<commit_message>
Updated excel products template for project defense demo
</commit_message>
<xml_diff>
--- a/src/datasheets/productsTemplate.xlsx
+++ b/src/datasheets/productsTemplate.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguelrc/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="24960" yWindow="2600" windowWidth="21540" windowHeight="16360" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -40,9 +53,6 @@
     <t>0887276149738</t>
   </si>
   <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHgAAAB4CAYAAAA5ZDbSAAAgAElEQVR4Xuy8d5xV1dX//z7l9j69d2CAGQYG6b0jIogNwZJYYokxMRqNGo0+aqKxxFgSNYpdLFEQRQELSJOhz9Cn997u3F7P+b3uAAo+eR6f5/v9/uXPPa/zuveee8+Zs9dnf9Zae+21tqCqqspP7UcrAeEngH+02A527CeAf9z4/gTwjxzfnwD+CeAfuwR+5P37yQb/BPCPXAI/8u79xOCfAP6RS+BH3r2fGPwTwD9yCfzIu/cTg38C+EcugR95935i8E8A/8gl8CPv3k8M/gngH7kEfuTd+4nBPwH8I5fAj7x7PzH4/w8Ax/LuIpEIsiwTUXzIooQgCIS9YWSDGVU8KQWFMIqioBV1/1YssfS92KEo0Vg2EJIkIgixc+rgEWux+8aO7zeVyMnvOfmdqsZe//1vT18be5YzmyieetD/B6B997yx51YH/04+l4ooiKc+x/oFoqD59j/Gvv9+/75/7vTn2GusD7HXmOxPt397D2K/jSKJcuxxBo+wGEGMyUgVERSBiHISH53uJD6x94KiKOrpBwqHwyiyjChANBxGI8YAEjmNcAyX2BFVomcB9e8AO1PGMSF8H9PT4Hx37Xdgxc4pyknh/VcD4t9h+D9JEP3+IPj+Nf+5L7HnOAnCaYAlSfr2/clBK337/Zkgnf597J6n/+/pfp/5HGfKIvZ/otGYfEVEUeLfjdnB50FBVWLgxhLrTgIuaCU8Hg9ms3kQ3Nj/EKLRqBp7E2NwY2MjPmcYJSLhsDsIRj1odFFEDciSZvAQRRmNzoAYY2LsBgjoDdpvgTjJ2JPdPP3+JLPVk+z8lrynGP3tue8Y/l+B933Gnhb06d/HBPND7X8C8Jmgnx5g/27wnD4XY/R/177t/6lRPohHjF2DwAsnCXkKpEFNEWNnOEw4EiYUChEMBgc/u91eQuEAgUiAUCREKCQRCYcIBP2D5zVRFa1Wy8KFCwfvHdMKQiQSGQQ41trb2zl8Yjuy6EDBhKwXUCKgEy0gRBHECELsNSIOjpCTh0pUCQ2OltgNY0KPvZ79WYNOqz+lumJqF/T6sz/r9JpTg+SkqGIdP82m00LWaL5ThbHffB/QM9XcfyXwH2Ls6UH0HWNP3unM68Lhk+bktOkJBSOn3g+eJRgMnFK9J6+NRKKD506CFRokUzQaIRQKfwte7PtYfwaBHbx/9FsynFbZWlmLImpQJD2qKGEL9ROJigQjELskqDpJS0tjyZIl36r9QRU9qKsFgaamJvZXh7j6pn8QxoTBZMGg8WLThbDa9NgcegwGGZOsYDKZsFgsGI0G9HoZjSyh12nQaWQkMYhOqxk8JxAdPGRJRCvFgBcGNb6gCmgkCVE6ac8iMVuGgkaCiBJBHgRYhFP+ADGVfYbJjSkCWT7bF4jde1BznFITMUV22naegmlQ2Ge2UDh41udwJDrIpsErY75DNEI0FAFJJBpTg6JIMBA+abaEmP1VEIgNTpVINIwiqGhiv1NOaqzYI0dR8QbC6AQFkSAe0UjU7yQSiN1WRNaoKHKIaFhB9Adj0gBJoq4R+sJ6/GKIsC9CMBCkz6fiCagE/BEaIqnoogYixgiyauHZKyKkpqQwb/68QRINqugYwKdHZ1tbG8er61h5xx6CRgFCesIEEc5wIgbZ9Z2ePTlC1SAaQUUvKuhk8PkTCEX9qJIXZIVoUEKJmtFICqEoqIIJWehCjoYHbYyilUiwhLBKNiyyHpNJJGoyoJXBIoaw6mUMJi0GxykAT6k6m/1snmq1mlNm4KSW0AgCJ63ld+37rI+x6MxmjIYG2RcOK0QiCmpYJBJUCYZi/okGj8cHagu+gIA/GMTl7iXoVfG4vYCeoB8OR+xEVC2CKhOVxEETV2RtZ4K2n8nFOjJSchA1Wkam5rP6zbeIL0hFNqVxzvwFaIJh9BaRY30HMZNIa6eXZ7eHKO+Zz6hCL6H+etxBkX6Pnn41SFQZgc5/FI88gr/NKyM7O4tzF83/VgP+DwAOIArfeXgn1efZNkfQ6lCVMETCKNEwDrMTv9dClGRUg5eg7CMYNWMQO7DLWlw9AcL6lJiORZQEBJ0IoThEuZZQpAtBzEMQjOjxI6gKXo2DqGhAE2w/Q40LaAXLWeCc6X0Oqndl0KX/9jexczqd/qxrlOjZnnjYEGNwzMmTUBUNYTWIogkRI5VBZ0CNCgh6HZ6BAKqqQdXrEP29GAxxqBEJk6QhpARjaggRiYgkoWq1lGhfZlRfKzmlSWT3tDMwEGZMvA6Ppw9/UhpJebls7m4gf0QxkX4f2j4ZdDbsI+MYMnwiPfVGBhrX0F1dhkZvBFMG9x24knqvkUcX7qMuECJXI/3vAY4IfiThbB7E1NSZLfKtwxDz/ES8ajoavRPZX4/QB8NNJpaNGkCrdBIXcTMqKweLrQ2touDzeej1DeCsFTjqzmGrWsKXboWIKQlkI7IYwRzqRRN245fNZ3nV33dtYo5LjLqDNhsIywIR6ewp2fdtsCQZzupLwCciyeKgs6LRaBGQCYZAq9Uz4PRgtVjxih5Mwkkv3x1VSYlE8UkawrKCGO4mGrYhqlpEZCKihEXfxwzL3wm3h2hPzsQoZzFpeCZXLZrB0b3bePy5v7H0gpmc8PXBgIjsNrH9aB1zSnJYUprFkbZqbBkpJHR0IuWOIcGoIUPp4YmaZJRuB7PytkF5De0Tr/7fAxwVAmi+B3D0e9NYnRj9lizRmPfm9rFwrIGRxp2UGI8xuXgIbk0+pJWi2DNp7+3BXXcCMXrSNksmDQNamWxTEKu7BnWgmt1lFj5rHsbGgTxcghGbNor3FKInAYyp37PZNzi9OOWVDzJYlAedkf+uicLZdjzGXlFS0GijyJooehlc3d14I1Ey8vNpPHKYc2dNYVx2Et7+TjrdLupavDT7LfRH45FiDqjYjxSzzepJBlvEekYqX1NoElh53nhW72jgqGpDiQiYA31cOGkIS0eqdIYD7DtQR5vqYNeJGjT0cNmChWRpHWz8eA1fH2vk3ntuo6XPh1+II0MbImNEPIQyqWnfT1OL/j8DHDPApz3H1tZWqqpqWH7XXvxGkINGomLMBp8tJK0qENFE0IZMBPR+tIJEIBogPpTIbPtazh3WydRUD/6x13HcFyHp0HH07iOElTYc0U7iQhFcCBhMEsqpSbIkRAkoGqLaDEJSClFTDkJ8PK7GLbx2bBxvu2YQ8vVjFy24EFGVTjSauLOwG3RszgikqIPTl5Oj4szpzpneeVRU0ftVfDoNEUUkOeLlsvPs1JQfZv+OL7nMBMdHjaAtdSwXDx1Ob3kjO6p20XasAr+7kXiNDo1oJTx0HOGgwED+EjxSAhpfNVIkjaBey3T7mzxzbi6fvvcGBrEPr8bKXmkkSePP5c7sNlo6W1n7z31kdnajDQewz5xE+KLF1G/djtheS/Gc8Ww/dpxf/OIONm74lBmLLsCano8acFOxbx+7vt4y6EZnFc8mLS2VRTEbPBhkis2T/w8AFgQDobCEydBNKBKHXQ5xibaV0hFvsDAznV1FCxFOiOTUv4zV34/VqOBSYH+tyi6PjfLeCFGTheTkZPRa7eDUwtcTRA43km3oYWaqlqwUCYPsJyqX0G3Nw9Pdze3l59IgOQiGJbSBCOoZ0Z9BEP8PABZlP6ovnojVRNRZwbIpmdSufZTlU2YTVzSFL7xObOiZP9TBfX9ai9+1g8XF48kfv4hjQRc2TxRV8lBdVs2xQAN9oUx6h15MXMBAVG5kXuI6rhpRwKF92xk/KY+gV6GquZfC3EmkzXJQ/ddNvLv7AH9YUUrX0MkE9u8gMOCiXUmhySRT3lZPUUY+F89ZiM0gExJVzOkZ+AWZgE9Co9cSVSOogsK+HdX/bwCOzUZ9soourGOKsZ1rR25gnK6Wg9Ouo79F4sKdr+JK68IVdrC9QcsHHRYCCTlMnjWOMRnJjE5Jxh3xEQn6CXhcg1OjRslFmhxPxC+yq6EJ16Emws07mJIXYHxKBMWYjw4vDxxewrrWUQRjjp8U+L9mcIQgmkgCqjzAwhEKza/cz8MPPsqDX+2k1pxDSWEBYy1eXrz3BUaOVLn15l9xtE/A0FNJomyhV9HSqTroMOkp9YbYXvklSTnT+arXzyTDp5xntdJ2YoCCJeNZs/Z50rLyKcqaQO7MEWx/aBMtYYXldy6ho2w1SVlxaB1TycwopHbbJxw81IArYqZNCNEheBAUmeTENKaOG09BRiZJKTbCkSCtPe2oEuwv9/y/ATiiEUiNaFmSWMGvUj5mILeYfw09n4fX/B5nQoATkpGyMi2rPcXMuGQKi84rwlHfykBDG59v3kxAJ5FtGUJKvB2TRkAjRLEOCJxQ+ug3qDirG8gtTqNw4iI2Ha7Av+srJlqamZemoLGm8cyJYbzSOZdOxfp/DXAAMybVh12pQt3xKk/+41HuevgTvKNnMm24g4xAF2Uvv8r5i/LIuvx3lL/3HnNn5rKrOZlXimciWXSMa9/PsD1fcLx8K1tbLWQ//iCZjRsZV38ETct2EkqKaWgX6er3cN31l6MZ2M8tjx5gbF4aF/3yNnw16ygYcQn+HOhpqGXjfzyNMERimCGLZP1QNBYtVbUVhBNjDlcHikHF5+/HLNiZPGUSKRkppKensvmbpn8P8OmITEtLC9XV1Sz/fTl+o4Qc0hIQBRzhDsI6BZeUR4KzE9Fm5ybrLi4eso6j+VeS4qunqPVTDKKDx49H+WftKH710DLG5CuwppIX9+5h8tBJnG+1EzT3IyYbqU5KHGSvmFGE166hcH8NbUNG0tO3D5tBoLTSidcd5esj5eiHpqJPLsC15j3mj2sjz6jy/oH53O26lKAi4hb60esSEQL+s6dNnAwDnmmDI9EIkZiDJmrQxCaomjQ0Na+TZ3Jx0egp3L9pCznnTyI1HM/weA91bz5HycxLMAybQVp6KxkVR2hecT2HbXmkdR6j7sG/8N5AHCkXXUBqqJXhJ47zeX0qbZpUIheNZf5kmczdH6A58iXnXnEJ5e++BV92kjEmnZQrRsGBbyj8+fOYDBH8m4/y+hcvsXLB+ayVLNS19nNeUQlFucnIqpfK9z4jSdUiJySwvu44wYEgHUIzGtVES+8A515wMxaLmSVLFw3OZganjTEb/N8BHNS4EVUNUigRm9JMR0IBj5vf5lepn/JG6ZPMK3+FVNMh2lwOpm8Zy+xFaTx+zSO89Y85HNsfx8VzR5Bijqcp3Ez/uAl85XVzzrBpxJ9o4zO5l6HHa+iva+TQuBSWzRuPesur7B4zHZM+jePZ8Vw+xc78PRupXL8bd5zIF0c6+Y/CTjRxEd45Noq7++4jFGpApwTR6Gw/CLCkiUXddAx4vJisNpRAG5G6di63H6EiMQVvg4+6cAn3XZHP3id+y5AZC4hmjWL6pGzadmzjkZm/QtDEc3vbKzzxH29x9zs3sur1rWiP1fDYOw/Rur+H9qp+NEcb+TB+ElsrKggrJQgrkrhwWh6X73+N3z74JE/fdRWurz4l/46nsKRYaXvpEz7eV8b9S36D6zwb24930uB3EepqoMHtY2n6BL7622OYk6wsf/Iu0g61Ub75deYW3kJF/yo215pJW7j0fw+wrPTSr8/EqHYSNA7hruBb3DnyIPcseoi/fPRbBJuLdS1x3HloKX/aMJxLDxWw5PW/cvfwQrKkbr4wpFJRoJI7ZC41TYlo16/hgeTX6O8OklunoWqgj8CAzL3pudx5UzoF3hxa/vYmyXoJrU6LI06hKnMYz9n/wPnXiogX3UL7g5cx8+0XyU8Jc/n+5XzO/MFQIpEfZnAsfBkLQERFiZBOxl/5EcNVicm5aby9rwVlwnD+ddmFvPTnq8kLRpCX3saQTB3hyuPcV3Aj7gwHL3ofY42thPzkETTc+Ud+dfsk1lb3cUduCZ7Efvrbenm2WkdB0jmM720m1PAFryhT+KpWwGoqJG1iPitnexglb2a0NZVjWz5jzb7jXDF9PGs7+9j4t/e40BTP1ddcQ8a1K9mwbQOHB5rpl/VMSsqnK9CKYaCTi3THeftwE3GJE5k+wcDmlon/e4AV1YWk0YNWYpFYwXPmD7l/8XP8cd/vsNh6eak6i9dco7jn/nEYPt7Nly1wy5AhfJrYTPaUm/nGXsbWN508K25j5InDHGwfQDknm+zifKSSftQWGx67H6vZTs92P0nKCeImTmX3V3sYajcRsUVx10lYPutGGKHjsG0KRw0F6KRqpnZvJiEUZGrDP2gWglgiZ0fcYtHg76toRRTQKRJ+WSRo1iF9+Xfm5Mkc8heROraQUfps2k48x6jKI3Rd+SQEyhnh7OLu3PtQzXHcf/RmPiqroNpRTKRgGcbrixmnE1nq7qTE8zV5gJRi4/PqBsq2bSNlzFU013ZBlQA1W0iafB474vMRGr3sOnqQSFBLzrRCFoTLmKTq6bS5aErVMyQtBa/Lx4fvr2XlgJWrFy4ieMMiDvS2o2tuIn6gh3f2lFM6JIVp4zO5/MqnWfno0z8McGVNHSvv3EfAKCKGdPhlH8lhHXFpWj5tvY1/XvMi19fcS6LawqvVeaxShvOb62dStuojFuszSMwWWT/zHGbW9PLPBjs3yS8ypKOb3p4o1sVF2JND9NZp+agln/TJxSToLDwb1vGXolXkm1M5/mk/Q7q76L18LHVfGhBcRpqCUfp9h5mddJi0bQGak9PYEJdPhiPKooaDvNqdzaO9vyVKmHAotuol4g970OkN365lnzTEKp6ogChYGDvURaDwPJJe/wVOxUOlU0YnZfPzm86j+NHfsa7012gT65mhi3K76UZC5hyu7ruHVz+sJCMxGymjmM5GN+GgH/85pSSNyWboHBsTBDf9L7/G8tIEDFlDqexuI9NoRY1E2FHVS3NjBht6qrElOBhhz2Wh+CGGjPH4jvbx9+P7eWx2Efs+Xk/iNb/iaNVO4q0eJiUUcjRk4POX3+LFG2fRnDCc9bs2cOmMoSRTwC8evpO77ruG+shEEhLiWbhw3mA07t/a4BM19Vx+596Tiw1hPbFAQCyq/JL+FYbkqAQSrYzo3ccXfjt/6i3l/lvP4+vHn6Vk2DQS47tZf+Es9hzsY8bRI/zes5mWWkgYH4+U4OHj+pFECyYRzdJi8XdR2dKJRZdJly9MXdwS/jTuBXJTrbR/UY+2uo+083L4rDaNzh4XU8zDOOzup6ajihW9m3k7uRTT2EsZVbGeEY3fkFPzPJLGiSTFYsBaIkHjYAxdlM5cPVIRDXYieoGEhtfJmvdrhIRk5KgX7VEDVrZz5KuXyA1ZaZ8ymiXmJDZSwG7bSOaL9Wx8/TlG3HMH/e89S0Z8KYGAC3RZdDZ56NXJhG1G4qdNJWVSGhc52hjefAxnVy3Jqcn0Cnbe+ccJdCUhpo++kp7ydxlTkky7R+WxR9/gZks9r1iHUGQ0c44tSHT3UUI3/ZImMQNP51EsSgcXZ1mxyn7WVHlYeo6VEfYS7n7kMf7wxE0cbRZwqzmkpqYwd95sZPlUgOf7Ttb3ARZUlXGOFta4n+GBX7zPIxUrCWj9jNs+j6eum8T69f9isS4ZJd/OMxNGEtxTxYLWHub3bEZnNpAzJZ+17Xl0xI1n5Agf+2ra6GyN0ielYDal01PTRubIdHz+TtzTr+av9ltISUmk992jhJvcpFyUxWbnAjadcJDjGGCiq5oTah5T5+2l/WAb+SYr8oEDPLx9Ei/5lhHWeLDZ9YRdMaBjc+UzwpkqmLUmZFsb6vHPaWvqQ7/iCiInWpCag1y+sIgZG/7Io5aVpJZoyHHBm+YbSU+WCf5rAqbL1hB9/jJSZ05maEocXRGVtmaZDEsS8QMONvQItPTXoM/UoyuYSuaIVH41IZHgobV8vKGSRUvGEdHn0b71z1y+/CouufsD7mjZxFvnLWRa8RK6i9Jx9aikBAQ6y3cSqdxH9pKJxBFHk7+PnD3/ZEA7nhEFdoZaGtn2ejUL/3YBFtO57C/bgs825H8PsEGvspFHceeOZHr85wQ0Fq7aWcSoixcQOP4x41tSGDZ7IbeEDlA4ORt/VEdJosDsT5+jYLKBhz6/AkNJDd1HPFT1JTIkcRhGOZG+vm4KR+ZyxYIp7GzsYn2Fix73bg591MaWO7ZjmZCFd38Q4ZMKUlbE8VbXUN55J4lwcSFZapglU2wYE9uZVPMNUW0f3ZU+pq9ZQdSYzEAQrMbYQmw4tsJ8hmctIEV9lGR2Ura9nNz8JAKWPEYlCSy1eHnw4y+Z7/GzM38O80IR/pU9m3bzEOY1f8SeKif5IxqxSGGSLBbmjoyjoiuIWQkjy1ms/aaOBNmEarHT0juapt460pKcLDu3gH+9/THLLp1NTnEm6serGHb7g9g/foGnNu5m7nW/JalkBg19fTTW7aJl+wEO7D7GFZfewiFVotGtRR1i4pxwE1QdxKct455kAy1rPRh/Poc+rQNncCt/fnwv9/zpuR8GuKa2jstv34/bpCAE9YyzVfOh533WLbmBSzofJOAt4NweB7cPycdf0ceQZB/v33Q1nR/5eFu9n4v32njxnSziunoIWXuplWfxwqdLiJc72FvexKiEVArG55M7ajj1LW08+UoFifV7uOE3E5hqSaHelMljv3+W1fcP4BgyGf/ur1H2d6Ex69EYLKheN+FwHx5vLOnMgF8bR/YwAV9XJV+PfJBfP36EvsgklHAIrUFCCCuDi/CosWwULao2SJFuN7uPiJCkIHl1nG924tVkM/u8xVQe3s/ewydIMOnZlXwlJTqV6j13YplwJaF9b7N4aR4dvQ3cZknFH99OSFPA0ztrKU0dR7nPTyBkJbpzI7Yx88kaOZFXVj/JdbfdS1ykk7qPHmTcH17isctWUCAN8N7hFtyWPchdI/jsoz9x2wNbWTFhDnFFiUTUbuboLRyzjuCbLh1mn5sybRL6jAy0B9fys7gtuDK1FDscfFPWyIzRS+iJS/3PAMcW/GNDPGaQYxkdx9p3svTWZmzeXl6+w8CM/Zs43qSjaHQ5Vq+B/Ip8Hls0iaptX7BANbH6/vk0bQjzrOdxBo6reI+r5D48HNMoDZJJxO/3sUH8C189tpu///1afF16ZuxqpuOp57j/gmFcdestiE4LO8VqZvRJeBxeTF8+SPvXWxE8euJHDkdM6SPgUXF3+UDnxZJmwJIaT5QAksUEaoCgswPxSCeuKpVfNqxko3Y2pv5WOuLM2MMyHqEQ1XcAg3YcQ7X3c6Q+HmtqIq62IHfF9fGkcxiTkup5flki9dECbvg0Sos0izHWj9D1dJLoKsM0dRh/sKgcDUJCNIIl1cC6HTKWggQC8c009lpxD+TQLmjISUxh07ZDYNFx4W+vpuPOC9h79escdf+VmRtr2bxlI+4eH0owyAsvPsXqV+HW80RaS61IFQJd8RHSjTPYY0vDvfo1Lr1hAeqat1niLGP+hHdwtmlImWHj3Ib7MOm94E4mp2jaDwNce9zD5j3v8ZDnHTqH6jA/3cJ7s1dwtf1tfN0hintG88tcExdUKrw10sonQzN4+suNTLbXIxqyiZZm0vxuFYn/kY8lJRY1ciJEZG7Rf0JibTJ/XnkbXz6ziKLJY2hv9zOQ2E+2N0L03dfIbP+GviQLwdJ0aNHRe6ic5GWjsBbkEl5XiWugBo9pCt2jZtBXXECwLYLXPYCihjCYjJh6qskIBUlr+hBz8lEUvZWX35/IvQ0T0IV6kGwTCBosFPXeR2NfHr2WAqKuKlYZI9ympnGB0MSn0XkEp8zEe0E65/XUkLnhXb6+5A4SBmD82v2MzHOzcOhnNIV6aWoy0dPZRW9+CgM+P7IuiT5XgKAvgy3r/HT80s7irhLMbQ+RMukDnri/BLtf4YmyTxmRnERcOMBfH/krIybO48Lls9j58UG2ff0Rd914Py+WuVld+zXjq/sQx06kscdLor6a29NK+DLQS9JrDyMWjuepvDup9upIzznA/am+Hwa47fgxZt77PC3yXo5deznxr69BnK+jcKCB2xpKWHTpcrrefIVEycs/rvgtwzeu5s+GfQx02fGbR/NqSje/Fxx0xPWReTGEbWlI3SpHtMU8+Ys93P7WA+C1kGop4cjxfzFh+9No20UiKe0Is0rofmk71uszCHZosNXItIxZSXPWBHrWryalZx+ZQhit2IpHcmOWAwRjuVyiikkLA14bTRoFfXIC+6sEolOupKgbRvlX8fSBOTzVPRUPpWR1/QW/O4w3LQVz7wAPR108pZe5SojyR/dlCHYvdt0Grp57LpYsgTff302jeTLxly9lZm+QhK+2Ys5oZP+BD8kqHU6SMUQ40kpShoOeztFs+FzhaFMDw+6/mcQ3/8b5505jrryd6Q9u4GdPPU66OYeROXqefvB5Qr4gy5afhyNnKlq1jdFF53Cio5HH7niC0Xlj6LRr0Xt6cQxPprlawmC3kNB4jGX+jzk85gGaj3/DpIbDHCuYQsb09B8G2FPTTOkz2zlc9ScSckUqtcmMH91Fl0/DqO1juaM0yrTqTtrOGc8D+mZ2BSrRHnTiK7Dw99SpRJwDXLJUpOIvNVxwbyqGuGbCCclE+7x8zO+YnrKIA1/vYmrVO+iqdqJmiTSrASxGLZ5iHWkVcCzrZ3RpHdC0n5yuA6S5j2EyqMhaEU9Y4XiPSGWPRKNLg1eJEEt7Mwk6QiYnc9McZEcGMKWKDAgRuq0Oqg3DMSkpFCtelu+YSfuej1CMQ+izJlEc6ecyTx07tf0st2ZyQ/9sELUk2z7HE/aSnmXlgkt+RZP7GJ+8WI1/9mKK555D0b46LIf6SRvzNYJpJ/4BParGStm+NPa2RsgqKSHJ1cu5ceX8boOX5R07sT7yBJ0umZRUC5Xr3uFEm5EJY0dz25XnsGvrVjQZw0mPSx5MbtfbwtjkVJwN+ykaFiGFFBpFPVXlG2n++gQVbTZy3XvwmRLwjFpGxcFtXHbZeT8McEP5cbavXsNSZVefwh8AACAASURBVBdJgVbqtGkkDW9E7jEyoymThwQP46ICncPOpUX6hItCLQhdqdxnLmJO6QCrqnIJtzVz+5gwCeFOhv5sGIKukmDEhCgYaNl3NQmbH8CiB29hPt0DTWjSewg2Z7Kr6BaE+lrGOHdgqT1AUrZILJftoxM29vR6cWSPYpecy4lugRxRoGDCENp8QbLNSfRpQnh97fT3+RErDbSJJ7hQq2GkbS/DczpwmxKRyKcgVeSDF0Se8KcR0OmYhUJmr49eS4DiZJn/6L0Em9RLguULpKiWsBLF53UxceI4Zs+ZRXn5AdZs6EWzeCVjSvPJ21eDprWGcfltbGzaz5ef6RAnJ5M75HzO3XUHXanz+OC9V1FyRjDqhl9hELwkHNnA+g01lIwtpr/dC0KQay6/kFHj8uk9dJAKp4bMvOH4IlES0ixkWSDJ78Zz6HW6TVn0t9RiczZAyM7xtk5aq7pxZE8mefGcwYyO2XOmD84cvs2qPNPJOlrbz8jeVShDh1K3r5qvT5Rzt243X7UMxW2+AOux17AmJnObLo+dQz+H/X4OmpNwzj2HR8oCFCaMxR108/spzbStOsHs261IRQHkXhvOt5zYq/xERrpokGTsKf0EA4ls1l1DQJQ4Z/sj5CfoCAddbOvLYlMjNJrHUjptFFq7ATU1l9o9W1l28RQS7AY2RfcziTya/EGydA4+bN/PguHzqO9rIWUgkTpLK0c3+eg/WMNYwxZSE08wPy0JvRDiH18O442jo1gR38GeVgMZ+U781ilsahlCnKGCOGMFoqontuwsxhL/vG6iSpglSxaTMKyIXZ9sZWezhazlFzHJkkhqbRur3n4RQQzjmDEH246nGHXOCsbse4QX+uLJvfJK/AY7hWofbz7/AQunl6DXRUmPiHQ4pnGgR8a09z1+c8Mcxi+Zy7927MXZ5yUpp4SmHj9D8/OYkJ9I57v3Uba1nKt/nooJL3aHQjAUx/pKN864i38Y4C/rykh9cxVrii/GKoWJOnt5Z+12tB4jTy4JUNDezEszR1Na1cwV0k6oyebNrCJycwZ49dBo2qw+8ocUoztextXZHWiczYw6P5PgS80Ykv04Z4tE1mswTNaws3YcW8ZO4mdr32Ko4zgBIrx/VODtzgzSp8whPKYUh7OX0YYovaNToa+aAmsux3QmLJ0DqB39HB+XyiUuK+ECM183NDH7788wzJBAh8aD1l5Kg8GGZ3gSXWYTa3bXMbH5WX42QiHPlcySd7M5X6fjyd5MFg/t5iNxOa7WBOIS3sYuu1FVPYGoE4fZgc/nRtZIBIN+4vU2Zl+5BJ0Ux7uv7aLFn8qKUR/x6r9ySL4oHfqT+J1uB49tEciWKgmMPRf3sGHMtUd4/S8vMzzZQunYImSxHyGQQKN+Jq373yZt7EQOHN7NmJYmrr98LuOuWMbnn22nTTXSPCyPviaF4pR4Zo5NRlO2Bsexz7CnyDjyE/FLLj5qXfjDAB+pPcE5t1/F5j89SVxB4WD8Nt/VROuRHrZ+8CI3d+iZelEa70e+YORxicMeAc9581l3oIOG5GLypRTe+qaDiZP03DuuCuW1/aRpPSQiUz8vhwxfL80dCm9MfJCxxz5mftsWJL3CzlotP9udzoqbzme9WMS8EYcZkTUGj9qJwZCNXNuKR8hgTI2TsXv+QN+AH9fIRO79pJKip2/DY09lun4CM4xfod3wMgPRCPo4OwaDG7kvQuibIPpOE7dO+gXzajYwcsw3+BsLKNsYz0NiEb92tHNXYBYGzzgcaQ9gw0pU0BMRnchRLYoSxmDU4fV6cOjNRLsEjMMNXPyzK/F1dvHM/Z8i6wtx53RzUeMH5ORfRPWBN1nvmIN+0TyKY9UOB8vobK9j0aLFEOhA9ArUxq3g2OEvMcohslMK8IseXFGJxp5KcstqWDhrBCsf+Q11W3axavthNBOvosPUhNIusnzqGLIcVVQ/+CfC4y/CZJf/e4BjtUm99d/Qds/T9BVKjNUk8Ub9MZrs4wmNncyIugoubqxgYXoGtcM2Ytqg4YvcoaSUmtnS2s4R/2K+dCSxCBlF18w5ngjX1P6DUIadgZwROCbJ1Pz1AM/+5htufrOYgqiRJnOUX3+eiW3WpRwUbNx6w3g+f/8DkhYls9Caw75umZFdIuc9eDcNBd3k/m4esjWd8O6jqGYz0tyDOFdnM5B6KW3ZPsb01KKbKLDu5QgdgWw6FQ2BTjd5PSeYm1VHVr4f3Xo/X4/NIinDxv63eninJ4VlqQPcWrcMS2KYeMtGYrkiYcVORHYjEyuziYULFGJ5fLrBlFmVQCCA1+slZ+Z0Zk9ZQdghUXbVPBbN/wV/WbOJnFQDrQklJBWlU2gI8+nzr7B05nQycxLwRlpI1M3m1eZE0nY/TnDSjRg1nYOLC2I4TF/IgdWcwb6jZQSP7+Ta1HRuePVB/JKb5bc/yeSld6MPiNy2Mh2Pt5t1L28nudBBVlYmM2dNG0z8H0y6OzPQEQN4j6uaTx5axyXBQ9Q0VLP8zivQpQ/gF30EDHO58097kEtreK5/P6YDTm5KOYflWSJbh1/Ap84EHsqN4NSbCGw9ys+r/ompwMZm1c+UWRIfVt5Au/Mwi93rSJGjvNGYQvnAcLaNv5Ybrgnw6rPrmH/lBIZ2JHLM5+WS8gHi3nmUhMeL0SUU4fAm8PjWI+yMLGFGUQJfae2ssj+DabgF08E2BKdEcEY3OsVKIH0kr69Koaa5iySbEdlrwWRtIBDQ03xoH7deYOePwWOM7krm0efgktJc3my9HtG0HYdpD+ZY+axiJiL7kGJVCoKKIMbi2gpiJDLowJyuJdIpMj6fysQbLiVHVFj7aQWN697HPGYyppEpZMUNw+IJ4HLKFKX0kODrpUA3mWdMI4l+cBfmeVdhDB3FbnAQ8oAiGMESJSFi5mB5E/qhmfhd3Rzf/BbXYua6j17AnJvCZTffwJN3/Z7nn9zOxdfFM9AT98MAK/U+Lr/8MtbMa+GRNisjs8bhuOVaOrwSOp2HeJOTt99/hj0H+9kxJUDf+Md47cWHyCgo5dm96ZS9fhGunhDD7rwI39AAA6FUbFY/txY/zLTdT7EstQG5OcANu0cTmTofRYojZ6oJl3SCvJwC1h8Lcm9VA+ayTeTfJGIPDKe2MsTfu4qZVDqFnNBuavDQ4BSxm2y0p43n6ri/kVjkIWG7FbWuHXWlBaJ2wgMj6N3YRHw4HtWQTLf+ABafmVadk7iBEuIXb2KbMJOdZWF2v+Llc84nTf4Io7YLvSygqJrBmmgpVqwTY7AYW2FWiIZjYc+TJaGxYjtRKxIY6CZsMhIRklh41TKEsAWxs5rWiJ22Tz6hOzISIWsaC0pDDA84ebdWpPXgJoYUZmIKquh1TlKsZvQ6LQ2eXuyJI9hTUYc1MZWoRsYng6yxo2tvp3zfh1xrNJD8sxtZe7CVX46r5d2DPi6aP/+HAa5ubOCqJReyZVGYss5EBpJHoF5wBTnmFlTZTUBj4q7aTWwaWkiOay2Hh16FGi3kn+91Mm24lnmzr0S8cRg2m0RVmp78YIgrp/+Bew59SIlzL3XRKH/eU0DLhOtJH6thuAPq3FWoYjYl3VqyVz9D8nUCBZJCebWR1cFLmJOfgCFcTiis0K3acWMkPGCg3h8hI1FizugUivesJZJkISFBxt/Vi2mRDzXQgpyYwoHdebz4GfQY9Aw3iYztD5MrfE6hzoDGkcqJAoGPmsw8/MJcslPXo5H0iNpYdn9ksFRFOlWEO8jiwbi2cKqG92SJpivgJaQESDI7CAWgU1EZnZ/CkHkrSAq5aWwJ8fHn27COXonkNyM0VzAlWU+O2UOV0k9/w17ml+Yyb3wB+3bup6Yjmc4Ohe5MI7U+J7nY0IREfBoLNQ6BFL+OQ1v3ML1gKFOnVdJpOodgfyujM4b89wA3NDTQWHOCcx/YzC89r5BSmIV48AjXH1iNTu1HCqrIqpG2E/2kJT+Cs1GHaEvnUMKzXHLHRxx8ahGBP/2W7PqjeAoc9IrdPD7yQX7Vu4Zh3RUcdzq4oSUHZcJFLLokhcrQUbS9FvQdSVy891VGJR9BHTkc7xYnzwhLiE+PMsGh0NYtoiToiAg5VHtCpCQHyQ3UMlqTREK4HTHawZGQGU1hFaOLC+mvbELfroHpVjTRfmSbQHtHHgfqFgwuiPerPo56k3DXnkBu38fkpmYmF7Sx2ZHJdW+cIF0cRsAWQggpmDQ+wrEylKhMRIgQ0QTRCYbBIvhYukiMxWJEQTAZ8bvdaHUimnCAECZ84QD5k2ZSNKKQRq+B5j6JhqYQIY+G0pw4dM11zByZQLGpg4DQQtnWeqaVJlJX04rbPIQmby/pZjOI6azuaCBeSCJB8CNqxzIw0E62dR2OoTMI2XQ0Hyhn8fiZ5ORkM236FKRTJTtn2eD6+npqmipY9lcLiftW8LeFRo7tCLLkvdsZlmEdTDYPy3pEux6x6c8EOzrQyhl8LD7CO29+ylPnSTgeeJPoGAOiNcjDaXcw1/s+47pbOOJSuWZgLAlTVzI/o5cuSy1io4m0DjOzKl8mbkKITI/KC+2LaEi1MNUBziY3gbg0em1apIBK2tAEprqaKOgK4zP7aY862RLJZr+aTkJiIj0McJP5AwpLTeiOiATbnQhTE5ANXXhDsRKVAj7cPARROxRTfAiLIZ4UYxuHqsM0NX3DbxbsZcDfyPVPTKbZ2YnOlBMrf0On+tCqCtFYzogURTq5PnNWUdtZJ7QCAZcXg2zA7Q8g2+xMnr0Qe2IqFbVe3JEETrR6SI1LItoSplDfxYx4P8WlEpu27KY7IJCfFY8a8tPqkQnSx8Iho/mm10dLrRm3OZO4psdImTSOnmACtiQZwRekNDWL/Px8Jk+Z8N2C/5lOVgzg6tZKrrynm0Drap4+p4xjncUsvKSAGVfORIqNVNFAyOxD0/BPgp42NH0m1kuX89WGCA8dfgWbxUFH6QDrnBeSlNTIgo4vqPSI3LZvMYG5M1hY7MRj6WftjiMU3lDKde+uZs4EJ8E9Bi7rfJiVKXvQeUO0+e1E7Bq6gj6G6uOYnhrFsv8Ijjwvtala3jueTSh/MjPijWRZLJS1dONp9lCXGcf1Gf9gWKEDsTaAprwVFibjN/jRBl30i/m8smY8vRjQkoQnFGZ8rh5/zwlGL11Ceu8fSUg9yl2/E9jUkoFFbyKkxioLY1ALSKqBYCRWKvpft1gyul6nx+v1o9ebiFVJ93d34sjKZuL5lzIgmOkJ6DnREKS+WWBI3mic27exYqyd5sZ9DM1WqXM5SY2I3LzEwu4WP9v2BkgxquwIXYpw9GE0kzPQaIeRZpbREGJ3+TGuXziX/Pw8Jk+Z+F8zuLKuiQv/eAyD0cHcgRsYl1VAgaRl0cu/JhAKYBYtBAU3uua1yHGNRCud9GXZaHo1l+JDOyDNx+G2JI5MWMrFvE93vZuLO6Zhu2QlGUkHGZ1bwgtvfsaa/EmsCJRxQ6iWa5fWIUenMF73TxY8eDs5qUlU61XMGi0TFZhsbEBv99PY5eP6yExGJBawvDSLnnA/jbXdNNU1YzaqNLcGSU/T0W6dxW/zX6C4IIDaEiR6qIeBJZnER3UE5Gq8Ujr1zdfRp9oIaVV6e2SMrma2Hm/il8sT0Q5UYE/byuENIR58z4A/okHRmganSBoxiirEym2+a9+vWAx6PWiMesJRFYPGgN/jx56QSHtXN+0eD5PnzWPOxMlUtas4tTo2l/XgcueRm6+j450a7ljgId+uRTOsm7e/amSJVWbqiixueWEI4fa3gAbEBdeTGA4z0FNFT6uHYSPzmZWZegrgCYP1wSfLec5YD44xuO7AYS5+6SAmZQbUX8MT0yVM9SaWfvUQ/V43DslGwO1CaNsMqfvRNnUTrcnAvWofdl0hBF1c/evPeWDPGDLdUW7cP4HauQvJSq3m+pLZvCc2MaVoMq859yC42xnRPImHCn6J0C3Qnmrms7idVNzxAFOS9MzOSiChdTMuoYcnPdms04/i/WVL6OjycOCbXUTkNLr728nPTyfNEY9HjnKktoF4NZWOUivLBp5j4hwRbU8Wwic99K+owxFKRiCMTyNR77ocwZcHpqEEZIGWjoN0VAVYMKudxkAhI01LCfbP5OrbywkbxuIMubDZvCgh68lNUGKV/LFCuO9VOUYCAVStjKrRDNpxJRRCb9QQ9YQGHTZf0E2X28iv772VbsVAZbcP2ZPLuooBogYdI+MSaNxVxl9mZaJGj2MpgY2fJtJXdwBHQjWGixej2VaPL9VKT9hDMJiIQ9vP+cOGUVCQz6TJ478D+PQmLLEKw6qqKiJNPUy7swVXRE+i6S3OS29mfH8nl3/8KKaQAyTnoLOhiBF0dX8mqvPh/NBI3M4G2uem8Ij4KPf1PoTDVcUde1OpKrmK3AJImWFFq2ax4M8PsyJdYOnNF2NqT2R0v8r8oufQ6dqI9mexRXstshRmyGcNpDeu4g1lGQ9Pvoon8vuxxWqddu5DQU9XVz+pSSZyc3NPbm0Uc3b0enz+ARo7nPQHHehTsrlR+woZUzwIkh3xSydqiZlAXhfGvgg+xcQ7x9J46d00+nWpsXpHks1TGJKzlzGlk4hP9zNVug+TZgOrnprNS2WbMMbNwxjuQKNPRG/tINidQ0R2ncXo2B4cZ7P65JZQp7dMin0X8riIcyTgCcNv77+fzfsbqPNKyNIQtpV3oaphbJY0kmr6+d1imTVb60jSf4U3L5fqLhPJ5gBGjQ6310+bN0JpfhzzcnIGGTxx0rj/GuC6qgHK3roT3YjFfLorDM1/Z1GqxB8+fBEVCdXfS0Cnx6T2Q/OzBBwmuHQfvSla7F2JrF+wgCXSy+zqSuTFvoUEMxIYOT1CU18fP9/4JePGdLFltYH2q69kTIaBIWnbsJs8RPQ1aA0GAh9fj7ZzC42uNlYOv51JnnR+Pg52nDhCzXH34M4zBYWFWO0WEuNt9Pb0Ims0GA0GHFYjWo1AT7+X2nYPbVEvknUs5yt3MG6JHm1HMpGdbahpEeQxdhSfd7B+uMGZzKGDcxDsvdQJnbgajZQfh296jOi18bxyST9jx62md08dl9/lQM7ORdVH0QjZKBxDUs8uY/1PAH+7f9jJ7ZgGAY6lECni4B5XfU4XhSNKGTF3Pr6Ann7BSHeDlQOdYRRjNlPD+4jsfp4GQw/mwnmYRANioAtnVMARb0OypyL0N/PzieN+GOBjFUf43QPlXHNZFluq7Vyv+QsH61v4zYN/JKUoASQLUa2K5Oon1PoBYrAPzR0HCOXHM2Xic+ysWUbYCjdWjKc6I5fSG9OoazRx3ocn+EVtBfJ0P8d7w9T6zYy7NpskuQq3kIhJ6UbztQTjooTNAYrK3+TO5FoMipNjVWZc7VWkJsSRPzQPrSFWdR9bZA9hs1kH56IaWYPBoCcaEWnr96KNzyAUSeb1tatpGAiyfvER0qZ40YVMRDcFCMf5EWeH0Peb8Wmc9Ak5PPbUaOIyUhFVA5lJvXT62qg4qtBlH849Lbcy4Y/T8Xi/4pbbtfT684gYBczmDILB7rMZHI1tA/Gdpz24qYtyNoMFWR5citTGdgaI7fsRUojt2rBg3mLGTp/JmhN1qAMOhujTcX36FufoN/GuZgWJxXF0dRxD6bdjTjWhjRWqW1Oo+WYbd192/g8DXHn0G257qou5y1NYs6qXOzI+JxA4yDlz5zHv13PRDFjBHoKgjWjHLpwbXsW23Ul9IIOesTlMVLbwal8BL3SWYJumcmFOPBV7VB6ufAl9XgL3955PezDA27fvZ+sXfqYsjI8FiJAiPjw5fegEE9G+dF5QV9JTlYa87StUo0pqcjoJCRYknRavP4jZbMUX9JGUlDQo3BjIUY0JSZdAX1Dk+XVfIUdcmOUmNC0J7C+rouLuY+imDSOgimg/r0dNyMQ3qR9LyE442kY0bjRvfjYP1aTBH9ai97mxyp0Yk23EKVGmPnczrufysenNPP6PftZtNiI7rMjS2RUVMQZ/3wmL7S5xpoqO+b4+IkTUKDoF9Brj4IxB4wWj2c6sJUtJVcJkafr4os/Jdn8qjsZKerwW/EYf8cYUvL39GIxBtJZktH1Orl8y7T8DfGZe9JEjRzhacZTH3qjk3EUlvPhGPWNyqnnRtYoPLYXcuepefJJjcN8MNEGkqBvlxlsR+gK8XnwPi41/JEFN5sqjY3CbZBKWZNPV0sArFZXEOftYlTIe74jz0Q60Mi2zHGNkB9aknP+vvTOBkqq61v/v3ltzVVdXVc90N81MA6JMgihKMIqKRo0TzlMc44SJmqhxiKJJFMc4xDmiYhJHREUQQRBkknnshu6m6Xmoea5b99Zb5zat6Bv8L54v/8Va1Fq9urqqbvU5+zt7n3PP2fv7cPXxGCWcmt6KkqeiW1zIVie/D77EgFVLjMrBovxOMloegaSEz+2h2CqRczhIZnUKnCbalHK2p/L4fMFnODMhpgzNJ9jdzt7uGB53GT7Fxyevv828W3SsP7NgsxSRXNSGw6oTmubDHu7EItlJuopZsu4omsL9MUkSZjmFI9vC6KTO7p+P5KTbf482PYl5IqxcqnH761ZUuRSrM44jpaErbmKpIA6xbW0zowmiiViGnKWn0qD37F3LCXY8qYeyMScRNGvGqZUpKmGV43S0ZbluZAr39IdYbbGihVpxaU5C9S0Eg2H2+NvJ91VgUzSiqRzJ+q08eP3FDBjQnyOPHI0k6Kp+WF0oAN7VUMsbn9RSVFTAjvUBPN6d3Kp9yrwuG0/MnU1WVBrLMSMLwZQOo18zg7Tu45VjL+Sa2GNsbnFyU3wUR//8MLoLbJw1/2NOD9WxzV/GC0fNpKLwJbTWCiLZSmZO/ZQNq1OMPseEFPOgmKPoih/FbUFNeGhwHc2clouw1y5ngi2PhMOO4rCh5DRwKOSZrGQVBx+lRrB++ULyUgGOHerAmmpnd6eGKeekqqSA8r5V7N5VR3dngPSbn/Lnu3IkjtNxmSrQFrRjTitkzhyGam5Fi27Dmz+EdVunsD1VTk61Mzr7JTn/TorrmokV2XB1abRraXwxM6Y8na5MN4trC5mruEkkUsg2D3ZZQUmmkW0KoUwcq2T+HsB6TtBQ9IArdrjTehprNISuD6bD18kdNPNmykmH6mPilEvRRw8mvbcVyW6mT2Eh8bZOGmt3s3dvHbGsHUcsxMM3XPjjANdvq2VMdT5Wl4ll81+haedGJltitOwOMe2jT8jFQwg+DZHJKEeCSFfdwsaC0YysrjXohKZ3HUfu+Em4pO1Ytyn8rW4h8UqZE5pO4DfVnXS1DGG93cY5g1Um7NxFYkwIqy+Fp28+ip4lk+3GWqCStGWw6oX8M3sLmV352FIdlBU6KUAmKjZbomZaykfx1w3N8PkiZpxbjhaKsq4+QyDpoLqfnapiN3ZbPoGon/L+FWzYvoVUByRmf8JDt8ZRj8pirRhE+p1abHsD5K4chmx2EpMakdfnkWjcRUdjms1rspT2zXJ4spzuikasTh/dqSJc6Tj2zizdzSHKTEEKqvpyb5edVZEcckkpdlXwdqXplhPYU9/xWQrPyoojR13wgO4DOGXHZW2m2+4ivquSmf3n8cfYCdidGZKNHdgdPgb94kzMFcWYZSu5UBI9ESUWCbGlpp3M3gae/N2vfhzg7TU59rx9OUcNOZKayG6CYRsTcjHM8RUc/fcPiJm34GI4OVE10N0Nv5rBR8Mn8svy5aQ1hamNU6FoNXHPyfyr6XO8JivLm0cSHBrG7e7PppCLwfZmpvlTSJ4NMNVD1xdWBp1vQ0pbxZ05Obkd2Z4iZSvGZlK5JzufIzYvp9SVJQpYSo7hnQ6Nua/M5p6JBfh8Jmrbk3S3S8QzLfxs8lhK8spp7wrg9bmNbcOcxUxXJMC2vTHyLF7kV2bx4HVFZKfpqJoV59I2unbWYRpXTe3CPXy6IsCFZw+hVO5g+8ATuSh7Cd1HHY2pC6bmtTJ627sMLymgLT+EOzSWF00Wzpz7Ir/e9R5zC8byVFcIzV6MLyPh1yPYsX7Pg7OinwY/pQjdMnpOJyt5CKZj/M7dwZspF5GsCLNeTNkkaZtCMirywn1MPO1cKComk8whqOrqd7fS+NUXzLr9iv8McC/brFgAbNmyhW0hnfRzVzCiqpKtcozWQI4SvZ2TYrVkr7wP16jRFDi9qKLoelc7kbvvYumkIzld/YYtBYVMrj2OG6akcK/0cnvsH2ztdvB7x+lcPcrFotUr8PWr4kZbf4pCcxjvuZJnky/R7/LhJJZK9D1VJVoTxTWoBCm3l7SnC0tE5FYN45OWlziu8yk+7HMnz8z9jJ93ruXkSRV0d2bZvqsZkx3GDRtCaVmZcdidzKSQsRMKRbHnWQlmErQHg/TNs+Lv6KZWGUj22Sd45uIEnsF2amtDfP5mI5eNNROoTvBI6d95feIZDNzzOTM6NnPOyCTW/gGycgolFyAlqB7F2bC/lUR5GQ59GHpsEm3L3sL21Aouze8mZz2FXGcHIV8Ca/aHfF29BKQCRBlLykR7noVwzSbuHpDg8dhgPFYTOUxImmC2i+Jw5qGJ1CF7HgVVQ/AOnMi27btpbFexBZt55Y8XG4cNYg7uJSP8lk5YALx582aW+lup+NslHFlZTb3ZQSRsIR3TGGLew1fOKq6971oUs4JuU8nMX4o2+1XWnyhzbCDDi9polihuOtUkf1Z3cmRDhhdNR9NncD4rapuQXZXcWeYjb/crXFT9W4rEyI6kePiMFXy5tIHjpx1BwtKOLeUUzJpki1uxyP2I63GWWGYwK3guq194hT8dlyLWbUGcfqE5GT7sMCMVNc/uwh8IUFhcTKe/C80kjgc0UqEEZt1EntVJup/TyGTs09DGpNK1+GtW0rzJwvhyEy/0O5LXzr6Hkk4nMz6/nkmT3HhcSVy0k0upbAtFSCcU2trcbGjWCesFWC15DHDsridXLwAAH+hJREFUJJMegN0bZugQK+OPquLRy5fzWtqB15TAI/uI575Pmdiz4OpZZIm5WDU7yQY7eLGslQtai/DYLOQkG4lEEoc9D8GhKWg2o6FuPIWlJLMSutlOMJomIRfjVBO8eO81Pw7wzpp6qufdSqb/GBpTKnZTli0tEcbLdexQBhAsGcidt5yCYAgLLloMn3yIb0oEfYPOIPko+h+3l/IvqnlRXUSyu5AH+5zML9zNrEkMZppnPcO3dDC7z9GsHlzGqNQ65m7VuWawhWkn7aZuaY6hJ5djSWbIamYo2kFOy8ds0kjZKxn13B3clJnPJr0A3d9O/9HDKSvug5kcnjyr0elAKIgzz2VsfrS3t2F1uY1cartVwZzL4O1uZpKvFm8uSXzPDnKdHl7tN54Vx1/GURu+YmxgK0eOWo/TO5Bw815ynTlWNyZYHbIQVl2osTRRbz661Y6KhtWcw2bpRzq7GmeuhGzYSzqymVOOH0f33jSPf1rLMMVO1Px99gGRGbI/wGlMBBpUHhtRz5/85STNMmZdMhhpBduew+EgFhPVE1Zks7WHaVeNGHN43FJGOhLm6btv/3GAt3zTzcnf3Ehj/6E0BaBA8tOuFjC8cyv1UTslUy+g8ucDKfGkDYrcpU8+ji/cTNqv8Vi6mok3O5j8TYAJDbW8Hh6Fd/RQOro7Kav0cdjqFuSyRm5xXMNZgzbS0uqgY5efzmyYl36dYfuqCCOPq8Lm7iAecKPkBTAXdpBO+rBm3DSbXNy7+RqKa5cypN8o8h0eg2FPy+YIh6OYrBYceU66AwG8hQUoOTMd7V3061uIM9nAEC/U/mMx3oK9qGqaPdWX8uW4yYxs62S6dzvFFU0E5SCuQAtaXZC1Sz0sCndRk7NiceXjcPho81jwhm1G6q2WDJOKBTBlg5AZgOxKIRW4SKU8lImUH1eaEl3inYUd2G3fvzcW1Mzf3SbJ6KEkdw/o4sZGN+U2F0kU1EwCm81BPJYymHvD4Qh2Twlen49ooJO0quKU0uiOErLJKA/efvePA7ytRuX4+l/jII+tneCWuljUlUezvz9rtA18+OoF7FkPg0c4UeylOPOSNH+5ho9fnM3KuAfzOSU8Vr8XW1OI12wn0KfKwtpgkjvTAaz+VkZXXcEd46PQZmJjw2oyaiGZlJlfHuFn0rTdtD3rwXeFFa+UIptwoFkDmIviyCok6ccjmd9Q9Y2brLoXd54T2a6QjKWIqTm6tRRHuPrSINdh7rRTMLiSeFcThyc24GpIU98wn/HjRlEv9WPDtN9TvWs540NbsJxSgaLWEYuswtwcZUedxLI6H18nw+jZfMwOBas9hzUkyLPddPobkC15oDhw5xWQcJYgJdtxCgoJPW4w6CaicUySCZPHR4U1w4KlLUiC4FQQncoh1JwJt+IiFYuhy3aKmrs4a5jCs34zCZeMM2ojJW5FTeLkSpCeJXE581AVi5Hsp6XiSHY3pGLIJhukEzx0z4MGwOPEHLyPvOJ7p0kbN26kvtVKydeX4E4kCNurqPfn81bmSFwJG8Wxl7hz5vXoaz9kwAWXkNWTZHIxUqYYeqyJuiUpZso13P/GZnxVEq+XXUf/phW4fBbG7+hkm8fDtikDUQJZos0RwkkVT1lfGlu7SEoSsy/cy4aGFIWDJIpNskFzJEtpY+dMl8IomWq6LDK/055j/KrlmDSw54lNC4WY2A7c3UJjXzcDTGXEkgEqLa0Mqv+YPbUdDCktpKbQydZhMznB04708muU/mqQkVMsyQG0hjUEaoO8vR7aVCcBxYMjz4aajKBIMolQkO6ODgryPVhL+5BRPKQyJsyyydg6TSRCBi2jWclDMcuY9Ax6RtD9KtgcPpSczoaV20h1e8QRHolcG8UFpeimCN3BNDf1zzK3xoJWnCHi6IMtmECxmVFMPTT9JtlEMqNjcTsJRyJGFondbidnspJMpFC0NA/8/l4D4LHjRv33AK/dtZJ+789m+Mw7eenRl9m1dxsXjSjjpPwGOiePZstiB4GtGzn5yYvId40gkanHqTiQrS20tye4JS/K2Jvmc+29MV7a+RzDt77G+F17kZwBRuTN5KUp2wlu6mBHZxTZYsPizCcQjrG1JcDzR3sYNL2GNY/FGHN1P+REHFWPo5mT2HyCgb4bOtxs8ozkw7o7sWz7giKTjLPYa8yJOVOGzWsbGTvEw/DwHhLrP0Vv1SibXMVrzuPZPeUybn/mPiwnWxj+s7sIWgrIz7kMIZJg0wr+9OIsuiUdixnyLdBVsxtBNZs1m7F7i7AXliCb7YQjLeQUJ7rsIpUWW5CqccCv6UKww4JszycZ8uMgjSJCqGxFMXuxSVnc5gBHjtZwhmDyL59mbd1mvlj6PERUrjr/WUoGD8OatpJRcgY5gVkM6N/dxoMPzeTiq69jV/MeItEoqUiM9Uu+YtHXq5n5yF+QcioP3tYTov9HgGtDX2N+bDFjH7yQPl3LUW1NLHwvQXLVSs69tR97Co+jub6TceecjSsYJun2odnbcMWLiWurueDxF3n4/vMZtnouMzedyI3OzXjfsfNRgQvb5TprNlYy2pplQW0b5ZWVZLM5gxM+3uxnXluErdc30dAl4ysvwpGfxOIzIfuDIkohe5pJSX2wyjqzzY/TvEFF37CZoupinBYLVimJT7EybsuzfDWvhZPG5nhm5GHsOvYrDt/xKIO2r+Hnl1yJVj4COZePFv2a7u3vsnKHD1NhOW999Sp93UOQpHZa92xAyTiwe/phKysnrUmkc2aiYh88l0aRdaLpNCaXB9ISaUEcL7Iw9QwOjx0lmyPWHSTPbSGnZHG6S7DIg2iv28jAil04Yq1cec0yttTV8dGyhwnmNI6sPg6rt4hjfKcybHI1M2c+aLDJz507jyWLl7C3uY0Lr7zMWED2Le3DB//4JxddeQ1bd+5k96YNvDV7zo8DvLE5wduzZvHsgxMo9negjOxDY7eTYePOh8huNt92Oofd+Sg55x4s1uG0OLsojkcIyRVYutdx2ZznOLz4bu7K3Edq1PX43/MTi7zDLc4/MPHoGCM2fEzUPJqgy8Le5ma8Xq+R2uItsLLjrJnc+tn5DD/bz9KXFX5xUQUZKU7OH8Hq9REoS+BNSnSEuij25vNUeC7OlWtojO1gZL8yyjo+Y0LtCppaJyJNXMVVVe9jqRjFjAeOZtxfr6bYNwy/uhBv/oOE4p+R+nAWb20ys0pVsbvNlEn5/OGm13n//cfZuGcNQ8b9grNPu4SbbzibqrIK7rr9TpoaGhky/GRmv/4E5118LrNeep6WvVuQcnn8ZeYs3n73dZYvW8Jf7nuaksIBxNUsf3v5aTr8q/FnOrn7ppeoLqhmffM2+hc4Wbf5A95e8gk+PZ+4qQXFLnNM1U1MP+8kbvjtzSxetIr8vFIuu+QqrrroYqqGDKKispIbr7mO0887hwkTjyUlxDrCQV546ZX/DPD+hw0bNmxgTV0n6ciXXOTfw1bLYKqvv5SCvZuo+WIRQ5WveHyelRuun4xr1GHEQnEkhxWnqYhcLoBqClLnb6Jx9U6OSzXgOMxJ8x272DhiOKGThxMRfI2N2/GHfAwfV8L2miS6NYzPMxDnmRdx768e4GfuVj68NUsLVtSuICPGOIlr+Ti1EF3hLgoH6WTULJl0Ac15p/L3nZfg83/Mr1reIvpSJ85T7SzK9WHGtPe5e9PLHOtpZ9A545CzEcxqO6n4MvL6LePr169g2c7t1CuFaFoOhyVG67ZW/jFnF6/NfYRvdixg3OCpXHzm77j6rqnkuWz87Y8LmL/yn+zeVsOWmi+4545X2bpjHa8ufJpq75Hc85snOe+myfzpjpdwF0rM+uv9nDn1MqoHjeb3vzqMIw4/ixvue4E3f3cdCYeV6+96ko8+f5qP17wNCcEzLXbyMpx67BWcPu06bv7DiUTSJkLBJP6tGVZ9vYwjJhxLNNHGp+8uZEftbu647TbaWvcY7Xv2mdd+HODdu6xYdzxPdboWe1kGqy+GXU1Q47mE5YePomnW3Tw8fTS5qok4ivqiy11E0hE8+V60QJRkRCU77zXUMd04P8tiXh/m+oJjeOoWmftfy4FY/VU4GTW4L+vXdhM1uzni0gk88KdGppU1EGlJMX1IhHMvrOeL55JMuNWKK15KjDacshXVmsbklFHTKSxWK9tqz2fwN/9iwecwZWyc84fdwYqhZ/P6y79h7EUy3nFjcPqdhO115O+ZT1soQ/HP6nj4qV/SGgwjmxRUyY4/1ET/0kE89Ns3eeW9P7Fi00dMHHEqv774AS65bRJul5Nn7/uIi2+ZisUi7mlznD71BsYefjw3PPRLZlw5k4EVQ/nDX67mmXs/ZuXSD6jduYR85+FccfVtPH/eMZw36yl8NgcPXXUk3ck0976ynS/Xz+eTTa+Ry1jQZMu3AJ93yvVcOuNINLMdu8tMR6fEW0/M5YsvVnPffTNY8/VaLrn8Gj784D1DGKSspJBZj/z1/wHgdWs55uTR5GeL2PX0ON4/6jk2m0sZEa1h1K5tVNUsYcyrV4ClGiWRIJMOY1HySaRT2BwK6En0Te8Sr1iJ8+Fi2gZkecB0LfcPm0mibRR/bMpjJPl4nWla872UFeVzb201Z3R9TqAzR6VrNeuaK/n42jCBkhDqUo2Kk/Ox2PKMQ33N1EbOEsek6LSucaAtiNBZI1E2sZLpo++hIuHh4frbKLnqeizJT8m4h2GzdUHzOvw7WnltcZQbH+jmteUPsX7rPKwZMzlTKfF0FKfFy1N3vc3zb9/Hxl2LGTP4BG689EHOu3E8pSVlPH3XHC64dTL5hSYjt7lv6SDuvuVFbnv4Cv5859+Y89pMPv9kNs+9tYtEWzvuTIZ40o9uM7Pg7luY/sI/kRMJnrjhKDKZLDOe38LitZ8xf9Wz6FYfmuHBacODzzntWs6+bRyFVh82wnSZXVz4s2s58ajzmPPWi1xy6eUMGnEEaiZDJpkyVG7++vgzPw7wkq3bOKtpF0WXXUHXmqeJRU0Uq0soEnWsX+5ErpLxTr+fXEkZsjkE9jLjNkLPJbHobWT2rEJvS6KXrCb9pYbl+DTvBp9nSvYF7CEXT68NgruPQc4yfOBA3rBOwT5vHr7KEEVxCdmRprbWxVlj6rnitDQLP97D5HMqkbMWwlotLq+GRSujdnUa+ycyyT1Ban8xgutGvMwti//FuWMaKT+1P7H8Khz1G5F8cfRgLdlNLXzZWMLsuhqeuHku5srhvPbG9TS0rUfTyykpLqatvoPn//IJc+Y/wSdfvsEZP7uC80+bweW3T8WT5+GpP7zJlb+fgmYx4ZC9xMN7eeSed2nv6mRk1QSuOasCVyrMn99qoHXr17x155VYFAmztxiL3MH0e+fiGTWBJ04cyO6syqx3t7Bs1ZssWvwcCXcZuvJdiD735Mu5/pHTSKxrw9HRinlcNSHFzN8fWUQyEWPuR5/yx1mPoqkaejaHmsrw1KOP/88Ar1u3jk07N3BKW4ydpXGGlAQI/mMO5RmZVMSPtV8VmbgJ/bKTKJowBjlTTC5TT7arHXNsFWlZwllyFjlfJfKyW8kOjJDcodPsPgap31UEF9zOF3uHoio20pJGYNQxLPuwi6M9G1CzCeSElX6VxTR3ptnekuKDC7ZhGSqxak4rJ1xuxeRMkBCpER8Po2XBTkNnadW087m98gEeWvRbJt9SwKC+Q1EjTWTl4VgsWwju/AxnRx5LVup87k4S291Bn6pjufmGpylwVhKMh7E67DQHtnPfn6/k0bvn4vUUEg6FDW2onDnHjLvPoMDp4+F753DNLcdhKfISTrVj0az84qizOfWM3xHe9jmv3nIWxYKm6byHOPr8X9PQHUPTYtii7Tz966mYPBU8/F4NreG92HHisDj4bP4rfLXhSboVH5pmxoTGKZMu4dzTpnPpicdSt2k3o4ssDPepdIw7jBsf+ISCvBLu//OveXf+ShwRCy1qGlcqzeOPP01FRTljxhxuHPj3sDfuRycsAN5RU0MfOYQ92kH1BA+7nr+P8cdNQLcPI92RoG3TNgoumYZS4CAXXIguH0b+iClICZF+4kdymlGyHqT659Gs29FbIVI4gDeK3mWarYXkZ5fz5pZq+h5ezGObD+eoxCcU2E0GaVm4K02+WzLOW3c3JTi9UuPy82uoW+in76U2lKhG97tWnJ81oWkunvnlb3hh/Bn89Z3pTP3DRbgKTYT9HUhyBLdiIpXahm2tn2/qzbzozzIwLbMr3kJB2UASMZmTjj+NfgPGEYllmf/FApo6a8kldK695joSiQSLF3/B+PFH89GC2eiyiVOmXcG7Hz1JUb4NJRYmtrOVPlIhZ5x9Fe3bV7B385dkUilCaStVI49h6vSrDEHJLxfO45ul/0KxuPAOO5PzLjqDtcuXE4m1YinIsmbnCkyWPDJOj3GIc1jBaPLSpbzy5NNkEgmqix1UKQkOcxThOeNUuiYdxrIFS7A7rWxdtI09AZWEZOXVB2b9OMALN67ngrEVBDYtxz4yH9tbcykdOYKNjXWsa2yG9iwn/eZM+h7nw9buJuc5BjJpupXleL1jEVE7l/CTk1aSbfgAkyi1dHh4rv0Grpt8ISwYxQO7S/i0333w8VxGlbUzyp2hKe0gq7nJSRGKfIUEOh2sat/JByfuJH+0ztI/dzGgQiOxWqEwI3HpHY/hzxvBX1+9maMeOxGKFHIpN7HkJmxZHVN0D8G6Jlr8ffjn2iCJwiJMZhNSxkx3pBObTSiUaUTUAN6CSqJxCcXqoK1pL3379iWTSRsb/YIrW2TVRDNxCvN85DIhso17MHUk6IuJYtmOZJaNdF2TVaE9nMWUgeI+blqDPdkdbcEuNF0op2lk7fnY1RS6ScNZlMVUaiNmLqBbTlPoHkheJsuODzfQ0GoiJ2UMXcjSPIXDnYZMGs5EDo/PxeYpR6B5Qe3OYYt7+WTeKp576u8/DvC2r9Zy8omlLPvX36hwWjGPOJL7n/+I4ycM49SpJ9G2ug67tIHqa07FGfFiMvvQIu3E8nbj8U5D7wyRkgJYbU2w5kVyfXRMe1RanCOwTnoGy1cXMTtyOi98GuEoXwfOrkZcZTlcdie7GzMMGTYYu2yioaaJmngnExU71561A/uSEpq+WE+5t5QTbr2f4RErd7W+jeeKArzO/mQtGqRlbNH3UTdFCHSFaE5V8+zmDsw2N0V6gs2SlX6OQjJ6glQsSKk3j3hGJPJZiadVZLPLkLETe71CN0mUiGa1EMlMiMoiH6XZBM0rd+KLaRTZrWQTWbDoOK0KWZF7JZsJxeLE0zlcHhdRVaUjlkaXFHwWB5GUil9LM9AOSUuO/GKZjF0mYXVRUFJG5+owrZvaiEp29kYyOOQsJklmUKGdYY4kFpcVXypNV57E4JiZHQPLaRvkRs8o2HJeTjp2xn8GWFXVb8UpRYje0tDI5F2L+Eb1U1w93Fj0vP6PPVQeNowbTiygac9e5r/8JjMevRdHuZes4kRVxH2kA0nS0SQNsoVImVoS7e8STa0l3R6g2ekhIr3PwILV3DzbTGjbx/gkwXeRxoqD/D59UbNCydSOIkkk4hrprI7VrDC0UMikmrBKNpION535AymP1pLfx4wiZi3ZiiQk6aQ8lGyQVDCNIhTITHbaoxEmHzvJ2K/2RxK4nA6jBCXg97Nz+3ZjV0j8nUqnsTuc6IZopJC365HoERrI4oBAKLCp0QSyqmNTU6iZLFktQ0bLEgkHe7b290nuxTpbySSTpNSMIYmnZWPkEu1ISg6zTcZuMpHfX0FSVCx2GavTwfoPU8TCGVRBeSzU4MwSpTaNYqFolBYyfTLDCiScgN0MkqKRkN20Fun4ywtpsnm5etKDRvnoaDEH78svMORlRUfEAbQ4bNjcXUv5K89SN7KShtX1TD33CNat2IPqEDyIPmq+yeIdaGHI4X1JaJqxH+u195xwCMMoiolMtkeVVNbMKKooxs6RcBSjSRmK1QY63PmGoARqCk1NgJoBa0+9T29qqSFMuY9isec1kVv8fT1hYeBePSRR2WAxOwxKBaFSmkjEqa9vYPLk4ygpKTXOhkXbUpm0of45fNgwampq+GrZMqMiz+PxGMqfYs7sLew25FkNHd/9ir1lGTUZQxG52GYzJpNAoMd+ve1N7ysQN9RYhfSPbEKVLMYZrvgR/ckGQ/gK8tH0FOFIkAJzHhldI6mrpLNZQ5XUrqcQWoqJlEY4pZOJd5JNRVHjYbRMilJ/nPZUBwmPE7/dw/TL/kBJSTGHHzESs/kHdMLiH4uMjq/r2nFF27HZCwjbnXgiGXSTgyJzkmbFj5r0oUgxtGySbFrFJFtJxFSj0l2kiRhGSoltAI2scSSewSSrJBMWctY92FMFkJ9vLMokk4RikY3fdpOIAD2GNECThQCnbBixx5BCutZkZKIYwlYipdVs+lY521AwV6wGGN3dfgIBPy5XntGuns+ZjfNrlzvPUCBV1QzJZJJspsdjhw4duk9N1UpWJK7rOeM68Q97VE97dExFhaEgHhf26pGJFXXCpu8BLHTEjBwrQwM4i6yLYpvvP+I5O3pOw2xWDFulwnFjrs8J1VWxAs7oSNk0kihCF0eGZjsmRTEiiWAZEL81UbmoJRFjLJxIkU3qBgnL2HFHfDvYJBGihfEEMEuWLKG+cTuuhEKXlKBMt9BpB7sukcKNT5XJK1ZISDYsisVQPNM1DYtXkJzJmC0Wo7rAYUljMduw29zY7A6E7q2siZMjE0lF6ACasQsd4l5JcXE4nhaK1SIkCtXrnlqe7yePixymHhnc7x49z0X0CIXCtLS0EovGSKVTRKNRg1y1ob6BHTt3GglQYqCIwm3hVaLPQmt3YP9BlJWVGeAKafSCQreRTC9eExrHvV7Z+9uog9qnAP5tO/bTvTXeF9kaBmlLz6mdGB+qLM6C953S5nJYNI3Ozk5mPTqLIUOqufDC6YZna2LQ6MLLhSocxhQgpNtzQttW1Y0BI7ZqjWggqiUSGSMBMiuDPxw0mO5Gjxn1nQcLgWjRDmHYYDCITVUIFbgp1iBj0bFnZRLZLGabhEjWtkkqsbhmHI8Z0cmYe74zueig0DsUyWLoZkMBVJdE6LYi6xnjNVkOk5WEgGPPpYJ0HGW/Ug8gk9GMnat9xY/GnCK0dsWn4vEEwUCAQDBoGCkcDhneGIvF2bp1C599tsDw/gEDBjBlyhSKioqNRZMIv8KThXFi8Ri1NbWsX7cBISck7nlPnDqV4cOHGFFEeGdpaakR3ouLSyguKjLOXw3Fe00MtO88e5963n4y9mLjp4fqoWf62+d1++5NRXTIGmLbsiEQYhSm7RPtFfYwxovBHrDPtN8KT+xnZ/FBvUf6V+SKJHQNuy4cNYPdLjI490m8fyse/IMQ8n/xZ6+ufM939yiI90rCimoPIySKNPB9Xqqqgo4/RzAYMpSzg4EwosRVXCdylBr21BpRZ+XKlYZHVlRUcOWVV3LaaacZHmlUHPaG/H3f+f0IgDHXCfBFAt+cOXN455136O7uNiLamWeeyeEjR1FYWGJEhPz8fMPr+w/oi8vlwuGw7TdF6EaoF99laCLres+0ZQzWjBE9eqOAeO+Haub/F/Y2fO/fDXAvqKKDvcrjwujptIrFYtonzqwZcvMixPr9fiNcCiOtWf0NTz31FIFgAJ/Xx9STjmfGjBmMHDnSeF94pgBePIQH9uoc7y9G+UND9g6wXt6r3vlebHR8+eWXzJnzD5YtXU5Xdyd9K6uM/ze0ejDhcNgYnCKMDx8+nPLyPka0EX3oXbT+cDAZw3qfnvEPNZgPaoB7Syb375Sm6aREOgQYxhIrWjEHCg8Qj507dzJv3jwWLlxo/C1C7aWXXszxxx9vfE4AIUDtWXz1eMoPDbp/hd9/Zexeo/aqgovv2f957/vCy8V3iWngvffe4+OPP2Xx4sVGO0S0mDZtGv369aOjo8OICFVVlcZmic/n+3YhJgZCbzv/r8D8r7733+rBwqtEqBM5RsFgFIfdYXR6+/btvPvev1i+fLlhoHHjxnHWWWcxcuRhRtgVq+GeBVgP+Zi4Zn8Z2d7X9h9Ivc/3/9x/Z9jegbB/WO1dIQsQxfeLwdn7vvDUbFbF7w/Q1NSMOEd/4403qK+vNxRVTzjheCZNmmTcfolIIBaBIrGhqqoKt9ttfM9B5cH7hx1jkSVuHfbNPeK+VPz0bBooxq2Y2FARc6f4nKjQHzNmDEcccYTxvLy8/P/LSP/feFUvYMLDDSKbXbsMtgSxryAWcGK+Fn089thjKSgoMKYRMYDEOkEs5MQg6mUp6P2u3qnjf9Oun2wO7vUAAZgAU3RUPG9qauKrr74yPFSE4cLCQoYNG2aEM+GlAsxe7xMdE+G2d47uXRz9bzv477heLMh6bu96vHz/SCDsEQgEjEEtAG9tbUVQRgpgq6urGT9+vLHaF9cL4IWNhE2ELX6Kx08Sons7JTooAJ07dy6hUMho7DHHHGN0QnSotzB6/8VPbygVHdrf+3vD8E/RyX/Hd/T2o3ctICLW/gXf4nXxGfGa8Fjh2d988w0rVqwwHGHw4MHGOkP89H72pwjjPwnAYgT3jrheb95/Jdkbwve/bei5L/1uLuq9leg1jOjkT9HBfwe4ov8/vA364aKuty+9IPdGrO9uE7PfRrCfcjH2kwD87zDiof9xYBY4BPCB2e2gueoQwAcNVAfW0EMAH5jdDpqrDgF80EB1YA09BPCB2e2gueoQwAcNVAfW0EMAH5jdDpqrDgF80EB1YA09BPCB2e2gueoQwAcNVAfW0EMAH5jdDpqrDgF80EB1YA09BPCB2e2gueoQwAcNVAfW0EMAH5jdDpqrDgF80EB1YA09BPCB2e2gueoQwAcNVAfW0EMAH5jdDpqrDgF80EB1YA09BPCB2e2gueo/AIR5jQyF5gA7AAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
     <t>Microondas con grill 800W</t>
   </si>
   <si>
@@ -52,38 +62,134 @@
     <t>4242002490915</t>
   </si>
   <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHgAAAB4CAYAAAA5ZDbSAAAgAElEQVR4Xu19B5Sc1ZXmV7m6ujontbKQhCQk2xgECGWEjdN6HLA9mAEDEslCIJFxmBl7PTveM4t3z4Sd2Tk7Ye2Z3Zldz9pICGVExoCwJBAo51buHCp0pX/Pd99//3pVaoE54z7a1XaBTlVX1f/+99737r3fDe+Vz3EcByOPS3YGfCMAX7LYysBGAL608R0B+BLHdwTgEYAv9Rm4xMc3YoNHAL7EZ+ASH96IBI8AfInPwCU+vBEJHgH4Ep+BS3x4IxI8AvAlPgOX+PBGJHgE4Et8Bi7x4Y1I8AjAl/gMXOLDG5HgEYAv8Rm4xIc3IsEjAF/iM3CJD29EgkcA/tfPACtzfT7fv76hkRY+8gwMmwTncnkMZgaRSAwilUoJwH6/X/7xkU6n0dPTI8988PNgMIjq6mo0NTUhl8uhv78fiUQChULBWyDRaBR1dXUIh8NIJpPyHX5XH2y/pqYGlZWVyGaz6Ovrw+DgILT8m88VFRXShvbFnjVdjB+1XFwX8FDX+cD/OEgAjvwPrne+6/j4l7zjzgOgleqOU5DXbJPPnId8oSDP8jqfA+e5kM/LWPmPY2XbM2ZMR2Us+tstumNHONmdXd0YSA1Kh23p5SQI0G6pvf6tE2z/Xf6ZDeBQy9jWEPY9h5pwG8RyzXKhaz8IeL0H27IXkg16eT8MaA4KPgXQEdDkvSGe7fcMuHn5Lp+RN39z7nnPysoYent7cOOSxR8d4AIAI4PmwVWWyRTQ09eHRCqFTCZjBumC6KConnUC/Ja6Lk6CkWIjzbrch37Nz82EccGcDzc/0vc/iiQWv+uKmjfG89szUmb6YMDX+dD3i/0quCJpg6+LX4HW9pyCA/N9A3TBKRipd4GnKMt3Cnn3uYC8U0Aun0dlrELm/8yp00gmE7jld7/+0QE23S8gk80hmaSa7UUqlUb+AjtgfpMJtiWgHC5bKlSVDyXBxQV3/k4cu322Z6v8D1LPQ2mFoST5g8Zof3aha23gi4AbCdd/AqzR0ygUiu9Tah0/pbYS/f29OHPqFDKDGRnj7916y0cHOJnO4OTpM0gmUubm4CpzuI4te2EmuXxw9nvlwNkTbX/2QSrUVoEXUtEftCg+yG7qdeXgfVC/y8dcvujKr9WFNpRky/1FUo3a5oOvAVXjELVM3lJVW4OTJ06g/ewZMeC003zc9nvf/BCAXV2XTKVxrqMTAwMDSKUNYfFUBoDe3l50dXUJ6VH17Pf7EA5H0DKqBfF4XL7T3d0thAtO3lXFQYRCIbS2jkJlPC6EqLujU4iXPbGhaARjx44VckRSxXvZ31GCNmbMGEQiEW+tfBgYCsiH2eELtWNrBlGqLhlUyuSNocihSqSyZCFLA6Xax3HnqVTCjQbKF/KIV8fh9wfRdvSIzK/YY1ewSCAvCDAbJBvrHUigo6ML/QMD7uo5nzRR5/Nf0X5SliHMrqqqCoFAQD4nwytZjbQp+bwwXn6H9+N3tJMkl5wwXlPbUC+Ml6BSJdmsmZ/zOrJirmZdfOWgXEiN/iYm5EKSWWIqXDup78kseAzYSBTf8FSuK5EfpHm8tlwDz2uzBcNpOG+0s0ePHEbWVcl225zTEoD5ISf3vffew/FTZ0WadDKdQh6FXE4+VwanVN2IohmADwHXHfLBH3DdomBUwAn6Awj4/e7nkPfYCT4rY1a3hX/r+3xm3/R5KJVrriPLKWVcPp8Zk8/HexhqaLdtM3W1zewTm3Fcxk81KYvFB2OK+L5rA3URsX+8rijRRrXaKvrC5qrYr6IadpeD3s/n89oPRsKor69H27FjOHmizRMaG1xeTc3oAcwPX37lVRw5clTUHyVCb2Y6Zpib/FcoqhHx5WR16cR6/k9xgoTRGvdIJ7j8dTnACqgNvk6mflf/LvrWvIdZLMWV7xITYbpmUZWrZbtv3uJxAZX7F9zFJcM06jHkD0g79oKkX04t0tZ2DKFQ2L1f0W1Sxl/ULO7CcVzX0a/zowuet2N/HTE7jY1N0n5/sh/79+wVc6caUUdcoEp35zsUjhiAC4W888zqNRg/8TL4XGlRwOwJtgG3V6dOikq0flbOBn0uvTfvG6JQfC6qLgXIMEWXULhuj+3+cFB6L7/faA6VUp18Xl/UBKpdihqB11DyfP6ixhAg/PxngjIBHzWN31uwfI8Ay3WupuH9qCna2trQ2dmOefMWlrhvJebLBYDjH0o9K/GytYPxeQvSftuJozhz+rTRFurNUb0YkXSFyA8P4IGBfudX236NpqYWmbChoju8mdq9oWyWriSbdOjkq0NOgNUmqRSRRKjNLbouKmW0v1SvPuQs+yZ9pJS6n9Ert6WQE69t6VhUvSsothbgZww2qLnQBUt7bgNoAxpAMSpngOJi8GHvnt3CE+ZcP0/+Ls6HWSxF6fWUjGd+iu8UeY49h9lsBuvXPydfS5OoSnyhlBN59/P7EQ5HjQQnEgPO2zvfRV1dgzcxNmvTybAJUjnI5VJrS7gCCKp2ddZ1vRVyJVEbmWzXdHHFijMv0Z6ianV1bAnA5bb7QqZAJ9n+XBaEz6hb2+7bf9tcQfiEawq8BUBJ9vmwb+8e8TTmzlvgBkHMQFXDeCbAHb/OI9vkPNnCZTSiGT+Fi5+vW7dW/s4ymOQrBlf853EPP8IRF+CBRL/z9g4DsHag3GDbdssGU9/X5/LPbNru5AtGo1guFifIfKcYuVFT4PMFPOn2JN5vvm8IUa7EBgZ8AWnGTJKJXbMN21YrILaNl0EHzAIiMVHCZEssr6NEG7CMirbB0Nf79+9Hf18v5sxbAL8bwRMJp5eQTov6jsfiiFVVo63tOKricVkYdP3CkYh4HXQ1R7UYbapzQYAz+Ry2bNqIfC7nxda9BeuSXAWa5iUUiuD22241Erxtxzuor290Q24aejOTqerNtglG0opx06LKLTrkysoNGAU63AJAuTov2mK1y4aBctVrxMZbQJ5KMiFS24754YfflSxibD4r2km1d7baVsAYCVLwy6VYpddW4SrB9nfZFgHu7enGdXPnI+QuGiOsPryzczuOHz+GbJYqfD7+6Ec/xOTJkyXhQpfnmmuuwb49e/HG66/jH/75557UqgTnnAI2b1yPbCYrZqDEzHBt09OQ0K3hD0UVnRzwJLjcRuhK14kcSnptibQlX1SrtQqpe5WBlxMw811KsmEN6tp4bbuBbUbNjForMmVe5020q8rFYeMEF0rdIgW03AYrwOIiuVKqgKqq1nvwfbXBXju0rwAOHjiAru5OXD9vAYKuEOjC6urswOHDR1BTU40JEyZi//59MpZgKISB/n7EKitRXVUl7PiTV13tuaTqlnLUGzesk5iCZuCKJNj1ZkRtkx8EEAqGcce3boMvmUo427YXJbjcTrjm4rywow2SDaRtv8sB1gSEEi9bxduLR9Ww3oOr10xUMWznuMyRRE0nWheiSi6BUMm0QS1/rSrallJh0ATTZcs26bJJlswXWbjPj/379qG7pwtz5s33XCmP+JRlRVQL2vOt/beFhp/rfNAGMyCk6c8iwCq5QwCcSiedN9/egcbG5vMCCjrpugptSR7KHVKbUbSTJhIlQNLWuiraU9uuDda/SxaEFekhwObeRb82n1fG77bvBhvMgnQDKpYPbpMmm3XL62CpKrfVOO0yv6PPIuX5ghc1k3YZ5CgUcPjQIXR1dWLuwoVwckXNUi40RfeuSB71nmrClHjpAmEbzz33rEgw7bS2qVrHqGbjs5PVU4LvvON2+FKptPPmr3egocGQLF1Z5VIhUax8HmdOnwInV29Md0DdEumcK/LFgIibeLAyIErv7c57C8FLUpjkhUq5uaboFsi1ZL+Sg1VyZVwWzVWqX6wRNB1fOev2/Gjxh00kiz4IxxaNVKAiFvPcqBIb7Rj3it1kyu7Y4SOgKr5+/kIEXL7ApDz8PvGnfWTGJGgSFZO3PbNUoMZgXjcYQDCXR5735yLXLBIgLJrSawNcIsUuwAHx00O4665vwZdODzpvbd8pANsTruTKU9Fw8J9/8jT+5u//FtlssYJCPy9/Vqkf+nOusgtdad53ayAkemaqH4xk8oVp2w0bCl9lNkuWggGG5EqDF3KBTiQ/1iVoR9dK7XrxHkBzUzP+/C//Gq2jR3sCoGMj2ZIJ9vuRK+Rx9NBhdHd1egD39vVg8eL5qEMIKb8DzlqDP4yefAYpJ4dGfxiMGWYdB9W+IAaQR9wXQBYF9COPWVd8DD/92T/SJ5BsHSWYyRr+U35UTraMpmJYOIilS+8kwCmRYAY6lBjpqlBbIOQLwBMPfBsbtj5fEmf9YJgujU+f+s73cOvtd3iLUidV7bO7tIwEd7Tj+gULhIj19vZh1szL0eAPIe1zUIEQYgCaq6I4m84h4hTQFI9hR28PFlTWY8dgD4JZaqQ8zhWyuPaaa7F67QbxGPh49tnVAq5m7cqZv/5NghkM+LF06VL4BgfTIsF0k2wWbdtdV+HjiQeWY/3zm/+/A/iJJ7+D2+9c6mkNVfUUAAWZqvT4kaPobD8nANNX7uvtwxVXTBUzUk2pgg+XxaqQDxRwXX0rurMZnEwMCImi1FZFqnCkq0M0UoeTwYwrr8Ta9Zul9koBJoMeCmDb/BDggN+HZcuWGYC37XgX9fXFSJaCq4BzIEwiP/XQCmx4fssQAJcmG0oLXtzPJP9nFC8H4Orhooh7OYyyxMVHUgLWvTzbYr/nGvLy5EhJJOj8ihACfNsdd5YkTETpW1kvXtV29Cg6zp0TkiUS3NOLj31surTeGAgh6ACfHT0B+wd6cHogiWn1tTibTGJyQwNOdnXhdD6NRDqPQSeHATj45CevwrPrNwmBY/tr1vxSqjXsQsRy8kjeIOzf78Pdd98N32AmIyyaKahy96HEx6WKfvABbBwCYMIWi2jAnzawWENE68hOMFmfc/O9VDnMuPB9Zq54X5acsFBM7EcggGw+6wUylA8omSOJ4KSR2fqDhuRJ6ZKb+dFB0/iSqMjfQUPGPKImKUj+Y0smAdHe2Y3EoKlSsR+PPf4kvnXX0pJcM/ts+828vu3YUbSfO4d5Cxch6AtIVOuKKy4XwlXrC6EuEEUsGsTMmhasP3MQV9c1IxwK4nQyhStjtfjZuQOoRhgxx49TThqzr5otEswYAj2JtWtWS5iSqdzyBVZU125c3efDPffcA18mk/VYtAJsIkmGwpuYqEQM8PiK5UMCXBkNY84nJpvEcz6PUCiIYCiAVDIlf8drajF56jQM9Peip6sT+VwWzaNaUVdbj8NHDiMWq8Tcuddj3bNrJGvD9FgmnfZKUiIVUZncVCIp1SEM8RHcUaNGoaomJv1jML7glpE2N9dL+a0/HIKvkEc4HEK0ggVpg0gMJJDOJFBVWSmlt8GgD3m3UDCdD+Leh58Gy5Lsx6OPPSEqWhMItg3WiaaaPXWiDefOnBUJpoqmBM+aNQ3NgTAGUUAin0PcH0U/MkKjawMhqWXrdRw0+f3IwEGvBHzMSpx9zTVYSwnOFyRevuYZSvCgxLuLXozm2M1zIOBmyADce++98GWyg84b27YLybJVs4IrBEJqr4DHH1yOjVu2lMSI+Xl1PIYlc2ahr4s5StYJGWkmpeekxOI1mDJtugG4uxO5wUE0jhqFuoYWHNj7HqKRSsxdNB/rn3nGU3uetAYCCFdEZb4zqTRisRgqKiKiAcaMbUW8ugrZwTRy2UEZXEVFpXwej1ciFo/LAhPPJxBAPpuTRUAmHeJEMNrEQAnJN8ObPh9u/fZ/QCLJkt+iqn74kcdwx9K7S5i/BkXsQMaJ4204e/oU5i+6wXB7x5H8uq3Ki96JSYcab4Bxd611Zn8l9igLXb0btrF69S/FD2bsWmMS5eFSE5xh2NYC+Fdv/RotLa3eRWp77UAHyzKfXPUgNm6m0Te1P/qorarEF5Zci+OHjyAcNnVWJAK8njcLRysx/YpZSKUG0NlxDtl0GvXNLWgdMx6HD+yB3xfGnAXXY90vfylNqvbga0aQWMUgiy9fEGmMRMKIRitQX18DSncoGEAhn5V7B4NhAbi2tgYVlZXU2zw0GblcwQ1YmbBoKBSQKhO6U06e2ZoMuBJu/fbTSEpNdxHglasewV133+OpRVs96hxwYtuOHcfZM6cwbwHrkTXh4UaZ3ISFbQaVpAUCQQEulyuaJRUsmwetXbtGTJoNsLZnh1Q55/R77r//fiPB297eicbmFg8wXZWeqpYIlIPHV67Ahs0bzwO4pqoSN39uAXa/+44BRDIvrOtirRYQCEVx5VVXI5FMoLerE8mBPtQ3N2PMmPE4eviQeLHXzZuHjWtWe3VLaoupAUKRqACcz+URrQgblRuOYPToVlTX1YgED6aTCEcCiEYrEa+MivqlfxqkBoiEkE5yd4WDaCSMysoKUXV52nkU5DuSoPAHcct9f3IewKseftRT0Xa+WRm0+qQnTpzA6RNtmDt/kZdsYL8TiX5UVVWL/efkHz58yN19EedqRn9vryQXRo0qCplGA1Xi2Q7dJN2tUQzLFnPTtpvEsX77/m/Dl80OOm++tR1No1o96bHTfPKmRFN8eGzlCmwcAuCG2mp87fMLsWvnDlN/FQqa7RSDWQkyhCsq8YlPXoVEMomezg4k+nvQ0NKCyy6bgr2794gUzV2wCOtX/8Kr+aIkiqoRgCsMwPk8ItGQgBSLVqClpQW1DbXIZ5lhSQjAkXAFaqrjqKmvQ093DxqbmuALAulECj6YMtNgkKTK1JcJyXLyEkrlQhtKRT/40CrcuYwq2kymAqrqUSX65MmTOHPihKQLmU3i96jN9ux9H/HKKowZMxaDg2m0t7dLSJNx61GtYzB29Fj5LisjWT2q5tF2w3jvNWuekYVAkmXbYFt6eW1ATKSD5QbgjPMmVfToMS6WGu81Ai2DkZQf8OhDD2DDpg3nSXBDXTW++pkF2LVzu0hOIEiAc+jv60coHEJjcysumzIVA4kEujvakUr0oa6pGVOnXo73d70HfzCAufMXYt0zv/Aq+hlqM5Tfj2DYFO4R4HAkiEg4jGg4LCSLALMgMJfLwB8ooCJaidraWlRWV6G3qxtNraORz6Vkh4BfEhRmT4/fbyRXwGFtN5PqTgF3PPSnSCS5X6qoolc8uBJ3EGDLNdJJtcGmBJ85eUIkmMxZeURb21G0to6RMmKO6X//759jyZIbMXnyVGTzeQz09eDggUOYPGVKSTTRNoO8nwJMFa3ms7wYwRAtRtdQBvCo0W5c1+yXUXD1WUiWALyppGyVn9fWxPGVm67Hvj374fcVEA5FxJ6QZEWiUUy4bKrYw+RAP3q7u5EdTKG6rhGTpkxx1XoIc+bPx4a1q5nVNW6P64ZQAjTQn81SRQcRCUUQCvrR2NiIxibj3uUKOWRSCVTW1KK1uQmspe7v4UJqRCjIRQokevqlEoLqmAvR78sjn0vD7wQMEQuFcfuK/4j+ARPM14cCrFtulCPYkSy+d7LtBE6eOIZ5CxdLbpaab8eOHbj22tno6xtAPF6FQ4f2Y+LEycJ5uGAHB1Mi1Rs3rsfV116LymgMRw4fxLjxE8S7sPkIVTSv+SAJVi3Dvq94wJXgN958G62jx3ruPpWVqgleoEmEJ1euwPohAK6uiuELi6/GybZTcAo5yWSQ0dJeMN85ftIUhKNRpJMJCQQ4+Syqahswdfp07H1vlzDiq6+7Ds+t/oXkcDWAz2v5mmAYlcRiMh8qKyoRjYQE4KpqMwl5J49sOimaoa66SiT4zKkTGD1homRZKKypvoRMZiDI7FAYoYCDTHIA4WiMWWgJxNz2wE/Q158oAXj5Aw+KBBNg6ZtbMKevlfWePX0abcePCsBMLiQTCQGE+d9Dhw5Kf7u6OjBp0mSZ00wmi0RiQFTzW2+9gaZRo3DFtBk4dfI4Lp82o7wOXmwwryPAqh04dl1oNuHiAB5csRy+XC7jvP6rbaKibcZm+8FSS+U4eOrhhwRgLavVWSDJWnzVVHT3dCAcigqodEsYVouEwhg3cbIEMgZSA+g4cxrpVAL1ja2YOm069rz/vqjcT1x1FV57+UUwiMEBEFRzfQgBV4ozuTwCARKlKCKRkNirWDQsr0ORMLq7OzGquUUS55U1Neg4247q2mpEqyok4JHNpIXkxasqhYARhHwuI9UmPj/Te2Hc9sDT6OsfKAH4nnvvx7L77hcBUFBtN0lfnzpxAseOHcUCquhwUMDdunUrrr/2GuzcuRPXzZsvJTf1tXXI5LLiaXCsBHjz2uew+FM34uMf/4TRSO6WWLH5Lg96bu0a2WSmElwkVcUgk83SXYCzzq/e2Ibm1tGeH6yj87JLbr3qY66KvhDAiVQCpPy0weoH0xVpbh2L2tp6JNMJdJ07h96+TrSMGofJUy/HrnfekcmvrKrCqRPHxVflfSviVbL3lZURDJrwQabf29spGiIaDUmdcFNTo+yq4+wT4AnjxkpbsXi1BFX8Pgc1DXXic9JXTqfSqK6qMC5JAQIwCUYkSskM4LYVP0FfX38JwHffc58ArGlHjReUpOp8Ptn4xVqrRQtvQN6tC2NDZ8+cRXV1lVRtmNiAX9wiBiz6ertx+uQp7Hr3Xdz/wANiflRrCj9wEz3UHs+ueUZCxhrJ4ud2UYJ+X4Vz5UMrKMEG4JZWQ7JMg24O103IcuVKLPqRlVi3YcMQEhzD4qsuRzrDzgfcZLhRQZT+usZm1NU1IpPNCIvu6+vE+IlTUFVTi+NHj4jU0laToHCFi58aqUBVdbUAEo3SNQqjrqERnR1nEQoGUVFhXKHpM6a5KUAfUqmE2NrpM2eKa9Xb3Yl8Jou6xlrZy1MoZCWVmOzrln09+VxB/GcwGBJi7V0Yv7f8T9DTWwowJXjpPfcZ8uLuAbarP1Rqzp4+g2PHjmDB/IWy468oTX6JJ3MumFbs7esT9d3Z0YnOzrM4fOgwvvjF38HY8eMlaqWpUhtgkr5nxY00e8H0MZSK1gW4auWD8OXzWVHRrVTRrhVWG8xGxL5xiyIgAD+3fv15ANdWx/DpOR9DKpk05IWlqPSD09yPlEFFRRVax45DNpdFb3cXujvb0dQyGlfNvgZvvv6ahEFpE8+dPi1hTHFfQmE0t7TIiqd6Zz8YZI9J2DKLiooY6uvrJHRZW1stLJl+bSbrYNaVs8QV6u/ulRh4d9c5NDQ1I5dJi2Rlk0kEIyEJBjCUyUR8d08nsjkHj//oZ+jpK1XRKsFKshQ4OxbNMZw5eQrHjx3GwoU3eAB7ILl2265aIREjc1dJ1LIgBnR07k1hg/nec2tWi3Yjiy4H2JbeUoBzWee1X72F0WPGetseuPrskhyV4O88umpIgBvra3DzTXPRN9AvE8qB01ZQQhIDvWLbaOPF5vR2o6vjHCZMmiISufPXb6OmtlYCAV3t7RK/5oIKRqNobGkWWxSN0L3wy7gjoYDYUt5nVOso5LIZ1NXVmGRGIYexEyfJQmCUK9XPTXMOkv29qK6rFYlOJfoR9PuQSadQXVsj9tsXMBvJI+Eolj38n9DZbYL5+li67B4su/d+U3hgZZBKSI3Ph/YzZ3HkyEFR0eqJ2O6U7sDXdvt6esRboKnRtgRsLV/QPVlu+oMAExcF2LbBCrAuDD4/8vBK+PK5rPPq629izNjxrr9bDLGxk1I6SybtOHjy4YeGBHhUUwOW33kz+vr7ZKJ1UJS+vXv2IBQ0doUA034nk/246pq5mDjpMry97U1kM4OYPuvjeGXLZmRzeYk3s+zTSHYIgbBh0wSrsbkeoUBAJJ6S7Tg5iYXz7I7+RNIERZyc2GZTyZmVRVAZjyASZUYrh2wmBRbaVMTCRlIkHZpBrgDc+9hforOrxzNT7Peddy3Dsnvv81wWO/6r0kLSdu70GRw9cvA8Ce5qPyd2k2O/fPoM0YYcz8njx6TEaPS4caZeLZeV4nmapnjcnFXCh5YESTLGlWDlR7Yf7PXF3QtmAM7nnFde/RXGjZ8odkINtOSAXVtcboNJEOxHS2M9Vt17KxJ0OcJktRGxw5Skt7dtk+BDf1+PhAdF1aaSuOlzX0RFLI7XXn1Z1OntS+/Gf/3zP5OACq9loIN2mQtGY9EEmLaTrL2hsV7ArwiHUBmPSeE4JzFWGUdFZQyhcBCDPd1IJfslkFJdHZNsUjo5iFw2LfHrIKMRVNSyDSYnpUjLv/93aO8oBfiOO5d6LFonsdwG0yydPXUKRw4dxMJFRoJ1Lg/t3ydjYknslMunCYD8jO8zKNPQ3CJ/00Sxrpp8p7KyCpMmTfJIFm03AebD9oO1H7a/rNrg0UdW0fwQ4DcwdtwEYYl8aFkrb2RWq8m0MBZNklUOcBMBvucWpFJJWZlGAsPSke3btqGmuhbnzp2V69geO3vT578kEvXayy+Izb7znnvxt3/1VyZaxTxvICSgSc5XJDYkdre2vha1NVWIRCOoqa5BvMqASXB6ursQjkbkerKA/t4uZNODQtK4iCjJtNOMZAUl0sSIVlCYtoMsfE4AD/3w73Gugyq6GMlatuwe3LHsHpkH1U6qCnUyJXPU3oGDB/ZhwcLFQJCmJIPO9g5cN2eOt7n10OHDSCYHcPLkaSxetAh9fT042nYChVweM6+4QtKcZPxk8m+89QY+8YkrjT/MdOEvfyGRMJYC6cMG2I5P8/PHHn3YAPzqa29izJhxco2u0PKccLaQB23w+o0bhfjYj6amejx+/21IpVMmFu0mHFi1v2fXLonIdHR0iIoS1eL3YclnviDS9vLzm+H4/Fh63334H//tp2Jj6BeTSyqwuq2DWyhr62okEkXAORnhKJMKjgG4qxOxWIWc4pPLpsRWZ1KDqIpXIBQJSUKCnCbgd+BjYCSXEZ7AoIk/WIAfEXz7e3+Js+2lAN9++x24+/7lbnGAmSMlWHaQofPMOew7sAeLFi1BgXZ+cBCd59oxfuIEU3ZTcLB37z40NNSjvb0DV155JQ4fPoh0Niex9XI8ST8AABgWSURBVEkTJ8qmbqLZ19eLV15/Fd/4xi0SgGFG7NlnfikhyL5epguN8i53kxRD9tEFOO+8/MrrGDdugucC2H6YNMNkg9+HJ1Y9OCTAzU31ePT+26RzusueQFFFH9izB8FgSKRX1RQZ9oIlN6GhsQkvbNogx0IsX7UK659ZLYMVKXePBKKKbmxukn07E8ZPRJ4hyUxaNAQ1hSF05pSB/p4exCS16CDO4Ibfh0TfAGKxCDLZQXGJKK2hYEgyUNxGwiRKJByE48uhkPNj5Q/+Bmfa6YYUJfiWW27F/SseLKl4ETLkFsZrUoAA7z+4FwsWLIYjOVmzWXyzm6BhOHTK5KmYOnWG9O2VV16W57kLFgr47+zcIdtDuZGe47vpc581Nd5uZShJFgHu7eECNMVPtg1WoVOt8sTjjzKIk3e2vvCKhM/Ux1NQaUdEkn2mNPVCADc11IqKHhigH+qTbAYflODjR44gFI2ioaFJJLinpwudHR2Yu2AxGlpG48VNG0Qj3Hnffdix7dde5T4BpuTTRvmDfiFR48aNE+C5kGhMCDqLUXO0rZlBJAcSaKznAWfsgw8Dvb0iCaNamQotIJ/Nm4PHJMnvIJsjJ3AkokXRZoHP43/8s/MA/sbvfhMrVjzoHttU3C1h72nieDs7O3Fo315R0fxMpYmsl/0XF9LvRyqZkEPiat0Nf/19fZIKrW+oN9yl3xzeRi/DfgjAPp/Mq7ZdDrBdCOAB/OJLr2H8+IneRfolkix5DYjb812q6E2bvL0xenMCvOKurwl9VzeJwQpWM5xsOy7uBztFtRKrigvA8xbcgJax47F1wzoB/pY77sDBvQfEjnNw7HgkEjV7dFAQRtnc3Cy3JFkiwCq9BZ7wRvuazSDu+syMhR86sF+CH7NmzRR3iAxaNMDgIEJBk3URjiHJeRNgeOLH/4BTZ7tLJPjr37gFDzywwt0HbO1HdgMfyqoJ8P7d72PR4iWem8T+7t69W8KqdIfY5507diASZZBmpriEhw4dEns9c9YsAfDo4cNSgsQMnPrGxGH92mdl/JpNUlNh56Xt7JYLcMF56eXXREWr2tGtIl6o0o1kCcAbN54HcHNDHR5f/i3Jb9IG8sZUo3v37kUmmUI6nUHAVdNk2CQWcxd9SnLQG9c+K2UzU6bPxLTLp+HUqdMCai6fE7CpeukOcYIamswOSJKoaChkwM6lMdDfh1QyLSk/Cg4T+tFoBEcPH5SFNevjV0hxmxwxRP88nxGpDYeNu+VQxecZynTwB0//DCfPdJWk7SjBy5c/4B0RoYDqxnH2iUCQZxzYs9tIMDe/OQ727d6DKVMuQzqbQXV1LU62tclC4pgYpOH4Tp8+jaaWFmH/bOfIgf2ymCurawzJdDeyKcDlRXfaH8VL/eOnnnycmqrgvPjSq5gwwVByPmyAJdjtls1+77GHhUXr7jaV4BpmkxZ9UoriqAqjFYbZMqSW6OuTmiNKo+wCdhyJFTM+Ha+qxZ73d6G/pxv+YBTTZ85A2j2miaZBpLfAfUAhk2d2bR4XCQHklpJMJiWbwc35IQUkEwOojMWEZacT/SLtJGbRWMyU5jBSRhYd5J4jRoxYBeqYOLPfj3/3F/9LWLS9uL/29d8VgGVbi5UT5l2VbKnqpASLm+T3yU78aCgsSf09e95D86hRGOjrw6SJkwRUSiKvmzFjBs62t2PXe7tEymdOnyEF7hu3bManPvUpL+hEgPl9G2BbRdslVsTNA5gSPHbseI8dMiwm1ZRuJIXI8L3vPkIJJikyB4jqo6oyihuummKyPyyJ4crMZqSTdN7NcX/G/UqmUph2xSxxTyprGtDU1IAdb72JUDgq9pUJcKnjYs43FJYyVLJh8fPc7SgEm/Fo4R6smghKcSwqYlH0dHUhwqKAaASxigqzsJyc1GDxGpayEmhKERdhrCKGYMiHwVQSuUwBP1u3DR09penCr3z1a1ix4iHXZTQ2WL0BPb7BcI5eHNhrJDjv7pjZv3cfItEgOs61S6UH67Y4Tp6Qc8VMzoMf6VQSx9vaBNzx48eLS0kzNpBK44YbbjBCl8th0/p1noq2bbCSKhtgAl8CsLJoXqir14tJWxLMig5TlFZ81FfHcdP1V7jHCpjoE+0oJdowTCbkTS30qJYxGMxl0NPTh/Hjp0hp6xUzZ2Dn9u1gRUQsFveYOCNfA719KDiGWft9DICQYYYkw2S0S14AZlGdJPUlmhaVOqxwkN+Nwuc3xX8MUcrWS6msNIsuGHKkvktKeLIF/GzDdnR0lcaiv/Tlr2LVqoc9G2xXUyiD1gjT7vd3GYBdFq7qU9OMnDXGzaVQsOD61Yyji69rFg/bp/THq6q8v/n+hufMEQ7MQunDDriIt+MKJe/7naeeMCr6hRdfERXNh6pkflFZtBS6OA6+/9gjeG7DOnFr7IdUVS6+Smwbc8GsbyJxysj3WPQekQAEJTgxkEYkFkHr6AnwBYI4zbMV04OIVcaMBglFZIBcsZKUl8oLIzH8R/LBB0tzaYv5TBVNVcw4N8OYtXX1yDNz5LAmOgqpAXSlnYSZddt6oCczTPRBWR8dRABP/3S9y6KLIyTAK1eu8gC2maodXBC/f897EqqkBIub5PPJzn+W47BESFRsby8a6muRc8zZHqmBfjDXzZg8P287fkwAHj9xkrBvfaiKtmPRNsDlEvzd7zxpAKaK1li0qh87VMlOMKolAG9ch1SZBLOi48ufvk6oPh0qBh3IDhljpl0z5xkPSiw5XlWDyZdPRXowg2S6gH27WYkZQm1dndk96Lg23ylIXtkETUwsWqNIWo7LwUvRXMGcfkf7Fo9FEWWoMsj9OUYbsQ2pmnRP5pGD3eSAE+MCyjFqPr7nw9/+4iWckUBH8fE7X/oKVq5c6SUa9LxdVY3KXQgwJZg2WAHmou7oaEdDQ6OEXjkv6WQSkYoKU/kJH86eOyveBwM3bIsxbZKvsRPGe2bBZtGML9gq2hZKXXAcswcwAx0KsE0u1JfTAy6///gjWLv+uSEArsRXPzMXuQxtG9loBql0Quqvgv4gAqGg2FqeUDt69DikMoM4fuQYJk6bhpPHjsLv584DgkXJMiqKKp3Vmexozk2fUZPoVhfaek1sFHLG3tNNYkE7iwUYnaI0sy1+j9WYtNcs7aEfrAV9QtwkTVRAAEH85O9X4+TpzhKA/80Xv+QBbBiqKWhQ9ayTTfLz3q53DMDu9la6SDfffLOcccWq0qNHjuDzn/0cunt7cPz4cSnmnzNnDnr6erF7zx6xwxXhiLiFb+/YLoWFyoqVRdsAE1xV/yrB7A8Xj6eiKcGjx47zVot+kb6vsES3ZOf3H38UazcQYKrJYqSnpiqOr39+kRAYH3JIJRISFjS7DYISTCfz7e7qlgp+hihZsB6va0TXubPI5x3UNzbJWRXcuSHHBtGWiNSaA84km8TV7xI8tkdXg6m+bJpnYaYktkyJiFfF5VDsaDgkZoGuG6s7CT5j6iR+lGjja9MkEHQeFOPHT/7uGbSdPFcC8Oe/8EVR0cbfLD9Nr7jPmBP/7jvbsfCGG2V6xExlMmge1YRdu3bh8sunS2xgzOjROHb0iMmWBUKYMGEC2k604ciRw2hpbcXECRMkMfHiCy/hS1/5sseilWSpDbbtu9TNWYeZEuDvffepoopmQl5FXUenBl+zSX/41ON4dp0CXNygxSK3W764BL293VKlyE7Th+UNCRxZbU93r9hnqmkOjOc4BSMxdJ49I+HCydMulyNxc1lOtoMMKzu8MyoN6HqIFlU3bTNVWiDoRz7DTFDaTR7QpQpIlCtWQbufE3eKtdQmgOtImQ41u+fPuiqb5UF/+tO1OHm6owTgz37uC0KyiifqFas1lNRwrgjwrnd2YM4Cs7uQ7x07dkzmgmB/cvZscY+4SbyjvR1zrr8ehVxByCVrpUk26xsbsW/3bvHfiQnBV7VLksU2y7ePyuJ395CpuTgP4DHjTUP2wyMTDFxks/jhd57EmnVrXQkuAkyS9eVPz0Ui2Y/cYFoiV9F4DFXVNSYIkUpJZSEBPnDggIDFstFgOIbTbUfh84dw2dTJOHzwoFctSK3MGJqqJwl+uIVoZOn17pETrHUq5AsiGSRK2WxB6rUkERE0JbhU0dzWQi7BNqgV/O4OQrYr+2kDPoT8wNN/88shAV65kizaFL6rSlaB0IUiErxzO+YuWiwxaFWdfnXp9IBTLjMSSnoGerQhM3amYTh5PQDV+OeMUzN+v3Hdc9IHW4JVRdsH27AZztHvf/+7RQkePc74wdp5W5+bQIeDHzz1BNauX4tkkkfpFXcBV8VjuOHqmTjX0SHFZbQbPAWehe9BfxZhqa+qlcAHdzEkE0lUVFZh5sdngn4iSUVDYyPSqUFkyLQTCSmsY6SHNpisnf0hEydhM/nSShkEC+AZ9Uom+iXaRbMymDY/K8BpkaREBbe+QGxtrDIq0k3fc2AgKX2pq4mLaxUMFvD0X69GR3eXt845Jzd+6iY88hgD9+4ZJq6ato9T4v24kN/d+WvMZ8mOWZ4lCQqNfCk5403Ujmv2zrbr+p6eV6YsmqVR6lIpwPYRy8bLCOIPfv97pQAruHpjvYEJegA//O5TePa5NecBzA6Pa26Ek8uaUCWdd9n7k5fKiUA4LKvQ7As2uVselsk9yVRFDJxQZcve3YJjzp+WA1AiooppYzlwAsyHnBudz6O+rs7kgjNmsxgPFONWFW4RpUQzg8SFQJC5N5nSwL+ZrmMFZldntwQnGpvqUFtTK4GFLa+87R2ZoPOx5MZPY9UjD0tehxOXd4FTNayrQQHm5jMCLPuYrZN2bYDLCRrbUO1gu17qHqofzGe6UMZtLu5LsgGm5rjpppswb+4cA/DWl1/FuDGmZIcXaZJBOy4GHMC//e6TeHbdWiQSpRJcotcvsT84Hzcs+RQeeuRh0VkGBEO0woGgu7/JmAIGUd57d4dsXWEVp7hg1iGkPK7JBGyoht3qmYC5Vl1AnT617TbASrLk1HwXYA3faliXambG9Gm49Zu3msVFgJ9/6RWMH1us6GAs2n6Iuvb58KPvPYXVa59FQmLOpQc1XGK4lqhoRqZWPfqIF8pVgG0VrQDvemc7rp+3UCRYj1ZU00dyWDwdyI1auduEbNuuLphep53ZvGG9aDL7t6YUYI3dt4xqxl133oF4ZdwsAgK86fkXcNkks/FJTurV+mg3esQbZXM5/Psf/gFWr1mN/gFTdWC7SqYTer7Gh8F9/jkYH3bFRfvc58P8+Qvx8GOPWkV37sFpcmSiSUDwmeTnvXd2yP5g8gLaYPnc5TZaEmWHLX2ScjTBHVW53qFO7nSKBi042Lplk3xPK2r4fVuCeZtldy/DuLHFbUgC8OYtL2DcRJNNUmaoq4cNkqUS9H/5p/+Ov/iLP0N7Z0fpD0gMB172WtH2f9P189tYDdaYFi9eggdWPuTNj86T2lexy/m8SNb777yDufMWSgkvY2Timbh5Z/sQU7uLMtfuIeS2LdbvGC7jw5bNG8VUMp+tNtiW4K98+XekDKikbQV4/KTLvJWoep9v6OtCniQpj1+9/jqOHDwkReySW6W/yp9XE2m3z382pMqoDlOKq3/ruU/GOad7yzBhccOb3FePQPROdjcn32lc3PxhdvCpe6d7eFQa9JS4krXiHkdR7hLatk91E/tM8L70la+ivtmUsNq2stxlIsDvbt8up8ky/kkflxEsumh6P15jqkbNYTMmjKqulzld3sftt3LIalAiW+LaOcBW1q/JHiue5lEkWWxn2rRp+OYt3zhvaRsVvXkrJk2Z6h0fXG5/OVB1pD3AXcdaJNz6qTWNqOj3eGajvqe+ml6TsxaEvuddpz/bptkt9wwLe1WrrRoKLN6z3IaV/61ExWa6tnQqQVIJk/2N1o+I6HX6TPb/7o7tmDNnPnLIy/YUhhxbW0Z7WR4CR5eTJIyP8rnTMfGzLRvWY+Eilv/wGMQ8nn9+sxA83RumfeU9lt51h7iV5Q9Dsra+hLETJnqd0AlTYHmRHimgINlAKoMrB0fYoXVGtJ4cILFmhiO5kcSVVPkFL9cOmaqL4m8ACViWhNsaRrWMDsz238s/U0Dt8emEqhTZUqrAmVw0Dx0tluuUg8s2OYZdO3fi+uvnI+tkJQ7AUwiam4vx5PMEwOI5JWaxUMCmdc/h2uvmiJvp53nRmzbC5w+cBzAPPJs4wVTFDgnw5q0vmmSDqypsdWWDpp37oGejXs1vIsm13sHhRTCzkjxwkHPPwrIHrQCJxpBwlvtTbm47njp2o24XAtuWals92uCW2CrLXy1XwwImU1NWuawNsM4byc/uXe9i9uzrUPCZPUTcKsp9URKhOu9XzCQP63KwYkrU9NHB85s3YcHCRWRwnopmfN78wqg5LPXGG5dg0cJFXknvkABvefFlry56qFVvq89ycO3PPBXMTltH95trDMCikphzct/ziuwtidU2JcnhqniVNHsBqIaxVfVQwNpqT1+rtNhqu1wqVR0bCZaNSSVEy1bnvC9V53s7d2D2NddJLGGgfwAVkQjqGk0tmc5dkdtw24y7o1N/YUY0muEjr736Km5YciP8rD/LF/DySy9IHxTgSZMm4u5lS88zRSULV/3gUaPMaapqF2w2batn+7Wqbu28NwCqWks1GzvD8xZNx/krKkZNuyHFssWgE0AJlsNRhpBWWxXbWsY2Kzaw5Xa6XFvZgNvAeQvAVdFawaiLQc0K36cN5kE0s2dfi7zPwUDfALKDg/LLbfyebXZ0jGTHOhavj+5vMGx/ewdu+sxnhXRxIbz44lYBkwuJ91u1aiXq60yRwIUexk164SWMHm1Od7Ef9sSVk6Ch1DRXmV5jd9omaJI0cAMpTO8pydCF5alc1/ezg+h2f4pSUNzLbEtyuSZSIPi+DXw50OXMmN+3JblEaq3fetCJJ4u+evZ1yPsKSA4M4OD+A1LK6/m21gTLeNi+u8mbGksEy40oHNh/AF/9+s1ywgE5yMsvvcQT3WT7zZe//EXMvnr2B4IrY1UJ5ikw5ROok1HO9Gy7p+ApESpvw84C6SLRUKjZJ1RKpjz1bP0MT7lqk3tZZTzlaln7YANpj2WomK/Oe7maLpfmoQDW9zgWAnzV1dei4Gd+2ScgazWpHMPq/po3XzP9qAvPFgzjTvKku7DkhyWhAB9efPFFqVAdM6ZVzoKWwsMPechPvG/aSgke7amKC0mxLbXlasUGSsiEJ83G9rJCQ/I7ZS6V3aaqfFGzZNXuKfHl97LVs5qM89Sc64KoqeEE6msbTH1fJbUcaH2/3D3i39REzGjp4uHz9rfewievu1ZMlCf9kh4sHpaq39eI1oV4AcHU+/Ka115+SbbZfP/73/9QyfXGQYB5pEB7e6cEK4qTp7/cpb8LXPzteFWnRek1K5PpwJ07d4gj7u7cMKdQFQqYMnWqnDIj17oskavUAGyCIfavWouKLVsMel9PPZsXXp+lP+6Rsh7gOlL9seUyFS1BDc2Dk0RZG/AUCFWjzJLxfnweipDRTTrRdkyqY6SuwS3zZSGBtKw/zhngqUDmdx/0p3DsBaZti+SyigQ+qZKprqrEwoULJb/9mz5Egm37ZKuMcuNtf684b2ap6ipcft/9+Kd/+EfU8HjggX6kBbw8urq7JQ9brh30HkO1rUDaEmLf94PIxYUm4EL30XsN1Z/y+fEWmOu32yaB1/PwGI6ZlZ6s6GD1xtbNW/CL//lzOSEoNZiW0tmPffxj+LP/8lfnmcbzCaSJ9pE1a/H9RwL4N/3yb/K9H/zhD/DjH/0RqqMx9KQTosa4UvV0md+kjUvtOxSB1f/yC9x+yzdRHa9Cf2JA3L+bv3Yzfvrzfx7W4YoE/zbv8PyWLXjyiSdxpu0kMtxzdPlUOVpefj/gw36J47fZkf+L2uIEv/7aa7hp8RLEIxXoSQ7IqQN//OMf4+FHHxnWnv7WAR7W3v4/3jh3evDAUpLNCRMnSqXJcD9GAB7uGb7I7Y8AfJEBGO7bjwA83DN8kdsfAfgiAzDctx8BeLhn+CK3PwLwRQZguG8/AvBwz/BFbn8E4IsMwHDffgTg4Z7hi9z+CMAXGYDhvv0IwMM9wxe5/RGALzIAw337EYCHe4YvcvsjAF9kAIb79iMAD/cMX+T2RwC+yAAM9+1HAB7uGb7I7Y8AfJEBGO7bjwA83DN8kdsfAfgiAzDctx8BeLhn+CK3PwLwRQZguG8/AvBwz/BFbv//AM6QhCjdHarLAAAAAElFTkSuQmCC</t>
+    <t>Batidora BP4541</t>
+  </si>
+  <si>
+    <t>Ufesa</t>
+  </si>
+  <si>
+    <t>8412897672055</t>
+  </si>
+  <si>
+    <t>Plancha vapor  FV2610X0</t>
+  </si>
+  <si>
+    <t>Tefal</t>
+  </si>
+  <si>
+    <t>3121042610105</t>
+  </si>
+  <si>
+    <t>Frigorifico Americano 3fal4651</t>
+  </si>
+  <si>
+    <t>Balay</t>
+  </si>
+  <si>
+    <t>4242006207922</t>
+  </si>
+  <si>
+    <t>Robot Aspirador ROOMBA 896</t>
+  </si>
+  <si>
+    <t>Irobot</t>
+  </si>
+  <si>
+    <t>5060359286475</t>
+  </si>
+  <si>
+    <t>Secador HP823200</t>
+  </si>
+  <si>
+    <t>Philips</t>
+  </si>
+  <si>
+    <t>8710103602019</t>
+  </si>
+  <si>
+    <t>Lavadora Xwe81283xweu</t>
+  </si>
+  <si>
+    <t>Indesit</t>
+  </si>
+  <si>
+    <t>8007842826050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitro 3EB785LQ </t>
+  </si>
+  <si>
+    <t>4242006249175</t>
+  </si>
+  <si>
+    <t>Tostadora LT330D</t>
+  </si>
+  <si>
+    <t>Moulinex</t>
+  </si>
+  <si>
+    <t>3016661148378</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAArwAAAK8CAMAAAA6ZJxxAAAB2lBMVEX+///n6eTn6ebq6+rw8vDi5eHt7e3////29/bp6+j19fXw8vLl5+Th4+Hv8e/z9PPt7uzl5+bFx8Ly9PPb3tvf4eDGyMPk5uKxtLHc397Z3NrW2NTU1tOyt7XNz8q0ubjO0czBw77S1M/DxcDu7+7e4Nvp6unc3ti/xMPJzMf///3i5OPg49/Kz8musa/f4d62u7rk5uX///7U2dXy9PHW3Ni1t7PAwr3R087c4uH4+Pirrqz9/f3IysXn6ejCxsXX2delpZza29aiopfr7OvHycTP09G5vr0AO5X7/Pru7+y4vLu9v7rN0dDS19WoqqmkpqW4urbMz87l5t+8wL+0sqO+wsHGycgBP5iqqZzc4dzJzMvLzciwrqDR1dKfoqEAQ5uEhYCrq6Gam5WHiIW8vK6fn5WnpZXh49z//v+QkpCbnZ2MjYqWl5AYFxm2tafCwrW/v7Hp6uN5eXcBUaK5uat/gH2Ul5fZ2tHKzs3FxrkhISXP0MLJyr0sKy4BSp1iYmVycnKvsarr7efW18hQUFMBNpFZWVw0NDdqa2tISEoICAj+/v47Oz1IcrNBQUNafrc0Z6v5+fElV5kNRpIdW6gRU5+6y9mnvM+HocB0k7ZCbKRTeauYr8cUVSZnAAG9g0lEQVR42oy9a3NV55UtvBEoExFJCEpBQtJRhECmueoFWRiQcHRUgmNhQIBdbQpTsk8lHyCd9ockdULKXXbaTudiDztQYBvj+L++z7rt9Ywx5xLZDgTQ1ta+zDWfeRmXngFmBjPArPpj/1+q/2Bm9a39I9Deo75zcw/Q39qvoXqk6tGRPxqqL5a/qm9vHr7/s+p/LW/0I+qnkX17c+/8STc/FHj0CI/qx+mhBwC9XvO15m5onmrzAP1/sfYZtG9X9rKbr2R/6//w/F/0G01/RP4Ots8I1n+W/feweeDsa/0fSh8bfaf/XPNPJ3vz0P6tfVezb6UP2vKfi/BL4DvlIWDmvgZ+Bf2vVr/30P/G/vuUf08/nJogyR+//8Jg2fto/W9AG7LWBBZ9JBTe/Q+o/2j9NzB7kH4Y5tHZPnUYkN+/H0z9R2qCd7X8tbraxmn2h/oSANo3G5Zd0uDn0r6w/I7t9Z99a/8Jt4/dhhL4WmsfNbs4jZ5KG7rt08gva7QvCBR02eWQhXX74uUpa4y7OM1CHPK5ZG9Ddh/A4AK7eS/yB7H8mdF106OPB2gzKuU8l2OR/TG7VmD5hQv68BBdZ+51Gedk0FWSxY6+GuhlLO9A87Ap8xqA1dXVy3v3XB/dv7mK803MITse6LnLZWJZlsw+0fw97l+u+WnWplu0LwrtWUex1QYLKPNAzpw83NqXIRcdX1d5ym+OtOxooAMkyxUU1pzckX/2mp3R5hWJnPayyt4JtJdTdv/8FGt+Rk8OyuwBNKsjuBrBmc0nfuQHZp526Gym6yx/Du056A4aMw4gzmdZEkOel1PwGgzY3D82sn7xwZUHx/e157z/ScheOdUT8Kck+PClwoPvlV0Z4GO9H0v9IoByaf9LWf1ifDkZ8ntRvZY9lfyM1FM6T4mQfKcnL+WR7K2iA9lcggEsrzqN33p9tnw5ZNdJj06h7HinHAp6Cvkh1NZ/0PjN7pKXHHq4WF4DtxmE01J2CkuZQ1cP/OvND4F+NsHm0Nr0zPzsiSM37kxvgo5+cOUChJcLxzm4HoP7N3/UUm1Obx6dNr4S4CfRP7WkrovOMWgK54sLfBL2LwM6+s0fD/7c5EwFc5dO0BEZ165SZ2cXdnZR9dr4az91UGPgDnroCecqrez0omvLpE3LEqS5FwRQJdwej5SOtXCQJ5M/16bhWwX2zMwvLW1fPHHwjQsXJuoCGFL+u8NHazwuE6VAzd4E+ObGOHXnF457010DAwmc/Bh2J1R+LVpeN4Pyf16MGv8ZUrjlr7dNdXwq5WUV2rO8/fH5OyZXhU+cgOnhXf6vByo53THCBUJ2pfMxo2UDJDSbiwPQk41be3BnzxeflBl522j6I+kkpmMfAE4uzM4szWxfPHP1jRufvbHZj17Qm0qJyqRO5H5dSqq8LA/iUQYD+oJ8OQh+L7RtM39FQz9E6l2Qz2eyHA7Lg0yqc64+glpXwg6ah7WUQNaLmhsaGNcj3PnVwWvBFzV/ZQev7126CpIo3Uj+AOhil0TrPiV513xTHX5gVK0DgJ3c3D83u710a/vamfeO3JjcOnB5VXvxfIbBKQGIDhH3keT9rKsH/Pvr5kOAhXVV9zAKmtn1TesnAAoV+D/kxwY/b1eI5p08/GdJb6EbXGiuh0zxQGMnuEO5DN62mKATWnoO97t1HVIaQnGnFTyITngRfFImVYFr8TtvMGB170/OHV67ePWNQ1fOnDnz3i/+/caFs1sX/v2PayM/ubwajRbDI9sXoJ0Na3hnfz8EVXHHRR+liq4LQaJGC0iO1iyLI6rHeDLXhjB4YELFLui06M/AJEdyo+OqGLRnArJaEdazdlbVHuP5zBCQYzgrhvKnwlUzd8FB/8eHFs0E8lZQz3GptBEcbaBPqT/TxeaeA2t3f3Hj//v5hcnJOzduvPHujRt37lyYXLn9wQe3t1b+17t3x1/btwpupdo3I2//88q7rXE7sn3WT6AdRtKH3y+r2sqF53b5zDJfD/UfDUHRmX9EYVnIfUb+s3Q5AO7BeT4vw353Rec7K56zcesAbss5VbvBBZrMmw32qExFdzKB9C3ZkQpJw26b5hIYaELBeTVMpQhOSWhfVf3sag+BvW9OH3r7wuTZs2cnJycv3KluF9Lt7MrW7eL2we3bW2fvvLe2cdnMsAr4owfuZcTtbFe9RHEERBeiH3TrvC1s0NyATyoq5B+Q5ErTfQ90UkBtHc0KXRqFG1ZJX+jyDP+V82iel/JRc5t58/mozst2qhHC/tgVo+GHqDVbx+ftBgfh6RkuLNsOrQjdy6/N35g8u3K2uE1eSKH7dhu8KZ5XVra2ygj+3+nXyts3D1wuv806Dn/Xy1pXk7vjvbqqE7lKOlYwO1VHpt2Oj0FQ95M1VtBw03vlJVDH/Wi4QDsOnh5or03tGFcP+fahvW8vH2fxTIXWEWiRBVnX0h6q2Rfb725PVPAD0LdklYrlj2f0z1IygFa4CB+iTLyrq/vHj0yufFZFbhG6b98oC4Z+9E6W8dsEcJGDL9zcWAXQg8xfwY+tP5ZfV/TmZPez+B1AdMbJo1n2Hpr7Xd6ONhIoOmjBoYMyQjbAz9OycSCyT9nn2WyoJOgA3e/Lhjrfw+TQAH74Hp/6+UKB13Om9WT2I6johyb86DTS1ygZwBWGinXhtt7/yH6xuzl28cLK2ckm5d648e4bR95Itxvp9na/epgsI/izIoDLGP7g9rs/27sKipXog4nONw4XwofAPUXr/A8WvTc7/D0f01FzZSZD2RxEkI+iZIOSXZ+mI1qzYJRGH59prCEqEmlmxitMB1OioVn5x55J34kcliH9PvzuKdtwgFEtJssOnVfr0ivHlplJqSMbuKz7zM4SEJagOPlXR7cvFEVulXBvvHHkyJGjR+pbHcE37pRBXOXgFL9lCt5K4ftvRfVQZG7w8SV9m3FrBEGEGAToggyOYDpjBdwIKc8o/I4Cef+ezWF5oE/nsDZDeeDme1JwjjLjsMjRe7oTB0N/fFdHoAma2HCfam5WAGlyeuaORpPVqG4XAemUGavDc3UwmibfQwn4UpfLwbOQcwVSElFBBkvQm5F36xq3SLhHDx49evRguh1tblUMpwCu64gmBRdVcKp+t/es1u2eaSPMSM98V85oFpOFRzAZVsQMnyzGn2sXPErgc1k05ZPXPDrAYCvCMDH+EjQn5yxnmuzdJoeG+VR15gttnp7TtNTBNNps2MtRaFBgLnZoCTobOQStCnQuAN9cw7cq3N9DoGiv+Mrq/pkLk0Wl8EYRuIcOHbqa/nelfztx9VAVxkfeaPJwWUT8r7IKLsP3/xzYTJk3HnII2MQh2MI5bfiqCTvlJi7hm4COKXQw/OUlPfXhyBOqYJAcKhsEUsn3B1REwYPqCKoIKFqMygzLAWigpKyndYkqkwXJDlsen57pPPO5Qt52+PW1nzju2KqjI4rkSjkPAJu7379QRG4RuFevnChuaS9xZjbdHsw+ePAg/f3KlatXrxaZuMzHZRJ+OxURP//5hf9VNHFbt89O7S3g6+lmijCUCRo6BlzgYSdgQTFm0RKuYyYYvmrIu+jWFATIl7FVHtswEM8gx0YBMt/Oama4SZf5ItyBBqj8i9YeOYQZ0PlBUzaAy0feTrsloQPsBosedKzCdGUJPydCgKGTEOmYQpT3OX++KFUvj/zizo03UlwWgftgdq68XUz/S7f0p9kifovbiSKAUx6+cvVgUUeUVcTbZQWRwjeVDvuqFYcb9skxhSB09MW7mW28woScRBAIgwXbx3b4FJWLhJRw7XgWXbrgUIJCFqVZWc9hDkYVQwZ1Emp5E+SeiFsp8NKoXlJYvBmlMbQDnoHndZB6ljo0bUN5M5L3ImZ8RZvstvysEtqcnkyxu3f8yNvvlpH74I9F1M7Pz2/P1Lft+fmLc3ercJ4tUnAZxEUZUeTfI2UfV9a/RfTO7VstmrZezkdAvsGjk0XWLdkxC7gTEfKh0TYT+TKNIi9/J82XpzL8l8ZWA9pkU+FGrr6S42gzgfDkH0nW6RDBjAYkOqJhZBXhyHijm0Eic8QculbsntVmkIK2a50hzXVHGQ0EWE/EKwIEkAEAOI+TJ/eOH01p99CJ92dnU66twnZ6em1turgV4XuxvhU5eHa2KiNSIVyk36J+eDdl3zL5bq3M70UdvBZTYhyGA9HWIkAK7HT+eNjKTmtKoGuJgyz689yVg7Bz4h9VBnKxwoiCBdlngcd8HfNT3mBDAIHU+GVJnkOiedReltzyrsNjZxiE3NXLdUCHwu1cRIVymChYJwgnBqzg/MmTlxcPplL3vffvFjm3Ctu14lf5exW9Kf2mWxG+ZRlRpeBUPKTGrk6/KXxT8t06O3M5WLdhh791bcNgHVtkxPRGlxSAzjUbutaANGlzo3Yes/JKDn6fDCUZcakbrvBAZ0uwk5ATIloj58On7HLouWuJUJboyg224yTCsSWCiFf4s6uyed3Tta31DKHz5zdHjh45eOXEmZvXilqhCN318an19HsVv9NV9VB8bbsK4Cp8Z5sALqrfN+ra4ezW5MIm8K/sdc3ijXk0M4+Q/gG4ATv1bN1baRkpGgR9Yz6QIPwxaKoFDX/h2Hh+NRUw9qAEJjAEkyk0MuN3fM4ebwyMirlO6CNePRDoxPYFsOt/KfMqY6PjwwSweeDQGwevvH/35rXt7ZnptfWp8eI2lW7r6bZWVQ5VIVHVwNvz1+oKoppCXK1HDyXq7OzWjd2rHYTtCFgB2zEjhpCbf+nd8d1fZ62he1eFw/ny04EKOoI3WwYTuU/XbAF0XPdLAbieqUl5toerzuvMyyUDAp70jiGDbtgN0JmUHRfPPLLarV8ohytKuf/V1x+8e+jE7Ny17VtLS2tT4wuLiwvjCwvj1a3IwEXynW5uM9Nl/KYIvlhn36J5O1qFb1E5rGyd2B8DjPCKSxg7/Bt8bRpPhj2Deadw9U8sP0U1fMF8hmjpnlUG0ugBAinMF/u6Ns8nvgwQE5CZ7AKh8IS8Mu8BFBK6AnLokZy9E8JPQMPmrNzv+E7jLjnry0HUMxIdyeAxOVAZMODy2o2DJ2ZvbqfYXS6S7kJxW0wRnP5XxPBUnX2rSrjNw/P9IVqRfA8dreveC5NbZ8c3oWQkMAbXRBRF35occpu/QgIP+PcHcj/GLEVvDqNyaDvtGAoenAuBtRGFSEe75h4hk5chCl8Ogu9EkzpUI00Iow1Lj8tzri8EISMwUgcCheurs3LGDUfk/OMr0+UHg9LHo7sBwOqBI0cf3L22vbRUxG4ZuIcPLza3wwtlAbFe3qaqUqKJ4Pl6/jBXJN+ydKjq3rNbb48R3ivqoRVP42fXnUCcUOmiG38TP4XwxNfxHWsLWUeZ6l6cg0oRWbobXUQwOXqWDuvE3Mr4nXCc0V7e7iq42WHjgWAnRAyGPPlavu/sAvB31LddW7hoCJc3HwkB+f6RE3PzqdadSmn38P3791PIXjpd3hZPLy6mfygL4PH21vRx04mS2YzPHhRtWzl0KMgWW8XEYTVmY+lyC/y2+a+oGEQOpoan7/NSSZnQKlgAR/WnHR9dQz7QubTIBvuAn5fmehykGZaPbgGhy5kDMZjgcWAK+pJhX/8z6IUzAtD6xJQACO0d/D7dnLTWK1pA3juGLR9xywMeYhW8gwfPlLG7XhS7i4spZi/VsTtyaWTk9GIRvPfHjx9vCopUSaT8Oz5VlcLb17bL2uFBOXQogzdF79adsSJ4EW/SHNjCnFpbfjj7ytDcXEXRK25y6xZjAS3QERx4OalbBQd8JAEuSr4gUFgOSIIg2wUvpjNpEJEpbFWJYskXUS/K27QCoho+r+/ytRsU+2r083JpEilVHb2DOVpGYA0qjfMuoX/Jre6dP5Emu2tVo5Zy7eBgCtvB9lYl3+KWwvbwwmL6ldq5upOrq4c6eg8dreveNHFY21zNXzFpakmnkD1JI9x4LhmY0wXNjfVzthshz6mlzcHaUK6A1+3y++guxIFHu+QwdSiwKu9WDIpAdAiPvF4wmbvBlbg6istr2h4Dl0g5hvXKzPHIYxKZe4dceZBjf2n1jIDhkh2GgAo46roGwNCD7bLYLWN3JMVtFbmXBgfPDQ6fGx4sg7kM3sWiEi6r4WoU0cwhtq+l8J2tyt5y5nDnzuTWjf04SdeKcf7nVAfB9TvaAEIyrRDPCFNA+Nts+kSqdEF1IvImCordma3ESp0WfJbSU5vHrsm7Ek6xwNJKgm+1CN9mTcPmZ2V6FeYEH+PxQY4qUJKfLxDByiVwCCluCMBXd564lc9d6zitz04vLxcVQRG7I2XgnjqVfjs3MVzdJsr4Xbxfd3Ap96YurhpDVMm33B4XqbeZ96aRw8rKyCroczDiF1skl5MPRWm8ko1iQpm8HHMLR9JyoHIqHvLSlng6efZRCQ8jWcBORrscltY1Dg4AoJBliWAWlHcTNJQ0NqleVi+Uw9qZMihM3W5xFmOhUFELYOinr/kMiJVcofD+7LTaPz+zNl6n3Sp0J84NT6SUe2DXgYHh4r8yegdHiv5tsfiVpd6pqaZySNFbjBwOVWXv22ngMLdJJydMdYLzZwS460un19hJzIGZ3JBRUY4JkHMQTpcrUgtFPIDWA7xrMO3Wz7msMSgRe1ozjUS5pKFOT6ngKgNdCSz79RVNNCFSsszNhDBX4LfBoGGk0NSl+2N4EJM/HUlB6fwAHuG1uVTtppIgtWdV6Ba3lG93DTS3MvvWAfyzcgBR1L1V8K436+My9aaRw6Fi4vBumjis3NgrEJTgg2cRJX90qNy0BcsjGOEImdxpyko01/0Qe8iioaKjgznNVMUzhDgwuPWYx4Y6RCQP6pxalaKfjWgi7qDosZoPPAQnH61nXShzgXPSMRAwTbU0ZQQfiZ6YzAeDoT01t8j3Gotz60XsLpaxO9GE7kAbugO7BprsW6TfOvEutNu3MvemkW+5rSibtiJ4z06OcYukhGGl+hoY/2nCyLVczcRUxVQWPqzfSrNTyHAcqlebg0cjcJc/wiMWulNXVMA7/KNZ/E9yzXOLqGoOBkHR51dTD68UAADJSDv4gyi1mLndizDIjfiHEKlShXkgaB3MHKWp/jGrazNF4q3SbhG2VaXbBu+u4Sr5nivCugjfouodn2oTb72wKMa9Rdl7pdq03ZlcWciFWcBzPd7xe4CrifxXrrXH16ywH3LALwxOSxNG7aMJFNq1xMIyjsGKDo4oMYgQ9QuzAMFj1pVqEe2IlUgmOpWyWOgFWkqIWn1Vs8xUCSHVAOOls3LBVXuMxyaiNnjmTEKKqvXQ/4dHl7eXxlPerdNu3aIV8TrURO+BgTcHDhS3qnNLU4fjx48X67bjx6eW15aWZmaKX9tl6i15FtXA4cLKXDYiE7F8gtt7WQp37JsbgErLzgdSAPV3kpqA2AN4Qn6wDHw1LsdBF91D+5pbdqNMHA0vBdsJkQZDwALqj8p2QjF5FXRBQABw6sqqRi2kFERLcVIWcBtvTnu6h62D4xGOXVyaur84MkjBOzCwu4zbKoDfPPDaawcOnCtHEGXwjlfBW9yWlqaXitvMTBO8J64cLPZsKXiPCukj2CLomeCLLXOC6F4QUcRkSb2b9esDbKUvNMFEtdBnQnb7EChxwGcQ+bpwpQ/qOIle4UBVxHF2QrA0gGxr4F53vQBEjy5vkRNdcU2y4iu8UHugwAeErCQolZ4nII9w7uLx8bJoyIrdofK/3WXsDg28ufHTjXMHDpxKwVuUvCnxpo3b1PL6+PJaEbjT6beaalED1K8eLOqGC5/d2PTMRXNVQq6aF4yJtBRWFhwdpuZmCNDpEq8toJKMOcAhrBGM6FRCL+pCXPhSGYIMgwxKXZXNQsZevjAEfzhUZ89zoHXswyM8bVl00kqyh4EnBq0QdXGd78zBezTqffMDOf8OjMwcv79YBe+5fsFQRm3x25vp18bar/7xySd/f+3cqf66IlW7y8WtqHfXaohvGjc0qfdQGbxn71zOTayYTWMBpshREXh9xkvKXDGG5k6qJSkddD7xAalQqsgHNxYiTYdI8sCpjljEvOLVGxjeIRtBYR1A7ZeE2a8oNzmOURMLXeYEof9kBEksTB3+ho4ioZo5aYznXaADdDqJctVnq//yaPXwdGrXytitC4ayVBhKtyYBL/79y3T70+ipc+eK3FsCdYrYXaqDt9yxbVcEobLoLVq2ctzwOhg5Cgi8UBoEpQowUoXDgIcKJmes2mTEmKbIFYOkG2QeaVKW5GRPR68jaITKlgImgk5gPy+DmjzEkCUe7amLhpr6oNehEW9B+ywawNDuga5jSGsKHfKaBwSaPG3ONsY6f9B9MmCbUyl4T9eDhnbIsLGxUfzf7t1DA3sufPLll3/769bogYEDKX4HT1+6f/9wEb1rKX5T7FYAyZkseBOyt8y8Z49Ray/+LoLwagMC5mXMqEwkVQ0VxclPtkChkUYCSiGAKqcHI13ICNa6jCIk3SDAvojMQqQvKaWDW9ZA4bUWbRX7z64Hv4wVYZCIERHsCEJicZA0HbgRTroI4ogWnWwyWar+1ARvlXib2F0/cuPd8YHdJ96+8WD9yu8++vKj3xw9t3vt7Q/+cPvfp04fvr94bfKXv/7PrV8Uc7L3tv7zN7/+4O25quatZB0OHi3hDWfHeKYVOdLlXwjcMN0E3STRoYMLpWzKwB7Esyiwg15Gx0ifJJ0cC1FVb2HeLIMHcYH6AvOdRVnavNsmtLHKfnhPMIUhExh+CwzhaTqIBwSQZ2oUobKwqozhBacQYREJHLO5VgXvcJ54xz746pO/HdkY+OvHn/z37X98lIqGj//0k3f//kmK4q/+79z90+/+Kf3xy4//Ork2tfLXj9OXP/rHr2dnquAt+JgHq7Lh7Fg2E9BdoooaeGebYO8P8uxzKkV+hCyDTwLoMfAm3J2Zt7r0W1XGdwHsyNgxwdYiz0JryJCsB2+XJkeWhTRjq0RHFGvurg3SjYdIBEJRNg7NGl5cIkeSj4Hg3lulbQsWtn3GTfCey2J3aPh3X375ydz16RSX//3LMjg//t3df6RwLcL3N4tL/5P++I/073+6+27xr1+lP351droZNqSa92AVvMfoPIPvVXKNAY/l944onJvFUJX3ZMZTXvG4jOC0ekEwIBbqE5YrJxvrWNKAlFdeYEiqHp3SqYrhoSiTWJeSUuB8Vb/wHngDZOJiqCK0pK7MyE/aI0MoJ7loiqNvCZRC1F+YhMJ+TSxH86gJ3nJKNpRq3NSobaz/9csv/2dx9E6K2l/O/78iSj94709ffvnF7cn0+z+2f57S7t+P/vqrT/509Q9/+/hvt9/9fynW/2O6wPSeKfq1q2XDNlk2bBlMV4yOQbjqXI8OQqFC7j1hOjmVnTetOHI5Sia8qTy16+pIItZhEUi011RRGSr4ASe1A8S0DLYjhcVmE64qDqlA/tHQY7cs8JLOU6dgyhhhxLzjf7Kdu3nrW5JKU94aSdTCG6Dx0Zcy70y/bBjaGLs+trF79/WrKZ/+7sC+X6eYfHvf7Y+//Ghr/5GUc/8+efa/P/ry46OTKRd/9bvf/Hrrzsy/ffCb30yupJD+5HYRvGfOlP1aXTZc2GuKMaSNCQ8iGcFggQsO43dY0kDRZ+FOWnHgcCoHCuXWfhC+aw7/0blf4NX7Ou7V+QdEck88BFZFcjmA6y/0nNuUlFxCpTbVzVe0Igkre56Oo3cQuhhqe27GokDUC3ipw9Wp+ak68w7sTsF7/frY2J6zab7wh917izQ7vftXH335yZH9vykK308+SVn44zvbXxSzs4+/+tXFqZW/f/HVJ0UB/I87M0XsljqSdfCuvL3J5BABGpt3KhHt5xzNQHq6MOJDm8JIpERWRUpVZXdwM/ZsYm9sHtar+gxdMHz0ySfKSuss4cc6TqoYjkCbhO1N4Raz9bPvhYhwKhq8RQFU/52ZllxvgTFY4gaAYJoBYjIrFwbo9IR7hJ/NLfeDd6wI3nT7Q8qvP9+z8bcvv/zrwEKa8n4xs+e/i67sH//44osv/npw6L3ffVV0cZ988MFX6Z+/+iKF9F+vzJexe6JSL0vThsmto7wAA/wFnHOeZH1LhHUBQJDAgps5Cugfju0vMqSR8mHHOax27oEpUYQXC9nQbpXWpfuvdOcO8ZOA5ejgQL0dnWXyCYhjqitjCU56XeA6zKHPuxVA3CgQmCASEpt683YDcK4M3qrkrYJ3tOzX7q4WJe//fX02pdm/Tx1LwfvV+1PXLnzwwZ0jv/nVbw7dSQXER79LtfHfzt69kwqL381fnC1ityp5j76ROJi3Z5UYKjgbOJtX3eiHukCATAO4+KWNlHn6udq95959LGQAZ5Ij9pfMxgDPzoRSSMcGPP4hko40ocqbCup63R3VppHuruckJ8QfmiSFecnuTOw8Fyj3v6MT00SKJds6h5hV5bCpp0X10I+OzS6NJ1zOcD/zju4fSfXCR7/7z5R4P7q97076v1+PjP0y1Qm/nvvlVx99/MvJFKt/mP5DEbxfFP3b3XT3j1O/Nttm3rLkvT3OO1g34yUoOLtCAM4tSmAB/ND0buanPYOdAQYpqWp+VH/GWVCplSJ2HkE0oqlYiOd1+5RYM1IzNITOgWA814sV4ci1g0H8UKyYMAfoSndKhRHa313TICSEKUM27+HovgkSObs9XqXeFLwpdEdH9wz87sv69vHV6/+RgnTl1PD4V8XELP364r31fxSzs6LOXflrUTwUs7S/XZgpZg1nqrxbgcq2NkS6xnzDld1DlIVBEwinkU8zJ9UpCh7A4P0oeGhFRA7F8QbbClZMgmc+kqlvAHWEjBS86kS0S3CyI4FMMDds+YHUg4nHMZdpJIURajbCdloLeQAVvL5IrGjrzazcsEWqk0ePVtfmlsfr4C1jd/T66+//TxGlf/3oo/+ZGP7VRx998d7wyNCD/ylC96M/HRwZLIa76Y9frCxsFSH98RfpLqlfS7F7pi8YmbDod/azAhVj56BvAJz/DA/nwWN4dAhjAq+mCgQiRnBiGISaECkN0odhtLzbUUcGAIoIZ05vJEuRvwWmxjiQWbFTpkSrjB4L8wa8JF3oiQUorXUBE4qQm4qLOL43DIRrHCWZU3lRf+vAmaWpqm4YKmN3z/Xrrx9e+Y+z58avnJh5bXjm6NG7CbdzemDk53/49X+8uziyMD6ytvXr3/zh7PzU9NSRP/zq1+/eTcZXV8rEe+JqMeM9UlQNk1uzm4rQNTdzyVkqPAZQ/TULhX9M1M0CDxooKYAXfvp9ua6AeeCgLO3U+D2Cest8nlA5Ha4ZkArREyYsYE9LF6UgzFa3IUQjeLquMplU/CkfdSkDX4qxcGFIKsL5XkjzEbNR8jpk793tqcUq9Y6l0N1T5N49lzcv79mzf/+egeHXNsY2KgLbmxsbQ8OnC97w4sS5UyML6wWk7PjCwtr29PR8KXZaj8mOlCuKrcVVnmiFaDhWmRCkriwvBDOHcMrF5tmyROLrKFQWAc/GvWsUG2iR0DgdexA3MsSClRGAQu3dwYFEmjyKa+zeZDQmguqWLVaApmRmC6Z5ASokEIo2F5GsMIWwLEEs7Snz+IbENre2UA7LBjaK4N0zWgx7i/82NhKobLiA7NTU4Ux4rxHtTXCc+VIup9QcuVqL/CdI2daFPUJqtIAdYzwGhzkonIwnROsB5nwnjetpcyQ60wmPCiHA+6moVp/5s9lLoFiAzRUEWsexophyuCI4dkplbwevhWq9ThcJ3YQZe0aojRbECIVAqSox4KZePIVnYzjZa7NKK52wAHDuwXQxb0jRu/t6E7zlrQreRnZkcGSklWyo5BoKIOR8rXJaapVdrQX+U7t2++7lVTh5ex3OQmS+oPMrnrV4lo5iR8S2mQ4/lrkikQzI7NUCFLA5JoZ5w/TwXESHfKWMfiNmGpWR5rbU3kciYg+3l0zPYpmm7vMAgfq02p9QZItKoDwFBwl0x6kD5+lLJD2on56YX69Sb1n0lnXD9TL9pugdKPnEBWt4pMq8SS+nUImsKMPzrcFKFbyVudWNVPGunCptXE0h1rJ0FG1CeOU6faPh8Khg0yAvs2XETnWls0hFOpKoCQGWJJGCZZzg2IzaEpgsK1ixhMoAgqcY+4ayia2AkOE0deu/9Mzr5XDxz17t7tpnVzRSNhBpLF/+8owyZE1LecBQHnWHMQCX5x6slak3Fb1Vy1YUvuWiuEm9E41kw0It81T7VMw34rwPHszWqIajR6oh79H9WAWZ3YtqGWTrydaKvF5jIHd2duSPyZWrwy6QobhzwgXIGtuEWRzo9ZtFRGGIMXVIr+yc83oD8Jh2HJl/B9LDDtqfETDh5dekpQwsBoCgrAHElcCCMsaNskVLW1W+WCrLgml69Wtz/ND0VFU3bPSDt0q9Y1XwTgz3g7c2q1grmGvbJX2irHdnKxR6UzVMrqyMb646yphpMUvLe4E8eGpZ2EyAMDdK8iJQZFZpSCRHW4RIgjqkVkI+UnU2sUgxRzZsdCJZZB3diehx0iQQ/05DsB4OPGeYmhRbn0CXjBaJ8Ua2VMGAJIbehGws7Uj7b+DqwNH59Sp4h64fOzbajBzK1JsYbSnvlpm3LBtKadO+QVBZNjyovDFP5MG7deMYgFXTzbgfVkP3k2F+0U5a3jEmwYguHAyByStkDhMtS0NvSAsoyAg9bvwL7fDOgQwbgq5KDOTlXoh/shPZ6i8pHLmGnOz5CteFA62ViG3GSEeDc58QfV+Z40MQgNLEG3T9DRj2n0h1QwmLHLheJd7ilga+Zcc2MNwI9Y4sVkXD+lrjD7Rdm1JUrq5V8Jb0tZX5yyJuByXZQVQ+2S4v342zIBYPxvmQcSenqs0HaniU/P3VABXTtx1O9dCL0jVsTltMwGMil24xpd01iQJyULnMftnQIZhPRuRs+E2D9wgkwuVhJnrOxkQc1P7jYsk+ej7sL5M115fXrqR5QwreiYGUbvc0wTtaFb1Dw4Mjp4p+rZ95a3OVmdoXsw3e5CZYieV8NnlK3FGIkZCTE9htRYaI4AqWoGUCOyP9aUKhmYD0AR2xaWMOFgsJxXEcYcwtNUJPkUDNdmf9nS7niuh+bgruJhw9CM9Kl5OkUAAXxUzCgivUjbWbjH0M2HdRbIhF74r5AyajuPbD3hy+Ml2BegcKdEMduz8dvf755xu7P//tO6dOXbp0/9LCSPF/48lUpZDHmV+6dStLvTXl/VCzGr4xJsQJ8uShPVeHV5PXmYDoOuYrM6dnBbHfYZErbhyhnUXQZLl2jVYaYUlqntMQaASHfsdeCl1sUvx1JIraivvtb9jYFi5iC/rpjhepCkAYurvGDl6WKqcHBJzYDjYzVzFY3TNbINJPp7qh6NiazDs2loJ3Y+i37zwcHPnZ6YfHjy8UKk+V2sjSdOYHVFu5ZsG79WAfrYEdAD/i9waj+sj1MnjdTtnBQUKADnhJh9ujUwvGKzS+vJkRVCxJ9PAigg86RMNMLGkD6pHKssXalD2ILABLqcETMOS98pZvUd0NB2JSs1DTwbZH6QVvPhw6Ctg7PbteBG+xpjjWRG855y2q3iSTM/Lw+OPH8/OPH0+vJS/Bx+tTqXJ4/Of5pcoP/qIEbyp5Zzaxg92UGQJp2tDcK+a5IMJv7WAvZaFfu3X8qEjOMVTiM4vwiU73IdjQwVFMWXVFqI6uZepaL/sOkmdTPZo7B5bf7F3ioouBx53YEwjEOa/+rOuaEGk9JyljHuxUEtkWH6xVmXeIg3f3xptDuwYvXRqfvvbH7757Udy+u3lr7XG6LVVOmNvz/cx7ogzef0/B+9nkz1aJ8intLNGhPYXPTVCZh8PccT9ZYhsmePU4kUKnKb+Tzoi8IUKsA7DDdig0m4PT51ODCNnteUX9LqImdO/X37CpzwO4rWX0tJrXm49mxt7RDjlX8IVOAZ0Es5CZuSUileCcG4uTm8MPEiL9dDVu6Be9Reb9/Lepali/dfPFjy//+fTZs+fPnv3w5PsXN5dS8K6Vs95aKKcO3oNV8K7cGaDNNgO/qRQ3UyFnGSop2sC5VagiH5ke5UTNOGFGkusOGIsozyG2JnOyY84Xjx3eA9qoymiGChYxHM2JIfBKrRdIvuhOwQHuiAXnRldQFp2MteEziRo6MWoCAh/VPbuxvuLqRkKkN7Oy6/W47ProsTJ2Fx6fefHyh2fP771178N0u/f8+bMnP363/DgNzGY4eGtUTurX3hgD1PbMROzKWANPlxdEIeSGTRtVf0GQ75do8JjrGy2i20BTjR7+sbRtyPcNig3wS2HIeIRwlNlFCMEKfLjloOgZJxUaHiN4TKKP5jtLZxQBGa0TSxYWVUBwCYClUh00Tp1tzLC6Ojq3Xc7KhgdKElu1pjg2eiyNGsZvfffyh+f37t37S7q9lQL43r3n9549eXFr/fF0sojfzoO3yrwpeK/uX1VmpQyrQ9QncZxB3CiiQBgj/8kRHMwMcMlPB2oQGBPiZQMiFBYCRafY+coNa714KbrTuyjfsjsZYnH/AO6S6TZ0A4nMI8OD5iCQtkJocM6FvJOqNij51iuaueODAA+rq6/PX5vqB2+/bEjB+87xWz/+89nzt9566y9/qaL3rRTHH374/On3Kflq5i0XbGnY8Nns3i4Ju3iooKPRYFvmxNr8mEIlMpz2VSC2HR3wRK30+0pJNG7bFWEfjTV1TWWmHGqbALfQ7ibM+GoHKJBgNHhe2cRwvwYHdmYhGFFayDmnMKeUpbA8p8pC1IocZqWkWsgELttX7Z+ZmyqJbAUevcQ2FA3bsY3h4zd//OF5E7epcCj+l0qHlH+fvfxueX26nvQmpZy6bPi3Eohe7teE1SoUZpjsEM27HGbFj3RqclAGw035+CKJPH1zvAo7nONvxAeAeZmcnSYQ5uCXHVoK8XQZHQ7ksS41Fxk9WJdtPGPwEJmC8ULIxG+FJM9ylowv10TDDs6xiWCgAjNro/oRAJzcN10G73CJR28GvdfHhhau9WO3SLpl+JaZt0i+T747/nj71q1rSVP67pl+w1Zm3plNQIWljTS+LLLrY7CXymCb03uSTkJxudGmMqepOvUnX21bF+RmB2C4R4lHVgyhC5a9KiRJNcY5wMFC9QC2sgoVeE1bN3OiZsLP1lmCqBEroppNyRBo6cGXBeqgwvwL4BEenT+JvWt3p+4PNsFbh+/oxsOlF/3YLYO3qRo+ff7hpx8+f3lreWkmBe/c3N0/NsFblg2T06sxnI415vQi9KYarvdWYSsEKuYKVIIwbp1/FWmVOJ/JyKFBz91QJoS9h2IoOuv2RABAxFMxlrgWvA7iibO1sv7M1TVOt9Lxqu87D74EwAkE8v2guQ7N0hgfrKrJDutBXXp92ztVS48MbBSYhip4f/ra4++e9GM3S79F9Kbb82ffL6/PzKTgnW0y76F+8BIxTVGDUi6AtZSysYloCBH4RidB8JIrhO6FgwUTIkeFHSNFMHTbpJlPtk6ppGOXEm5qWUVSiKoW8paCFtBjGyzoETwjMia7RrSGDsq2G9yb045ng1ylvhk7VfCQpLmwHgHncfLy1Jnlumwo690Sl3Ps4dz337zlg7cYOaTo/f3vnz99cfjx/LWbc3XNWwXvG1XmNfOKMqFuZ8yGISlwRO0xOQj7iU+XS5kQB/3UC11rgBBIGzw1GYBFc2MGsBg6FuDm1Xn8QrZDYEHslxoOm65nDNKmqoGSN1aRPYc4DENIJcJ9MHZqYnkZ0YPi9woyeqq/+eTJvf3gHetDG44Nrb/44R6HbvFfVTrcS8H76fMnt9b/XAZvf0lRQhs+m95EDzBC30g0qgqrKuQ7hTO4dprFSqk4hvOhccAgy7V0wOYecVoMCJixrk4nM3IHxRz28+7Sy7FoUd1Fr1CJsxwS6UXG4D1fo+E2IiaIH+iBifGIhBlYNAmRAjcJOMjso+zXzqfgXburwbvn84czL5/9RW913fvW87JyePbi8J+3b87912zFpDhU6UNOnp3Z7BErNKfNmSj2iouPqY4TYM62nneF6HjpDkoMfXdJ0dBpkCslAoFlhJqQdUEdgxGJddErOjwyzTeJYZUd23XC2ppXgA+K/nSFtBerhJ6AOaQa8CrEYJ591AXrg+dDKATmUQDwCCexb22uCd49BQOzyLyfL0jifaspGlLwPn+rmDh8+taT5ePz11Lw/rFmUpQbtgufzW+aKDERfBGK7PMAQMizlLZKDq8ATymSbnmDHL1VzlzAQcJoBxtg+OBhBuFeGSEyRcAprtzxtimxsSGPWd16uxdaaRqr1Bj3HWxjwkIVsdoAW+JK0+UVL+Dcw8Q0QTN3822PyuDdP31tqh+81bBh9J0pSbx10XCvmpcVq+JPP3z23ULq2P5rrgzeE2XwFvTLuctmCBxR8pEsvSxRGDbRJGUReiCEz8Eb77AyZz7WheO6BARVKTa9OpcO5rnkRGxsItsotdZxntEs6QhZnKBD4pQdTJof0wu1f2LWmphdwCk8WOD/pvv9Th1V794iF68TitH3Hej10qjs5P6Za1OLdfA2aN53/vj18ypmOfFW44Y05/3w029///z702tl8NZFb515T+w9f54Fs9kHmbtOpWM7+jS6YLTOddt9jILEQqSPKDg+onubwPtzsjsEeSxLeu8SkDcgORnfqZs5HDgi4xGLUMbO746irseQomiP7Gzj1JAoSDye1+sWSBAHPpGkhdsbR5hXNSTpWQrePdsJ2zBSKD41LKDRodMvnpaR226G/9JUDQU+59tvv/nm6dNvn1x6PN9QKSpwQwreswdfPw9d+6scEETgmcfgZB0swt+xTQNMtWkCSXJdcIg6g/tmV2oivJhgwXoYvipADIGX2QXCKRXkUpIPVkvq0GrNen5m6yD0OkR3Yy4gVGFRm1owpY5mnmpUhUDPSF+r8yLrldOG1WPbM7VS5PUG2DB8//tndfDWt7/0txTFqCxF7tdf//Obp98dn68pmCl4rx48WAbvu2O8BzSotgRChTupGiFts2gDsUKDZ7qyC5zOmY25gd511y3oLdiJeRcu51cQeQ+7/YFoFNDAyZErdxgtGKIxLvLMCwcrZxlE6F8YpCsrJAI6sn8Pb/ehyhu6RYO6OhG2wPK2v/6GXi9NG1Z3X1taGMmDd8/1ieWXz8use4+i914NzPn2aRm8T5+9eDjTz7y1HUVyHX7z5HkyistFXyBDPtBIDOrBygxOgxobMcmauJcKkiDZB15NgKGpAeOXVXWkU2KYHLyWZLBhY7wyNYROuVQwHI7oI7tsRP/YZw8jph2xAKvooyvux5FZOwZLfvQuDq+O5kLtERvHsppDEbtWgNGvLVfBO9QG760nz9usmyL2LZ94nzz5+tmPu6br4K1UR4oV29kLp+DE2eHE81lNFoHUR6TkZQqTgMjyqP8E7RsJTAgxUrfIZUJ6JYtVynVz1CUTogL1WqtGQ1Y4gykE7EeSBiI1xgwD0ZMhhAqGdJB6YiYK4MobRBxJRl6Llp7uqr1BtLfpaxwRez3D6ubItUIyJ22H+8E7Nnjzn22tcK8M3r+0sdsE75Nn3w+tVW7vzazsaDHonVo9T0CEoP1SpDjvW0nb3aGho+mTI1FRlxQwzxzhCvHHBxGl5T4IStqN1l6wDrCvM9qN5T11/4agw/ei1Do+6ZsIwktKKpQSxr2Z170EKaWSsKwI2MqhBFmiMYFDt24mmAEYa+Gv7h0v+rUqeOtJ2cbD734oq4QsePu4nBS9dew++ebJm8sJE3lmtvRtLZX2UtG7cvcyzhuhXaCwDXFXVD0GY993iKIjA89UAQzmTYcEqYqoqQCckLlD2ZgaPKqWeEDLRLx2VpcmtxgRZxj/M6ErwUhowrkBIeJXG7xRGnvJs86yEmRYuIzKMjoYTBWpHB40lxaJIG3ts+oZTu6fnr6/OFgH77HRClGWBW8RsRy836bYLYP36T/fPFwFbxW9pY3VhZU3RnEegnE2AW5CZ1HiosK4UaWqwESh3sh8WfAF5AxKNktgpVQjBpUD5nhqsEEwBIHoSKTaYOYtNh1Kkk3nfG+GoMNUmQl6yr0Q+m8eh5eP6VkNlg0GAusfMWU1OBMm5GBHhs4GSjQMDc7033oAsDo6s3Z/pEREDo0eK4N3z+6H3z1NdUIWvPfaircoeVO3VgTvDz8cuJTkpfvBe6h0fD87OcyHgHW4yjA7TUg5EGKaUbUsmnuOcMTS1BC/J6ieiXAJhVUXyYR0ulG6Ra1X1okE+QJ5HIt2xjEQPfC/FBhGjucNaDowPwN09KkduB87SKcxIjLfyHklvRydwxW+qJ2imjZsDifNkZHBU8k4e6NZsO1++OJpqnLvleFbRmwTu/eqquGHIvG+fPL06aUUvBeb4C3WFKXqyPpmuMLsJAF1AKvgpQoQva2OShbutNwH6ukt7ieonl2XWJ4uVgLNGASIsOiTd6ZEhA11fm4BqcgZqoIImNJaqC0A5G/Gtp5gaUxKl+TzaISQFhsSBlXR0NPhrQCxJGu+1juJywvzxxeKFcXwcLNg2zO08OJpnXbrmM0Sb1E1lMGbxg1PL92vBKazWVkK3hP7AB2Adf+tS3nmX32A+LHcbrHr+02xl4zwCiV7xMs1vkJz7EXHpcuWcl5xMmpGI/GToI31FPlGJTJ3/MtjGFqQIbY1pIYVNCqEOZ1LZhzQogfMGXTzP1hgM5tdewnZMDO9sFiZYI41JKChhy+eVdOGJmzz4P3m6Q918D59tnw/kx25UndsW3fGFMfImFS/w0asf2W65BC7CkUROAcvE3sJhEcmxA7dax4F0rTwC9/IyMRYhU4+QC+knHMPZWoEL+Erq1Pp/+l+qEVHTNVkuWWCV1bnAwcxQ1a4LwgUvcJ40Mkv1ChOdDayDcLJ1Y2Lhax/GbzXG/7lxsN/e9qAyN5iDlAiAX3T9Gtp0LucZ94m9Z5dGfa2GOYV0NXoFqYfmBkT+Kl8Nx2UmyikwSLJCjgnAVfPii9pt3BwIPRlMkeywMdcpFCEFW3wWdV5VkULSWM0v1uK9FyNRmsF6GIgaBTVOSWgRfOm0YRy65SdTLxp2HWNAae0iDPD5uLF4wuldfZwf1KWat4yeO/VA4e/5KOGql+rovfrLPOWEr0Hq7rh9tomvA6SJA+Erhws1sL7IsjW1zhZOEE6JxjhdI3YjZ29zGP9P8HDK0UDbhZq8LjXvIAzZ/ArO1YhnLjdqa7T/P6teaSepyrzqB3ss6buYubUfeBIJbpIAVxghwRp0GJtBwhJ1trh8szM+EIxa0jBW4N5U/CebkZl98rY/UuWeFPJW9S8X2dlw+xcNm4oUJFbV/fl3oiiGuE0FQTvlYUa4GFnXG2oDavFWg2+HIVih+GkwXRYA/O69zo8ihHADgjXiVoKg0F2WQHJSJtDRCC8nphyQp2vwHgEmR0iUMOOIKqm2Dlj+JWK++um39OYOanV37EKXJ+bXjidBW81522Dt029Teb9/dMy835dZt5LLnhT0Xtn5c6os8igZhnmnH8FJu8g1gJydsbnAv3gxECIIEGtE4+li7KOUEiHWRrmtAMVwBBMACI90Ehkyuk6BSMb8NzL3a/nFE4D4R2dzXotMRYM0hWK2A+ztTCgZkgiislC9FD2HIPZVyfm1hdKuZzkPtwnAW08/GMWvH/h9dq3T/tlQxqVjbcNWxO8RdH7pkhaGS+uoGBIYbCJ9ZPH56m4AIMKjDk6XgHZvHg+zO/OZMEgEJlIfMH8hwP4iavDNYQj3R0lqEUL21XkgTN8T8V9ZKfNkEVBxJiM5MlzCKLnomL4Ys3EeBNBVqnkDqnp0/PYXLs4Xmfe1spqz9jpEttwr8bkNLCG/qTsaRu8y7UXWxu85bBsajPbT1BgsAexMvfFaIdIpmwH5qeUHgGeS7FQU0KTm3yOaEHwemYmLF4rhPL/CDdi1rWk8InUvGY7mxjBnGwZJFqsBuYYX+nB5I4W5yLPQpUSS2ixjWU2Q1NgLCIEXF7d8dzEPPq6HxP75sqStw7eZkkxNnjrSRa8GQy9zbwlMOeHc0uNLUUevBe23r/slUkVwZAvqx2yS1VRzQdsDqEW5wtTCUmS6yHAbKRM4pG6crjyVACOzqFdFfvBIeQFm8VTNpZyDoLSfLFCzMAIEhkYseWdgAW7ITiXZ890MNOKQ9YhTmnba7ipuEFc6QB4NHRmaXxxsD/mrbANe66n4L13r8bv6rChAvOWmffZ1weWSmxDUzZcrYN35e19J+HkwVTWxolWOKxWVBWpM4CpkBhk7aROnIi2XGrZYcHuT0hHpkAs2WEzmjxHM8jQCMFo2WJLrJgwF9EwFRiXeQ8HO2CBzboRn1psE+mHYdrmlJgD51Mokh20vechGjd27RR8gYO3Hjek4H15716OJyu5a1XNm0ZlPzTB+2Tg1rWLJYet2g+XwVuwKVbGVtm4iCjtulgURHmwHGT/SzX02mkTZ8zDFHUEdWFE4A0VYXQ7cQZiD+QjqkOBJ5A5c75VMIvNCF7Nms9RZZF0L0SYMsjOkU6TSMNABDnQJSkJEpMD2NwxD36q0lijb3V7bmm87teGCtWGOvNOTL18fq9dDJdVQxO7ReotRmUpfJ+9LIO3j22oMm8Bb7g9vnqSJ5fOnRPmbBBo+a0+PrzN4l4u1uFntWNyvlU7PdWijWxDX9U87RSUOkcIRgqAB/AAYTx3iPbxseMr8l4Im+FeS4X13VKTgZEQJgHDV93ChQASxjoIyhACkcDBdTWAR/sebFcyZcWw4XpfZu/68Pj3z3NYQ581/OGnv//006Zs+PrZ9wPb12jD1nRstx/UBq4ulzrAGY++ufty6IPg4dhP0P8z7eFEfwc6oIGx8kOHJoiT9H9VMoa5bZHzlAlypW4Yu6zZosWbn0v0uAXibBipAMteJbJ8gWKTHUwhojiLpqkM7v0qxQKoPDauLPWDd+N6f8M2uuvw99/WmbfGNTQ7iiJ4v6k7tq+f/zgxf60clZ04UTVshw7Wa4o7l1cDTr9TOneHl19DGGSj7kB0cKU1PK6Mayi6HvyTETNRyDhJQZ7KMDLauQbuseFaypg1zYevYm9N2Myq5wERFoC1DRvUjUaRlIyfV11y6LJHh5bqjgKVnJPxXKDh4jbe+gTx6NHPkpdKnnkb6vuuxR+fVd1aTl+rgvf3n37bz7wvBv987Vo5562D92DdsX22MqpuDw4wyBe+gsFob+4aLm/xxkuYGI6JWATCEyjNaYgHjAcF+4osigWeCyEfT3FJ2t96/iWPsaKxsF9b5DQgplgFuVvIv50QT5jbIaumrVhx5AwbNioT7WoTBR4eqMEMM3Nl8A7XY949jaj/wMP/8/StPHjvueBN4fv02Xf3y+CdbZcUdfBO3h4k/Wf2/IFnB+RjIDEEhVeh8To6JnWtmVeiFnEN6FxDIVIKSubuV/R5na0WIiMhXdAJtBtK2zdnmxkAd80BPALP+QbPKye8UEgkoXPDCci0T12Gg50v+W1LmQKVTDdR0wD8ZqvfXu+9O5OCd6Ts1wbaxJvADe+897T0T3mLecNV8H76TZV5047i/n8lncjZbM5bjRvuXLg9R/6oTKYTprdeo7oSBMcK4FwpSFnTwFUd3AViULtjKAOHka8GHjJ30cE1EpwNqcB4Apcf5QdZ7LFhofmc+G2KNkNPCev+MgWvH2XQyPbVUkzAlyOuKxAFTwaziNUCT+XVN97sJ+/PLPeHDXnwbrxz7WueNmSZt6kb/vnN15eW/ytl3lnJvIV79taNRCF2k/08rMSdmQTeHNqfNnHObM6vfBnLwVKpgqpVXKmpWkA0p2KqvhPmi2auCHxRzZzxJ6I6IBB/5pxozmnE27i2HDb4aDWFF/DR7QS7FUEZ7ZyhUzS2sBPdKbCEnGpEsIYgDBMPblWe2SUgstJEf71csb0z9eR5Jaonwfv7Nni/fvby1OObNy822+GqYUsK02XH9tleHkjreklm4RGFEHAIKXibSK42DSrb57T8dDkNYeRrketdJlUVzxmrBEyvDrcpNvQyB98J7NE8Sc5N0KSHaoT21HRSFzweNOck/3zV5j6IaIGCaPighkWdUnQBaRmrU3eXUvCO1FD0Y23mvT5x+OXzD+95uZEq8/6+Dt7vR/588+LFJvM2o7JKK/L2a15YQDtIb5KmZkXh/EW0MGna4JXnvQg/RNTcKWW4vskY7StmN85D1hDYnqugCc/jaFbgjdhzRTDrTsLw3V92mvcEjir0YbjKJAMqepq7dqSqHMJgMDgoKARSqmbZ3giMipzNmbnlMvMWJS8H7/DpH59p8DaJNwXvNwV9OA0bTtfBW9e8h5LuSN2xXfjfayrZwXg5VfLx3Qc6Cbdiw8RqIE6fidD52g4onp/FWhDI3nhWMIFZ+ANgIwzzzLOYLW8WSbSbhzqKJLaYUMo6vOfqZEYL8I6DpQegF1t+tjHcSVASwlynjXKgd6GWMOqw20TO63PzU4XrcCFTxjXv9V2JP1xYrnHwVok3RW856U3DhoU/X7t48ebd/nr4UDNuSB3bofO8WFTxNzCen60O+KIjyptH8RlhGlXczPug59eNdBEIbeI9PZCbthh7Fu0jOndi0GNDQVodEW+heCtCG5deMEuHSvcE6pKOzQplDJkMdKFIFrdoFvU4EErLhDqj6RmADb2/PXV/sT/mvd4G7+hQkh0pg/c5Vw2/r25F0fvkmx++O/7n+eTDVgfvlX7wFuOGrQubsvITbIOI20D6CBDmzBm7QlBiSpHIh4OhZRLNJxwAHn7i5QpMJQuxPnu0O4uALjsicDuUcAKwvLMRciYu+ZLCQutWFl7yR4aqj7jFO83bVfM+mh/pbkm3IKwq177IVWDkQT94B6rtcBO713c/TFJ7beq9l1cNdfB+/ezJpaWLycG1zLwVtKEcNyRPoBsXLny2NUrKjcEwkSH3+tmqIiYc6NeNISF+SEDE8oIYh7EGuwaS88cEfLghZFx0eAaExljqcP5KwHCXhIm/FFpgDjptdB0aJJQP0P4uWH6FenoKCOTeDyFwT+oXCPVrdXx2RoK3WQ9f3xhZ//5ZZXfZ6o30E281bvj2+0vJfTgJ9DbBe+VqNiub/OAwVgET4TFjdI10LAIRhXtvgzUmHVukimfBsEHdtWT5Y1F77zMU+bj4JbhjkOhy2WIvdxgiQIAS+IT6iQ6am4vUnt+QWPAOWujoKvsik32RoMu519Btk4l2Cul4itAD7fzbujf1a9Nt8G5kNe/o9WPDj5PuSIHEuaftWpN5C3Xe+e3kqDLbZt562lAGb1pTEH6IalbQ5sRY7tQB6yCe50Le5ewnny3U71INVQAejXJ+Q+i6o3RwBls6XZBAJVohcs6iKqABif5Tp5A7fyvERFCVWALwjxc45yqdlWSj7QrLWUENJFm72Sn90JdoGZAgDY8AAPsvzq2N94N37HqGbbh+bOD4d1+XIMh7WbtGwVvool8sg7dPYWuCt1wQb72xilX/BHi7DRWP5Lo2Xy0IpCS/F23tQF4PjnvjCSiQN9G07AvJRmSMwycDb4sCR/W8ZJEMpcU8aK6Xjz0IKW1gcGegtA3rGeP1nEOqPCYP0TLgKuJ6jb1bWcCP+beije78r0iU0/NsAWz88eZSIW7aZN489X7+21NrL799zsHbj900bvj6h2dPpqa250sW0JkzZ3JgThm8Fz6b3FcGLxSkSfbKuVMn4yPBRP6cDGVAjI0UezZjadQQRAm5l9PkZZSOufUVz92diBnUi0OWHaq9SBal1CEIJUM2JrFGAnFOeqzLz2chLWU7pK8lh6h/npl4lcNtgJVWwhe6G6KINGJtYHUewMSZ7eWO4D32+efnxtOktw7edjPcD96nT599f2m5Ct65NnjbzHvh7NmBsuhldp0eNo5GY0Ik5Qs9x/QG5CqQfq4w94QmQYWfOpFDKlVYsKSNd8HwIB+tP6GCBcIuQli+wsKBmTotMWIjr0d7wvBUCQGhyhFDwNRxgiW8GPukUsqkawURsiZlZMiRpi0AHgF2vqQApeC93wZvPm0YGzs3XgzLPqwFIj+89ykF77dPv3n24tKtKnjv5pm3TL3FrGxyaw0lncL8VrjLuwseyMctnYn0thc4FclZB4+10FnLhT7B3kLxSahih6Jr/UjXEeCc4ZDTi3Gz5S7IukNemKlISM/tCAN4rezCVNqMg52koRhQwmJXJgWPg1PQxN8J2uYlTJl5N9dS8N7nzDvaD96NA4dvvkz6OCWwTCreMvN+889bp7e3L6bgvTnHZUM5KyuC98HqKsjDhFejrqRlDSTH/CfCv1qsCUVY/G2l3IBKNTAmLeh+mLItgFSdWTiSg3lUGboFbk3acTYk9IsKZ+FqHX4ZPVo/u9ZXajYBRweSViY8UpEfdCMcJxcVuXVZpHvZXq2P8AgA9s3M3loukA1Nw5Zv2H6ysevw4x+/SdHbD97ft9H7aerYvnl5abxIvMWGrQreK03mrcYNF1ZuXF6F6H267XogBgidXnUI4u6kldupL+bRtSKPpkIyuj6JplMI6IoWjOGdnmKQY+ENLd0W1ZxVlXOYIDUss77ru6IfOBWT3w4k0pipIUaILBbF2py8qoHjo0DZBNzQE82xGDacP4k9F+cSpmyxhuVI8B67/vnpx//2dVnz8oy3Lhu+efpieHm7TL2JgVknXs68K5NjfrBlAfDeHV4KylX5H0fsFV1YCJ5a9AFy+WPOrYAH2vrBs3cDgtvxkia+JltnTxpYXnnHNgaOK3DQFO3IwozZkgJx3lddQNXPyfnegfRRTsdUyTPaPCHYDTk5Z+HN5KOfR3Ye2JjLgzchIrPoTX/5fHD55svnzbShxTXUs7Jv/3lrYmm73FEUVUObedvgPXv2VNkYkj2MDk+MV2fGqmZmMuRVkLixMS8pCBDZWoR5mIqphY2JqYs50LvJ+pNaY4t3a6azOK5QeEnOphfZD2LFKX0Mt6PMP/4eEYxcA0iMSuK4U1TG7aKvbAVtJLZaJitptxk2iyQyikFvEbwTDy4uNcFb4HLyzDuagndieSkR2eqyQYve33/7/ZsPp2coeLOGrRz0Tq7M8NiPVsLBhFv9mtnQg63rZahODjK8lFbNGnGw7XI+CUjt1kV9F3yGw84E6jWB1LgSQREhy+AIzL7n6xKs6nVUXW7D4CyQ2AiSiaqQCQRXIWC9fro0LGonIl3GfLVYlg2riw/m6+CdqLbDx9ppQxG8uy4tv/fP5/mYN4/ep9+N3Z+eKXYUbfCeqLcU9aB3cuXKJncCZKACodgGyrL8hsmwVl00/VTBYxMcPEem5xbDLxErfni4tyI0AH+dRYjyINwsAGLCYRvUu1oih2O/p+0Bwo071IqSo9qNiD2m3KGoSCKW1yoyTIVoezktwmLacHJzKg0bKPPmeN6fHvvtrkvrt75/Vov0at3w7csDu6amZ2ZmipJ3tqkbSvvhpmxIwXtj3/lsQUNkJ5jaGYhrlx70FunpkmI1j/sZOiaCbVxYewHaiKuALrSYSIXBqdZZrCbZBZzsEuRTfnBsBivAHMicN6a0h6tC3izxMJjkYdlDjXG5xtVtcPhAFsaiK648+B5wHntnyuC9nzds7Zw3Be9vT00tfffPFLl/KaysOHo/ffZidHB9OqXeJnhP9IX2+jXv5NkLu02vNzPn/y3ja1EB0vUxizN4RWhxwzZH3syX7+B315kvRXxni6ysJGtBDGnNO7/7ShWRjJMGr2LUIEIAwaO1mRfiPiC+pKLYANl1evkuU/M7BIL1DAk0N/fNXQXy5RTkxM3X5XsunrmVdhRZwzaaNWxF5j03/jil3nvJPbsYOtR6OdXt+ZMDQw+L4J0J1sNF2VBuKc5O/ky8MwhjzYIdjiDMjFxCprMfBcUKrX6oToaYMYpApAg5RpBIh1KHRdQx7KQatoPpmp9wqO+vm0IDnRBLICwbcnVXUS9XNUavg6rQck8KCBXZPRYNseJAB1gyv7x6Zdf5k7m7RfCermvePHhHi1HZb4cOLDxe+u7J82o5XG+IaybFs+9e37VQBe/cXFY29Bu2KnjPTusujRk3EfxRqYOmLgXO4zL41p2GwwjlHwX6DD82kJ2UgNWcXoFOgugHRAMFdk5TcWKDB7ZD4DVEv6dGqa/bABWBtsA5RuB5xrpissn17Ej6LaCGCkk5ig54xdXmXeuZncfAbD94Swobz3lTwzb05unHf556UQ0cqtT7aRG9KX6fv/zp9eHj02XZMJdn3oY+XAfvyolNkQaOIC3g1wkh8QYMRHdHI8kS4v7Bkae9YLE4TLvnE4gQEC4YwUqIpwiSVUMLbfoOp2IC1YeI5SU7V1TWdwOC6MW6TtUUQqPyPB4XAQdPCjgyng1kFjkq+jlo++Ui855fHUyTspJ+OeFHZeW0YXcRvI9vvfz2w8QF+rCqGiqtsk+f3vrpRpqkFdMGKRsqJkUz6F05si84YwIcf2QhovzqADIeqcnoldEFCkcH1FsHN2QpTQhdOEd5GKudyKIiV2T3J0UOyfYWlfAAdNV/EqaI55/1iEKi5xwATXYy5gYjT1nUuIMN5K9RQCyO8mUjr/8hHWRZNgC2ufDg2tJyX6jMz3k3UvCuP378+Lt/Pn/reaWK/mkZvZ8+f/bjTzdeO7W8NJPmvCV5+Ayv2I4044atOxsCo89lQPKKnsgJYMsVPh+px1VwWKQAx75hsso0xBKNCCVsu3gNgYwNAukxdFKAZWPAwjw6mjOVZzcybHSYgVbuCXB1KvzrAQC/s/SnW/4HXu1AHLJEJwcmFmKiCCUqwQRbLrUnLq+XwbuYB+8eDt6BwfGl6cfLZeFwr595P/3w+cuNjaFdC/3gDcuGaksxOeJdQMlKDa7WVMxZDh7jzs4E2+xrJDhvAbFYiWgR5um9bgFhcM2a9P0BRhJa+HFbB+fAGkDReLcRPCEEUK3mO3ssUJQD8wK3HfbiUrA7ra0R4ZMZmcysdsdT5PUH1Po22zL2ANs3/WB7aYqDt43eYwlWtjEweH8tRe/S988+7AtLF7H75NLnGxu/PV5UvNsXs4atzwNqg3dljYp/SBthvOUSJTBOlMYy8bQsYyih2NhANBH5FysFeGV0L3UD4ixFVa4DRHhFHTLt7KTb00mMiAgYOR/oljdnD+uSQdHMpIvODC7RTjV2BGMBaJ8TQNWFt2P0spQEGOEOec/2g5m1LHh3962AGkzkxsDE4tT09ONyXvZhQap4nlLvWyl2N978ye6iXysSbxG7s/0dxSECN0yubN3dFKxnXl4J3EzIVR2eZZ7Rxq+SML50FQvhWrl9UMFZ+AlUJL+AYLgVLJHRtWpWZ9gYHaA6650YAgtcXVu5J4+nU766A9FnPgxMvKa3OZAoZP0s1sXhg5KvCJlWgH0HzMzG5mZT8N4Pgne0H7znTk+tra0tLd/6/ofnz2s25rOXl958c/fG0GAdvFnZ0JS8B9sV29Yv9lGVH8Gn4Jfq3NPSUoz1lNSQVpaZTj7ScTjd2cZ+C3BqUTDWbjbIVFgfOZRoiLTPgrVCXLt4TmZUQweXTM/cksJp83gXBQVJmXdeydlF+eie6Zuq22A+34NMGXiykmW31x6UwdsIlRXBS/Thsd27B4ZHxtfWbq1NLy+/ePnDs2+fP3/29MmLS4MHhtLXTq9XsTuXBW8l3HC0BTec3Xr7GHN6+C8m5iq5Ogpyul8AXDcnNIlYq0iFHkQzA6zjb4EvioeaQYlW3T6AnokcuqfEEiaCyjKLnAyDBYqzQTQ2VHE9Im0ueBdMmrLEowVTaUmhSD8dYQoJ6w/q5aCcI8bBDJ+ogjdB0c81mfcYBe/QwPDg+Nrjxyn5Pl6+9d2LH3/88cV3y4MPH7459Pnnu8r9mmbeKxy8F85uTZ5iEVOFabDCKcMRBNUMJ7+t6qfeCzOYhsM8jilvOlg1FNprqpt5LAqlmy78q0ZCHRlVtXAcdSImAclYuudoel7JT0A5dMZDBpvs9mjq9wN+V80vXgT4m+PXCAgtqjOri1fmyrKh0jfN5XlHyzlvCt6h4cHF9cd/np5aXn58/PDhnx2+f//S4OA77wwPDX0+vLC+VCIiL3LmzVZsZeZdGYeYIucKb8L0YcwCTPXGMq64dHgQ7WFDhCcjp2CnBwed+6PbfEp5g8J7lK2CrGpJnsDioilUK3PSURZx2KxLPKqFREK0sfKVvYkmth8XOjMYUy04IGCydPNgOtefESMGwOWpq3NN5q2nDdmUt1hSpHFYCt6px4+n16am1tfXjx9fuH//9KlTKU8PfT6UpmjlpGyegTl9+vAbdfBurSEwbbdoeuqedmA3suNL7xK4Cd8MhO+u95pCYJ4dsG6gEBeq2WHwVtaOPQRzSuwWiUvDafqqwmqHZ1sHntflS+N/MEHvsxEr+2JQf6FIR2ITOqtsFe80leToZ7m901fy4BVh9BS7Y2NjKXhPjy/dWppePz4+ldLv/UuXLp0afGciBe9vB6eWmjFvELxH+8F7+9oqt6SRowY4WfD7ZCwgKNLqAR2MeScmKvTMS5F35tXiX9AViv3r3sPh7EK4e8Hw1yVuxQbFZUiUeRXCQOosJpNdv2SDMvpdzt9BTdklIa+MEegnA6buQ8D+7SsXZ5aLYUM+5x1tM+/YWJF5B8eXl5bWirw7vpyKhksPHz58551duz7ftbjc7Cgu5sAcl3lvv3cZ3apbnmVpjldur8yf6F46o5Ofic5UHQIKA2aQALoDE+tQtE9qSHjV8zBHq2iOm8soHd8vR6znkMymWCJTN3ivyisgJZl1ifZnPITMYcFOvy+3aeNZaPOFPXNXLiahsgYROUxLiqps2D00PDG4sP54bTnVvOvHD//sZyl0H55688DEbz8fuJ+CeqbkDhMYvZjzHqqROUXwrtz+xX4D7BF0r5Yb7/LQRfXVBDvK6sU8xdamwTF2xbGDd0Em+jWsPKdDXUjnYr71JC9jRGM30mXUjsuZXSqSiInokUghiwf03HoDPPMx8ml1SzCxAjKv0uKVYZn4ox6XjnXNn47gOpqnNfbgxLUSznu6Dt6cBpTmDlXwpqJ3LZW8y6ngPT5+ON354eDguXMTAxvDi+tr023mfZC5AdWqI4XKadpS3L4x+gjAIyh+HAKjF6SD+Xzmdr2C1BEHUekrmFkhuBvmAiAsSgWwpdZSEFEoYai5I1wksrnbE30PmEMNSs3utGkYatmOygQtKfOKnG7uj0BAp3a5UplyI5wjeZ48FZpmeoEKaI/cY3s/qYO3ApXV2tJt5j1WNWzDace2VlYNKXhTmj5d3H1iYmj34Pj62loBKqumDWRlVQk3NMF75yeA2SOiRgPKtjQm85pgasxpYAYzRpCMOhBDPegIzAEkZFAelCLoZJ0Ro9ADuD1dR1pr8HgLbtwMr43rrCDg+ZhuLtELeDUxlg+izShsZaIQmJPfFNNhagBlx+E3QMyhd2N0ANh4cKaANtxvEm9Ffc+Dd2xjIAVvsWNbn2qCd7EM3uGhgZEyeKdnguA9SOCG2xcGHI1HwLaS9ISMydQnosFkJE6lVThypsMF8PbHdDspQJsOnaWADmG+5g16s9BvBR4dJ0KpomXAw19hhcKvz3o5bqyrCRBNQTVWUtSaTJ67yRKUlWK0cICpcGLKALD7/RS8fVCZBG+J5x3bXQZv2rGtrWfBO1gG7+kUvNPTfVTZA8m8WfCenUC/5hX0veibM2iQyX8mg24W4VT2tRijMSRKFfbUjFiHX/BVaqTL4PR9HByNN0ZOFd0sGH+Z01VGZGMVYSoCQ85eMGSMNJpyNzRZcovxBK0eReWAW1mFMXuuB3vSiuUY6XvsfvDHBlRWESmGMmH0YlRWQCKHJyaKBfHa2vHjdfSOlMG7e2BxvKgaSix6m3mvXMl5QHXwrvwMq8AjKKyXQKhgUKNTnBaRUnPq00ZbCsWKdS5TAbe3c3paCHDzTis3GG9ZUE5bV9K2QBTCQm94VefjfVkgfU2y/k4OvvsBAmAFhL/BdjJwIzhG+zrVEjiQOw2DLV850WLotffv1mVDNufNg3esmjYMLtTBuz4+XmXeZHy1eziVwtNl5u03bM2krIRE1rYURfBuTa2u+iNdyE5UWRB4BgFD0tRl0bxOgpFAKkgwEoIOUa6DRfLeJqsvx6IMik2GMSCIQVVQ5wZL9HdCQy9t7eB7OJ7zWlAJwPHvhFGBKGPDeRn4f3ftJTrXTHAjVDPzcqIA3twxeAsO28ZQGbxprLBWVA3Hp+rgnRgcGJpYmCrLhu0GE1ln3kP9xNto5mxtTW8CljR6LOrIXznAjUgKr+AUBVu5jvar6zug7zycKghUq9MCbr54ATvh3EDKSWnvYA0WbzYfzZZD5E8jOiIoSJno0toH8nU+dLrfWk9hV/caN0cWM2LGGwrpKQXvzVsSvGSoUs95JwZP1+OG9SJ4T5c170BaDq9Xo7KLF/PgLUBlRyvhhn7w3t7ehJWjMpcc1X2LkhRXnCRYqniakE4F9oADmwaqcYC6AcXWPw6Du5MACDpRZeECzDraP0SkTz94c7O9CA7U23GcZ+rPpDhwo3kRe5QZTRRySCA7ezJXAIyx94s7QFqg4vfVA+/P3Vougvd0G7wJVJaXDWXmLTu2fvBWNe9APWwo5XKamreBRB6sqRQNJvL23ctN5gVpvTosASuy5EMTNZML7+ZJQmw4IZ7w4jWBTisrB8vZGfwSOGViZ90zp9tgohUjqSr4z+1TYgBPzwvm6FxDFMbynKdQMNMUY+KKl+OsHc5KrErIJpvsuskTozICOvf+3PbS+MLi6ZYGNJor5rSZtxw3jJe3xULMdzAFbz1saPC8c23w1i6CRxvNnK3bJ/aeB9Wfbjkp0kEKXhXteMrcon7Fh5U5q/e8ylWIAzrgtg7dHao6ueA1DxbWb2d+ccDJlSAHXomUiJgZeebVwZZqV4IpriwLy6DkfMIr2HSIagm7PXmxV5WkJNIP44EAYHOwDN7FxYWMSbGHg3eoDd6pPHjTpGxxqg7eypKibtjK9XDFA8qC9+D+k+cLXUp1jnFuEWyHIMpYxmthJYabm5VxVhYWspkOJSLqTuibKjN3h0TUA/lfoQHB61923ctjFlQ0yMN3+m9TL5NtEOZC5yAk19YVRK+H6zuwuRqLml9t6snC0zm1/IQBm4MPrpWZd2HEc9jK2rcI3l2pYSvHDVMJVdYG7+4E5l2T4D2RocoOEjLnyJ5KpNdZl1D4mJ6NBudz2kHH0Zmr4P/Nsa6hCpycuiXz6y4YTtATkTEL+8iZ+jbAeUDJjhvMwpFtjjFr2r27xpdsxqTg/bnbrYsVWgbnFyyIiCTHGgWinyeqh2BPd6ntnCRq/7jeHKmCtxb1L4O3WQ9XYPSibCiDd3Gtn3qb4J3oryiq4J2j4O2rlVXInLfHzqNeDxN1z0llmze/FolvMXIj7RfWgSBdaHmDhesoZPpIEkYYvaHajrPw8wN+tXoNlLycYA7MYbEs+F1EBcCjiOYOPVNhKwQoRTiQh7EhtkwmFBHllsdOfTZnESpbPKfRGmuUNNGxeboM3vE2eKsNGy0phnYNlsE7TcE7MZCQDVP1oKweN9RVg9KHy+C9s3HyvEGVCfPhNBvV8st2Trc0xAZEOYyVVrgb9r4CJFsA0YeBt7NwqpQyIrNImcsiQwk3xfNqUkI67BBfdex6J2qdBV/P2QQpZUIcOVXa1Jz3jVOiEOaxUn0iKTPzJpmSMxiTtrn44NrMciobakTkcBO8NCrbNVEOeqenq+BdKIN3eMgFbzUqa72Hy6rhjbLmTeCG1wDDI1K68etHP6Vi71UnIi6vXrkFBBaAaMER2dXMaZFAoFwuGfrwdbpjYqenPliO9YJuwLNwy8wzjZw1EBQZiT6qjGoWfUK0FtJekiNJMyqDapRmQUWI+F/mnxRNgYwFOZocdHnxTBm8pxs4b1U21Kl3tEDmpBVbWTakQe90GjdM9YN39+6RNnjn5/rYhoo83GdSNGXD5IHSw4U5rxDkqhg1QGVS2DwC5s3vzCnsse272Aa6pRBrYsBL5wns0NFvZUyhW2ER3WPVHwQj3QDJHnCMvaJmrLUJA6xHmpHm8LUKYAzs8rxllSnQL</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAooAAAKKCAMAAACNqoq+AAABblBMVEX+/v6hrLKnsri4v8S1vMKptLqwub////+qtbukr7WuuL6msbe2vsOeqK+lsLajrrSgqrGdp627w8ezu8Gcpay/x8qVoKaXoajQ1dhlcHaKlZuyur9pc3rBycyrtrzCys3S19rW29+QmqBjbnSyu8FibHKttr1rdn2bpKvN09a5wcXU2dzGztGOmZ+Un6W9xMiao6qtt717hY6Zo6mIkpnIz9N9iJCBjJRqdXt/ipJ4gotncnhueYFtd3+SnKJ0foXL0dR2gIjDy86hqrBganCDjpbFzdCNl5zY3eGFkJhxfIS6uraFj5X09fft7/BweoNcaW+2vsHo6utyen+Eio5+hYne4eOYnqFbZGqosLTi5udXYWattbkpMDMvOD1fZ21udnuxubxGUFalq66gpae2t7I3P0SMkZVPWV89R01nb3T///7///+9v7smJyewsaxlZGX6+/xcW113dXd7enxra2xwcHNKQiduXSSJcyZzd6SnAADl2klEQVR42uxdj1PbRhZeOzhCtW1ZjGPnmpRSN6XGCcYeddKb6xXIuBM6OfDNBQg1AcJBJtBk5ma4du7vv/fe7mrfyiYYF7tI0bMt6XOI9evT2/fefisJ4ThCOPDCqZopIBcltICDJvTC9YAzBSB3JRlAOPps0JeJBiLcc7msZ+Y4qONjAC7J31G/MgoIf1tMHJhrJf6AXWyOk2gg9DchEzV99Al2hgB9oMYDzsRBSM/4A3P4mY9MJBD8QhSmcTDEc8IDwoC+cIVuSa4G2p9OAwgWY8Qc6NNkucdEAhGJ6FjjGi47YbuugAj9qYohrwVCrk8MqC1MBNCHTxgXkVBg2mO1oANFy4k6URBGkpzTVwAWIEwahBdT/IFjTknCgRDD91j7PtPqMTCeyxJCGLZPFlwe5cYO2Och4UCEUZYp4BjnOMzNfcxf3g5ggoq4AyesoYVxVUKB0AwM64qsisjjaA6swsmoQK9lGoBFHXEHLHQUTqKBsMrXYQJj1XwGakDjpUkOj+UmCXjiGXvAgndHJBpotyUEd5esUGeCaPvUj1HHnE7KYiqmiQC60hg23QkGzC+axFl8NCUeXmscFZjfnBSwinExB/wyE4kGrLxtegV5Q86K2jzQvNXFgWT1QbBXsoHghWsbmLwjAiIF2NHAFHs0eYUq7oD7EJFswAvbwhToBLMBEKnAjgh4ojthYBWp4g6SGHYMA1wMEV6IrCPejhtZxBhyeHQwLd0RC/eTAT4RcQ5rCYRdHxEsQREDwFy5IwLBariTBcavJAGw6kXywaA8IpQmDZfOWi307QNDuoviCxwemycahKxkJR7BNMRG6MXAoJh2dDC1NNRJBvgURLODugjT02JVb5wBMFbtWZjy0YSBMO12/AEvBYtkAyfa42z3pA1XfY3TFWJ6DVNwLRCmiVbOmDyQyiFSOcTtkUOw8pXd8cycm9UBZbpnWJB9JRBsBNdkgXBYn1H8gRgodiQVWMJtMVKFbkz1TDiGaNIgMnAn3kDwXvwkA9byOmKIMmRow26PihkR2EOuJg1YzT7eIJVDpHKIVA4xdTmEyVyiKQl/28CMV3FGB9MbzpgkOYSRCvDhV0kEIpKUCIeLcswYKwuMV5XgHdwTBaGuIwmAH/2Eg1QOkcohbpMcQgxTtF/eNcrGIIjRgcNH00wS2JFH3IHVJZZoIGy/yDUuPEcR0YRl3HhOTB4MqHVjD8SnAPgouYFeFc6hSwYDjeOMJz42SfABZQkAiRs7NhSw/GRYMfpylc21lQpm4OqkQbIEA+ZOWk7CgXUDkuhNuayQcjA7vuZdG/h9LCcJWA97/MEnkrI4Dhs3ZXoseBealWU7tnRRsNvnjACmV4fjF0LcweVSvUQCLie0xuuZql0E8ArNiGB6PeysTJ8IwO9Hm2iQyiFSOcTtkEPYdyqJpNqXDBYU7N6dzqhAmJvbTRzwm9zHHPDuB5FoEBl1b39na2sdm7RjJxVTAMmL6z8BS+UQqRwilUOkcohUDpHKIVI5RCqHSOUQqRwilUOkcohUDpHKIVI5RCqHSOUQqRwilUOkcohUDpHKIVI5RCqHmLocwrYLZakcYmpyiI8Yf5KrY92xxy5b8VsLCBa2CGsd/HHTH3D2QVi5neBPuhksRTj2g2WHPjGYnYBI8cux7l0aeeq1I6m31eu93N9/9dXCwsLjxwvrz58/AVv/aiuVQ0xHDiEueitvT40d3LnzrztPFh6/6vW2LkRUWCBYHdScx0v0BxJLx4L+ZWsLTray/f3eBRByC879/v5LfJGpmbTeywHrXdO2tnC1uGaYyE3QM8suXv7jbX1zd/fZ2tr28cPjtd3dHVyG987mwf5FKoeYghxC7J8dn787eof2K01OTn49OT//7+s3b755/z9px8e//bb9O9ja77tDbMe2s/C1c2ZsQ8026vW9en3jbGd37/7F/sbxs92zHfmHm5swUb9BP0q/PfDzV9vmDq17U64P3srOIsb/z+6b1+dosOsnJ7jwmgznP539HEs5hP2MSWHdT82x7hxm3Z772kDwu/D8ASCWfvncX9t+sf3ixYvtf66RIwDbXttGe0Hg2bO/7T7d3X36VJ6173e+39zc/O4MXt99DrYB742N5eWN5Xp9tQ6f1t7qXmuvCtNqUAuCdqNR8btFv9v1vH6/f9BHO+h+/fqX96/fPF31srnFxQcP7t797O7df3c6i4uLuWy/7/a55fr9bD+b7V9hB3qGf+lJcNqF1ynA01MPvvNOu7ApfqXSCBpv8QVbuFdr1IJiN5Pplrtd+Df414rfCNq+7zdqfr+/tzTEgdx2IKyb1fGHqH304VBCRCrKI4Abyv0/LL2fWwhWq7UqkKYWAGsaDZpU4IT5Rb8orZspl7vljLRyxvM8F16eWyr1S2D5fD6bhXd2NpfN5ubn52fhPQsTtE5nvvMZGJLtERryruB+e350ePSwWCoUms25lXv3VuZWVubAmtLmmnPSmmqCXzWbd8Bg2tQGsFAozMzApACLMJ8pwDd3ZmYePJqZodXd7cw/KhRgtRLBlnRgezrzOdrC2VwumwPDHYD9KLke7SPtH+xwcfbe8+zCtG7Bf6OA96QMPOKQpx12LjJ2pUL8QSDWvyks1eqrYK1qq1WtgVWr+A5qZAFaLWgHNengGo12G7ycXyG+on8hJyINWSvZ2y3DpFzGT2hAZ0Vl4HL1h5Ojw3d/rZSzyIXZkL7AZaIGGn45mwXC5GCSQ+rg32bVn9AHAVwIeRevBiBSyXVLeRcNLhRAGa8EE7hk4B9cXC8wjbYlgxsnjXYC96gRBJU2XpK439UqHo965c4X/QWeDYjYgJjJIT6sfw1UXCYqtpCKko+tFp2RoKrI2G63aSapqJ0nclEuSi5KShY1KRUDi+WinHkZQ0V39S/nh4fvvvXdTqczC1QkLzVPXiqnGTlLtAMM7naWFvBrbuCQkXzgy1z1dol2yDwPaEiE9DxioIfrRybS9YKbRdsJewAf3w8afqVWa8DO0a4GdBSqy5XmF/37MdVG2EqHkYQF48gJb+j5pmL9J/SKLWQiuAF6o9WUT7SpiKQDwwkwUnpHZURFX51dnBD7wBN2u12cERWACcSKTMZd/eHk8PDoRz+DrhBI+FkHp4vzOaKgsix5PeUEteX1J4/tqSvZRzwsEe1wUpLxg+cxGnpeF2OMchc3ED5dXxtufaNdgV2Evaq1ZSMAFyYck3ql+aS7bkp2LBS75SDSQg8Ru7BHuNgB4OV6iUvA8EdvXBdAA72OVESXKDmI9NNUBASMk0RE7hEVfekSsYGuUDgJ04punHV8qZwhLGSIkDrQVHwEKp4f/ufox6KHflC2vmCdeekHQ+aVqP2W3NNf5VWbXJLeMJxL9iEvceZmFPvdDJHf80KvXFZbiBtLAUY7qMidbLQbMiKpUfvcai1X5p54S9MYtnHTIH5yiKX3haVglahITXNQs01RsU1ERA62yTFWpH+saC+o8xsdJ6qmmQWLKlIkvwi2+pCo6GeoRVZszM3PZkNPqKg4YJKKMvpzZaOcL5EHlF7QLcl1SN4THTMuTWWIaKJE5RLRxatWuY3+UB8ComJj7nlxPZ7aCOEwhxkpvLC7g0YB7wgcEbA+g/HBh593mveVV1RZC6Nj0NZUlKGhr7MW6RHJQ/oy7C9y60oS0lRxkbIF5Z2AF0DFE0nFXBgcUibCHCBmtJCEKKzntMCp6FEDLVtmVweHknuKhvBxdZTKqIgRBTHRrxAV2+QYzVVIVGzPPc8sjaFW+bMB762KdB9/pM5nKHJtYOvTxgCi158Dr1iT+XNVR4dh9lxrN4iKFZmdqGQFnSLW3xq+pqI6uUUVKGorK15yKlJT6bU4FWVCQq1y3nCu5GJKXCIy5szXWdlAKyoSCTUVM5KKLuUrmoqyfWbGqEiBL+wPBIptuuZqA1Rsftl8Zd1XOCYgdnII0TtorrdXKVsJ/WFgspUAqSgb5UY7zJl9X/OxaDXNMlD0bfcoE2jlEUOvqKnoyfY5DA6Rinnp/JCK0gZb6az8J1emKmG+oqjoYnnQUyQsZ8L1Z2yvqDKuBr5hF7E2EKVi3V+5t7QVRzlEVIwYyZ9vLPG9uf6h3sHcerBqUmbNQp03S68oiYcORFcSVd7MWKioSC1zsay9IlExIxMGVxVWIJFwWxQr/r3osmw5q/Ji8oxERXR+edeNsJByZ23SCSr+ucqoUu3pJtlQUdeXKIn2ZSlAUxFjD7wYA31JwvUJVLwnqci6XGMBxDDuOFY/3eCwv6HDAK8Gzs08yBqoiA20dol4NmqB9ohhkKiphx5RUVHWEjURoa1WfCQS+oqQMl0p6xBRZRmY5lYlFct5FSFmB6mIdWtsjZGKunoT+kNst7GqSI5RNtZ8Sh0mYaISRge60AlZv7mgJBXR+VMZJwgjlCpSceXLpZ5d54gJiDxy2LGGQPPI0X70IRe/jwR4HvR/9s7tRY7rCON028d0q9Wne5zZWYFQSwLhjLRiPJuJchGJdRkiNiJro5cFB73oJWAC+v8fM6fqq8vpGeXFbIOhN0LeWTlm7P1tXb76qvrXvEgo3lsKiiv+LqTxCgdFQVGaFHzKxf5Cg6LMWoTNvs1GLECxiJSaSXOpOUH/VETj0GuH1JtELhAb1zY33LEkBoVJ0m9SuI1O1S46KxF7y9IcEXv/rjnccxWcfvp2UHP444f92dt7P+Y767+JF79BO8QBxUdLi4pAcbfdqoKDsQqHQhYWSRRuF0uMViCJcO/S5x+MIsFYcBtbECyrvyQU3xdR1RtXMjb+o4yUkDkrA0fQqIMVqDgkc1PwVRGTMfTZuUfgxmBI4z1l6C230VtREjYJxevZDjGBHYJQXPygIo5ViUShkLh2+UxmFISiJxFB0mVlNAymKRbSQ9er36cE/b6zliSheMyhAYjPCEpGkRWdNGQu0KygjeHoK6FRh9+FR7Fltwe/dYzUFUYWdYDio+vZDjGFHSKh2G522rVQiqJOxZWJjKLMmCUfmwti4XsYmvcZi8URioVDsW5ksMeNNIRDdvpAvwGRGLKUTGUiMimPMUORcnUtbXrhUzRQ5DkQwiKi4lpQXEpk3DkU3z26nu0QE9ghBEVUR7utVYhb1664cGil4cLFx+VCW5Z+fwLF4kRU/CwoBvXihFK0nOBV7exzZrKMrC8Sil1RU7NCc75kxyGRW+Ujpyj2rrVqfUCX/oU76e0xirMd4rbtED9+/P5iv0IYOM8LxLXLykvQpvW+qtkcJ5GaT0RFxtE1EgTKhqLiq5qNjkFCY8Zfpmq7/pol7gRjQ8ViRKeSdO0OZrDiKC72iIpOBmUPB4s6kqjZe5SjONshprBDEIqbLfXM52m2srPETHoN9yoLeoFp80JbZQ6OretXtG/J2tdCSjf+re7q878nk9irCM8tXBCVZ1CSsuRsaqqjQ5FJ5JacAiLjqLWizJ3RPzOK/BaT+t4yiKwvQjF1LNJ/EETF2Q4xgR2CUYR8sxMURW+jaIjXmo41KqL2V3OiF3H60bQti4p1HVcHFD8fUCwz100VSsWvlPJQCcxeUtPSQKXk3Nx1EhN9VOy6HiiaRYNrWt91OfFeUEw/nwnFi+vZDjGBHQIJWmXt7Zp2UXx9uIRd21D0LLbtWMLJ5mzJisDOMMSqgkd0cYOoqOmXzGAV2SGCrwphjLDhMyuLqX2pZRLdRJbPi6KOxHzdWedy+NzeXOtcGtq5LKSNRj2SrGIkdu8Sis8vrmc7xCR2CELRhMQ1zGC+U7GIeAJFLr96C4iSFQsNTJ37gMk6bv5GKDbcNMMkC5s2ZEY/63PSdwMUVeBJKFKNyHPoohAUJQijiT/6yJRubBWo2K0ovri4nu0Q09ghqG2xVkXKRJ+TR1lZZs570enSDlbrfA99r4FQOuYO82HgQyh+/s+bksVE6Z+rgC9kw0BnEDMcpYVhJ3dy59BeS4SJtuhkYcrsYf0+E7oz2+JiYeWIKTqG4myHmMAOcXZRnAuK/J0QFBdjFM2kDU3ENSqteBOBYleoNwZhkZCJsBoyii+rQcgLVaVDl6oMZa7diMSoJWRZquQts2eeS7PSXYxQVLm9cFHclbunxi6patn0Z68vZjvENHaIT2ePixW5Y7drMeBI8TTKyub92ruYKK3zvjU3GHkROs8hS30UtwhJTtBvEoqBCPMouogYrHdRFOElixgClmxrZBY5KnIg9l2TKxhhpET/Yr3LGlExFYvY5tmu+gev0bbMdojbtkMcUOzOl0vvwFkjXXkQ93val6Jv4eGTvZDYu80+1zp3qi27fSdCkfNoLShSDEzNS1WJKcJm0YKpzl1kEkMGCRN7qP7E3M+2q5xvtnOZmSM4Gc33HsWF6QXrrdTOq/0DiYqzHeK27RCCIvTdZdalIBbumTzn/UvfRsl6qmSLCQdhqFMMfNNCIaxsUCsygI0UhzwApHXnymyMTRR7WPol1lm10DawitWY+6FYTM0zGBTrIr9HaDn4QVr42ZEIizqLXhUPn17Mdohp7BAHFOtz1mtI623lKIQWhT21JcKc3w7oDL3C/GCsIQIAcsqyqs1BkczZiuJQ1ZGTsMVBWnWpKtm4p21nWbASWUdH0uinI3NeclTk4w4SFdW0OOqincVX5oDsT4fKnVL0Zp9QnO0Qk9ghgOJygb0j15o4zbDN9BDnMHDz3ZGkXfhBHy2J1ugs0gSZE/TLy8sGOmIwz+KBQ+g66o+QDiahKH1M41Cs2SQWMYpGTM5sixmKe1G88yngglclaIkCCfrh08ezHWIaO8Sns6ufz9Vz0+YQpl5EmhFnhi4s+0kULHpfmXUSETEVRsNC/yOw4uYnQvHOHdeh6ByaE7Tfh/busWj+sTGKond3piseo1j4uNh/EUUKjYbibIe4dTvEpwdXP++WJtH0bluv/z9xkGcnUhZqn+qiIi411B7FiLYDKP7hmzvZ4A93cKxWrHJ3hNjFfIImrRIncuqoS9E23DmK3i5J70cgcoLeri0qvn36eLZDTGOHuH9Ace2WAZRFuuzgXNB9/k01a6pjskZQrN0uC8zWNQ+NBavNe0LxyR0/6aM4WOE2U4lzOW7jtORll9I5GQlFVRZrttLqD4BtRMsPiiVo6fqPUVxmKN67mu0Q09gh7j+8KpetWr56uTLSHnkaunFUhCEG0UdP3aFxcLIz2/8pPTNNTcxRDGVVVpyQJSqGMvhDEc3IPsYlY/qns1ZJdSI2DNg1xuv6cjJCG/p8WO5ZpCk0o6gnMYDibIeYwg6RUMT+skxQ8Ftf9C4td06fofSL212yY6/JWPIyTP+6oRIlwTKKr4AiupNK59C8WSBEShXZZBYeHj8nRwR83IJizZERt3Q0NDKKtWcxfda6WTQGf4u1Tly4VpSoONshbt0OcUAxoEjsj5ekshgIf0NXawakwQaPmPWrMuNL2kq2qCJ1In2Ro+Kf7j6RlfwAkxh3LCWuRVhk1OGfOHUoMlIFquv5UBj5nBMStXkYa2mwbCu6dRMYtG4y/GNvyKp4R1FxtkNMYIf48PDqY9u7jdHM5GWdsCvAEIZQo3WWi7Vsw25UwzKg7jZbjVcyin/96gkBKDBmHbPqipk9x/sZS76pw8piHYnRKNtXDa2kpvUCufOEEZD96zmNceGlbptFH1B8dDPbIaaxQ3x4m1C0sV3vFRsQCFmQ0qCaYLgArGU/HgEJDi5xMURba3aSzeHV6hVQpIuy7qIiX5OtFMVQhtFtCF81xkZRhG9MLBINtg1q848lm4StGXSFH0svFqP1RTrPslYUZzvE7dshEop7G+iJaoNZBQjETWGuxJD8lDvdUkZOdse/MhS9aCMoPksJeuDZSlXxiMUmLb51CTKFHu1cNUJgRJDE7UW8oUYLRkaxyHUANC9tvjO21Jvkq45RnO0QE9ghKCqa+utqQwqKBF3T6CnDGM0Gw1vxWgnSH/iiTleo9CuVhkaPYlWmw8d06zPIzC8EP4MZpekTKFItEFEayLtDmrYC1jlqfYren4qKpOisuucXN7MdYho7xP0UFV045EkKJhdOj6mj+wJWkSN6EaCIvnb8EfLyL/3+sVy9SSj+mVEMl4PExaHyV8VKvQNfnvgHizMHynlTYl1fr+poCetRHCve7G9rBcdWN6MNxdkOMYkdIrUtimIHS40PfRb3vEzYyHe/cf1tLv7lGRa9cYB4eP7GJehBUQxs1WHrom6l8o27xlJ0cDtXXCvKJkxTCpINlqT5F+aCnQ2Jivy22F4PjOHaAIVGRMXZDjGFHSIl6N4XiKlNOZWCyxj1fJIecBhfKG5imR9yh2zItV9CDU9Kkaj4daDHEwxknHUNDOAdhUAHe+P4j74okOm0NFVNlGlMLctYxUkW9zZ8lwtVu/PuBSfo2Q5x+3aID+9uLsX638lhhegPx3knjLoScoUFj7UgTpzbS2Qa/gvvCqSqMFQVUPz261BVw+WAiTM1LvJIDE+z7UOPC0X8WWzc+5EYDq+uZOna6kULjc4BfITienlA8fHNbIeYxg5xQPET1Gsc+dBQgsdUHZdo4zKQk262o2f6TJDHD/AzgvDBKP7j27vpTwcOiWihq+AeE5Rtoh69k+OpII7tQMjBUSerdI+CYpGv/3kUk0XnvE4oznaISewQhCJdsYZYkzzWuF3Y6Dc7uDCF7zpvLbOVC75r3L+hODkoWmUAiMPAMKbfNgnFX/71/d1SURzw9w+Vj4oKY+PeCfawmpPPL5AbjB5Fl6Thbus6u0mrk+hezueijwaKsx1iEjuEoojldvHuUxoO5ZdQDPZaWpEqlH6NuQo606uURf5rUBTPDMWgUbHikyVm0Mk0nTB6nUdJdPQq5riuv9YroJio68MzjqKiSjqSoGc7xAR2iA/Pb77pYhcVRY6KXJlVRqHbTW7kxA07ahg6XtkLchYMX638B3XKCchQBUrQv/yTUOTHqSmKeIxLaeMXjsHZD0UZvoCiVYqkdNe1E0PlZkSnm1djFBcexsMvi4qzHeKW7RD/TSjerwnFGPkQeybH2PpT9nSzspJqsAwSAKvBx0B8MT34FK/SU1A5SScUXyYU//jgq0Ao8hOEAiVpF02DecWsEg3lyQ9uWGqNipjCiF9SUTy9BJhdszcH465G2zLbISawQzy/+V1s5LkU43aEK0DfggSJV2HgwYjOSaQ6TI/qQ01IKCYWE6XDnctLepXIA4oPnyFB8wNxFUUOq5XrXEKQRt1dNjnmUVFs5LG6GJinL3beYu5Q1MNOfWutNEmMu/r11b9nO8REdogXKSqaVqP5lyRprgAJlfSKAJMUim4XFeABQEJp+O7wkWLfd/L1yxQLqzKkR0qSmJ1S9AZR8VlZDYf/J/19w6BBUxSgSoKxW0bV1H0KxsYZ08hMVtexYxaj71iKEYqF7br0egm0NRRnO8QEdoj/sXd2vW0cVxiW9our4Yq0yMgJsvAmCNhFxDixN65a5CYw7CJBgdgojdapZFqA7As76I3jxv39nfM5Z5Z0arsWYQEcS0vOckXk4sk7c2bec+bYq2Lsnwkm1sYcBcn61wiKHPGGaKTFiSCCWLaOgdRROc871+FB5WVnUcxlkYePhG54F1qWu+Oi8SZO6iVhrUERz2XTk3mHI1v3NlrIsQkvjCIV6zv4mFHc2iE2YYc4Ps0ExUQHXxmDm1J544VBkDCaGcK7Jaue/xDQa0tURY9iUQCM/i2MyS2My42g2CCK3wKKn342l1We0EqlPOT/raAoeTC9oNosfo4kF1Bj6HVZgJLWHYrG04yRje23TlQVt3aIi7ZDeBQXwyQcPi86CK+NzPNKlji4tsKlv9e2pb/gCAyi2Dog0qDoFEXnG2IIb7tOULzjUWyFcwKxCUuQuYzRZmWHN6jz+JhoHseNPc2kpRKLWE5nbGpKqUtsdzfKSQXLHB+IdPAlongp7RA2wjVBtcbQJpKOYh+zAfOGnXXz0bfvEIpcqiaR+RnpUiOrL4xii6Ovp6+hMZgboIi8IYoNAcgodtIcNpRGbKWgOKHlncbMFYM6yjAt88NE1nBym8GvY7aueWs5HZgrBpc5bf2tKyUQoRjOMNg/uHli5ooD6zj40DvRCKiLLr35407c2bEWnTfvhBXN/6sDKFa0XwxRCc0OG+aiw/i3awJ11HAi6PDVOSatAwBBFYE0ungU/acukChQdq65Sij+MGnyhkd+RREGfBRk9urkUXqB1cO8Z0AbRrn7tDkd9qHJ/WvSt+VAyqhm7n7Yfzk4uDkiVRxEy8aXojMwK4s71jH2+hE3jJcDXQ56k86OmYO+c8ejePs0RUmByIJnaV0pTOBo2jjXoNR5tjx8RYucKYqMGzHaeDl0gUbmj1nEnitiFPF/gIZ4xPGZouxOPBIsd3miey+J1qdlheyN1prVlZBRTPahqSKoKYG7Ur+Eyy9ChScs88QoDt6nL28znRC/hG3naMZo1hUH1ufw9p339F++c39++3TOYYg2UcEOZdE1rsNOiwwiax0S2PHMz0lsgjfgpxX2YKAmOotCXoHQq98+IhSBw5JnkaKKDi4dmbpLjujLMrbj5knIll53SKBm16gkjvTg8jHv/El6Qa8ssoTUXhZvDo9orvi7+7YfYucS2iEIxaUMkK1pMLlD1kjNHAiagoU8stI5hbJT3TMs4k/BLBY1vLUoQpiN36ADNI3QZVPqDk4uCS92lNZ9at5uLHu1ao1AMpG0CS1nr+2Od6P6TlTy7q5kPsKM8cvkiFRxa4e4eDsEoFiWS1QlET7RtEKmdoQU/hoUBTXnApeMovnh5vha17WgePbLj36AxrBHUSyZxbxxjaCoBRd5NBaLRCmL3Rz8l3my6rU1vt8Rl7zTBG6tGNE7AnB3n/Ie/Qid6Lri1g5x0XYIQLEplzQgA4UFTfMcwHNOPDFMhF3BVyGR33UMqKAYNfyOGbypZ6CKdUGqiCi6sNQTZDEvO5pAWhRzk5KaaLExjbB/B8Vhzz8rp7D1z13jsAWz9UEWP0p4rnhZ7RAhbNGVRl34GYRI1o7mb6nCO++pwyjiuEwTPMFtpdVG25yHSUmsBVwnWMrTcZvR13hV9G+DKpYtjv02fmYUu0bNtpiMgEcY6D64RTFfUcXgNdezU0emopPUsugbadnDuLvPLB4kMleMrfqXoTMYWOGLPrPDsumE1XK7Rv4/O+8rgvYoTiBSLtYBWBcADvwGtmakbowlPYGvBT1Z81Pw3Iz5w7/xV/wy/5BH8U+Pzh7/8vUxzBVptonbMR2rYidzxka3XsSyk3CmdJKHMozJ6k5gKMCoGYCaxzjWOiu40Dje7ee7gDZiNH0QzxUvT+vlU+3EdojXbXy82x50BPg7dzyKR4AiTQU1uhDqaj+e0i8jN5vOZkEjawKLMaPGdM6kIY8zhhMegGtA8QagSMvfuDrZtV2jq5HQKUujjZIjzZ3E1NfhpJiSM2wk+0qPeNGSFiOpHb/H0jheqZJ2RY8GPMiPHnpVHFiD1eXo7KzmVu3YaHpdZxCG7Lfo9D1A79j5F6miOw8zP1bBMJrWs6lQNpv6xiJZ86e1PKkoagNw6Y1/eDoFBn3zN6fu4+8enZ2BKjZlq+GOg1UjeuWFypZNEiyNSdiXFL9uHmSxlDqhoSoob0YnkorKKfrmTKM1Calm8uhV8eHpr8b0Z7Xgw+5cPjuEV8UbMvU772FFbNVA35SVMbRp9Iy5OY1QZP78+8xfPMuIcwEoPn7y9XWeK2oIjoviBkWksVuHovga9XQNUkh8L0nZtuwY148facLV3igM2Cup+lJqLPnk4YNft3aIjdghJoAioARLfrOYQtLAOsv8q/+te5CGxwRAhDZjFkkAZyKEU7hk0wy/rSBV/OK6qqJIMqwg4eAMbFJcL66ghnfJNX0rLDmWNFiXtOY4TGy+6lCyALncqEwaJT2V5o5jc9pQWOEhFLd2iI3YIQDF86KmkGKG+CF9BFYGjAmKRKaihvT5jv/s9ShOiUL/TEZXaP4Pbn33z7OzJ4girlGG2Nwpip1BEcNplkH0NAYSZaNaAus8ygSMAukRF/fRbJcQxuhpBoriFUVxa4fYiB1icvTgsIDxc0YRhcGNUSQhy4ij6bSqMtZBeIhRnPIt/0qyN1UxNChmC0Ixq6Y3EcXvr09aDpko1rYo0oANloqG7d8BRUuieiZkW3rYr6yjNI6GJh2QjwQ0+dHjcTivlU9KYlXc2iE2YIcAFAHEKaJjUCQVQ9KqjFUReTI9AA8G3Zo6Nd6sSEBpTM6yWVBD3/Eg+046vflnRtE1TsL2mQhj59RCwd4fWAjXyWHYDeQ0L0kwjBy0UVGJYXTaxkivnBwt80XrlKABOkdV3NohLt4OMbh/w6M4Q6IynhoCVwtqJGFVmlb0gJczUr0K7uO9jGAEAPFmRX9D3+b/AG5U2rifZl96FB8/+f74RtEyh45XH3VjW60TzuGaI+cZlJwjWJZR8QmtW2ssjGVU0IITvLlA+MhWMJFqY3s9zw6juLVDbMQOASgiScRUjRPFgCLQk3oUCTHiyr9JM71TEYGpv8mfInAEraEQ2gwvWTVHFM8ARUcowmQxQlHiGBZFcupQ8KIFnyyL+JIkZSjgrVTmPRR5iUfqUxlh1KL2iuKSVXFrh7hwO8S9G588uLaoWMk0tkBw0opfsbGmVSljlUo3tbAhjqkCmvHfR0Bm6Tz76CdC8bBteXubN2hkl1usPAXYI8lQ3lD1O8nJssLIQGq1lNjAGIrrhFJ4mrdvxJHPOhoxi3uA4ucYtmztEBuwQyCKEEhIRMGDsgDkr4IivaTSqipwlgqU2jN0QpvTPXqZC4rf3D7sluypoC2ZNZvfMEC3jdh2bM2TUA5KlnjKUDg5JAzmWvBW1XG0yiKpo6DIATWjuLVDXLwdYnD/0KM41YFWmnBXBfIYxIov3KmYToYyM5gyrAqyR5BVNZ1UBz/9DVA8PnSd7H7L9mARbT+iRoI9nJ3ejaKYl2L9bihjlWRSfN20PV1KTJ2bknfsZaRDFIZaPWJvZOzeHLssvzqlueLWDnHhdgiP4mc4J9RRNWPUqnUQ9m8H0RTgzBMRyEyll8R5NUn3/4oo3r5WF+CKZPhm61SxMyiWrIYsjvTWFsszkXWpBZf7aTDWVjscGXWUAjuyHcgobu0QG7FDIIqqZjI0r7bK/KxQutLm8gG88fDNicQ5dyfp3T8iikfXaC2bg5SZyKLjfx0pY+tcCymFkrgfxmnJztaBOi4XmkSFTqJz2vQ4mVEAMqo6BixewQF6a4fYgB0CUbyzUPyqSsECfuaEETIErxUzthbVuaGQ/ooxnPjOYkH35nP63iuI4tWjw3aJ1vFz3PHpC6ME163jtP4oOZWLAeAWtSzvsJ2MRuokqvKztpJEEs5+GwYU+TiG8VjClq0d4uLtEPcAxUp1TPHxl8lkPmd00gkApXwG1vjjVGilfpWyAKZ6a3F+vuR2vlgIit8c31gmeJjz+OTkJGlgD9CyyBPFAny9lInV0TqO2BohT7vtrFCWUli0tDkxa4uaSFHQJITUe1E8PR77AXprh9iUHeLw8wd3dBzlNxOSMrpOJpO5ACVkKYDzgGRqP+n9QTpd/PzqBbf/PM2q9Mqnf/Eofnw8Sfb/4e+9euV/Xv39vGtLF5m+C1zMoYybFjMPOem/0T5UCMBCFm27LFqQQ5lG5pQuCMuNpQYueU8Vh/2DNvZktdFH0le6z0+3dojN2CHuXSMUkTsAD0icyA8BiSwGIJVTxi+Nbxt09aPFeffs5XP89/L5iy+WdbqLKN46nu7//O+X0n47GeZl51yMIlvHHOXeMIqYkYj3KD+7w3oVi8XdfJlzkj+hSBZbTl3NGUWtWSrHTFP97qEe0CVZWYTi1g6xCTvEvWt+gMZIAhWQ/8mbVFRxEgCbhHs4jBsQBdyJqiITPO1Onr0g3J6/fPHs6TLb/fQPgOIP7dUfPYovXrwEafzt7u4oKdu1KMpmIKfFypWzZSGV2kNZPz04X4YS9Fhzj1a+m1yq7uSUKsgLjeHUA5OQJZe98a776vT+1g7xX/bOtzeNKwvjNTYjjJuwgMdeeQTTIuR16dQTQmhVVSU1VBCpTbQ4485Od7TJCLZEWa26Esaff+/5d+8d7LSvwqu5DniYGZw3Pz3n3jvnPGcn6RCkij2RswaOXiMEzvB435zNodiwxZKPRBUbJsTTda+0WK3vNkCjIm41SLy9GaI4Ti9nawBxc3d7u75d1ie1Uju/ajGPAinH1qDI0ZkNy84r7fl8mcy9NG2rf23p0ibrap06Uc6vpk0TDs2iNLA8PCQUi3SIXbhDvPQ/u55yMGYM4SBkLsPGQ8PIH6ujTCphhGEopOr7vWQZrdW429zdbN6s4omDKL47HZdGs7ebu020WkUKxfhJfZG0q46UxcgTwKqp8JdfZITSZjDb52ma9ebLZZbOD9JSCixqVygtkvy0Ou+Cd7TVCESiNdXwsyoW6RA7SIcYf3Yd9GzO9pFAxClsuOroIRx7mrweSKj9B8L739n3kgWiuN7cRpv/reI6qeK7wbTUOVMo3q1m0Q2gOKhPkkrVMTVaTq4GWxwmHA0nKCWcOe+nvWwVJWn6e/J7UjoHFulpYdV06WCJ1F5Q5fJDa2p+NIhJZDVRxSId4uOnQ4y/vB72bDmTwxAGYAVY4iXCk46M4mE0bxj8+DthKMIYCoq3ShbXiOJSUGRVvFOiiCieKFUEc0ZnG0V49au2z4Rdda2ITL1w9XyWNeY//XuxnKRVdtsTXz72h4K974pMG413qNXvID91ZBSLdIiPnw7xn1eAYoNowyEY6hN40oWTbkNfyIOLgAqtpIrmMjDZTPOqKCg+8dPRbK1QVAGaUDyeHJb7jtSo6rJqkD62hiKB7JuATZlkqbt4HcVuI/vvT8tZJ7HcHU2/mD4V95cfcFAul7amj3RQy768flWkQ+zEHQJVscEi6Gr0WNj0cF1XvRpbZxk3Ody6aESyN38AxR//9du7i3Ean61RFTWKSVrV5dJdqayGYsSMfaEQTbJDMSg6qbt6Gy3DbJEkcXQz6YMXD5lPmRSKftvU9mv70NKHG7aVSjXn8+tXRTrETtIhFIqvfkCGXEJOEwn0CV2uSyzyYagvMH+uBHPXApqUE27vzc+3Uax99SOoolpBn93lVRFQREWkAocuu0+w+YROZ8SCWStQZ9nqJlousmQZr16/vYDtRnk+U6H2HZJ+a3XLKt/LbNwahGKRDrGLdIiX488Vii7+0BsRx8iFhkSm0bVpY+DkXkRRfw+vENHzPs8Vcyj+9g43c+7suSKg2EcOde2qJ1X9hKL2TPHMnNFxzp3SozjqLLNFvHr+/rtjCuikihV8OKjXLtLlo5xrl/VwQ00K0EU6xC7SIRBFgczdgo4Q2zohH+zoLcwRlG4+rKvAvl9NSBXvCMXjbRQjRvH0YpLAXFFXC8KbR7EaSPTEMaArFhZSd+Bk6eLnVRzH0dXbN1eHkNXDk8V2hXPAuTSmJFWCZcm1zTdttVCUuWKRDrELd4gpoSiIIVPhAwDaR2GLbrW/ItyxtIJCGjh7TpJTxXpTUMxOcyieXIAqgiGFFK3ikZ42euLUg3Xb1Zy5WZbMolk8i15/93ZUVTJ53pe6GEydOO9XSiVdMN3WO9+lD3eA0QG6SIfYQTrEy8BWRRytlvvHQ93wwXt0NA9tGW14CsVba1/x4DGieDH1Bp27zdpG8bDUd6AEkU1NSBtNoPY8Dt/s6CO7PV61my5nM4j0z89ST1wmpEarrzcW2R/P2EvYPYkqpUpOG/WypUiH+PjpEMMXRhVb1vsWffblFoCoYQz/hMmW67uNpqC4ZhQPCcVx83i0hWItPXe6UPBlVLGJVhO8mhaNdDzRSZgXwpV5Opgtl6uok0Ilq4rY8FgaWTznMG0aW261LNSnrGwJQPHQ06pYpEN87HQIG0UCDF+WOppjPuG38sL4pyrqhvNUoai3uAcLQXE6r+dQjBFFj4wouJaairPFFcrpstUekwiBGn2Ve1mSpEm6jBfzeVNF7X6awpoF3Mng8aA8AjTVWTqbsWx6Z+ndRhZHQrFIh9hJOgSi2BLZQ8nj4TJx6s1vMYstupUv5yJ6LmprfYXv+oSiLFs2s+VinwL0cbBfj/UK+m4dj57UkxKjqElkowASQu0xxUsYFamh8sDL5oOb2SJL4kGaZUmp65FhI6XvQNuttq7OqkiDdLtfdU4rqZy6rFWxSIfYRToEq6IoYMuGMT9cJJIo9H2Dq/qCT3S2rLkkQwu3KhXtZbBvuFYCeLPZxMtF70hQnAwwHSJSKN5exZcDRNHjKlg0RAEkLVX0cvNGUkVFYjaPb1bxLF7GnXj2c10Rigb2mHRLnbioG2Zb18dw4g4vYMrbZdWoio+bssVdpEN87HQIQPELwchnDIEeoM2H0aIP+I7XkD06IVrJwkmTSMMy3j+Gb+xng7izunn9/vXq/XuD4kXQ2zt+vb7dnMWnJ3Hn2cloMEnKhCJ6nxjTEx2Su+zb2KX9HVpJKxSTTrSaRSs1OlG0wIoY43PCKNotOawyQVZFU4Sgp41HzRfXRTrEjtIhNIqCDrCjGfS3hr7cYhR9UkW/NfZFKn0hWqPoK1U8uTw9jc+uvuo+fTsCFDuEYlirX938/PTTYcupnTwbxct6TVRRCrPJtULrIqEIu41dNmCGXW8vqw3UfxDHg3ipgEw8LhcEFB1uCJxbT7eluSC1uGSxtGxPcDwmFIt0iB24QxCKyJXLlI01jfwZTtDw7SNLMdXn8RjRBfbGDCH80N2txsFgdDkaffX1qfv196OBQnHEKD5+9Dw6+yb4rNX+yyWiuIcosqWJHk2xFGUb2yYZ2prdHFxUZ16moNybJGoFXa1mjGKVk2ylOwwTea/7rxbKto3ir0U6xI7SIQBFgE6xM0aiLN7oc/7It3/5Y6G1xR/or8Df860/BCheAopPTxtPv1cBunHU+TugOFQoXkXPvvWHbnVy+SyOl4/2jgjFfXTl0Shqf1H2sW12PYtEtJ6vdh0STVpoZ5mkkVHat25UxAbLbaxB4JYc97pRkzIezV/8WqRD7Cgd4odfQBXHGEpF/3xCkuTRYlH0bzz1fYvSe6RaH6Zw93Qcfjq4PDkhFP+mAnSj1HmjUKwP3aQOKLaGbmXvFFCs7yWp12RHEx2nm3rpYu/v6O2catczRvbycNDJuo7ph0R94frcKokcRdl3nl8UxStW0oRaRx+8KNIhdpUOISj6rfuil2PNnJoiYIDYNLh3G4Bn3YooBuNw/+JkcAoBmlE8GgmKk6tvz77xv2hVagOFYlxfKBTZgIytGWkxzU7L7GprW9IrPZTuCI4nzT1gs6dr90OiREeuQKBSGUFROgy3K3acRhRxrlikQ+wkHQJQ9P2pHZXtMbXezSmNon05mBr6hFe4IwBV3D8+HZxeGlU0KC6uIkDRbSOKgyWhuJ9zwiP8cMa4hWKXZNGz5NDsges08KrDht9SMOhwYbXd4Fq2HyW9ER0mIEB/UqRD7MQdQqH4V/9hIUTZmxq64CBAyKb40mOM4jgNptMcivh1eAvGbg9R7CCKlwrFx4ji8bCVAooqQIeVvYFatiCKzoE4Rolr3oHZ885NHZtd3vN2TNcY88B6uzjG4TWMZFAwhv1zLvVvSzIZaWPZQrFIh/j46RBfKBQZtACEbUoCxxQpjOhFJwL5rbgbBvoj8zgMphaA+GUeat1S30IR54oXCsUaoOgGjfLexbNRx0bRGEaxzVnz/orarGC68nSaUMRtR+eBrpemHyu725ImttvcaV0Sv7FPu5orKhSLdIidpEMwikDXlNQOkFQwDQNmaTgM7IEf1WVAEQcBGwCcGt9gyCjid4fTVggonnS+PrFR/OfF0E+Tq29m37rTRrl2fMYoege2GZmJ1Ha/DQ7S2AsGH8F4XWvQI5l7IFa1IZRj1bTqTuyIIvbUEo+y0vyX61efFOkQO0mHABSnonwBqdqYCCKWZJhjpFGfCeh2uYdgHSKWwTDg2/3w0eDJ4BJR/J5Q/IdC8RhRjADFXvmwrlCMNYq2YR46Ke8bFD9lFJvcRYEbCHLqtzyL8bom19uSxTycPG0UJqvc9bJvo1ikQ+wkHSKPIgMZMEwEErwFmkJ+M+9w+9CgqGEN9OnhcBxOBheIYk/2FRHF4P/sne1PG0kSxjceY4EZQH5LRjuKM7asiPEQiCFwh3Vr+fAKciK7Okthvc5ms+sj5nQ6IfbDRvz7111VXV0946D7wnyaiV/mxeTTT091VT/dJVAEVZx9nigUp356j1Hc07Ysdmmmph7IZM/WHRsYsHvQYFVuL1GtyuYHsOIAKzxkmoBAPaC+qwOcrFYo/ljYIXKyQwCKe2Jct2d5Quk7PhYY4jF2bknlPBZU0kP94/OWQvG1CtD7/cPfZ6yKteMXi/nf312cAIpKFWegiovpNL3hLe8tb7YKRw8Zu3fKjXS3N9v/UmwvUSESF6bB5WBgKuDtNnUsoicwfiz5CsVvCjtELnYIjeIepSkCxVUAOpd76dt7KUzpbDzWrzSKBwbFs8V8+O7VSWtPBegtE6AX4TSzkyiJo0HRtoihxjGNFIey8sjbm9jtQzWOWOmGTU8qGKMruL66soC6T/tlew1QLOwQudghEEU6IONgFDVFyBQceMeBzIAn8MOfmL87HuPHnkZx91n3cN9PoRgqFLsqg/bXtiegiipAqwht9sTjLUipBYdpH0N9OWyJBwK1Mdk2qNEb6yJlLKEzbKxWafD40g4XBzB1bUaQgzXvpx9/+KawQ+RihwgMik6MBprGiBQSOWauAMsx3SXV42+kV97G3z9XKDYViqM0io2PShVPD84UiltmrLhoTGlzRs9sP+qlW3AIFG2gDjlcS5mENf3Uw1odC3O2AOqo6PiS9s5b8MSMPgjFwg6Rhx1Co3jM+bBNkxEkEr+xPSxehCV+xARnfIx/Z356HI/HcTw+fnGtUDzqnox6Q4Fi81yhqMaKp/XnPUARVVFvkezub9v3uPmGOLGi6IvmrKJNK9ttbV0nzCyhzlR8qhbF9b5GsbBD5GKHYBTdJMWgZrmLs19xjFcx/jC2rMb4SDE4RhbPrnebzaORQtGq4n9+2T0/m2pVPFEoljYnF0YVpx5vY1un7b99DNIcrlklMT77DZHDQJfMsuObYBpFhcdtD2NqjlUJ6TqrYmGHeHQ7hFVFkY2IMMzQabjgfRzTlQVu7Mim+D2fnV+/JhSHEsUzQLF7Un/R29yeXHQVils6QHtym2Xeat728fA9buhmB4wrUBSrDkLj3EkLYWgLPoRnaG5U2qiKhR0iDztE8EGhaIOyCMaAHqH08GHhi0kp4zjgG3Br7/p1bVeguDH6BVA8Vyj+o3uoVHG7tAMo1ihA0w6itK+o5zYnsoVvMWAU84IUr8vYVJiYNCiGwukYVipinwmaxYYrGDQO+pBBF3aIPOwQCsVoLAPxGIIq61n8f7KoPoMgpYUMpwrU89pW7TWg+FeLYlOhuBi+kSgeEYq0va3ZdznbrEi4GX3qlFl2RZLaWZtO69Y0Ic6BTsBO5zOsmHBHvRnFwg7x+HaICFG0sdUqXADvwDkNYit4gTr0B/88EE8DfEyn8Z5GcXf/dDWKQ0JxplHcgbFi3e73bXOXlCaWjWnHN0tgoPevj93T8U3Gsmz9u2I24jGbn5jteGQEr/apxF3YIR7fDsEoxvQRW9AYQ4YO6AqcgwC0V4EFlR/Fx/NmrdmUKP5sULxSKPafV7Y3CcX5x48Nz+6vLJrGOF3efJlUlymDwTdpY4PkMUSnY3Yqpmf1sULOxx7tzkObRVXrWFcs7BA52CEEinJgiAwZEQxIEhE1+oyiCC6iDJ0Op3hAgG6OTvdN2rIPacuLcy+8ejM69FvVlSj23aZameaVLor6Hnehxt7oFKiZRbvThHXx6At0PfZCJ4IrVax/gGJOYYfIwQ6R/GRRtJGWdTGWPAWEHnIIKBKP6jN6AMZIozip7XZPRpUsiipt6dWrG4ziXKHIvRCcZlqpmUDb9JxMEj57JsDHQ/PUJrcOeQrGotggFNHpmAKRVbGwQ+Rhh1CqmPDwMHCic+YA+hA+YC/CO3RJDwnRIIr4r9RLBegtQLGKKG5qFH9uKhSnV+8Uiv3qRmnj1UijqF1iXqYhArdwk/3cPLfaLeZhfE9WwLHozShiRo1bQ5mVMDKjabBiIoqFHSIXO4RGMXb0MBDxmJEkugRukXNlZBL/IYkWzyAaz2u1LVRFGCuWAMUaoPgGUNwsbWAGvQJFqOiYFr6ir6oicSoP37eN0n00T5h5QDsVY9YMuisHKXY3xFBSfQ3qTom7sEM8ph2CUaTRYcxJSJwKyykIU6yZL35HFkf11ihOdtVYcSWKw57fBhQvDIr9NIp17l/JXVXhcFAklbT6yN5GitSNsCxnBp0NotI2M62hg35hh8jNDoEojm35RVIYyRxFH0mGxsx1YEJ3IIO2QnEyqY1OVYDWKLYIxTNAcTTs9dsbpW0doGdNjeK0v6p/FmP4NRRNSl0Wkdp36t5Y+DaTMmkUcdbaunDDBaQthR0iFzuEVEUSw5gHhpGTpGgQkyRZDWX0EKSJQfFk9NJB8fy8Tyiu72RQPMgMFkVnXxOfvannoOi5y1a5BE4rBcthWWgi7VVm4nVoZ2YI1wVl0IUdIgc7hEKxE3PRMBIJCkdhkjegMIEv/alvdQBOQyl+REmG1CSSKOq0pbUGKG6d7yGKFY3iJqBYAxt3n9samb6DDoruUNHD4GxRFDUeXNTvLBYspyYIw7L0llksGcXCDpGLHQJQjEkLTUBeoXsJIJgQiMQl3YTHkXmOd92/TOL55BoD9OF3TwWKWhW/HQ2r/vrO2mZXO3OajCI1g7G6WM/MuxCKKI1yYtAm075NphnDhl0js8Jbxum1QvHgQ2GHyMsOgarIqQnVZhKG0SihBq3DoMkP9epEiYHR6GNChNLv4vmWUsX909HLw98zKO4Pq721nbWSRnG2SyhSOyLszObYdKYig8ZcZZpBkTJpj4uPYsNGA6MzLUNjR5loq0tEsbBD5GKH0ChywiyKMwRdJ+no18oDHiWJvMIbCf4JogskdgDFLY3i8DsI0E81ihOFon9IKK4TihMcK1LPDUIxRWOq6j31jYGM70NdZwq6adNqM1Vd5jKkk9I0WDXNWcWgWNghHt8OkRCKkRuVcf5YFHTEWZyedKZkJ7ZPTV1I0w1IB/PJzmTrKQRoRvG3iRor+lffzq4GvdJOu9TtXiCKrIpOe+k+u8bcCZi+52PFUQ4jdWCmYaRJX3xPmsqIy0wh3DGbIYqFHSIXOwSjGAUi50jG00t9hPCaqg98Ty/Ll/Bkeqv/LW7hHt4VTy8vb/Hr8gzTHD1WRBQHQhX/CaqoUByuVzY1irNud/ZaonggmgMjglIeaRkWOSXUbU/OwniMopNRN2x0ZqkUuYxBET8WVhULO8Rj2yEUim9ZFSkbTqLOeHm3/Opx6V5cfv2Xy1bUgf9SoTgHFFWAfipRrPtXF0+H61oV15QqChSdVqycuSCP0rFDKw48Uk1P1hzNYJK8E3qaumFE0SbYvs8eM8Glvh0eFHaI/OwQiGIUYBZsco6x5uvy0rzwWxy3t1L7vn609IAx0mPF6/mTiQ7QQydAn9enGsW2QnHQHnW7GRSxzaqsMZJHwq01ZsePmj5MaSh58cXiVd+KIj+S8Zp+QygWdohc7BDJhx/e2hK2KRp2EEXBYArGzzNF4y0S+QCQyxeU/SCKz0AVnzko+levng3XqttPKlWF4mx2JAI0tVStm3/WOEahWushDBExfLtzgj4HaI92DjUVb194y8piP9GyX3ZwZVUs7BA52CE0iqICaCo3YwPeEj+WfA5qePfHH+/fv5/NZtd3ywfl8TmhGCCKf9EoHikU15+ZAO1pFEvVjSeVykinLUdbBkXZu1JOAOI6g7pMWzwK1J65wwGaCt9C+8rucmpxQwRs+nmv9aGwQ+Rlh7AomsqLfmtVNEJoABSieHv35cuf7/+8Use/l0jiahiXLaruWBQPAcW2i+JadWOnFwKKM724pdGvUzN0CNAHZp2LMxVYl2teyLBDTjKhj33a4cSHJaskeLYEnlrob41mgC+hWNghHt8O8V9HFe1sydtxCsRlisbZ+89Lndl8/kwJ8/JrqqgLjIjiDqL4N1bF73UG3b+6UCi2GUUI0A2vbppWmmoOoYg0cqw23BGKRif7nl2D0DeeCY+dZDQPI5cnpCUSs/CwVdghcrNDdNwATfH0LaqiARCDsDkO1Lt11tKnrdvnBwfm3u3talXs4FixtKHSli6pokLxRqvimULxFaD4JAxngGLtmlVRDBZlwgIo2tVX5qB5QZvDeJy56JlBQ6Rv98rLuCd4uEj7LiOKhR0iFzuEQJEHiqiKlLYo7dP/lnd3Mx0+Hzqo/nO3XLqq2EEUtxWKr9oSxR2DYqm986SiUezOnsGKgv6B6ITuDBelb6y+YvrFCCJA6FkxZD+Zv2KNDO/A07A7lPmMYmGHyMUOgSgmlkNEBwO0RurOFBivbu5v7u8/3X/Sr0+/qrMbOIPzX+/v72++mGritSzmwCxgPJ+vbasM2qDYPvrt5l/fb6gA7V11EcVqQ1e4FYrXGkVKWzhIA459KnT/j70z/k0rOeI45vEMGBsbMPGpTyHF4pDv+XIYkcspkuo0cSu/hqp3pHU4UpyWM9iNToZfTrLz33dmdnZ39j2cc2IFyRKLDbuA/dNHMzuz350xIDosloWGzLkIw6paw6QsZys2jvpevzgbDJZyiEXJIX61VlGfFtMjMnnFyQxghAFB8xRwm/KQEzWHz97PLrsziKkvVViNO0i1V6zDXnEwTMNe8dhF8duXCsVCDqxij6wiybjxyl9V7BZb5Wqr5d52KeuMjikjIdyzxdFIeUJtJGMlJjJutRPTiprMY7CUQyxODmGsojaKJGIgFMkqIorj/hhQfD81+F3jIAKvPsDslBG96gOK/f64O5tIq4gDUMwhin9wUEQH7T09BBT9lZUAUOzrJkKe9tAttVvURy4iv6h51Imdspd019ZA9kJ8CHtoUMzEZN5GESFRXMohvrwcAlB880eHRTRjCsUu+Wc+1xu/m2rrd/Xhw4frK3DL0+n1NUzxven5+9PTf/FZIPwRhy12rzjwC+CgLYo/n//yNVrFUKPY8MgqqrqzHEEbGjm92HJQtAJvcxJoouxYTTwiUSW9TdO2ddlf1VbdqbBoDL8QLOUQi5ND1F8DikZ5qPVd0TddHbWMYczGZ2f9UxdFmME711fE4vR0+u78dHoCXwQPDX9gwpa6sYp+YRNQzCkUh2gVv85/j2HL7s6LorKKh7v9QyXjliiqTDe8MIpleRTIIglzRG2OY3T+Rye9Q705ZADXY1WURQEoLrYDM5JDZJdyiIXIIcgqGgE2yQ/3LYpg185maiCKmkZA8UqtcIoowup0evrbhL88u9RWsR5pFIeM4j8pgkar+BeDYj69srXq9Q8fs1UMXKvIMtpWmY+kW4k70mUJXyyiie0N+cK+eyeQ2xJl5J0ro8xZyiEWIodAFO09AHU04ljFGR+lHKNBPJ0a08jj+koFM6fvfzmd/ta9BBghbLEOmlEEBz0crACKaYGictAnh50XRUQxfEAozrGKyjfL+wVznHRYDhOaHc/NHXrr8m6qF5fOxq5E6wsF90QBce/lEIxinU9FWLJNKJJZnFHY0p91x+/Pz6/OebxLTGhcXHb7F/2zbhJFsoorHUIRvL1F0QMU99BBbzXKHUDxkNtllN28oo5XlIKR4xe7VQwdpQ6f+OlkolXlaCMo5LHi+mklqIjL0PQmSWezSznEQuQQCsU67xI59cJWkWDCBA2idTa+cfRpO4lPuLeUVrHLKEZfDYfNgUYRlTk7CsVHnndyePAi729tVFqMopLmtKRRtOIcjWArdi21bDKKoZEqekLFndwVurUigqASqzaG61FrKYdYmByCUNQImlssjKJK5qizP9bgTDBTo3KO5o0z5nY2nlxOMGQ5s8kcbRWHw2F6E1F8Sg5ao/iy1wMH/Tyf3tqqsFXsWBRb1ZY9b5lz5mK3hviim71Q1saervRsUR3RIzBDN/Mztp6OU0Rsld00Xz5dyiEWUR1CoWjuS+1LFNVekeOWsY5I9Bvm1X6kJwkUwSoOfH+z84PeK/oPEMVNRPEp7BXzhY2NhotiuaXdszn5S8LophF79kFHz564UCDq5oirVMRhoP1zrDZygDVzlnKIxckhXrODdi72WRS7HBTjQTS+TNQP/874SZ8945fkGfSEkznooIf+AFAsEIotPIPGFPdDRHHnxWZeoYgy7o7joFWwUm2VY5FzWA5D55qLOmdRsgdv3aP8IdrETC/DbQxMHQiOkzPGEcNDl5+lGp9rumw3oZhdyiEWI4d4rSJoe4XUhi0qcFGaG1bldO3cSnUuL+PvuHKIiKzicIhWMZ9AESPolU1AsdUBEHU1bkaRSKyK6y1lGSfT5rCnI2XVtiBjqzfFAhNR2lMO1bF3VfUxp4UtgNwOOYJeyiEWIIdQVjE2GMUuX6JiS3jrYaWNBkWIoMFBP3uiUXzwb4niJqOIyRxUiWGxT3HkRyS6mRrhk+MVum3PDLE/rHAj84apBq8s36pisGEaujRkPxdCcSmHWEx1CELRuWYvkzlKmvPJY9JNnEGzg35SFCh+LaxiaaNR7exShUXOcbeqbrhiGwpJErU61hNVIER5BwfFhtP2jzq0NIJGsqXVatO0EAr5tGUph1iAHMJF0bGKXf3UNfZxcpNcu+vcyDLjkbKKhGJzsEcojs/YQTOK3yGK26VKdUxn0BpFdbTiiB/crkIhny2HrHJYd8o92JYZIlFjmghhN4zR2pptakXNrNY0iWvci9IPzcHfUg7xxeUQN6PYnUy6nznMX1YNirBXLGz/AA76v2gVKYIGB11FFPdebK3slSoPx2QVOccdls0O0V5lYfmN2R7aSwJuM6FKvKQsd51UPdNUY9O1drvZVH3Km/xQ/U+bzRo2Kce5aje5lEMsRA4RfcQq6gv34nJB9xPpfOg46L1nT4pP/zQmFNVesVoJNIoZdNDHx7rjZDjnaM/e4tN62B7aRa8nFIeZjKkDZiFsVBrKFnJb8pGaDBHFJg7dhbdNK2IRx9BbNstYmByCUdxPoDi7VWWIyUeWEzeZM2rmYa9YeIqnLa20RjEITvoHzwHFjXVCcZdQHMRQtFdNKU1Ih3kIYsg3BjLrzlGyaxaBwUoDwxHV8FkZQtX9GQeaxia/DRNY1GoKxVpbW8V7KIdwsjrCGtqgJrH4PJiyqZSIfj578Ss56GSRsOgrys0k8zWfOl7ag7/Ran6PUOxQLW5EceUlovhg78fSVmdj/eH48fHjY0osDnSxT33Nz20hZMviyA4FFkBO2lADgkZFd6Yi9tYsiu22RrFWY2dNz7AEFmtIpO+pZI7OyUmbcw8Wwu2KlKDUSSQXWcd23maRknvIz18oFOd4aCXTUQlHc0SNXEW6yqJb3E7N9uN5of2IrSxaxQHsFYsxFEeA4var0tZOaf3RGPzzrkbRC4XawYYmjtxL3QdwUtjIoM7YmBQhhiC0F6RfxBHh44Hg5drqHZzX2rVcjia5Wnr9Lff4s4dj92ThCg6ybvblIycnKZH3u80iK44B77SIhS0RPWgGkyh6gz/2MX+84V8e4p/gv1D/FVEcAop/c1F81BqNTnZKzze2DkoZQtHcbumZPKIXb2TF0TIJXysiVAk4j623iA3Z7JmCkyZZPUZOjyZC12b4cohhDp9xnl6ndpNCQZK9PwtjJlOSzNTNmq2YcvETF9k7LiSKBiCydJLIG4dhjf/BTYNR3LMoHioUy4ziRmcj83J8fEFxC91u6XkiayOKHsfqvYtEdsWksFfdrpEcF/OoGRJzhBxNeOHnfN/nGb6f7gGK2ZQ8pLgfC3e7KNy2pXHOwkojUqnbLmzG8m4Li2ICoygJVmQNZ+T+QTSnHG1d63BJOksoHjz7u0TxP0ePykNCcW9jZ8N7SVbxWGdzvGRlMOdAz4bMogd5w7R9DkZgCikqbuqwmE1gu53j4WvweO6n6VnN0SoWejqCzsr88T1YmGPilDyRtsqabCq5uIs+LXXnhQhb4mwJV60+NKaQPxZOnVda7sh1kM3B9j6iWGmmtzWK5YFEceP5NqAYfltiq0jZHGMWTTEHqbkWokPR1dR0vCdNA1lC9Mt6H6gtYJttH7KXZvBglqYnesUJfl7ovaUmvDY8zd6PRUqYwvjm7OYz4ayNcG6/kLHwHRYSRcGXokvhaDxx3TBo94N2axglK3Xva124QrE39EsCxf8RiiGiePQKUSx/fwQgXhwfahR7pvwSWkKPr0bZZmnJTlQqTF7j5GGbM9YYhpBTJm/sp3M1DSJYwTRjCADij8+vBfVOIcNhS1bEAvdhcR/lEPNT3Cbg0JQ5CCpA1VeiBH98lVpcl8EiecDWcAgo5imvWC7uglX8aeVhOGwiiuCgt8M/n7FV7BydDdsBBshW5CC6CUgIdR9JjJWDVYMi5QhrOliukc/VjjjtWkEmkmHUo0AspouVN6//sZRDLEYOEc3JKxobWI+ijwQuyQ3lvt4m7scGWMXRaOhvE4poFfMKxaqL4sXxxQWH0ICirPRlrqTgDzbPdY9TOGuz5gybq1Eo+hyWMIrIpLKKaTkKZBEZxTyiuJRDLEYOEUcxMjYxMhxqH2xSNfNd8hyrWK9LFNEqFp8himFxFxz0T0eAYg5RPNh+UCoDikAio9hcxfIMSmwjbkdVGpi35nbOSvjPyi48WG7HSOQ4uWaCY4GiANA36OGkgHO1LmwGbxWKSznEl5dDIIqRMG4WsUiGL1H9Bvgcg2h1ZnGrCA4aWFQo9sfjMP9Yoeil/ZNO6VVnD1D8BlBEs0iX/nJrAV9Ydrr8OHlDCpWBPx2rrCn4tDHM6QQNTRIEFniIabEIP/l8Eae03AzIQS/lEIuSQ7CfjYXQv2MAXRDJEM7xzNxlDVEMRsO9Z38FFHcAxU2N4iBNKB4wikBin+IWvx1UTB0R2waSzCEr/1dHmL3G82NU20CI0mQUbdLQJGz8OZ6YgCsWFYRpJK+YBxBhEI/4Syguq0MsTg4Ry8xENyYMb+xqJaGcg6IKWwjFPDpoQPEYUPz5qNojFH/cOfhum1G8uNgFFDfT7SBg8Suh6LRrXjV2kE6NR+iYa7U1TF6rcxPKWfv/Z+/8ettGrigOKquFZZUiGSsiYWETWSiy1MpS6DKy4SDLqCYqq4GBwKgV11mhgGqjTrHf/33n/psZ0gyQl+UTJxJFOq8/nHvPnUNyTzeFZQSNDPaAxR7KIWGIy/M8OHS8H0kVmzjEnx6HKKNYRnJ99F2KKPW5LIbygO/R0cKo4qcyinH+fhAqFCNSxfHs9iHw2ifQB4pV4T29od5U3kHwlVNdO4XiyT5WZOAPN+3Up93as6txi1rALqshUYjqhxj2hEEC0VEYOk7H2aEqNnGIOuIQJduytolcf4csTu1GsSCE/FpeAlKp4vVuCw4ae8Vnjkaxu0nzT4OEUbxEVUwDpwUomtuj9N1PmLzGIQ2lbDhnw3PDPXEm6tRMCkULWwJgj2qxOiB6lhYq/hw8OHDecVAVmzhELXGI9ReD4vq76nGFYy5V46l+TbTgyCgqVfTItjiz3xSK7ovrXhd6RYVi/AupIk1znO5rvg9AbtT7Kw9rZGRDDDKQ+ye6PaywyJYzQfVDDfQARqV9NocAoQco+oSi57MqNnGIGuIQNorfyZ59oTk07znlF/HabyiPAMUD6RVBFX2wLf8OXlx3eps0/qgKdMIFmlWxu1XWRGcP0alQvoa38/ZfS9rwNYVdgcTylMa45K4uw8IeUAjYeVKThUVGEZWRUGziELXEIRjFaUX3V90YEnJPzPKoKIoj++3k0YhQbPc1iu4hovjm2utswodPgzBLn49YFS+zMHDutvtolsUxI4qQOcRsw76VNQTPLBsppVU2KFCQHZs6h0uxuXDgzFcLL9wTcdBNHOJPj0MIiibzWri9YFrWxKkkHWR+w8YEz+jhteZtvubdvgtEMT4/65wBiteC4tDpbNKHT3OF4pspq+JlNujnnfbrAoakiTrpZRKHmPMqqaEMC3tWa8jiR6zJ0fDH10Sgz8txt6iKTRyijjgEoTgtRrqm2hIfmRR3wZYcVU1sLCFkNYzo/b6A4na4a/UFRVLF3/pvhrkHw5x5OE7fHN0/XnGzGOdea0vTQ+4OT0ze0FBIqQawKO0KNbSmM7bsyfKlDMt1xQq2bFuaOEQNcQhB0RZDKdDFHZNp8Q+6URwdkVExCEYaxBHr4jGoYitAFMPbh+vg7df//R9Q9B1SxVn64khUEVHstunWZHTMQOJLAZGCrtQb7lHMqxBi4H2Tbk/GgxUcIoi6DtscurTw1EdVbOIQNT0dwqiitWlX5UqOrLpckkMe3YyYPI3iaMSqqFAcHsDG37lXQPH5LndIFRWKa6OKiatQPLHuWd43avh6T4f+JWBTiSIUZWkFrXpM+KlDbvHnKOyAPPjnBoyiOqAqNnGI2l6W8Zng48/0SC7LjsRqDqfmjQbTqdHDiPvDKBJB5H9QoHe7O6WKHhboH9y3X/8DKA5d510YvFcoJqCKV1eKxkOw0F6vvW8nHHhWI9NDGGG39yq9spgUcMjIYEkVLf783HXz3M39XH0sSUQW4RBvPzdxiDpflnGkhe+oQvIMc/y/Iz2xGRUmNsghK2GkcSRhRBShV2QUA0QxRhRBFQez+IX0iofjeRrkvdYJT7JPcEOPFyAIQrjHGS97Q5n2TnrWmNBQaBQwN0uwU2c2hbAC/MbbJg5R38syLBS/sX9sC2NRB6fyHixuDQsYRpOJUciV6hWHrVhQPOhjgU5/2QWA4sdsrlBc31/dXCldfDvLQmWhWxCx2T/hDT0ZXktf2OYvbueJS+4UKSxgmDOFviEwCAL1dfHrWn9Uqw/ffpC0mjhErS/LEC0cldzw1PybWi9GHU1tiyJOxRBIhwmiyH8BFFWBTlWvePWv29uHg/ifgqKPKGaqQAOKj+pD0xyvtfdS0l57hZBX204Xkj/pPdkyqSjJxGAuvLn4oZOgCGLQj/uKxH4/vWviEPU9HaIKRTOmNvBNp+YF5jaGURlF4hBVcRLJ7wX2iojiR4XiMPkHo9h3oUADij+t729AFa/eKhRj1+nC/Z94d5REbPRS/FHCodfFNBfvm3S88szQHswYHaxaGkJccUy/4V0Th6jv6RD83pZReURo7+I9XVFU5g+hGzGHE1oGyQss0BUoxojiOJulrz7fKxKVLioLPQcUW+09PT5s29mGbqfHARuSQ1ZC255oYyJe2Lc0j5GjGqzrsQ1ikiQpiCKi2MQh6ohD/G69Qmg00o3hSCi04zWygyIeWaM4KtZlLM0TOkyIRERxN9waFFNC8dk2cd89BO/H2RhRvLlSH0AxCRyFG+W92k9Cr6CKcOh0cFOZ90u8kg7SbJAMiY9DGmGOqi+Dx0jSH2Klh+obp6lCMU5FFZs4RB1Ph0AUS0EaKsSWCFoTbEKQPMqk2B5GWg55LRnI5eQCbyjon3GvOEzP/qscdPhsmwabB/eTsi0hooi+RaGYuk6ny/coW3fgcXvIDWIPazJObDzboORoUnKDYlBURC1/9sKarCBMUBOTFH7TwV0Th6jv6RCAog1dwRybZtCQGPHscGSpoRiVSNRQUJSFKN7F56eMYogoDv6yTfuAIhToC0DxTJnox8Nxlga+x8Prto6+UvhVdpU9kMNOhUHBOQ3ODP2CFzHOuIggKCH9KA4RwzThNb9r4hD1PR1CULRVUFpE2rWLirvKpkdkHYyoHFtlGSBU/5aLpVrqYom94k4VaIXiB4Xij+G5hWLwfjaeJStURdDFQ8jm+F7X3JksGS8QQzHLgF7HkyiDPTPESWHull2xoTCWOhyTBMovYpimYSqLUGziEPU8HaKkiprFCrcSlZ0yY6hPGMPlkn+IRbguopjuI4pfBz+0BukmtlA8u8FpznjQV76lW6jJveLUsOCVxaDQ7olbIYbMIBViUUBUQSWBdEQtDHEpHENCcd3EIWp7WQa9mvyJTxaLInkGbZgnPLy2NXCiLwA70EN1WCgQFwTkYvKTQnG7Tc5PHUsVv84Bxb+TKqYXX+5ukMWrtwrFGJrFLiawNYkUbpDEf6kwgzfJZaPkG31h3DcokhbGTKDWwTAUGIFGQrGJQ9QQh/hdo6jYi6xuUItgyTHbA8NJuStcmrVAAgHGJR5ecIqbUdwfCIpzQnE2S18Biuc3xkJ3ej1zRxRByHXZTA6toQ0ZlG9wGIsrMb4EjQnXZUNgOIDFwhjOvXUTh6grDjE1KFL0X/eGU5NskJmhqcqRqcbqG2FJXto1eTFZAIq4EMXhtSrQp4Li/BRQzBDFxCUUP4MqnkOFPpxZKPKdAB4HsE3K62myi/ZNbCUM9KAQxBDbQlBAkkExJ+oiHDCLgzksucoExSYOUU8cwviTaMQfE3y1LUpkQ8gyKFoozeGCBLG4AMVngmJ2e6tRvANVzBFFLNCnqIoKxbTve/CcBn2b/NNcg2PNDUvzmqI/Zh0kZ6yrsFZCJFCtuVJDInGOF+qbOesmDlFnHML45EizGEXlzRQDYaR0cKKbQoMj6eCS1fB4QcfjY0Rxp1B8KKN4cJeFjGICKJ6Shz6EQISvRLCDNwKwT+GgIacafI4Yqk/wrd6wbzBMxBkjg6x6AzkD7ojA+TzLsrksRLGJQ9QTh5gSihEnXvV3ZM8MJWdD1RkxlHpcxFAWAKgWHeEECvTWoHhCKI4VioMPD/mvZFvuSRVvHnEXGm4AZcNs3Xdi5oau61d5ZasxZHuCFTkNLQqBONa9ATWHBj5kkWHMxqyKTRyihqdDEIqR7KEIhBX7yxPLqCxti7K0CNRnvFarFRwMij6i+DIjFId34/mHh3uNIqniDUxzEtevTr1aE8OSHmotTGI6xtqTaGs8mFvciRCiFsKHSKRLQHKWr5s4RF1xCLItnG6o7BBlEyUyUxsZ2SyXBS1kAOlsBet4dQE/FwpFvCVfUNzL/gYozhSKmULxZ4VivFIobk5vNmyhU9d/kvMqpVuZPxNjkKoM5ljZk0TGM2CJB4OC/GUofroUZ9ULUWziEPU8HYJVUd8qWtZDiTfwdsrS9so4rBEIGUWUQfy9UOv4gtYx9YqJoNjWKM4AxV8Px7Pk+Mv9ZnO62ZAqztPAvgmKAzauzhZqIYwRRd46iUkUU/HF2hVLLziYa9ljFOUwFvzG4zEe4FdUsYlD1BCHML1iZN0ZZQcPzW7KxOoOFzQwNIK4OmYpvFhBRSYUZa3eoINmFMdlFH8+VA4aUFSaCCw+Xs5ulW/RLOqxoUFRR2wsFHlqrVEUb6KlkF2JoDhG/MaIojrnS14Z/OESUWziELXEIQRFM8ou+hUd9iJRXJj+cGn3h8fA3zGCeIEfJPGVZvH59gBR3OSE4vgdoHi5QxRzheJluBJV3JCFjl26C8BUZj2wUT996Q4RxVi2kfXWiRZFqcqZrsTjcVZE8Q/2zu43bSwN49LQRtkO0YokQNaUpkVRN2ECpGDswsyEOJHjeuXpKqW0omJXyaZqNPf5/7Xn/TjnvMdQzVV95RcwTq5/et6v52ABIEbPhLfzrrRDFGWHeMlti2lczPhQtCkHYo54YeaG2CGPsThkObw0JBKAhxDwBShirTi8yuYdhWIPUezd3ScaRVTFBakiGblrZGvYtFNm7yvvlGv7dm0yMmMbMaTh2lDnZUSQsrDOxJ0eELhGo1d7V9ohirJDvOS2Za1dJhQP7F7PTLH13IbnNdyZWACRPeSw3YY3fLqrm5uWUkUXxWSFKN7feolHKA4XBsUzQnGjz8v6rTkrj+wWeSSm1o0NXQmh1unlhFCKoYoEP6iKpR2iGDuEQNFenZWKptA0K3pmw+OaS52OWQUh2njRUa+3CUWlijsKxeTzklD0FIodrBU9r3n9AVQRgltoxRwcisor4b4YH+IaD9Z5I2d3grNrzaAGkcq/nsueBbAjGKSrl5AqlnaIYn4dQqH4Ln9gz45vGMkLO0hUgghSSPUhyiE3JpeHAkUCsa4YVO+2endVgm7dEYpJ5/PPGsUrT6F4BarYuP6wJFVcUAvdPK7l3dfo/jcLPXQanuHg+swu8BwU3caY5VBT2MtHAm+4UHhe4tdKO0RhdggXRcGhI4o6OZMo8</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAgGBgcGBQgHBwcJCQgKDBQNDAsLDBkSEw8UHRofHh0aHBwgJC4nICIsIxwcKDcpLDAxNDQ0Hyc5PTgyPC4zNDIBCQkJDAsMGA0NGDIhHCEyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMv/CABEIAVoBBAMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAACAAEDBAUGBwj/2gAIAQEAAAAA9/Sg529YTu7u6dJkzJMw53QmkmHm+YnTu6d0yTMmTCzCz1e82kmo4udqZUWs2UOzLBM0Q15atcRAXrNHp+jKGvhYu3mVgtRNd0KGpf5OnS3/ACnznmxW52PtDY+P7woa2BlbWeF2ymQAc/NcZq9R5X57zmxlanXevzYuN7+8FTOqT04NF8iOWt5b6+3MwdVa5DlObEdjc7KPGyvoF4M6plQGySsaOfzu/HEZgACEYRBFj0PoNQ4fjBdNfNzs7dzEQgDBGEdRqTVoNGDJ+g0HKnFGIp1Gb0mCCA5I44gAGZVcX6KQcbeAAFk8Ep3Rz6GnSzaTziIiyp4X0Qg4bVAAFAegwBFiZfSBFFnY16dhZ6WH9DoOC2QAWC7LHHl0KVaXSnCEIuefXdKlh/QyDz/cAFHfUeRyeNZa7kWbl7apQQYg9CT0MP6FTee7ojHdeLluJqc2TbeLSfrdjqoc+tg6W8VDD+hUPnm+CVqHluCy+Puha3uYid+k6fq6mXW5ztL1DE+g3HzzfGvqQ5HmOPzMVrQ01xmjnz3el1O052tmxdtQxfoND530LR3IfPeOwsOexLbvc/NQafS6vo69Wpgd7Fj/AEEh866KtpR53luJhqpZvN1uRkUaV/X63VrVqeL0GjkfQKbznoqmpFzPnGYxaVLntf2Tg+Sfe52Tp+grw0M8Omy/oBN5x0lTSi4/zjNLv+a4ZaOlHvVtrZx6/QQRZ9LM7DM9/dvOOkq6EfIedzZ+jxuOejsHrZZW+0OSCGhRyOxoe/JvOejrX4+d8zixa3M6t3r6PRzb+V5d2WnrQQ51HH7Oh76l510UNwM7yijkDLi6+9z3a3LfqHD+T9J0kFfOoZvY5/vqXnXQ1r4B59w0XQcthzT09vpO20qWHldJVq5+Nd3s/wB8TeedACnHH85x7eBXkhLZ6za1ocTC63KpUMLqLVD3p28/3QjtsHM8Hz1a/NNo6G0VjDyO8n5elQw/QKdH3pLgNsAllGLA47lMcdbpLSmxr/c3eXpUsHV6rKo+9JuD2RaO0zBnYvMY8LW7F3o+jr4dSjl5vbWMml7w64TYBmGywiFWCtBJpW6tGlVrZmD1WqORS95TcPrCzM07CwgkMVaCGCrn8/0OwIZFP3dPxGoLJkJkLCABHFXhgw6W/oCAY1P3dNxemLJkzMiYACKKrlZ97UMQAMWn7q64vSFMkyZRCEUUFaK1OQgEYBjUvdUuN0GZMkmTIREREREI4wAMaj7olx98UySZMkzCLAIgEcYAGNR9xT8lcFJkkmTJMIgICEYRxjjUPcEuWssySSZJMzIQEAEI44wx8/29PyxJOkkkzJhYREAGMI4wyaftybmXTpJJJMzIWEQAAAI4OZm9rS5uGJkmdJMmZhEAjCMI444MXQ9pdc5BCyZ0kkzJhAAjCMY4wgx9L2RNg1K6STpJmSYACMIwAIxhyug9RThGkkkzskmSZJkzMyZ7zpM6SZ0kkkkkkkkkkkl//8QAFwEBAQEBAAAAAAAAAAAAAAAAAAECA//aAAgBAhAAAABaQCpDSCoLcxS668JLm0jUGsAAFCItgWFi5WwWa1JrObm2Bbz3G8wsC5tTOhYE1UkUApc50lAXVZ57iUC2pigCWiAAlAAAAAAAAAAJQKIEtAAhagUGQAAP/8QAFwEBAQEBAAAAAAAAAAAAAAAAAAECA//aAAgBAxAAAAAhQAIACWkJnl31GdUIGdgBKIoWCVCyiwQITVAgahm0EWagsAiomioEsC2LAlRJemVQBIuoAECgARQAiooAQCgCAKAQAoCWUABCgAAAA//EADYQAAEEAQIEBAQGAQMFAAAAAAEAAgMEBQYREhMUIRAVMTIgJDQ1ByIjJTNBMBYXRSY2QlBR/9oACAEBAAEIAPG3crUYDPaOu8a6Qsgh1NUmAJ88poZuovOqi85qoZisV5tWXmtZeaVl5nWXmdVeZVV5nVXmlVeaVF5tUXm9NecUl5xSXnVELzvHqXPUY2Eth1xg3zcqaORksbZI/hlljhYXy5LUl528eJloZS/Y599tCZjeFvQTLoZkKMy6KVdHKuklXSyLpXrpXLpnLpnFGo5dK5dKV0xRrrpyjXKNcrpijWK6cj0nqxXY+C3j7GX07OfLsNqaplgI3+L3iNjnkt4nmR+ZfkGjehWkzEs8TpeTICr02VF97acMubfMxsjXNZ+o69K8UJJIIp8tI2MmGTPmSJs4mjhYOZGfyLr6/NMSklbEBu2GzLKGPmbNXbG4izu8xyT5KrWk5csFiOxEJYrWZxlGbk2zqXBI6lwSOpMGjqTBo6kwaizWNtycmoyjkGRhqZUyAc0zXnlrXEaO1Ta8wjx1zws/TvR9pWRLjkq8arxyHG45t6C5Ba3ENiWWPI2g17YRFW3cYWyvUssljEXhJXfvFA0QVWXRIIK2LbFMHyRkCM7xYyQ5Y5RzYy61G1SPbEwMZgrf7O5WbbK9lojnpSZi498OOgfVoxwya41RV0v+IlqW1q3VFbUox7a8jeB5b46Wz0Gn789ixp7U1bPa8wTYWHYvanuWRf8ApuWNmcy7BI3wtfSyI/xrISFuXq8MU089Go8wRiGFrBJUn8xsWGSwWnNgVFskdfhk3+ANDonNNyaxIwMg5kdazADYm7bi/YjqxOEbcq25lHwKuLDbBbHiYLFbGRx2tdaodpj8Q7MjdXarfqUY9r7LmvsPc2tlqsbIgbszZ7Je3S2oTpu9asNwOq3Z7V+nqzq9ZsNqxMnu7FZJ36TljTxWa/jb+klRd+kp4opJGyPNKoWNYRsAAHssG27aubcEXGInOfG1zydgSrGUutlHIOVyXAQKuTuuLuq1JmLGNxU4qwXbleWazNh7k9rDNdNJPMyVlduXiuZCvG6DDaa6DiaqdNtcbrdZbD56PVU+YxGqtC6r1ayk2yfwT1Cj+CuoQv8AZfUIWm/w81Jpi/Nbjbgc/dzuMuXhs3faR/ZZR36LliO9ul43PopkX/ohPKsZ7EVXFs7dT4V3s/1Fi/6Oosb/AF/qKh/Q1BSPo7I0bZAkjr1J9tq2I4B8vOyGzWnqWRpWFtoSiFsVWtHXgkdud0Tue7ZGtRshGyEbIRtNCNtqNtiNtidaYUbDEZmlPfuO2Vf8u9Yf6zH+NvvSnAfMGw8RzF7VOqrknDR0FkZNnWqmk212gJuFDQhiQEMWAm44BQUg14VauGAEuy0NaIthAIHdFEIhEIooop1khzgnykQOkEFi6+Bkk77cu7C2pkLUrmR2Z8jk45eGOCWSVjjJlIOdj5iMR9bjh4y/xPUfAZownRMTq8R9TWhRrRLkR/1yWhcAC4V08fEXHlArkhS38bC/lv6mN43hdJP/AE6eUe6TI04vqILFK59M6BqdAE6AJ1cI1wjWajWaumaulYulYslCI8bZc2k0MkrOb4S/xPUT/nYAiiij47INJT7cTZzXhbRyU/eYYXHetiItrM4K7pXO92Tuup0zLHTyz7N3kO5z2+lujRvd7kuDjjG9CV+Wpd7FXJ1rrC6vxA+hRR+DK/arSp++r4y/xPUbv3OsEUUUfADdTTxVQwPZjrNr82QhjhqwCCsXIuRfsnOWXGTncYK9CnmKU0hjJRcnuReshi6eReJZp5Mhh93W692KxG18e+6Pht4ZftibSpd5qg8Zf4nph/daiKKKKDd06SWSc1adSnDR4nsc5Fyc/ZWc5SgcWCTOWJP4ps1Kx20pz8IP54c9VedmxXDKAW8biE/cernovTnkHcXsTJBI+3iMbmY7TSC1wcNwtkAsz9ntKh9RT8ZP4npn3amnIooN3TzLPP0dWGCGnXEEDnJzlk85XoExrJZqawxz7kWXsXCWYqGrNaY/rGUsA2KR0wwumn4o3pXY7S0tR9qE4THQ1orVKpNmIxw1aupIhN097lxWGcTJ45IXbPLt08rL402ni3Uw+ZE4LJGuDgCPDNfZrSx/e1SHi/8AjcmfdqaPqitu6nkezghgr1o6VcQxucnOWa1CQ59WjbynLm6aradRos52Uu6ju3pOBlHP36LXiGWy57YyZJgcVwqnYG80bZb9h8LqxhtXaLw1mO1YLkDauUrSz49ot4jGZenmaxAvUnVjxte5SFZmnJx+ZU8Jlo7cLCB3HhnPstpY3vdojxf7HJv3WmnIolrGF7sbE5zXX5XlOK1HmiwuoVbt57pRRp38pBh6boab5pZ5C+WvvyS5jWufJu4tMlloa/8AJiDvDY5N5rlaby53gRGSRmzo3PD+I4rIvge2SPnMtOZkMfhsxFlKpZJkqTqcvZ6ce6mBxGWa+PHW22a7XALO/ZbKxn3Ch4v9jk37rTR9StlPGLluKiXuJJJcVnMmMZQdI3J3nV4yGzytx9RwE8/UyOkeIwT3jPEQGRiIQknBUYrDCDn430IHQucS5/Zr43x8Uksp4/ywz7ncxSmFwc3GWgC2SOKw+pcF6CPIV8pjJWqQJ6yNVt6nLXdpnJO3ayVp3AKz32WysV9zx/i72FN+6U0fUof/AFYlvHFNdc8pxWob5u5aThgkdavTXDqGzG0RwMiDjwbEf+DYGFu20jy4cIxd+SlcjlWstRw6gnjfXp1DK0uMkLGjZkkJDk1pZ3DX7MO1Cy6Ixk0nOsiEx9PDj4nVKrwnhSDupwaWcLm42wLFRj1n/sthYj7tjR4u9pQ+500fUq+98dGQRNjjgiZDE4rLW+hxliwMtP0OLc4WzJXx8dOHIYuSe7XjbaxliKNrQIzAPz1Wvsn8rmV2jhEUDJncLNNfhvPmsbPeNnHR1RLXbKwRntOwu7ta48RaaNGSaZrm2KEEVUuiwfK8tYY5fz12PRG4UjVKFnGbVI7I01Y3a6E6g+yzrDd8zjB4u9pX/JU0fUqyS/KYyuHJy1hNw46GEZ9zZrlKq63x2bRlaLrK+TgsnL6oblGRVcbhfw/nmYLmczdmrUkNesJjLIsZAZpWxtw9wYvDQ1Ganohlt80cmw33pGN8wZJe0i2esJoTjr2MsB7TZa7mB2BsfpxQqIcTJWLZTDspgrkIsVJoDpiw4TVy7UB/ZZlhPvuKHifQr/kaiPuKjHFqOMpyctZO/VptWTk4tQR7zy8G0ccunrOSlIjpHTGn5ncnUmvhba+vjnulkcXyssRRFVMm8HZkNszNdu3KSNdwjGQR3YyX2oMdDNwyYbJ9O0Ma9uPyDe13T0II4alblWq7m1RvZa1bKUbhTBSDsVhncqywLPHfByrB99QYkeJ9Cv8AkKiPqVX++zJyctYM/VrPU8XHqEb4zHRPtSWZ7uVrZTJPjZcz7qNywYMnqKC2CAbznlMm4/WpIN+1ZzmA7NpF7t1WmmoREts5J0j3k09RV6j42EavdLYbFFLPO3HBz69eNuHjeaY+ciRClHZTKRY87WpFnD+wvWBG+osR4n0Q+uqo+4qJpGbBTk5aqh5lSN6yG0GYqSukifLHNVfLS8teWRZqJuRx7bEFWlNZfsxmHEbOKajBAyUb1JYYodwb3Fc7Ur4dGGltkxWGuaG6by8TIbub/CRtiHqsLLhLUOV8vtZO/Njoq1Cpjbcduqx8dMbSveipfRTKVYs8cznLOjbBPWnxvqTEfAPrqqd6lE8N+s4ORWWgE2PkB1BWcabyTZLeXabkLr2ySObhoH5Se3LLfxb8ZiYuVC9u54sdPWftxAU5Idk5sbMgWNxEGO4Gl9yWsfyRYWu90rSMdYhgx7eLLUW6j1V1UGTZdo5ixXs6djPSuldEOXRe5FTKY+qncGsc52n4y8VN9QDbCyBad76lxPwD62snepVslsHMB2/op7Q5pac9j+VaeDGwVJ58dYr4sZOSOtKzGVMVoi5SkNuWBjo3W6kL5N4qcAjG5tXpIWgNZZc93GaN1+wDceQ/bfE13RM45r+RYysWywvdJPFVjz+mm5vUWSyMcAdWtQ16drhDxEx3opj6qYrMP4cfK0aeg47zNtRfaJVpvvqfE/A0fOV073FEbghUnfLCMlFZyiLFcyNz2IdZh50OPycPKNS9Ys2ce4c6/wAmSUvrGtFLBIXOxE7GmWtYx1oAMsVsQDwF2OxDAdm0qgYHBtWzNK1vIjxNeaIll2rDWjO+QsMbWD52NsZS61rRjZI8c7jkOymPZSlZB3OyMMA03X4Y3THUX2iRaZ76pxPwRj5yBP8AcUU13JttciinAEEHK4vlSGSPP4FwL7tQTzthHJmliYQZa8UNqEOjqQOgsRzhleTiDTDA42HubUrSNfC0cl5kleGSRsmeDLqHy6EOdZzz55DMd7GRuADB4VmMg3fmrghhNNkpUpViRscb5H0Y32JXTOowCvUYwai+zyLS/fVWJ+CMfOQp3uKKkYJIyw15TLHs8oqSNsrC117GOicXMy+l22XPsUZIpq0j68tjEv5hkqMzGbou4ZqWuXQjmGrruKd8fNdriCLfgbqrmkcg6ifOx7LDJWRue5mPw97LSAsxOFrYuPhiuXG0GFrJ3Fzi4ylSnuVlZefK2mzBUeZMJXbbDZai+zyLSvfVmK+CMfNxp3uPi7eOQSsDg9oc0opzQ4EGzjWvJczIYivcj5V27ouRpLqUmFuVnFtnyuGZHCva4cEOEfsC4YwPcGmrpXITkbY7SdOoRJZjhLm/ls5BkDSyrK4kkmVSlZC0KsJcqNN80uxpVW1oGtBWovs8i0l31bivgYPmmJ/uKPi13IcSuxG4KKKdG142dJQjd3a6hMO7ZsbFKd7Hk2NJTMVjYz2q1mt7ROiEY/PJYrxEltm1LP73lSFSf2rliOtE6SQMluWebJisaIGB7iEVqL7PItId9XYv4GfVNT/cUfga4wnsHBzQ5p8SEey5sg9DPIR36qVvZr7EzvV5TynJ/opFdtxVI+KQsnv2eZJjcUIgHvDQ0bAhELUX2iRaN76vxfwMHzTU73Hw28fRbFpLmNlDjwu2RRRCKKcnJ6enKQ7DdXcq0Ex1YMdNam5stPFxwAE8AA2BCITgtR/Z5FovvrDGfA0bXAne4/Bt4kBw2ds9nt57fR4II3BRRTk5PU8scTS6SfLR921317uQP69XDMYAXR1mRDYEIhEIhELUg/aJFonvrDGfAPrE73H/AAnv6mBhO7SyZvtLrDU6acJ1ix/T5brva+C9L2c3DNc7ifHjY2JtdjB24dkWohEIohELUo/ZpFobvrHG/A0fNp3uPx7fCQiAi0IsCLQtkQiEQiE4IhEIhELUw/ZpFoUf9ZY34Gj5sp3uP+TZEIhEIhEIhEIhEIhOCIRCIWph+yyLQffWeN+Bo+acne4/5iEQiEQiEQiEQiE4IhEIhamH7JItBf8AemN+BrfmXp3uP+coohEIhEIhEIhOCIRC1MP2SVaAaTrTHfAxp5nE13Ulx24bC4bC4LC4LC4LC5c65c65c65c65c65c65c65dhGOwjHZRisoxWUYrSMVpGK0jDbRhtow3EYbiMF1GC7/Woo7Jws3M/D1vDrSh8DPRy5/D7upYupjXUxrqY11Ma6mNdTGupjXURrqI11Ma6iJdRGjYjRsxI2Y0bUSNuJG3CjbhRuQo3YUbsKdegTr8ClyULQds/dktxcB0ANta0PgaPylPR/zFFFORRRRCcE4JwUg7LIt3aQtBjbWtD4Gj8hKej/lKKKKKKKKKKciFIOyuNJK0VHwa2x/wSRui4mOkRK3W63W/hut1ut1uFuFuESEXBFwRcESEXBFwRcEXBFwRcESFIRsVZILlofF2bGoYMg3xfGyQbSClVHp0dVdFVXR1V0VVdFVXRVV0VRdFUXRVF0VRdDURoUz6+X0l5fSXl9JeXUV5dRXltFeWUF5Xj15TjivKMavJ8YvJcWvJMWjg8UfVmExUbuJrWtY0Nb/6P//EAEoQAAEDAQQDCwkGBAUDBQAAAAEAAgMRBBIhMUFRYQUQICJScYGRk7HREzJCU5KhssHSFCNUguHwMEBickOUorPxM3PCJERQY6P/2gAIAQEACT8A35mQxj0nmis1tm1ObGAD1kH3Jpjroe9o+akj7Vvins7VniiO0Z9SI7Rn1KnaM+pEdoz6kR2jPqTh2jPFPb2jfFSM9tvipWe23xUrPbb4qVntt8VKz22+KlZ7bfFSs9tvipme23xUzPbb4qdntt8VaIx+ceKeZTobGQSebFTSWV9affxlo6SKgdKe17HCrXNNQRsPCe1jRmXGgW5k8mj7RNGWt6AaE9NOlC0Sv1uFabAMgrLIBp4hxVnl9gqzy9mVZ5ezKgl9gqCX2CoJezKgk9g+Cgk7M+Chk7M+Chk7M+Chk7M+Chk9gqJ/sFRP9gqJ/sFRSewVG/2Con+wVE/2Co3+wVG72SmP9gqF5dkJQw1HPhijJLZq1dA9hMbubS07R70ySyWrTBOKE/2nJ3fs4GQFUAX69WwKWIPFPu5HBt4UcTiQccB71NZ22ZwJe6OUOIFNHEFceZWubqZ9Knsvkg28Y3vDXADP0ThliprIGG4SWzAuukgOoLmOFaK3OcwZ3iynuCljY+6C2R54o5zjhtVps2NHktlaQY6HjDia7vQSpbI1l5oe9koNdd0XM889itLTj5z3NHdRaz3lOf5QeiI3V7kC5xwa1uZTjHUXh5NoPWTn1BSvJe+4GyMBGnVTUm3JKVpWoI1g6VLddS9ShOHQnXmHI0pVbo2Szy0rclnaw010JW7W53+aZ4rdrc7/ADTPFbs7n/5pnit2dz/80zxW7O5/+aZ4rdKxzTuBuMZO1xOGoGq3VeTcIJMbSb5OeOgaluiXt9NrYwK8xzCJClMsEhuRudiWO0Cuo5b+redRj2uDh5O9XiP06NPPlpT4LRaWx0e+SyFwJvYkBuA605xpnVhb3hSXW/ZyaCC8a3hje6culMs5pGADLYy8gVOVMkyxVLrprYHkkbSM07ygAugfZjQDVdPnc2lR1I3PqCbMWgYDC7TA4+b0KLc8tFLwdYyATjrp+6qKyUArSOAN41cCsqnvKlZ5M+aDZ2h127Tz86ZHoVl8o12D5LwFwc2fUhRoGARytNoHVK9QucJJC9773mG7SuJ00pgnMc0Na19+zMkDaVIxcRjjXSpGyPbWrmxhgzPojLUtyY90PtG50UbQ8geTN52IqCty2WE2Zrmvc1wcZC6mJoBqPWqmmsU37D9rEsPkmgOa0sN5rqglrh6NMtKsBspjklLnF7SXViI9FraIkgOwqa6BvmjmzsIO28N/UtS4xAc4N8vcLiGv9H0vlmopIn3CXMbbWgto49BUkkgzvPdeJ6U15LrOWMPlqNLq4C7oO3m1BQ2iojYHiK0hgBGzSmyNIJp5SS+ac/ByN4e8qMGQimLgANFeZTzmQx3GRit112hJI1+KIIORGlNaxtS6jRQVJqT1qd7SHC7cycW1JB2UcE2Z0bo3ACLlHOo6K1RBmqSQDW6MABXTgOslbnNthtO5kcVC66WcdxqMDqW5osf2QPAN+8X3i3PAZU96AAOokjrKMrAwNDmhreMQI8ei67PZrKc5wuMaXOGJIaAT1hWT7SbRZX2agfcLLxabzTQ0Iu+9WN0Is87yJHzeUc6sZGJoNScXF7qY6NPz39NpjH+ob/IK1KJjnsrdcWgltcDQ9KssJYzBrTGKDmQoBkmvMZY7ESUodAy96s1pkc6g8nLOw3RrrrTCxxGLSQadSBNBkFYZLl0cWRlDWudQcstCsfHBbmw0pTjelryW58owFPJNrjprUqzziZxDGWgMBjjLnUqTXRXVnRCBxbLd44Pl3EE1N8cYHKhrnVSEzNdJCZaYuuPcy900qmuc0tqZHDCuPV+vOi4RyvuG43jNGIqa5DDUnF1XE4jLxQxO8dz3MnsTLK9lpke1zS15dUUaRpCm3IgFkDwyk0ri69SteJ/SrfuX2kn0K3bl9pJ9Ct25naSfQpNy7QZITCWGeVtBea6tQyubQvsUUFjmMrhHaZZHOq0igvDBVxNTU13tS02qP4xv+rd3LVvbp2ONwzDpm16qrdGB39pr3K1V5mO8FM480bvBOkP5CvK+yoDJqvsBVli2VYP3oCihjvUrdFPkohJE8vY9pyIqQrRllIYGGYfn1/1UrprXFRhkUbQ1rRoG+1NKaU0oFAoHqVepE9SKO9qX4mL4hv8Aq3dyPFAJNNQFVZbayxF33cEbHNZTReOk86iMY5KY6vMmO9lMd7Ka7qTT1IHqWA1nBUmkphd80c58EauJJJ1k4n+FZ5jQ0rQUO0YqN5IaSGaTsVjbG4t40bZalrtWQFNoVklu3qOrSowzAritz5onurxm0LRQnM1wwotzPKAOIJDzrwOWlQmIg0AJrXavOawkdS/ERfEN/klNFTXRsKaEwJnvKa72z4oydo7xTpO1d4p0naO8U5/tu8VfcTypHHvKLvaKLvaKt0flOQ2W87qBqrLunLtZZpgOsgBbk7qn8tO9y3L3Wb+Rzu4lfbbP/wB+KZg6yKK2tm2Rz3u4p8naO8U+TtHeKfJ2jvFPl7R3iny9o7xT5e0d4p8vaO8U+XtXeKfL2rvFPl7V3inyg+TOPlHHRzqt4Ssoa4jEb/JK0uPcf4LJLTaRnDA284c+hvO4hTQWFnJjHlpevBrT7SjltrtdrkL2+wKM9yjjgZyYmBg9ycTzlMD5HPZGwONBee4NFTqq5Nbdf5e48YGsUtxwIx1toa444DJPcOYqw2ac8qSIF3tZjrVutdkOhjn+Xj9l9SOghWNtriH+NYSS4c8Zx6i5TNkDTRwGBadRBxB5/wCB6s9y9bH8Q3+SVy/keHedI80jiY28951ADNSOs8RyssD+Of75BlzN6yoo4IRkyNt0c+07eDZ7LLY3spIJQS4mujjDZ4hWOyNc8uBkfNJKaVJABc6uJNTljU8GNzLS0UbaYXXJW/mGY2GoQ+12Mf8AuoWUcwf/AGMHxNw1gJ7XscKtc01BGw8L1ZXro/iG/wAkr1nyPCa184AL3u8yEHS75DM82Ic6W0PFJLQ/znbByW7B7zwJPKvHoxC9TnOQUDIxrkdU9Q8VbWRnUA0d6t4HO4BboRnZfCla4a1RDfNCrscpN6Syk3Y5TrbyHbcjp1q8x7HXHxvF1zHanDQUeB6sr10fxDf5JXrR3HgkNkpellIqIW69pOgfIJpawGpJNXPcc3OOknf+9nphG05c50K0COEf4bTRvi794KxmVrc5n8SNvTl71uvG51MY7KCQ3nOAPvVskPkW3ncWppWmFBTM61aba1mhvkLpPW5SW0MZIGOvsaSK6aVOGC3Ylga/BhwaT3e4rdCy7oU/wnG7Ieg0J6CVFJY5waFsow/fOiGk5EYgptNR0Hfc2LdCMUDjg2VvIfs1HMcya6ORjiySN/nMcMweByCvXx/EN/UV60d3AaH2mY3Y2nLa47AMT4kJxca3pJHedI45uPhoFBo33gOGEkw9HY3bt0KN1otbz5oxx1kq0C227MWdp+6i5zp5hgnlkbfNaBRrRsGSnIc8ULnaOYZKR99zq3a4HbRRNvcupqh98RxXd4Uznwl1fJSYgHZq6E94aD5jjUdGpMbaosgJPOb/AGuzCtJtVjr95Z5PPZ0aRtCzHnRuzbt/VG9Ecnath32k2mNtJY25zxjR/cNHVqTw5rgC1w0jf5C/ERfEN/UV64b5DWtFSScAE0iW0N+7aRjHFmBsJ849A0b7yH0++kB80ckbT7kPvTg5wwuD96dCxmeKSTaXbBqHenHHWmANGkjFxWZKGDAs1kTQ9K0mqdRw80/JDGuKe5rm45qkFsbi9jBRr9ZA16wmi+BdljPeES6J+LHfLfwstqcXNAyZLm5vM7Fw2go473IX4iL4hv6l65u+KxkeVn/sB838xoNovLM71DM83ImnS7XzDNOLp5CcTiSTmU6szxWV2r+n95o11BdOxeaMgmi8BWqoZHmqFN4cYCiwC6UeKVhXBwGtHjB33jcgQfkVS6GF4Olrh+6b7rpcKsfyHDFrug0QuPqWvZyXg0cOve5K/ExfEN/UvXt79/O0ycT/ALbahvQeM78++axQVjZz+kevDoTaxxG5Hz6/n0hOJcal52/uiHnYhGus6944aUTdaQSNis4gZG0NoNO1YAZlZ7+LNI1I4OwPyTL1ateNBH7IQIZWr5DnKdZ2ahwMGWlvlB/e2gd1i6ego6FyfmvxUPxjf1L17O/eNJn0jjOp7jdb7yELsUbQxg1NAoPcN7zmMN3+44D30R+8dxQ46zpVQ4MvuprpV3VxQqkvf5Pbg2p9yhc1xFC6mjYiMEwiPS6iacNa06URdbUMFfOIWBY6jlimGqbdO1UI0jYsDERUHn/VCh9PaVm3iO+Xh0cDOzytf+XzXe4k9COWS1DvX4uH4xv6l69nfveaZXSvGxjCR/qub5/6korzAE99EaNJqe5Ggx78URdZIXG9lUinyUXlZX5iNpzT/JspVsAOJ59SDWtZgA0YBFZE4qUMDsSK0WTjWoQqUAATmUA6orxcwmlzB1on70g0Iyx0oUvxlw6HfqVpZUc4x7q8DKRhYekUWb2C9z0xWod6/GQ/GOB69neN7Jljk63Pj8Dv5APJ/wBKxusaBszPyQc95FSBorj81JckNlbI2MjzjgC3noSU2CC1NYC4OxcMNSDqHAynM8yddJ5RxRvFSFg/pwV9xArUuJUjmjVWoTbLJUZONwlNks7hp85vWFMy0Q6LjqkdCLQ/UcFZ2TNkqDiRdw86o1GidxI6taKZgg4e9elVvWKcH0Jnt/1FaQO9fjYPjHA9ezvG9+GbT2jv5XXD3hcgHvCka2KK7UnAVB/4RfFHTyYc04imRA+WwKzbmWmRrQ2SeYElwFaNqTiQ27XaVuZYYXk1rBHdI96aDzmqjjG2iha7oUVKimFUwDnaVZWSCmd39FCxpA80il7ZpW5FlEhNL5BBG1WN7ZHGgLJGCvSWo3bPdrH5MirsCHVphnkRsQHlDRx2EkYLQ6vVwdFod3r+nvX42H4xwPXs+Ib2TrM6vQ5n1b4828O4/IrJ3EP76VeMMj2teIzjUE0pz19ydG+Uk+UkzDdFG6+fq1oNjnYOO1uFXZHroPcmOkdSpAyHOVKwHRHHiek5Kzt/MK96jYMNDQiKVRBTqNrjqW5jJZDnLELhHipzNHSojkwc1QlrmuIo4Gox0JrXGzxgycUHDQOodVE/yZJ49nxNP6gTo2LJkbiekUHvI4PpWl9PbI+S/p71+Mh+IcD1zPiG96RdGTsLSe9rd/0eN0ZH3EoUks773QMCjRsgaHHkuGR91ObnQaHOJrQYdAUdyxxMDZn5Yk0FDr8NiDDFeLJXsGJdUlpPO0jqOihTstCNEaH+k0T3Xa6SnFzv6nIN6FgE4ig05lMYPIxiOM6A4nziRmcqc1dVQ+OVryHAih2e5GprdGzT4LOV10cwxPvu9XANABUocZ1HkbTitbe8L8ZF8Q4Hrmd+8CTG4SUGm6QadNKIgjWN4VBwITatdxXV0/8AIogTH6J0kHIj95hOEE4ddZI8ENkbq5x+8k5/2w2xshu0LS0Agd5HOBrR8pCRdLXYimo7PeE97CRW4Tl4/vJSVQcBrRTqHnRLinCENF65m8j+3R00Ck8hHT0jxqbdXfzZoOghDxWlSSdZ1lWuP7PeoJXCgNBSg15U96aBZxgXPFDM44V2bNQRqyIXAdes9JrwDxpaRj8xp80MGBa294X4uPvHA9czv384j5PoGXupvjjNGPyP71pn/qYa0byhpb4Jl+yyYh4HGjdrHzH6gltohIoyal5rxqd0KMNaDeuPNQ3XQ5og3XX3GU0AbjWlMiDQKe9GBUCTGtaVoRjp0hWalRUOaQ6u1R0BOINcBXmxKhvP0YFwphUkVG1NLb4owA3QNZqKH3ptxl664tHGGjTpT3Pc84tfjTXTBPcxp845XhqGmnV1KkdmaKRWbIyH+qmjZ+iF6WQ4CmDRr5gi574QKvdm4ZY8DzYh5V3OcB/5IZ5LW3vC/FR9/A9a34t/zZQGHn9HvI6RvioOYQq0phdXGaJuf9zdutTAVyqKtdsI/ZGjUYnw7acWumhH71ryE5AoCa3qaRVvzaV5QSxYNNA8AEkkUaa9YU5fHevuLw4OOeGIGCFnkaXNLC66KNGymqimhYA68+r8xU4UB1UVob98QMI3VDKZZAJ0kt1oADW1I1n9lGOzAigdM6rncw09XSg52p8uZ5h8z+ia6WV5o1o/eSo+0yee4dw2IgyOxlI0am75Aa0EknQECJJ33qHQNA6qIaFym94X4lnA9a3v38iF/wBRuDtu3p/eW+KgoVGzSrsc5xfEcGSeBUbmP9KGQZjuIUpjfndrdPQjI+FvoyRiRo6TVOsrZm0uhrHM+EhT2E3hV5de4p6XYqWxkZcSZ7B7nqCwvZyrhl9wBVpMd3BvkGY9GIw5wowZHHF7hU++v70JhEeRlfg0ePME0vmdg6QjE7BqGxEOtRHRH+qJJOJJ3/NwdKdmgdPcNqHFblvcpveF+IbwPWt71r3xWmDgNIRqDiDvioWDlZ2vb6JOY5joVoEjfVzYEczh4KzzRNHpXL7esVCdZZecivvVgszxroxWazxHZcFFaGOOhrXFx6lF5NnKfxR1Zo/aJB6JFGDo0/vBBrI2ilcmtCNXZGU59GpHfF6Rxoxuso3pHm892sob3Kb3hevHA9YO9a+BjGcxyTr/AH/ziNfAAIKJYesIB42FWNjzrfGD3hWGDoYArFZwdsYKhut1MZTuVyPa92PUgZnbeK3qzKdgMmjADo4BoBkNJOoIcc4NboYNSHG3+U3vC9eO48D1g71r4NTHpGrmRqDp4Tj0otPO0JwHM0KV9NVeEak+a0ZuOxCp9Foyb+u1DHgcpveF675HgesHetfCNCcxoKF12o6eb+KBK/leiPFEve7NxQxQ4HKb3het/wDE8D1nz/gCoTrw5LvFAsO3LrRqOG9rG63GijdM7Xk3rTyGerbgOnWghwuU3vC9YfhPA9Z81r/ghVadbTRS12OFUxjukhQD2/0Vnb7f6KOJvPUqdwGpgA/VVe7W41KaEEOHym94XLd8J4HrPmtf8UIIIIfwuU3vXLd8DuB6z5rX/N8pveuU/wCB3A9Ye9a/5vlN7wtcn+27gesPf/OcpveFo8of/wA3cB1ONiCKhCIDaT4J0XUU+L2T4qSL2D4qWLsz4qWLsz9Smj7I/Upo+yP1KaPsj9Smj7I/Upo+yP1KaPsj9Smj7I/Upo+yP1KaLsj9Sni7E/Up4uxP1K0RdifqVoi7E/UrRF2J+pWiHsT9StEPYH6laIewP1K0QdifqVog7E/Up7P2R+pT2fs3eKls4bVuLWurmNFU4uNJKkin+G7RwNZQrtQd1KvUq9Sr1KvUiepE9SJ6kT1InqRPUiepE9SJ6kT1InqRPUiepE9SJ6kT1InqRPUi7qRd1JriVxWA1DQtUn+27gaz/O6pP9t3A1n+d1Sf7buAKEH+RPAO+eCwizWYPvPIwJLS2g2414DGuGpwqrNF7AVmi9gKzQ+wFZofYCs0XsBWaH2ArND7AVlh7MKzQ+wFZYezCssPZhWWHswrJB2YVjg7MKxwdmFY4OzCsdn7JvgrHZ+yb4KxWfsm+CsVn7JvgrDZuyb4KwWbsm+CsFm7Jq3Ps3ZNW59m7ILc+z9mFufZ+zC3Nsgdr8i2vcmgNGQA/wDhP//EACQRAAMAAQMDBAMAAAAAAAAAAAABEQIQIDEDEjAEIUBBUFFg/9oACAECAQE/ACERCEIQhCEIQnwFlBuj3Y4vLgfTySOl6Z9RWmSjgiLTLFZciUU0Q9ZsbZj1MseGc718J+XnY96xo2lwWndBTIamxD3JDZRD0WX7GtHo91LRImvd7l2Pc1RYpFKNlTHj4/opGdo8RMQ/FKJCKNn2IfjukGhrzXRk/qYT8N//xAAjEQEAAgIBAwQDAAAAAAAAAAABABECEDADITEEEiBAQVBw/9oACAEDAQE/APvJcCvm5BDMnV9QdNqpi2XoAb04D5gV24qJlhjl5P2S1AXzKntncg3xsDTDSQeS5e6gcV1FXVQJTB5K1cGJGHEadBPxGHMMuP0L/iH/2Q==</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSgBBwcHCggKEwoKEygaFhooKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKP/CABEIArwCvAMBIgACEQEDEQH/xAAdAAEAAgMBAQEBAAAAAAAAAAAAAQIDBAUGCAcJ/9oACAEBAAAAAPqkAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAMNZmUyEgACQAJABCIimS4AAAFOdztSZryded7saGiy9mnMxz09nlYK7XVkhCBBEkERWtKY8WLDgwYOj+j3AAAI5/J51EiUylMgIAQIQhCFUVita1rSlMeO+Hz37X1QAANTjcfBWIiCAJEgJAImAgIiIVikVpXHucnh4/3TqgADDxeHz4jR5eGNzsaPOxx1t/k6VMnfcjBXY71hAgEECIRERCJiIq3POcur926gAFfGed4WvjrWJTa1rze9rXm1pmUzKayJJlYmU1IKxMwlfNHlNWsW/eOmADz3heUmVIWrWYhExCYCYm1pTN05LWta1pve800+kSklK+/wADxdERk/eOmADwutEppERFYitK1ikViKxFSZm02nJa1r5LZb3y3yWnzPb7M3lNZmFcfjvGasoZf3jpgA8RqoIiIitYpSK0ikVisRUWtNpnJNr2y2y3y5L5LZPMdXtsnP3M0SUrg8b5DVtKcv7z0gAeHwQgisVitaRjrWsVisREREzNrTabzfJe982TLbJe3m+j3Vvyfq/l+5iw/ov6dhxeP8bq2tM5f3zoAA8RgiZhWsUrRSuOKRWiikIiLrTa15te+S98uXJkyXt5rod40tjYrM1imPyXh9W9rTm/fOgADxWtMEK1rWla0pSK1rWtYqiJTMze9rWyXyTmzZclr2830O5M2RKFYr5Lw2ne1rZv33oAA8XrxaY4HyfzyRIEkkyla0zMyss3/qLsWtkv5npd38d/IcG3qbeG98H7p+oeS8Hp2te+X9+6AAPGYIlXxHxtqgAAAAAPsf8AQZve3nOh3/nb5u2exdsanFxfVP7l5DwWnN73y/v/AEAAeMwFqeG+N9UAAAAAB9jfoNpvbz2/3/nb5s7fa5W5tcnma31T+6+O8FpTe98v0B0AAeMwk08N8b6q3vKZcWT0Ohqek4vS4VqNrHtb/Tmu9t33sOTC3fzr8gPsX9BWvbz2/wCg+d/nXDnw72ltaVfq/wDdPHeB0Zve+X6B6AAPJasxEeH+NNVl/Wedlw5PYcvneu8x3PK5sefLba6ffxbW11c2fNr0zPAfNh9hfoa+SODvd3S0r3muTBV1dzyHgtG1r5Mv0D0AAeV0is+G+NNVl/YuHlwX9pyuX7Pz/S8re19idrqdyMm/u5d6mTFbP+efNx9gfoc3tPD2e/bBtYMWS9dmE+Q8JoWve+X6C6AAPKayk18P8Z6rN+x+ey69/b8nl+0890vLZGbLfZ6vpK5Ojub21GvNn5781n19+h2tkniZ++8p6vQ8b2t/Y6kRfyPhdGb3vl+hd4AHlNeIR4f4x1WX9j4GXX63e5nO9l5rr+VtbNmna3/SMvYt0cmCa3eE+bT69/Q5tkvws/e0Olrcv3GPmeE9RHTnyHh9Ccl7ZPoncAB5PXmqvifjDVZf1nn5q9Ps8vl+14e55pknPkzdTtbl+xlzdXnXY9j8/wDmg+uf0S1r34eb0PI6/mvS7/N894z9H2tt5DxGhOS9sn0VuAA8rqSq8R8Y6jL+q4703O9zON6/h15M7S+/Xc9btYfRbGr1bc3Nm1/EfMx9b/otrXni5+7bh9zDr8jw3qfczW3kPE6M5LWv9GbgAPK6s1mPE/F+oy/rlZrX0OjyfceXxcp0o3L16PoOnh9Rk53bw6GzfQ8V81n1r+jTktbiZe/a1cfN4uf1kpjyHitJkvN/o3cAB5TXTWPFfF2oz/u0Q4Xb52l6Dk5+Dm6WXJtYep0ez08W9hrl1KbmbxnzIfWf6La17cbJ35otbz/oraufI8f4vSnJdf6P2wAeTwTEPFfFuoz/AEvXLi8Hipue38N7LwO1nz7HX6u50dmm5m4/TtrV2MHjfmc+sf0W2S08W/fx6Oj3b8ju63F3O1fxnjdGcl1vpHbAB5PFNEeK+LtNn+lcexqeM0J6fuvz73Hh9nZvt+i6u92djmZ9Hl9jWrFreO+aD6w/Q73vbjT39D2GPxm36PyHX7up5f0XjvGaM5bLfSW2ADyeKIh4v4t02b6Zri0/KX19r3X5z+heWz4uj2PVYs+/g5t9nn9HHipmw+W+Zz6r/RrXyW47va/Ex7vV8/3cHIp6Lp+O8foTltF/pPbAB5XXmsPF/FumzfSWONHzubTy+4/Pv0PmYdl1O/hK6nS1eF6/DWMtPLfNJ9U/o05L35DvT5v02pzu/wCf3t3z/odjx/kNCctot9K7YAPM6c1h4v4t02X6Lpi5PEmN31XivXdTW1qdXuM1dGm3g877rHFrR5b5kPqj9Gm97cmO/p9vlU39bZw4upo7Xj/IaM5Zi30zsAA8zpXpE+L+LNNf9Zru6mtbH6LPl83s22OTbPtZovm1tjay5dO+/i4X4efUv6PabTzI73PjR3uL2dvzHosOr6fx/kdOck1v9NbAAPMaqsPG/FmkyfsV6a0Z9zX3/Qc/RzV0cloWrqbl8+eMd82Xj/hJ9R/pNlrcyndty+xh0+pyehn4HoJ8l5DTnIi/03sAA8vqWrV474s0mT9qnWxzr7PpuVwdq917Xz5M+PndPJfNMXzYuR+DH1H+j3Wtyqd2eF6HDr9Lmbd/O+k2PIeR1JyRFvp7OADzGlasT4/4q0mT9upztS3Ww22tXNWJZ8FdzJgwb+3PRm2XNXi/Ox9QfpF0252Dv6vsPEdXNxPXeXzel8n1vKeS07Xit/p/OADy+nMQ8h8V6LJ+4aWO2/r2nb5nY5M42KMm5tal8u/k6VpupyvnU+nP0qbTPPw93V4faxcP2Pno7fmu91/I+T1ZyUW+oM4APK6yDx/xXosn7Fr7+TR73Cw+o830ePki+ON/b3uZv4t+dvLM7Otxvns+m/0e82tzsHem83ulZNfJeU1ZyUT9Q5wAeV1ZiK+T+KtE9BltgXq6HP2tTNhz4rXtt625GPPh2oxbury/Mn0v+k2taefrd61pyTZeYtXyXldW16PX/vUgA8zoTVXyvxTogAAAAAPpT9Iva08/B27WvabTaZPJ+U17Xr0voneAA8voyV8t8Vc4AAAAAB9I/pNrXtz9ftTa95m02sr5Ty2Cck/v3qAAHltJMVxflfgsWOla1xxWsVrFYisQhBBUE2/b+3e1raGr29KsXyWstbY2PK+Ywzk/Vv1EAA8ppzE1x0rjpjpSmOlKY6UrXHWta1hEQCZtNsuSbWtfR1ezg9taKxSLR43s+U8zin1/73IAB5PRtEVpjrSlcdcdMcY8dK0rSlIrFURATKbWvkte1raWr2NH1c0ipWPNd/y3m8W99GdIAAeT0IIpipGOuOlaUpSmOlYpirFYiIiEJmU2ta972tbT0ezy+1SsQirm+n8v5zF+6e4AADyOlWEY8da46UpGOlKVx1pWmKIrEVVQJTabWte95vq8/s8PDWqEQ3fWeY877z9sAAB5TlwiMdaVrStK48dKUx1rSmOKxFYiIhMJm0za9rXtfX53amU2uTM5PMan0RtgAA1+TNaq1xxWPyv81pg+ieuwxGPGrUpREQmtZTEzMRM2V176XG8nEet9KTFo/VbAAAAAfi/x1rav9OswAAAAAA+AfO6P17+4gAAAAAHE/EtD3X66AAAAAAH4T4Dc+hfSAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH/8QAGAEBAQEBAQAAAAAAAAAAAAAAAAECAwT/2gAIAQIQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA0AAAACQAXVCUSoqVKASZAttJSFAASwCZBqgqABYCgQmQbBSACoqLBYJkG6QqAWCwKECZBuyYCwFhTdRzku9CZBtcZmVlQkiTrvpUcsta6QmQbrGcc5ohM5xnOfb6OiwWAmQbXGefNuIsxnOM59vo6LCoCZBsznni2WEzic859vo6LFIsJkGzOcc7ZZUxmYzn1+jpYVCwmQbM5xzLVZ5yc859no6CywsJkGzOcczS2ZznOc59Xo6WAFiZBsznnzl1aSZmM59PfosAVJkGzOefOXVqyZmc59HboLAVJkGzOccpbqrGWc579egqWCs5BsznOSqqRJN76AqCs5BszkAADoBSLMAbWRYAANIAGAG6ioogApLKgzAGxSFQAFSoLnIAoAAABUEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAD/8QAGAEBAQEBAQAAAAAAAAAAAAAAAAECAwT/2gAIAQMQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAgAAABC0ATIAAAAlLoCSAlSygAAC6BmAAAALAsLoGAAAAUURC6BgAAAFAELoGDfQASoDiq+jtefn5yW6Bg31EoFLc54Fvq764+bllboGY31W4qi3Vt5c+AtSplboGU31W4qpWrbrlz4CgZNaBlOnRZKsLpda444BYqQ1oGTXUSrlaurrljgAqQ1oGTXWVZEW3Wrrlz4wWUkW6Bk11lXKS23V1eWeEAENaBk30WsIWrq3GeEAENaBk30WsxC223OeEACTegZNdZqyRBbbczhAAjWgZTfUEIUo4QAI1oGU31AAA4QARdgZRQsUAMygEdAGABFABKlBN0BgASgACUF0AIFuQAAAFAACwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAP/EAEUQAAEDAgIECwYDBgYCAwEAAAEAAgMEEQUSBhATIRQVFiAiMTIzNVFUIzA0QVJTNkJhByQlQGJxJkNQVWNkRIFFkaBy/9oACAEBAAEMAf8A9erpWN7TgttH9YW1j+oLas+oLaM+oLaM+oLO36gs7fqCzt+oLM3zCzN8wszfMLMPMLMPMLMPMLMPMLMPMK48wrjzCzDzCzDzCuPMK48wrjzCuPMK48wrjzCuPMK481ceauPNXHmrjzVx5q4V1dXV1dX97dXHmsw8wszfqCzs+pqM0Y65GJrmuF2kEfzLnNb2iApKxg7Aun1L3/OwzK6zJ5JHRdlUtG6Q9KpkXFjfvyrixv35VDRRR9pz3kENbZu5SxOl653gcAB/8iVcXj1EqZQtB6U0rhEGRizQpMz+qUtRo79dTKuAf9mZcA/7MqhiZF83uL3EjomykpnPNzUyLgJ9VKuAu9VKoaUM7c0j0HABZlmWZZlmWZZlmWZZlmWZZ1mWdZ1nW0W0W1W1W2W3W3XCD5rhB81wgo1BRqHeaM7vNGZ3mjKfNOkK3vO5U1QKN4dmTHB7Gub1fypNutSVkTOo5jJXPd2eiHPJ3k3V1dXWZZlmWZZlnWdZ1nWdZ1nWdZ1tFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFtFnWdZ1nWdZ1nWdZ1mWZZlmWZZldEolFyZGXb3bhPUNjGVikkLjclYV4bTfyktRFH2nb5cRP+W2yknfJ23ErMsyzrOs6zrOs6zrOs6zrOs6zrOs6zrOs6zrOs6zrMsyzLMsyzLMsyzLMrrMrq6urq6usyzK6usyzLMsyzK6urq6zK6urq6vc2HW2MMGaRVVXfosRN9WFeG038jJKyMXe4BS4kwd23MpqyWXrdYZlfVI+b/LjTm1p6lsa76itjXeZUNLUGxlnc1BmRnzeZduewyydFWnqWxrfNy2Nb/UoKWQb5Z3FPGXstLlKKonossjDW/wBS2Nb/AFqOnrHO6T3MUEBYOnI55kzfkjT21RO4OWyrPNy2dZ/WoKepcfaSvaGNyttcnn31XV1dXV1dXV1dXV1dXV1dZlmWZZlmWZZlmV1dX1taXncjkp2XPXU1TpDu6idQ61hfh1N757gxpc42bU6RU0TiGRTSKfSZzuzDIwPxkE3MUhJxhv2XrjkfZcuOx9h647H2Hrjz/geuPP8AgeuPP+B648/4Xrjv/hcuOx9l6GND7T1xw37T1xu37T1xs37T1xq37blxo37blxm37blxk37blxiPocuMG/Q5cPb9Dlw4fQ5cNH0FcMH0FcM/oK4X/Q5cK/ocuE/0FcJ/oK4T/QVwr+grhP8AQVwn+lcI/RcIHkuEBcIC24W3C24W2H6Laj9Ftf7Laf2Wf+yz/wBlmP6K5/RF9iAcoOb/APlX/sr/ANl/9L/61X5u9dXyTAXmzGklsDi7p3aqioZA2zeuaZ0jrkq+tvWsM8Op/e4rXPpssVO1r6ipjr6nvsQdbiyb1r1xZN6xy4sl9YVxVL6wriqX1ZXFcvq1xZL6pcWS+qC4tl9UFxdN6oLi6f1LVwCf1LVwGf1DVwKo9QxcDqPUMXBKn1DFwWo9QxcGqfUMXB6n1DFsan77Fsan77Fsan78a2VT9+NbOp+9GslT96NbOp+9GtnVfejWSq+9GstV95iy1X3o1lqvvxrLV/fjWSr+/GslX9+NbOr9RGtnV+ojWyq/vxrZ1f341sav78a2NV6iJbCr9REthV/fiWwq/vxLg9X9+JcHq/UQrg1Z9+FcFrPUQrglX6mFcEqvVQrglX6qFT56OllnqpGvbh1FVVNHFO+eNj+LKj1bFxZUeqYuK6j1TFxXUeqYuK6j1Ua4qqPUxriqo9TGuK6j1Ma4rqPURLiyo9REuLan78K4tqfvwJmHzB15ZYnNMMMOVwWI1uaM5CnPLjc81vWsM8Pp/e1wvic5RVlbnn3x96NQ1DmDqQ1Dr1gLSXdglUVgxLsJpCTc6xrvzbolY3K5jHAHdf2T+c1YZ4fT+9rvEZvf/PUdR5p94ENQ5gQQQ1DV8kOpaS+BVawPwej1hS1cMUpjJc58M0c0YfC4OavnqGonU5Y52d6/y385qwzw+n97XeIz8wDVbWfcFHm/P3w5o1BBBDm6S+BVawPwei1g71QtquN6jJwna6HB+ykvnDNJmvGkuIOY1xlqGvOJz3jquUFOJosUr48Na6pq5xh/JqqbhcVa2t0YbWN0hxrjFzHSlFHesd7IX5H85qw/4Gn97W+Iz8wazqPOKK+XO+fub6roFX9wCghzQtJfA6tYJ4NRcyWlhkkzvZ04Y2QsDImBjLr/AN6rq+srHu7C/I7UOY1Yf8BT+9rfEZtXy5x1HUdfzR1FH3BV/c3Q1DWNTU1A79Q1XWkfgdWsD8Ho0VdDmhXRW5X1Y/3TUew7nNWH/AU/va3xCZHm43W8X4fLOBd1fpNislQSKyVg5RYv6+dcosX9fMuUeL+vmXKPF/XzLlHi/r5lyjxf10y5SYv66VcpMX9dKuUmL+ulXKTF/XSrlJi/rZFykxf1si5SYv62RcpMW9bIuUmLetkXKTFvWPXKTFvWPXKTFvWPXKXFvWPXKXFvVuXKXFvVuXKbFvVuXKbFvVFcp8W9UVymxb1RXKjFvVFcqcW9QuVOK+oXKrFvUBcqsW++Fyrxb74XKzFvvhcrMW++Fytxb74XK7F/vhcrsX++Fyvxf74VHppicMzXTObKzC6tlfRQ1MXY1X1fJaReCVYWB+DUSC/aLjlbgvADQSZENNscLM23YuXmNfeanaa440E7aNDTvGye/Ynaa460E7eNR6dY482E0afpxjjBczRJum2OuaCJYk7TzG2uttYloDjFXjOH1E1a5rnWWP8AdNTuw7nBYf8AAU/vazxGbWNemXgVQqnvf9H0E/DFHr/VAr5LSHwWqWBeDUaC/bF2cKQe4CwJtZjGszNLjURspquRkmeSMwQ1FGJaWExSexp6OB1TG+V5pYI6mR2V4in2E2HSTRxyRlm1yjKejI1wN3L9kng9WitIO6an9g80ILD/AICn97WeIT87THwGoVT3n+j6Cfhij1jXpB4LVrAvBqJBfth7GFao2vdVRxBvQ6WWrnpYtpJUPfJkbWBzFVU8/wC7sgie5k0eZ2Imna6R1Wx0eHQiVpbIxrixpa6yeXXIcbr9kng1Zq0i7pqf2DzQgsP+Ap/e1niM/MOrTLwKdVPea2i7gEMPgDWdBcEg33Ym0UBy3jRooOl0FFRQF8d47oYVSZX+yUuG0zQy0abQU/S9mqrB6NlFTPbDZ3F1Nd/s1V4TSMwuCQRWeaCnu85EaCm2fZRoKfaO9khh9Pk6guLqbOPZKPDqYsN2puGUpMfs1TYRRuMt47qTAqAQs6FlxFRcIktCVxBQbK260Oj1A6eG8DlDo1hpiluxxT9GsO2MREZCOjGGtqpv3ZzkNGcL4Pa1wNGsNM1NemLUNGsMHCPYlyl0awwUw9mWrk1hnDwOCFaS4BS0uFPq6TMTr0D/AAvR6wvmisf8Fq1gXg1Emr9sPYwtMDMu9Z3fUUyUxx9B7mudI55u5xJbM4Q7ppAmSvZfI9zVM7OCXXJa4t6iibnev2R+DVastIu5an93zQgsP+Ap/e1wHDZDztMfAp1U95ri71ikZaFpIXlu3gbiSvJRWDxcBAbm7lUDoncm/JVnwDLDec25VnhDT+Y9X6Hrd13Nt/Vlb2/nmFsvyyxfk67s6v0pTle2/U8h20IvmkDbOvk2bL7cWz7SnIs3sbOHc2Lzf/nEXzShuzcDs9kLmqb3u2iy5BYMyOtkYD1PB2kpGfagM6vZbLTT8OSZuvXoF+GKTWNePeDVawHwai1VVJTVYaKunhmHE2Ff7bRoYLhX+20a4kwo/wDxlGuJMJ/22iXEeFX8No1xFhP+2UaOB4SP/jKNcR4T/tlGuJMK/wBso1SUtPSMLaSCKFq0iPsmKTu+aEFh/wABT+9rfjX6rczTHwOdVPea4u9Yq2wihVyEOy26v12UZs5vkOyqnsBA7lWH+HweRPa86o3wVn0n83mbWPVl/MevM236ZR1jec0R3Dqsz8qpu0U+NoB6XRfcSP6Ts7DvG9uzprl0fazRyPbGS0bjIHR2JNpJHbWTKJNqyRoyg22cTx7Lt5y92R5be8jhZwNjGHO24N5Nrph+GprHdr0D/DFJrGoLHvB6pYEf4NRoatvFtdntGbS6qqhtNA6aQ9ETzzfDwgMDK370FzUTQj97h6FPO2pp2TR9lEq+rSLumKXscwIILD/gKf3td8a9W1fPVZaY+Bzqp7zXD30axEgMZ5i9xbchYMKuot/V1flaqk+zcvpVV4axFVHgx37yj1u67n/1Zp6XzuOyPKL8vmzsqm7YTicsm8qUdI+Ud9p1m9IOjH5S32LRcp4DYZLXUou8t+TLmYG5zR7o4/J17EJ17ym5QvnjHy0y/Dk3z5mgf4YpENQ1474PVrAvBaPUEYzsRE0OEzr5CAbOk9lTyGvfHLFFVV1d7LCINlTwYVijd7qyYOnnmp48mLxx1FLVxSPihbQPZCwdQvvJ1XWkXcsUvd8wagqEWooB72t+Nfq+XM0x8DnVT3uuHvmKvILYd5Qvf5IWACyk3uqNo3q/s1UdlHcFVeGxLN2lP4LZE9pHrKv1pvyTVGbBqZv8yoXEdTSnOd0hkTsxzkmICn2rnMs1t6XNZh+UuYU7c3VI2Xpi++TP03F0eT24qYY/82Jr8vabldn2N7ss/acJewNvLGXdrLGY9MSeTT8zC069A/wxSaxqCx3werWBeD0auqqd8ZjjgZtJ2UFQI8z668kEmfO19hJUU3GVYIHk8GjyxMDI2hrXvU0rZWOjk3rAqgsnmonG4rRUO2YpZAw0japsjuEuBaOvVpF3TFL3esawqL4OD3tb8dJztL/BJ1U95ri71iqZLxsG+9r38gNyPWqTqevyBVIs1DeFL4bGj+dTAnBtwRid0r7llG/pIgB1t92EfpZli+IEJhc3cmk2bvKpO8kB639l3VYMJlcOlnw+2Ut6OWAb4R+aoaTRzKN20oWk5QHh3CXgZ9q8DZB7RGWR3yQfU7qmt1zANJcdlsm34RGDm22lw/w1U5bczQL8M0usa8c8Iq1gXg1Gh1Kok4NXU1VJ3VTXMYzNmGXCJHzuqqog7Oh6JqHJ0llLMqqfK0m6wSTb6QSOHVX0pqmNLJMj6SMw0scbrZkVpD3LVJ3esawqL4OD3tb8c/naYeCTKp7zXF3rE8IBAK3UqY94h3bFVdgqPeFLI3gIjG953fMJ2Z0MxcTd/Ueq35j15pQMocMuVl8w681rx7rWkbvjNkz5ppybN56iwiWUb81m5T3ezguK2mJzZqRvQB6OSoH7pY5VHeOoqGi935cju52QvwiG+ba0pytkZdtpO5F8tpQXVLx0tpTuBZ/l5NMN+jMua3M0C/DFLq6kNeOeEVawHwajQW636HCKEyZuDNQsG2AADn7Il35ZJrhTSrF62zdjH0pdFcONJTvll775ooatIu5Ype71jWFRfBwe9rfjX87S7wSZVXe64u9YnNWXr3LL1bll61FuKaOgqkdAblAbEktzCokbNh+0AYG/N6lFoPlld2neZ6vlYAuh/qiYLDs5WDezzbvpY9wTR2VGzO2VvzgdnpGF2W1yZz2tpFEZaIhlrULhLDSyDtTfDz2VWP3Fjxa2fPNtGl+eKwDAMuzku0QSXKeejKQd7wMxacuQTNFTG/OVpVKH6N1QYHczQH8M02u+vHPCatYF4NR86Wka6+RzozJhkzzvqujQ4PT00mexfK3cObpD3TVL3escyj+Dg97W/HP5h3atLvBZ1Vd4NcHfxp9Mbv3Lgx6O5cHO/cuD2sSox0nIygNapZM1wqIXc5GhHApJonva/YzMDs5YpHu2Fn08gTyP/TQXONs14bBjmHLljPSBvvZawF22hymJ43ZmjcVDYdZbaKQNkqmZioiCd1i3DZBE4OkLmnDpWQMfG97QySpidE4B106T2DhmKp5dmeCi8jmSVZcxzY0I6t0VnPaAIJiJGyPktwaMPJdncGRNa6NojIOlQ/wzVAX5mgX4aptQ1hY34TVLAfBqNDU+WOM2e4NWdp6ntRQC4ZUZNpwT2fUgm1EJdYSNuHtLywPaXatIu5apexrGsKj+Eg97W/Hv1W8uZpd4LOqrvBrp/iIkcu7cFu6SawdEqqAbBJZQ9ac/tJjryNWDdKqcCr5MNuDZEkySFxJM+/Rdl72I3u67hWLpGuJN442bhZRtALCL3oJRCx4yAujlneG5nq7+n0nXdHIc7Q6RNpi5xLnPy0NHEJAwxi7KSIvhmyHNOBwd6aM0BADszMrSX2bZpOeIdLO09AlS22ZJtldfhJHTMsZbYHo7PSr8OVF+rXoF+GqbmhY34TVLAT/B6PVLKyGIySOytmgnrA1wo6rIcNqBK1/BKlMlzuc0hzHySsgY6SVwYxjZ30mTZ1IpmvDxmaQWy1LIXtZ0nyS0EkgfenrQqaI0tncGqmtY4PaHNILVpF3TFL3eoIcyj+Eg97W/HyK+u2/Vpd4JOqrvBrg7+NO7T96HU1Nd171VuvB1qHddO61F3wWD7qwWU27DXG5Tjven/hoIt7SDfmg3fbemflKgjLnMFiqWm6DXb1srWG+zId0vaJe0Na47slncILbSZ6UjOTuyDqiB65XXimte8bv3bflyNzbcj2m1jIyMLSzZ/KMFPv7axOcub5x7Jl9tGCXbTSTfo5XEczQI/wCGKbUENeM+E1SwHwajV10XYrRNl7DqoA9aNWLdarqzNiNGG9pwa/FaNkvYqavK071htRtqitDexgzmtdWTu77ho81UVwDOtYVUbWasa3sLSPumKXsaxrCo/hIPe1niMms69LfBZ1V94NcHfxpx/VXV+pVLvZPTTuTKd7ndSdGWSrCt1WpvCnech3uVOM+jrh1l8Vr9VslnEWOa39stPCS9lw69KxvQtltA0NbCAN77DP1XzNyflyySe2l7e1M7AN2y2UExNSO3tIjeP8tnBuyF7WpXDZy2vtCWWt7LZMd7SK5dnaRs3dSmtksSMmY8Icbv2jHABvZy6TG+j1UDzNAfw1BzLoLGfCqpYF4PSaqiFs8YaS4F8GJZt09M4bDFPrpVQYeYZdvUSCWepgbO0XJY6akxGU5dvBloaVlHBs47lVFNIXulpZBHJwfE/wDrJ1HiMvRc6BgoKVlFBs47krSLumKbsaxrCpPhIfe1zf34uV+Z8lpbvwSdVXeDXD30aLt5Xy+a8lV7oXJo3Zio62QNsjLtHPJWHfFFSn+F7+p43v8AOgF8Cd1ZZG9KTtZy0W/LkZHaTfmztkaGttkyUNzNGd+aLfD+Wz79C/Vmttt5zzPFuuPZ5ztzvftKXKCLGPIx1tnv31cxZTSuaelSzkuLCRkDztS7M7PGejHa2W/VvKkccspvvPeW+TCS5putIr8navmaA/hqDWNeMeFVSwLwek1vrJ2zPbZtrqqkfDGHRgE0tXNLLG14arqrrJYp3NZlLaOd8xkzqd7o6eRzBmcK6a4HRtTSOfBG9ws660iPsmqbsaghrCpPhIfe1/xZ5pC0s8EnVV3g1w98xGePpDK5cJjsDYp9QwA7nKpkLw0v6DS83It0bdRVjaT5nDGZZsxTpP3KZg7Tt1zutgNSxjqlskjgquBjS/I+J8NiJT2to5oLdzo9myJ+0aSenR5GBoc9gEdTCGxkytvwynAcNs1GaCRjiHNLZ3M2klnOznLfKHx5Yn+0hcXqMjI1oe1V7S6kfbeqZj9o42IDInGQAKKN3QcOyInBjR83xOvJu3mI5ibNythdniFjn0hidxBXkDmaBfhuDVfUEFi3hdUsC8HpNUzpM8cNOAZm4c2OO76uodJFJd0jDbNCyatqHsjk2MFXDwWIujmkkRmYIDMT7OjpJp4xNVzvhUztjUNjc/O2eSQOjigAdPwJ0Ud31sjpIJBIHDdnWkR9kxTdjnBU/wAPF72u+MKvrCK0s8EnVV3g1x9tqcf1Qa5xdZMds29Ep5uXK3UgbXW0dtAGJgMTXAnptd0DmPRxnD9m90tM7PFHCRd9wpHvzutdZnHrIy9Ine94Jle0gCQ2ZO+7ekbsnNhubZtTu7qIo1Z6Vo4wn1L3OPUhUPzfJPqHZIB1FtRJl7RW1fk3u3XILyC7M1/y2nQc9wMfTfmEz7O6RTpXZLOd0WyPM980m0Dy1nRd0cYkc7CJ2uO7XoB+GokNY6tWLeGVKwLwikV1NIaWpgqrEx1mLRbPM2Vpbg4kk29S/cIKwUL5oJuisSxEv9nF05TTP4pFMDd/GzJYr3yvjmdX4pDs98dRLwWrgqXD2VbibchIeMuA55GT1Mlw1aQ9yxS9nWNYVP8ADx+9rvjTztLPBJ1V94NcfeMTmNzv8vk1PtdyPyVt5TKckAus0BkUOYixc95k6LN5a0tbJc9JtcyCF8UtpGTileZODT5RwXK1wEsRGxcHdtiNO927PGhhznFpzhMwx929IIYc7KCXLggb1yAJ1Myz/aJ1My56ZsYLO3Z7u7LOqwpez1rY2a/zMXRN8mQROEw69o2O7B2cuw7O9GE+0Iccwit+ZmzbFcszP6WLQWwmrcJLnXoB+HItXyQ14r4ZVLA/CKTWaSh2+d0FPtVLGyZhZKxr20lNSRXdSRwjVXwUT27StjjIhjjhjDYGNYw9W/q4FhpftNlT3aQWjL2VpD3LVL2dY1hU/wAPH72vH76dXy12Wlfgs6q+8GuPvGot3jqR6nJ3yXnchdMWy2TpHDNfrjjc8jNuDWMp43OcApqnbNn6IanPe9zvmdk/KSeoi2ay6d+pBrv/AE0Ou3pG7RuA6RTWizDlQsM3RajbKexZ1w5w6WYubl+WQC74ic12kFpCcG5Ord1vfbPnDW9W7I1vSYSXXydF1intOUi/Ryv2+bMc7A+zQLWxfMcJqrt3a9APw5FzQsV8NqVgXhFIrouDQSTYbKOasFWx78gIspJo4AHSuDVRtZDE1gL811UPjdKxmZhkp7NgY1rg5TN2kMjCcqjhid2alhELNnE1l76tIe5apezzgqfuI/e4gf3zmXRK0q8FnVX3g1x94xHrcnnqT5OvKj1pmZx6KscovvIqGRuOQF76h0tQMrjYEN2EtgbljRcWRByuNui7rPXfd5Cw7Q3HM35dWVoj6Bc43OS3Rur7kPz9eaQtsezlJ6f5s7COj1ZWHc3z/K/zb+bqys7YPSzMtlaPl+X5p/5+tAXktvUfU11ysZbbBqvmaAH/AA5GhrCusU8OqVgR/hFJqyNnr6aCbup6sMbuKpZxJVVLGjo4QIzNU1T98uK1gdA5rkap3FPCR2qURUFK2KJVlaOH09u1IxtRXU9PL3NRVtZHlFg2gnEslRG3srSDuGqTs6wjqb1qDuI/e4gf33m9a0p8FnVZ3o1x941SfqnuB6wnMaRcXUdOX/IotbFuAudm+UZndkxZSRlRU0WSGTcbu6j5W/dn3BzOy7+rL+b82YWt+XKL3b15h1W3WHU1fUhbIb2s/tne7Nu6t2WOMnI66b0RZA5mOsCmDe7fvY3pAJnZaVbopw3vG/MLXv0crR3Y33xa5wmu6769APw6znYn4dUrA/CKTVURGXI5jsks5xKQ5RDEsPpRSREE5pJop43vlpLFGlra1+WdgghMTDDsco2cwr4WCNjOEMw+im4SKmssH1cDpMkkL8k1RxjIcopd+GUnBISHHNKtIO5apOzzh1qDuY/e1/x552lHg06rO8GuPvGIzNzTbitoDszZyjMYMufMFJVx5IwBZpna4vvdQ10EcQe5lzNUh7pboTs6DkH08zJo3HfUTwhxczNk28bopIbi5qGZdpmNg9u02d23E7Mu0zmwkYHNZmbfax5c2dbRnR6QVM+AyHauu2aenuXx9GOOWITOjLI3EysPtGv6DmshMUUk7czXxnNkebZoxBmdM2zHDavjBO0ZNFs9pnZsmuF4mu7Ye20lj0nvj2WbNHsb/vQac22jczZkgsyYy9gwaozFuXXoB+Hmax1oasS8PqFgXhFLrBV+YCgdYRWkHdNUnZ58HcR+9rweH/oNV9elHg06rO8HMGKz9LzbjE7dnYBOxmoJkJ6+NJrM3IYrMM642mysb8uNZrvNt4xWWzBbczH6ljpSBvdikjmtblGUY3OHvflGbjSTZCPKMnHE222thn4zfsjHkGTjiXaskyNzcavySNyNtxtJ7LoNTcXkDpTs2rjd+yZGYm5ePn8JM2wjzDGDwcw7FuXj720UhpY7tx2zZxwSNOxzNDDHwZibj9qp83BIkMbtSOg4KxHSEGenk4FGm6QAGp/c2J+OtdSxw8FAPKNnD21PAhaPHWNpp4uCXOJ4qa2mggbEI269APw81Dr1BdSv+qxH4CoWB+E0qvrGr5oahzdIO6an9k87R3CziFTmkH7uBYWHV7zEfighzPmtJvB51Wd6P9H0B/D41goasQ+AnWCeE02u+5BX13Q/vqOvH+6an9R1hFYdRyV1UyGIb6Kljo6ZkMIs33uI/GBX1BHVpCC7Cpg0XNc0tlbf/R9AfAFdDUDqxD4GdYIf4XTK6ugdyBQXzV1dA8wrHe6Cf1HWE1pe8NaLuwDDBh1L0u/99iPxo5zt60k0YixCYPpKVkSOgsvyDUdBZ/6UdBqjyauQ9R5NXIio8guRFR5BciajyC5F1HkuRdR5LkZUeS5GVHkuRtT5LkdUeS5H1PkuR9T5LkhU+S5IVPkuSFT5LkjUrkjUrkjVfquSVT+q5JVP6rklU+RXJKq/Vck6nyK5J1XkVyTqvJy5J1Pk5ck6r6XLknV+TlyTq/pcuSdX9LlySrPpcuSVZ9LlySrPpeuSNb9L03RGszAFrwsHoW4bh8VMzfqGsKu+CnWCn+FUuqapjheGuJuK2ID8y4dD5vXD4fNy4dB9RXDYD+dcNg+4Fw6Af5oXD6f7rUa+m+61U9VDPmEMgeSsd7oJ/UeZonhVgK2obv8Af4l8cOedZ5x1FHfzT/KhA6xq3Kt+DnWC+FU2qjdbGmraH6itofMraHzK2h+oraHzK2h8ysx8ys58ytofMrNfH6ok6sd7oJ3z16O4YcQqrvHsAAAABYe/xP45qHOJ1XROq6KOo6zrP89W/BzrBj/C6ZXUBtjDVtEZFtFtFtFtFtFtVtVA6+OVR1Y53bU7VRU0lXUshiF3YfSR0NIyCLq/kMT+Oarq+snVdFXV9V9V9RR1X5p/nK34WZYN4ZT6s1sVajKjKtr+q2q2q2q2q2q2iozfF6k6sa7sJyC0XwvgdNtpR7f+RxP49q/vzOpX5hRRR1HUdZ/0Cs+FmWD+F02qrbKyqZMyMyA1E/pJlwib0ky4TN6WZcKl9LMuEy+lmXCZPTTLhUnpplwt/p5Vwx/p5VhWd9bNMWFrbrG+wEVorhfCp+EzD2P8lijbVkb9+q/MOu6Os6jrujzCf5oIaqr4WVYP4ZTc0FXV9yBVyr/qrq91dY0egqCilrauOFjHAUsDKWnZDELM/kp4WzMyvXFkf3ZVxbH92RHDGfKaQLixv35VxW370i4rb96RHCm/KeQLij/sPXFA9Q9cT/8AZejg27dUvvpdNXaOwR1D3wzQM0xqHdUcadplM3tRsR03f9thOF4RVVFIyWsmjjfxF/2SuIv+yVxC71S4gd6pHR93qgjo/JbdVNXJ6b1TFyel9UxHR2X1TFydm9UxcnJvVMXJyb1TEdHJ/lUxrk5UepiXJuo9TEuTdR6mJcm6j1ES5N1HqIVybqPURLk3UeoiR0cqflPCuTlX96BcnKr70C5OVX3oVycqvvQrk7V/dgXJ2r+7AuT1X92Bcnqv7sCOAVnyfAuIK36oFxDWfVAuIqz6oFxFWfVAuI6zzhUmBVkkbmZoQotHKukhZDBJFKw4NiH0wKfDcSi6qUSJ4xCPtYZUp+kVPFI6ORpa/lLSDruuU9FfrKwad+MMkdQQl7eLcQ9KuLsQ9KuLq/0q4ur/AE5XAK4f+K5cBrvSvVNgVRWVYfXs2NO1oa0NaAB/P/tajz6J51A/cp3KIZpWBQNyQxt/0nSxmx0rxNqkd0UHWK/ZKz+A1Ev+kYzhlPi+HS0VYHGGX9l1Hc8HxCoYB+yuMv8Aa4o/Lgn7P8GwyZkzmyVU3+k6U6AjFcTlr6Sr2Usv7NcVIsyqoVR/stqC8GsxGJrdH8Hp8Dw5tHSF5Z/+03//xABEEAAAAwQDDQYDCAEEAwEAAAAAARECEiFBMVFxAxATICIyQlJhcoGR4TBzobHB0SOSojNAQ1BTYoLwwhSy0uIEYKDx/9oACAEBAA0/Af8A7LrRaNn3zZiWYm072wWi0Wi0bCFotFo2tCwbBbe3k/JJkDJS+77P/QXC+6VEKz/9DcL7lWYqLE2mQtIbw3hUVI2i0b3UbwtL3FRXthkLS9xvF7jaY23rSFpe4tL3FSxFZ/lbhdsVJit1CGwbRx9hx9hYfsLD9hun7DdP2G6Y3T9hutew3WvYWNewsP2Fh+wsP2Fh+wsP2Fh+wsP2HH2HEcfuHG9x9hx9hx9hx9sS0Wi0HREWi0Wi0Wi0Wi0Wi0Wi2/UeO4XatxJ6hkqzGqzcyIhuEO7Id2Q7sh3ZDuyHdkO6Id0Q7oh3RDuiHdDuh3Y7sd2O7Hdjux3fUd31G51Hd9RudRudRudRudRudRudRudRudRudRudR3fUd31G4O76ju+o7vqO76ju+o7vqO66ju+o7vqO66jueo7nqO56hglImLnSYujLxlg1Qd0O6HdDuh3Y7sd2O7Hdjux3Y7sVMsIYPzqDJpjuF2rrBef5oheYO5l2xkyf1dQpeuO4Xaoz5fmjowTOIVLLDBtmVqDZ2Kf5EIY7hdqjPl+aOjBM4jrT+DNkplrbV8A4xnUvf3wQYS4HcyZZbwhwJXDKBcQf/nkdxaykwKlwdQXVi7pdzYulzutyOTy5J7Bg7jh3ybR58lXaoNm45VzIyYOB0LiJ/kQhjuF5dqjPl+aOjBM4lDzLRsmfIFIuxT/IhDHwZeXaoz+aODBF2yf5EIY+DLy7VGcZkoCojFotFotFot7PhesFgsFgsFgsFgsFgsFgsFgsFgsFgsE2UF0ZXGcGCK9dX3oVILBYN0bo3RujdB/sG4QZujpISSvf9iEMfBl5dq6zjIELy/J0PzxnBgivfE/xvGS0hhknmXkiYwpXNlboqwF2eNCujqEqBi4FdTYemaQXiGW2WYtvKqi0GMKXleT/ACIKWPg2fLtUZxkCF5fk6H54zgwRXvif43jaZZVAd3dZyX0Z/qAiaN1lhEqgCuTKtOvEpxPzBNs3Nkiyof0g3dGjdRIERSvEMKXle6kFx8Gz5dqjPrjIELyvmChvW1A9mb7iEK4+A/2x8R/uBzTMj4izOj4D/bHxFafaR8BZmx8Q+0TyZ9HIRhqgjPKSkatQXPTZUNSuFYhlJQIQ1/YJV9nHxBPZbv2iH4BGvhTZhSoe+2dhmqiUg3fhQVtSpUZOU79jlJEp8BlZTv22UkNXiEb+BBWEIorQYwif6kmIZqo7SDK5/C/UWkyOQdWhMBlJHW4AjuiXZxSbSSSCp/poLmqr1AYNh40QieWCeuJHzxnBgivLdP8AEeQtB6poKzMEVDwOo0FZtLfwpeV7/sQXHwbPl2pss+uMgQvK+8QnsjOsS5yqEPOdYlzkIecxo89GoT5zrEuchpJTTpViXOQfaerlnCKVcBG3iI7tA+qgQ3aBBK+Ag9z0ho/NohG1RHqdIK0i5lEpr1C7MJm8kBnc1TM/lNegJlhxac78PrsDrb6I9nfidAt0R4/hKkjpXqHyqwyOckHwn0zKdPbYHPhrv/h9dg+K86mF/lJOgO6FR9irnNQ7cXcJSinm7MSPnjODBFeZowjBNIO5Z9h3LPsO5ZHcsjuWR3LI7lkdyyO5ZBxMrmyRXupBcfBs+Xaul64yBC8r7xCXPRB085iCc5CfOYgnOQ0vm0ho89ET5zGjz0RFecxhW3apZoitfERsH1UC3JoELaBBauIQk5yrCZXPSqGWkcn+JzGVLLomQeLSyM3WBYN1c7+JTIOsv1Z+nq8AjbpGcCytE9LiFbii3RHZsUJtB3RkzIm/h5mvSoJm5OrBoo6JaRBw30nl6ZaPALdUJpr4fBqkz61Am2UMy+LmalCbQZXFXTeJVOmo9mJleeM4MEV/VejeJJ1mg17tBbGafIVYE/8AkJ3S5G8RWlT5hslLF6kFx8Gz5dq6z64yBC8r7xCL1edPxEuchSfOYlzkJ85hIc9GsT5zqEuchOMadKoRSO2VYwjSxjKkpCM4CNvIWworFkaKhCcKKxD+pMQXnOoIaRojLWCNrWdrMrQrUH4ZuuHii7HN1AeDg9D5tGwIzwy5fqf2sO3VYGa5U2dC0PN5OEMizf1J2ewfZynEPM/Tnb7AyuUHjMjytbQsBMNTRMuv8T+1hbrlOGcv05W+4NtjJfM9D9SVnuCZuP7Uyj+a3Ej54zgwZX3HDYO5meVrvUUxUVoKjuaEGdImYcBscPwQfqkzm7zPqGW2TQmYIuL1ILj4Nny7V1n1x0LyvvEIw4yrE0tnUKPHxHWdQIvWVYOnnOodfEdfAF7y1hHz8BhGvSc7BGXpIRn6izZULdlYhL0mMmfrIIVdf1CMtv0hG9OMpzsCtSaMs3UBtFB4zPN1/QEVzVGIU6ulaDR2H75an9qBM3V5INFEqWtMPtkuDNxXP05Who2DiatZuv6Blm5vIwhFlaRadoNltzJMyPL0S0ARtmZPI3m687LATbESZMmM2bE7QbFyR7Kg9o6pbMTK88ZwYIr11N1gjo2mewVYMnffxDButELlG6JpbAVBFeMoC5HkbsvURM6I0ViKEUqOt/qQXHcZ8u1dZ9cZA6V94gRnQe2dQlz8R18B18RDz8Anr9Q6+AL38R1+kZXn4jCNekpWgl/u0RlCioeNFYshRUDNm3mCQjhtnWEhzlUHGj5HOsZcsngUjCnDTzawy2zo5EWdUJc3VzqdE5ECZykL9+nrcNoS6kTxZCrolIw81QmGRyuhAy3czyS+FmzKlegcubio9nfhnLiHLo+iPZ34lfAG3dCiXwc2RUr1D1zRUw2adB0J1Dtyecrf09tmJleeM4MGV5kmmGz1Vn4CtRdWiK57SIqQ02v0lfKIJiPj7hgmkqNSmGSTJv8AUguO4z5dq6z64yB0r6kOviOvgOviOvgJ8/EJDnKoT5zrHWVQRTJkqI6VYikIUyqDJHs51iNgjbQD2ZNA+qgQlDiG2WGir4CfOYZM/PRBPrQ9KnYHj7vM5qGnWJP5sEkPhvGRZFOntsDnw1T9T8PrsDdzujUEflnbLBhGkU/gq5KahbmjyYZHToknUEVzWh3P06uAdujimTuf+HWdoebVEwubMqE6B+5qRNfCV2Z0kfQYO5uvb+jWWIrXnjOGMGV+lIu8qL077chdMXqQXHcZ8u1cZ9cZA6V94hLnKoT5zrEucqhPnOsS5yqE+elWJc5VDSsWY0UIkLK0auIitdMwbJmVVMhG0R3aATX8qApbtAyU1uAZNxrmuUEyeeiDZaI66dIZZRPJUqjrDx1YTMqoQKwcDyFdmdKh25OqZE0WVoFPiDYafSeX+Jq8NoueEaIjPJkrpzPYDaPKIviJg9ShNoNq5qRNrc82bdJHs9wwyxaRP6OuDYuqmUTPK0i0BhG4G3kZkrp6ewW5qaZRZOpO32BsXNTKJHlz1bMRWvPGwYwZY2yjkNjHUazWN1ILjuM+XauM+uMgdK+8QWOzK0ho/NojS+bSEueiFjzmJc9ET56QQ05yBllssnTHSIErrJzNZdQyw2ybbJlFaxGwRtoqEaTyaKxDeoqGTpQ4nIIw0zGNMq6QkY7Z1AiaRWtsqwrTRNTiUYB6gmjdzNcPMZRkbxZOpMNNMNMk9AyemegGWWiLKzcuX6n9rCXUjNDNf46NoJo2iYJpIOfqegI7nFoklqTt9g2yxCJrlV6AYZukCaSC62lYH2ifNkzLN/T9QZ3M3VUzhrys9wzcmF0U+JPXtxFa88ZwxgyvootvuvvPQRFxCJUI7/UguO4Xl2rjPrjIHSvvF5hcn5tHqNL5tLoNH5tHqNL5tKrgFhzkJ85iXOVYMo851Bk2ncpJ6JzBvKczjOoE02lVMjnYI28hHShRWCOrZqiE4UVgnf6kw2TKHVGvRDBQyf3fWGibVCpjVojL0zqLTnZ7B+ZNan6fqHrlCnR15We4ubNzKDKEWVNnTtDTDSQOOXIvw/7UCK6qVB8WtKwP5x3M3fs9SkLcjIjNW6DoblZaCZZeh+/T1+AMrq6rKs52iWiCban8TM16AtzVGciibMz6DBMuvEpZ+hUVuzEVrzxnDGDK8UwlTDJnzNQVP2da1hmlhokMgVJmHXXjuEXea+AOZBvNubBPNHwDakaMMTTbsBMobTVzKtZWg4qV7qQXHcLy7Vxn1xkDpX3iGl82lUFyY/u0axpR/dpaoKiP7pawWPOdQlzlWOvgEhzlWDfWa2lojKnt8QbTc1mWjo2iM/WYjFNmqFoXZrCEtmqMn+rIZKwoyplpAyhCnKlqBkrosjKMz0rAZ3RDwZuHkyYke0E3mr8T7P8AUo4B64qbmRmzYpMGzczZWJnlaB6PEEy2+lOfp63AHhUNolY4FIwTVEMLmV0IFuTzpfD/AJFSvQOsuKmv+H12Ambo86j9OnssB3Q+5zOaj4aPJhKDzZJ1GCJ5xF+009tm3Eea88ZwxgyvE+2RHrEUPW+02bPBDUETV0Iq2io9bzLZHxMog7qbBnUyVBX2Wy5mUf7tvdSC47heXa4Nn/LGQOlfeILCP75awn809Uf9paw/7fSF9fEH7+AL38Qh+fgMvZXPSEfPwBG3sOU52DKikOUhG2isLq5ObUIJrUVhWHoQ4lMGTDtZ5WgejxCG/wDPp63DaEujqlkq9oVGPiKiYVHSzjoToH6vg/Z1UqEuSKmEoPNknUZD9Dudp7bA604qJn/h9dg+KRuo/LO2DCa3wsyulQlzRUwlGiVBkDZZfTf09XhtCXR1TySjonMPHFCwmZq0IFuakTSscWpAriTrxomXo62I8154zhjBleI1ZaZpZOshW0RkY/kEQjIkJktgZN5ltmlkxrumvIKrTR0tHWGs4jzWhvn7CtTa8AZvNNHS0dd7qQXHcLy7U2GfXGQOlfeIH/y+kEe3W+oH/wAvpH/aesKfGVQL3nWDo5yqBEa851j4iKSlPNqEV61gjbRSVmVBSMZW9RMwpyyM2ocH83kFZXUontGQ7Q9PN2DIfgSZ2n0CZCpr6HXYEujyI9Tp7LAraL9nRI6V6haYYTMqoQG4ZkR5E6TkfQEyw5WWVoV8QjT1Z5elq8B8Q0NpC4NB7OdyszU9QeDUiaMy+bRs9wTBJJMuWv8A2sGV0ihmsZs6IfPJfPU/U9AWDi6ZJ/DSt9gdxKtpcv6LPbEfb88bBmMGV8jgaUmubeWJIsjBwgVOdFeBc71aZoKSI7TDwLmGWTMirCoZu0Fr2BpkjO91ILjuF5dq4XrjIHSvvEJ5J609YSyT1paonk/unrDRZSJxlUJ851iXOVQOnnMJCG2QRs2kp/kIpVwF0YbZaIkXjsBG0hkeQcJTEan83kgWvIzaxkpQ9QMh7KyeNQImXVMlLK0a+IaI3o05elq8ARXR3KhTonMGbUYPZs2ZB6jC5OZrhxhDMkOlqhnSBkwqNfumegCJpEP98tcZcXTOWrIPUPnqfqeg+FF0y+jSt9gbJJSa5ctT+1BkrqpKhlGbWkMIcXDdzNQfCpNWuDUgVwykgZZelrYj7fnjYMxg711NCeoZKZmK4JyQMGhpMXI0buhErTR1ECibN0Q1Dry7A1Fm5XNMktpnMNwZM6VqMXU0ZWgqzMbjLvLqGDRpL3UguO6XauF5njIHSvqJc5VDS5zB0Ge9o1DS5zEuchPnMdZA1f56QdbT5tENPH+4iXSKQjOHARopomQWvJorH1UVCGlCisZNvUQXnOoJBSOvxBk1QR+UhGZ1VhaXTq1QyyRZxmtM5BCrr8Qh11y1RlUGh85g2qUyc3VBEwimrXA5BMr5tKsZaLm8Kg9rZebWDceTN4kMFkvUZ2jiYRvzxsGYcvMKy2kiOYrUXUydLYUw22d0ubR0NLK0NwZZKZgrkTPEiBZzB0smLib7bRWQIETTDZ6qz8BWourROWEVN7qQXHdLtXC8zxkDpX1IT56Q0fm0RPnpCXOQnzmJc5CfOYinOQNhoj+Yqagb8FgUdGsNPQaKMpSCtaUKKwpyjm6oXWhm6wyZRoqmMmfrIQnt+oGRz2/SCen6zCnFw0oqBHRPN1hk0FDkEJOcqgRNLznWFaRc0L/PNGQqFk8Q7k/NogibVM7iH/4ZoRhFLK4DBGpMlHO0qsTCN+eNgzDl9aXSVbxyaJRQbTF4oPNEJEySENoR7ZaJJe6kFx3S7VwvM8ZA6V9RL5tET+bSqEucqxPnOoSQ9sqxPnOoSrOMqwh5JHt0qgTBtFH97PMGv92CP9WYjLZUF1tlYWqFFQgkY0VyGSsDTiUxBOcqghrznWMpIQ4FIGZwLOorC1ZGbUMlKHuAQnqEztIE86pwp0RlUGT9E9ge1sjNrCMIudwrBlH5tKoE+ink8DmHqsrN1RkKhw4nIFcWkU0TKkeliYRvzxsGYcvFMEZGuDN00JM7nzvGcNoSlsjIz53mDecNk25VEGSJlSDTJkoefVDMnlOa0RBTvdS7B0u1wZeZ4yB0r6kJ/NOoW7ZViZ8fAdfET5+AKLxyj4ibZ2+AjRb4hx1a8spSEf6sxlShykI20VhaoUVDxorGTKHEhkpXwEF5zEU5yCNKlPEKe7QF2PZoyVTN4hCdjt0awZNLXTpVBWtLJorBmUsrN1RkThzkCZhsyvq/tYN+S/TIE3Q8errhLnFE+nSB3Fo6FLOq0cTCN42DMOXjVs2dZJXmTI7FDLZ3JhdAiHkDuRNeApaam0dZi6NOHtJAZHdG2dZJeIoSQubRJxle6l2Dpdrgy8zx3b6iMOPiOvgC9/EdfpBcij9QMzTn4AlXn4iKQ2+AMo/MVNYikIcKhlW8xGWTRUPqoClLJoEEr4DJWriJc9EIa85jKSMOAjvUVBS0smisZNMD4FMISpbPVBE0kdsj0gZtRdWWqFKD37dcIxIySNWkDLnlS1QT8FQ/mmDbpdyc3VCXNFpPdOQwLbyQPO0q8TCt4zhhy8wbzDVQ18JD3DZvNtVmG8+5tGinWR1g87LVo7EDrqbAUGWiaRrioZzLmRqm0xc4smdFhjWfJ0Nm821tvdS7B0u1wbPmeMgdvqQudMDjGVQulEKIzrFxpJ01OMtUXShkiOvS1hc6YbZVC6E7cySiOlWGFM4QplULopFDbOsXJk2jhClcmoNqRLncQyrSaPDaDMy/dQKU0aARoulQGkNFhxDCEdfCsN0RpjOoMEbxLRGVYbNomYqZ2lIEpuG2dWsHiJ7hqhomGiZZNV4yFzInj1Yz1g28TEM6MtUE8bq5REmsHiVtMiibIMmHCPOPdOQZZPCVs5WnX/8AoM23WjL4Zns29Q9AoYVHa6EBOPoWTTpg7i249QeVoYmEbxnDDnbdS7B0u1wZeZ4yB3EaztoueZHNF0z45wYzY0BvOjSGM2NAbztoYizGgXUnW9pBk1Ig2TpmCNQiAzUMEhBuJi50C6QMMGpAyRJA2nlWIuZIRLTaLttzbBc512hokdkDaefWIuRESLBq0XYkzsywMNGb70TBEjj+wXQyMmn80XMomqm1iYVv0xnDDnbdSx7nnbdnbOeuO7+T4Vr0xnDDnbdSxjpOogz49tg/XGQJ+T4Zr0xnDDnbdSxTNCIg3Fs/Tt8H649LSNQXYN4b43hvDeG8N8bw3hvDeG8N4bw3hvDeIbxC0haQtIWkLSFpC0haQtIWkLSFpDgOA4DgOAsIWENqEGYmdZ4zhh28dQ3TG6YsFmMVJVXupYp/Zkfn9wwfr+aOGHb2DPssCx63upYlzi1t2AvuGD9fzRww7ewZ9lgmPW91K+0YKk6z+44P1/NHDDt7Bn2WCY8zvdSv3QvlL7lgvX80dMO3kRGRwvcBwHD3HD3HD3H8fcWs+4NhlmKbb3Ur1zOH7j+5nczLx/NHTDvbQ8w1F52BEGSQvufkOHsOHsOHsOHsOHsLCFhDdIbpDdIbpC6NuFkmRkeI2RNEzc2VQuI3BuDu+o7vqO76ju+o7vqO76ju+o3Oo3Oo3Oo3DG6Y3TG6Y3TG6Y3TG6YsMcRxHEcRxHEcRxFp+w3j9hvH7DeP2G8fsN4/YNEivHDwDBITTRumY7zoP2XQhsZUMmhsnSR37mZE0rSDvCG+yN9kb7I3mfcbzPuGNBVNv2BUEX5Bc7swfmXrfMyBMkX5Th2jvt3dORF+UXSl00MVNsE17D9tx6hg1I7scCOz8qusW2G2VJRtaa/4iq5MmfmgI3jabOJn/wDad//EACsQAQACAgEDAgYDAQEBAQAAAAEAESExQVFhcYHwEJGhscHRMOHxIEBQoP/aAAgBAQABPxD/APXq3QnpcH1H/ah/bz/bn+nP9yf6k/0J/tT/AGp/tT/Wn+tP9af60/1J/uT/AHJ/rT/Wn+5P9if7E/2J/sT/AGJ/sTtPnO0+c7D5zsPnOw+c7D5zuHzlOp85TqSnUlOpKdSU6ks6ks6ks6ks6y+8s/5s6yzqSnUnafOI/un+zEt/KTRDyZ308r/9Rtid2Woj6uCXx4GEy3AwETHnZSxN8ASzd3khw/OI4JJ5Q+UruE1zUvjoohFlvy3w9f8Aohr9pZ16puEkJ7Vx3cKl4gKPtfWHCEcsyhC+uUWg30BPav3Hg+f/AHELbOFD6MABo6tysrKysr8L3fD5zznnPOHdPOeU8p5zyj3Tyj3y3WWOYs5YyPWR67851bOoRXKO5zr0VdrDGGOVgM25tkfqzJ2f/MAVAHLLgToafOXRXsZfnF1S6vxyfL/g+c8p2Q7p5Tynn/x/KeU8p5Slb/5jy/4OnweU8p5fB5TynlPKX6xfWX6y8e+K6y/WK6xXWLinmPdGGGHH4rRv4CLOm4sQ3EqO/wAX/ktafUMZYQ8j8ogvZFxPOJ6ynWU6xPWecT1j3ys85XrK9Z5yvWec85XrPOec8p5zynlPL/iHd8Fvgt/yV/5PmPxDL8N74xnGGGLUNxeIvdPEQKUR0q2y7Z7l0/8ADRm92Xoy8BLYdeyRTzFPMVeZmFvf9iP7HpfmWufkv3H+r/uUoHKfdaSsBJyi37ENwQ60v7xjYOwh/rP7g7SnvdFKiOQr1sjDKVwgfVmXR6fsRrhHiRHSoKsN1CvosyNBm5R4oIjhl6qV948qHg/PwWJ9fiS4k3NHyUpBBNOXLKJiXLly/gv+EA6PhYe6cJ5/C0+J5fwRFiyvHHWNyjKIVT1IvwDXusfzBaDaaCKmjhY+efpCU+eHzipM5S/iGkP9fJGCZGp2IqQVPY/aAkgzByfABoSsNDDQQ80KTR8LAgX9UP8AC/SH9B+kF/Q/qH9S/qXf2/qU/wBf1KPs/Er7P1K37ft8KW4PL/U9tnuf5PL9f1A8/f8Aqe5f6gnAfP8AU8Ht4mbRXr+p4Yd0h34LuRCnX5n9Q96/qX/2/qW4+t+odD536na+Z+oTWxo5Nb4m2436zV1+XLevyYr/AIxfHyTDj6IN8HyT5fJM9Po/cz0+j9wKa+j9y3ZfM/c7CGDMqBo4KZhmyiVXT4F+GUe79P5a3zbDXw1Zc4A36Q1zWxHwfuKbhhfljefBU0S2W8Mfb3M5fcd5f7j6xLXtO8RL9h5mKz2neUfrfuZvxP3E2hvT+5Q/i/uZfxf3OhV79Z7V+5X733l5MZxX+zCP7kH99jo/OxRzeuOn87Ab99x/vYx/lwg/lx/oYE/dgTH1EbvuoOrvn+5mmFN/XQLv1HB1H1Qf2aC38+P9dHSt84G187Bz/MQL+xA5Z8xATlPFIeFlTNmm3nUC8pVls0q8a4lvL6f3Mf437n+K/c/xX7nH7PrPbf3H238z3P8AcP2X95/u/wByrXz/AO5SbPX+4bAdqT1WNtasWlUS1dGs94e3D4COPmfWM1VZcuL8b3/p/Kq7bV7AL7rB2qUxxKXvMwcQqm6nM8yq1cDMHaomNxy53EK7xDkuc4qOViFRDMQrGJxmdOIhW5RcpjPyJi41u473Cqw5mEbuHmoVqBgtj1GB2nm4ZcQHLAz1n1QQ6zKFViyFBqHjHmLQuCfUnSJbeV+02/smaXFURjthHKK1dqkGjmDb0hnmYXGLXWdjBszmGqJ85fWNHD8J2RgPUBfyRB1ryRcHH/G5Pf8Ap/KuH/VHtExouAdAgeveDTVErNNSuxEKneo26j6SscXOfzLrZE5VmO9fKaYi81NJXmY23HeWoOagzzHEqu8aObmKth6wpcupjnEHNNxrj6TzcDplmnPeK7uZWC03Ba012g55nEtjpBW4M5uO3Nzk5IFibq5rJNQ3+EzDs+5F7TiCdaTvFHnERDB1Yc9ha9YiVqX1dE2J0YI456SwopdXXabsKs3mApbMNMWrhXGqmdwYWHGP3PylwZcv4bz2/p/L7T1TpWoGK6yh2sDOWiVhiq0yqiF3mDWY2Nx6xb3HnczcTzH4A1uL2iTHiVO6M53Odx1ePSPU+BqEd9px1nS4UuGHMokPExUJ0nYE0SnWdrKXNqYNQ8/KGTNTjG4L9nZLYvYSzeJ6BCAvWMrUEir5qpeXGaeFQhgAJfQ3fff6ahx3VqlL1NTxKipMKcDJquMYmykIUFULQjOTUeTIO2Oww5tcesuoqdOKnZV94TiLGZWB8rG/mflLgwfgTcnvfR/LbH7VDB1ld7IVesQeGVedRzj7QVjmOZ6IxMdvg32m+aJ2St53PYj4jrPwxcwPwPWMOpGq5l1xLxLqDntLLBzNpY4hR0we0GDjJBXFQdQcVUHzUzVUydYjVhvFwrFjcEeMSyohMxc3ukZ3PwQcai0tPpC2uY2YMEAOBUWeZZAigrLt8vWOLlqX3VG3N4ls8xhcek2JuDOp38Ljy/lLzFBgwizPcej+X3foxbKr4qrmDROdTXEsx9fgSjmLpHHWajtzMGLbmOLEtrGYtOpfaXnpFzFtzLvUURUHBFqEHMXNEFa6Qc6g1qGEUud0Gqg9GJ5YLxKRVup2kWx6x4Gkmg59YjpFu9rIzGf4zDIviAOz2lufrFyWNTNMMOcxxq4nie9xPWXTWY90ardSp95zHHz/AJS8wYS4Tae69H8oz++mI3RLsyQShqZ+faXivuRB/AOLiThkrBefhULXxcvB6+Qi2/lJ/pk/1z9T/QP1PYH6nsz9T3Z+p7s/Uw/o/U/zD9T/ADz9T/P/AEn+cfqf4j9T/LfqBfofqf4Cf5af4+f5eA8npgHCQ3SSiEKWr3fvAPd+897/AHPb/wBz2f8Ac6/v+Z7f+4dCpdSzs3MtYiOzqfOFjcMsE30g1gWGb+kWRv8AYjv2OIhc1DDFQUN6fuwhjUtJ4412hafZxaVF4B+oMKBxk0fSLhQL0z9O0R2gXk/qXcC6wf12ZXl6WP1HjROZG/NTgPCHK6lcXJHHyfl8BgwYfB7r0fym8tfpZhO8a4uaZlZhd5bhH3+Jvr2D/wCPdt9TymmbMfOBjS5aZb/EsyFrzLoucn6kXveICy7IDH1hQapVXHLE3Wssu4XXIApfZfpGgcCo1LlAKx85RE7ABUaG7pglC8zopi7M1CZ1pWYTwVQfWFXBww98M3RVu4bvrzd0U+Xh4Psv4EIfF906P5a5mv1saABS4HeBntKDmcvSNYPb9n/x/dOqDd41DJwMHOMwa6waGcBvL7kWIp/TBnJWNkFZLz8DOYgi4aFtPMq3HycIK2N+ph9tyO6sk0b56SwWjZoMCjQdHSPYku4LtTNmG9WRuXVYQBfJcyqgVNar2x10J+evxDf2LulZnV1RP6Z9mO4Qh8CnunR/LTJ7yAK1qFH6hk5qB5fpHLDrnI+/D4oTtBMy1Vl7quASRVGupWIAYjQob7WwEtsmjqfYcQM4RVYyr01M44HkylH6xipSvorf2ji+1cdr2JcUFvtB9/PXtE8vI48L2Jlr34o0K6L56wVC2aeFZvmGIE9B+K2eYCrgmt4Gb1GsflHlXKFni0GB5OHpBC23z/Fcxxa418mrH8oKVnbwbf06MULLBQlAAN9FsXFdaAUBMlO9dzvEEFYeObHNfMoVJuygii9Grp6PaOuJSQZJHanyMO4QQ7CAAbwxpsgUVMcF4M9GdCuTvHZtHUx82vmLKTlguaha1umtMAtn1RSv6AOrT1IuUbz0Hy88pw9SNWGy9g1bcuLisL4UtC1lRDDG/wDhdhr70DO8TGC6jBcQ7MTAoYLS+f4m83/TMM58RC+v0QwYK7bh0YoY3xm0etRq/lKFTpBY5SFgN9PEbT219vlHYiKHp+bFhYqIirVtlMvuUcsOIPkx3eH2YwhD4NJ7p0fyiIU2nrBQQO08RS7C5Vuo4tPuw+PvnWGbZXPX+rrowbBZCaVBUVgU0Y9riDnHpp/j6x4ICFT6XPpMfbjTv9j2gD9Rr3+47wBr01/z9e0IuG5QcP5td+0qAiGczGvpfPaVSBh0DG9mk8d4y4h1XKz0PmJtDl1WNHhXjtMAq5pj5HN/3L8M3bD6KlAxc2rl1c3/AFBnoc1Y58K895W2sMVVv83jvBosC7VjD59b7R70txTxrxxKFwkt+sdztCDBEAph6TaMTBQa508sNNYvKVArxFXvcmvCGNO8arDparr0XEi245q6u5vF4aJa2wrWubo33+vMQqDxMW255NOi6gphRYRDCr9dV+yJNQBw1Gj2KrPzQoU0tHkOn0alKwpJU70N+ef+F56+/LxmY7R6Bbjq731hr8krRbviIN1/hhQd4jtVNxd1Y1BIxOqpEVlPu4jo914gnt3ymJv23aMbfd0hY37TtGvHtO0To1FV60EXO4WLM8F4fZiwgw+J7p0fym8HpxSlaj1Sk2LKtlVmtQc9xp9+Hx986wHNZG6D+rnfaDHHBTXyfnqPYtQWr2+YnPJsyr2eIyr7EF8ny3GXfHDq9q7xh4jh/lrfaZGenH3+O8wedsqrXfnjfabF6cN19M8d5kd0yEzvdtfMecnHiwxp08RULyVt3rh3f9xXZu1WHUaqOmW59Tu3cXopdY20aT+4WJ6E9TtsfEZjbZl1ftc9oxW8qKJk+k3rv0lBgq77rO4uzzfSBsrJWjSvDVaz46wAF1cWz66WPbxGrW8UK08NbsvfpEMXwW1l0Z7+bpL0Jepaj1l2gqUApKIcVNMO3ViSCwR7zSmmNa6xlrVhqK3FXceJewIdz4DHedM9ItvUhDRx8jDBzsAKUtqltvm6RuesDcbTT0mP+Mfe3g2vE05YswIqvnmbac8+sYt1+GL5QdwT5evp3BD0lPJwqAKBa8ZmUZaZq6gWPMbA/Up+cX4a7YHVSh3I790L5r8QbbPWUuDMLdoOX8xAXafteIwYfAvg906P5bIl9qNB2+ZeMlvadk1eMws5umDBGv34fHjb/IQisvoC32fCUbgS9j3d3rNhts0P6PSbgbwZf6cblgt0VUcfh3x0g8uhuY9zfacxtN7vP3HeD1Hq/wBPWO1Eu3Gyw0rv136Razo6Aw2+xm0dDWR6QdyZ2WVrwa08vaJwNmTWWDfA7ymuVx7jxGyvKZ9id4jaWcbPk4eP3G3k0KvJl19yPDOEwO/d1+InY4yEaf8AB/MtIKiqXIYox/tzLgxahLi1y8fqXF7lj8rz+pQbuaEpty7L+nMd4aGZRAsD7oZGBBCMWPbbjXd4NAatn3nWMigtaC9JCadmHZCy+1qNOVa5bCNfY5h0IKTYOLT/AKqgWoiRWOWfS+SLpqraHUVWvfz/AMXo984gerMLiJ5xLQhndSoXfuFfZ4mA9OIsNNdF4mHEbYFUGAy5PniBg1MO1PWufEQsoLHgzSKjx4qbcZDEZ4YPn8owb+0IBmBLr24cxXZrkjCTB8IWqQqrxzDVwAy1VvidlnmZPE6m4vkT9jxGEPgH4O032H8uN8hkHRMcsSxxxEW8k08was4ftNXvw+PsnWaQA2FJnlXQ76kKwaLgvc/cQ4rVYOTsi5btznf9hir8Amc7aSKldGzn3dfiK6Zo1lx2+/1gR7779/t9IrocWQbKw2+z9xwWbTOnPcffHYyoWsgY1mTK23e3b/SLB3wt0PX4/UbKt2l39veXs07Gr/0+JZBt77FYf9v1KjdLpZvL/jL0oosow7/b6xlstCrZx0P1fqXSdio0Hdx/04ipRZnUWqGPPnrBSypamWTQ17MCYhemA23b5XniBO1O43xvfbvqQkYqwSDJdgdjxAzEobYFnJb+brFF3TNTfV6DfzdYkIlnRFuXLs3CesOwJzWtZdY6SxYDSrpu1DX9EU0uDaPG21r5OkyOAaytyr9R26f8Pof6wzcOuos7aO0KrOViopmOhzj97xCw0sAJalQotXAMvy5l6OxJ36VwhWCltsGhEeRESONCCVWcnrxfYesJY+h0BDBbgNgYTzjTFabS88j0oeAji7AOVOw9XXaOj0wVK0Or53ekXRcVxXWcpn7HiLD4BhuKexdH8rSouS8F4ZYbg2UBKRbl2yr0Lfaa/Zj4++dZsC5ky+7jr2g1ZqxQvHb8ntlVDFou8xGxxXXETRW5OrOXPv8AKA23obvHu93GU4fOe33+kSl8O+Pf7uc/It8o46Pu/UBdTIWM2Ybft9JS2booUca88Huai9ueNv2R3xSgbiw8h7yyDe1d0+XXaApBWM4efe+8FAUeVaJxag7eZlFFqtQRGH3EWHA8ve326TKy8A4V3xq8HfrFzX4re2OS+49+sowhaEKV3ek7eOkpvtu9IiXa1vnx0jqhycCy3NXaeLlI5pxim/N7s/cIFrhJoq1N95xdxGK7Rand7aY3rpFvKCIHcdtpkx80K2WXKRfkoduFQq1q0iAB6qG/C4OleIttOBt2+SBukJl0zesYfwhL4uDDJp6+i77f8O7imx9cEHF95ebZ1/mKYy3DoOYsV23iPf6iugpDsBxlNafawLxcc6a+CutwHwITjvSq/KEScn6KT7MrbxCrcpejgfEVf0Dr/h84sAEeSj0G/NPETXMtj6wWqfpK</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAlgAAAJYCAMAAACJuGjuAAAABGdBTUEAALGPC/xhBQAAAAFzUkdCAK7OHOkAAAIiUExURf//+wBRZeDg4ABccdLV1OXm5dnc2////+Tk5P///t7e3s/S0dHU09zd3QBWbgBabgBTZ9XY193d3QBUaQBWawBbb9/f3wBBUwA3SNfa2eLi4gBZbdbZ2ABNYdra2gBLXAAkMtDT0gBPY+Hh4QApOABLXQBccgAYJtvb2+fn53BydAA9TAAyQ9TW1QBDVf/+/wBFVwBecgAxP9TX1gAgLgAtPQAcKQBAUQBUas/R0P7/+u/v7QAnNP39/enp6AA6SwA9UABfdAA1RMvOzcnLy83QzwBNXgBgdwBJWwBJWABke21vcQArO+3t7dnZ2fDw8AATInV3eevr63p8fgAIF9fX1tXT07W2trm6uwANHb2+vgBHW2VmZ8TFxWprbTc4OsbIyABBTsHCwfPz893h4LCysvv7+vb39l1fYTAyNICBg6utrT0+QKCho+Hk5KanqVZXWs7NzkVHSZmbnc3Y2NTV2X2bqE5QUae0wABcaYWGiNzS0Zyuuo+mssna0dPa3wBUX9bj3+Pb2Ojg4uXc3/r//ouNj93h57K8ye85J5KUlsTO1sba3OLS2s/j573Gz93o6+Pu8yUmKGeRnLq/yOA0HI+4wK7K0dbr8bbZ2u/h52meqKHCyn6utu/Y3C5yfcLg5AhyfUt3gd+Og1qIkTmAi+NnW+iyrNzFuutSSEeQm/D8/e3LyOh6cSZjb+mfl9pNNtCrnRKGkiBWY8hlXBtASzhWTvIAARcySURBVHja7L37U5Pn1v8vkRwIBCBAgACBEJCwA8gZUAiQBBA3BHeeDSAMz3AMM3XUYWyd0sNHRK17arfFsaNYtdaOzjxTZ/rD3vP9/77vta7ruu87IZ7o7q7qvfCsbfcur671vtbxyBHTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPNNNNMM80000wzzTTTTDPtg7MTppn2B5j5X5Zpppn2HlnOn2d/5j/btPf6kzs4SN/gOzL9V8QPtB+aZoL1dnZi8ISA6gg+TvBHclBaEh/mv34TrENZErYpbI1senr6JNnUVCKROGl6rA8aLPsfaIPJzaTO1bQwgiqRCIeb1uw5dtM+VPtDwbIPbjJZazpXU+ytwFXYagVZgyZbJliHsJxkurtSXDVZrVbvtAmWCdbhydK5Oqm8FWHlcDg8IMv8FJhgHS4YalydnGZ3BazAlcPqCHgtzs0c02WZYB3KkgqrqRR35fV6AxaPK4Ekl8mWCdZhguFmmmg3cOV0B61JuwmWCdbhZNbatAqCIgoyVcDKFXT54p5NM+tggnUosOxJkbwKc45B91auYDAY980ETbJMsA5p0wldtDsYKw+w8sV98fjMzKx7kKqJ5qfCBOvtBXyiSYorryauwFWcuZr1O+yDJlgmWIexTcGVQ1LldvkYqpmWllnY1pTdTJSaYB3Gjm/qUdDJUZC4Iqz8/v7+/q1pu+mxTLAOod9z7GsOr4OxklyRuwJW/f2jo6Nb0VGQZZZ3TLDe1igHuhbwethduQzuClhtwaKx2FRO0sxnmWC9dcYB0ISdFk4xKG81S95qKwqqwNXyslmQNsF6e49FLmuTRDui4IweBdlXkS3HlraSXJA24TLBeku47NM+d9AoroAVcbUFd7W8tLxqsVOvsiniTbDeWsAnWpBol+Jqa1RgFdsirMgWHHBXZj7LBOttwRq050zFW5AQJXcFqkhZkbhaWlrFF3xdCNvNTgcTrEMI+EH71OxsHlJXo0JbLS9Lb7VKtrC6miA1Zn5OTLDeOhomKSE6qzQ7UyWhwgeMUvDm69AE6y3tOHIOUb98Cy6zZl+SWLGtzi9M25NmQdoE661fhjk5gVh/VERBPQYqm1+YX12zm4lSE6y3BmswafcsqyDIXCmihIGsTbMgbYJ1KLjcyzHNXVH8Y7I0m1veNAvSJliHSjvMLCnRrsVARdXc3PzGsjm5Y4J1CEvap41RkLmaI6Skzc/FkuanxQTrEALeHl7V/dV8Klbss2bMwR0TrEOZTyorEQZ1pMSP5+fNjlITrMOFw1mNLJ0rKbJgG0tJsxhtgnUoAe9kpsCWwV2BKPqygWA4aoJlgnUYnTVoH51nsNhHbUhHBVM/9pk5BxOsQ4TCQXtCSzDMpWIlybKCLFNnmWC97ctw0N4/t6DA2hBgMVuCrvm5hYTdzDqYYL21xhrM2VyY07HaMJj0WQvmSJgJ1tuDhUSVdU4KLP5IQYvzpKvTZiw0wTpEOLQ7lbpisM4JpITLIrbmue/P9FomWG/rtexW9SY0uCrlsSj/sDplN9MOJlhvr7Pssxu6xxL+6tyGkSwoeBMsE6y3DIUQ8MkllRTV4uA5GQuZrvklc3eWCdYhnJZ9bX5OQ2t+7px0WETVPMfChZlBu1mRNsF6ewEf1kIhCjng6pzQ8Gh/54LP6mqc7qKYnyYTrLcV8O4NidbChgyE8F0LoiZNYC25zAy8CdYhdJbdL96CC/rTcH5eCCxqW8Ycq9cEywTrEAYBP28sF6LMI1Ok7LFWl2LWHHMXvAnWIQT8goiFspQzP7dhBGtpeXnLHJA2wTqMgG9KaUye07JYAqylWLR/2uwoNcF6e51ld8/Np7a9p3ms/rhZkDbBevtYmIMWmvn09ixNYi3HotHsijWTLBOst0drMzYvxnU0usRcNEVCAiu3ZX3T/FSZYL01WTlrS/Mpo/aCKw2s0eyKC8lXZR34CvFx87NpgpUu4BNq48y8Nhe9oIdCv7/K2ZTkqJmCV87LsvJmtt4ES3Bg92ij0XJ+h4Iji/dYLJqbV2QLJAYN2AyS5YifJHFebGrq5MmTazhAnRxMJnmXLsOVwymwHPFTLjqawH1UHgu1nZnVtKVGmsdikVVk8U6Jy4e4X85IiXN1CavD4nG7fbCg0+twNE01hafCJ6dPrq3hDyZVo6Bg0fRjHx9YOUn/qtzDxnStCq4o3cBk5WF7aUvLTDzu9gas4enNtUSTl289uXHswun0gCmrtamJTow1hfHRFLbi3hiOjk1Pr60RYIMSMFOJfVShkE5XROXWrKVVxdcqq3fe1h1bJsSiW/2zMz6nMxAOB3BAxe30eLDh2+fxNjU5rE2SrDADlWpTU9PkwsyC9scFlhDw03LdLSFEaNE2Zf6qjMgazS6yrQdw48IZdHkCnuBsiy9A15/ovCb7LIlWWCdsSpj4IYXIZHIwR1dhpu76wMHKybHGRmnnLe3pXlK+aykmvgdT/uyiCpvN5rRVtfj9nT630xX3tzgDdPnJ47EEAnQL0comImITA5YAXPgydZLkPb4yZyenBV4yUWFi8CGDBaHl2urHRQG+WKE2dbOniiH3brNVVHW25PlHsSF+NK+oKuibHZ11B5wksTwAC2QRW3RkjFwX3Qjm0CjwCrPjOmkwegcwXabH+tDBgoCP99PpJnyJqg24+IhmF1V1+vujUeYNmOXmZlcEZ7f8QVzngQmwCCt84ZCIL2TCe1llZORQmFB0TQs7OYVnZtIk6wMGi9Ofm3j64cZAbm7/qDwwgMjoz8vt5zsWy8J79ftbKlqiWzMeV9Al3JV0WV7htHS0hN9ykK4Pa3FRxEKdLv4RXo6DKi2RY+quDwosIeDphtNMdnYuySzCKjYq3NeyOIsSi+ZlZ1dUjcZagi4fwCJ/5WSwGC0LmWBLREXNeTFlmu5KGCKjpAvPRiS++HoBfWOC9SGBBQUfnvHFZ/3RZaGtYhz+lkTeQQj4zqKK7NhoRUU86IoHg0GXS8ZCEvAe/t7ChCnnxcLLQWfO8XgUTkynS4uMUPPItk5x+pWzryZYHxBYdFQu6Z2ZjcZE0GMvJTLwDNlobl5nZ2fVaLTKVoErrS5fMOjzuYAW8HIxYkJyKQemzKsCJJHlsCrf1RROCYxSdU2Rppc5epOu9x4sMHVj0D6YnAp0RrUrO7KsIzocCKuWluyKoqi/oqKqoqqoqsJXEfRVKEMiwuaS5uboaLHodAXkm9Ghq3qRljBkurQHI/2Y4aIykN28ofj+giXylMm1sK1fqqlVWdKBqqJ4iIdirj+7paKoqiXWCawMVlVlIAsWJHO5AZdbui6PFhx116U/GvWomDCyhZ8KuCgNYmLynoJFinkzYfPHtP3vepWQqMrNJaw6i0hedRqhKiqiL/hapPEVFOYSkdEpTOLlsah0l8aXTpfMdbHvwpcE5eqnpjdNIf8+h8KcaU9uTHU2iODHOXhQJbDKA1dVRRX+WBEHQUlVUUsLvinqJANaDBf3OQQ5ILpdBrScBt0lA6OmuKz6i1FKevlslGyZmLxnYA2yjsHlVf+SoVFGUBVlI678eYRVZ0uRzR+l0EfGPLUI07kqqpKOi0KiK+jSNJcS9RZddxk8lyAMFg7ruVSKjRIuKK4kay3zZvV7ApZQMFN+CdWCSCroXEFaEVfZ2eyYKkbBVZHEqrMlW5jkqkgAJ0Ok5rk00wOjrrtExsshsvUOrQLEr0WRS9XejMRWTo65rut9CYV4dK3Nsp+SvmpZ81VU2snlKEhOCUUdW26Mn4MwkERcKX9V1FkkwTI8ERVY5LHU95rrknwJt0Uf0m+JGpBMdIlEvUBr+iTyEGtm7ed9CYU4MscJdXJUulhnI6b8MgpSoINur5JcVYEnwqpTOquiVH9F+PnYY6XDpbku5bx0zeVNfy82yc4b8V7kLNeU1FsmXu8yWNQ1Oji1RalPUROU0S9XM78/TwY68GTrBFcs2EmyK3VVpJsCC5nTuBEqhkmXWy5Cyu1OyaWmaC79qdjUpHV1iYBIaPE7Uea3THreTbDsmy5OU8Wi6gVI0c8vTQooklNFlLqKtrC/Uo9A5aw0KV/FyspW4dO5SjGiiz7cGlbSb2mPRY+muZTTkq3O4rU4paVPRfLU5OqdBAufl6mtJcPrD8FPhD4lytklVakYN+qv6FQMpfkpPQSCK0200/fkoTKFRMNrUVfzmuYy6C2wxY031B4RNqAFKW+i826CdTzpAlZRNPWxosLzz8/PP80ILs5YsbLyR21V/CIskglRyVVFKljksQxgGSFSPyZHpf08Q2lR67zRCj/MFfsvvWhNIdF0We8WWDm8MHnNv7xFXBFSRFWeyBxoyakWLc7RK7Ai2llhcFeilKObwWFlFO2axgrqIl7l5t1pCXpR+RH5UxUUm8hxCUWv5JbKQAyaOYh3xmNRK10YLchRwZXfPwvTlXgnWrJmRMYzXhHn8FfR76ea4AGQZDCUUAGroM2Xlr8KZgqB7NFEMxe5r9R4mBIRBVpNiixuR5X98+S30H3K/5mY9i54rBz7oGU5thUTWGUTVECpSoa9dD9EP5qJptSdJUUpv2BTZehgBjN4Ls17uV0cLX3qpSh757UUqp6CEC30wncRZUrJi/ZAc6TsHQELgWMzDske4yjoJ6yIqxlb0CZhoYRBBZ52/GNuXxjN8/kqKtJREqaBZRO/ZgRJD4l6vsHguYxJiLTUqZrO0LNbKCpe09ttkN0isOhjas30WH82WDlcGlybXUYQ3CLFPktgzcwQSvSJps49kS2QXQq+OOp/RZ+OXvH54LN8BICCh6GiV2AwLa2gwJHfZ8xnBV3Sk+mZB5ehH8Iju1F1Ka8mf1TBOqweidzWDLdFrYGm5/qzwBokPTIN0U6yvd/fL6nyxfGpl5/coILmU4RANIr6vvwy3p8X9O3G0YiMUULX9evMQZC/S8uqG0OfQOXA7/lchnQpC6w0S6snGkrVMil/TZSrCS7Ve0pC3hwj+1M9FrgaXd7aEvJKOiuf6MyTJhzRFRHmfL7dn/55fetT2C6M/BX3tQMwkBh02VIDmh7vVF7BnfrLGeDLCJZQW+lkGRpt1LSiNpBhdtf8qR5rEFnR5Zh6DGpc0eeTPqkU5IiXIBYy7O5edzhu3rz588/37u7fvnrV44Jj8wXdrqvCbFev4NvvbrvS4NDZ0n/NqNrT4MoYCqWWd8oeiEAgxW9Z1UNRdNjwfDWjtWYWEv8EsER1bRpZdlJXlGOY4TDo0+rC+Jy61hHqfFj74Wjau33r0eO7z58+Pb3T/vjeD7d+3t/fu5MIX/PADfniLLbcNvg37DACBRoQznTIFCwZ4TMkTdP9Vkr+wXIgIFo5GS+bt2QlUb4RecnSoAnWfzEval/b0tyV8FeahHbt0qd4/cqVoGdv7/aDzy8/354IhcpDod7eieHy8tDKzm9Pnl3+6h+3rtykHOWPP167dn2Xw6MLTQr41DsN5n6Jqd9zSQ8WTGvYSq30OA1gGZ+IKm0q3FYThUWVfgBhSMjTSjgTrP9mHFzrp+cgsgyzSrYHNTmEGIg33vre/oN7d5+2Nnd3RMpXWicmJsrKWtvaJlpXQpFIR0cksjLx7yfP7n79+f3vbsODTSWaHAHakuVSzzknp6JkIEuHTPu5S3dcRs2lIqbu//R6TyC1dwt8WR3a0E+TntriWo9Zof5vgmXf9CN5JWQ7cUUCS+gcajnYDfrW9/Zuff3LRCQyNNy22Aprw9cy+qa1rHVx8VRNzcTEykqonAgbWtlpf/Ls4b1H0YoLcBhhh8XNdOlTExY9lL3Mi6X002g/CaaApbRWQDdjbsshHRgXeyj5sIbclonWf1Nj2TdnYyJ7xVx9+c9/Ui+L67rLBiWOmObd++7xk7Lu7vIycFTWGxoaKo9EIvhazjYUorDYWwb3NXHqFDzZMP1+eW/vzjZi5L373+3fuZNAeKyqCq47LTdvegPXhVks6yT4RYx0psssV7qwT++TVy1bhqRpQG9pxhereihSiCaygBY1yXND/8er5f9bYOXYkylcwSoYLBsGmYMVrr3bj35Zqa+P9La2MlMKKPrhEFlI2vDwMPBCfJyoqakZa5iYaA3Bg3WEJn775fK9B7f3p0l9uXfdTpvt6jqACkjAPCI+MllOY4eDETCZpVc/VjI+vbNGkeXVewNBF/ksTpeuUWKLSz05psf6wy0Zjyl9RTWc+KefIpcedNuu2pz/vH7n9uPTHQPNCHu9Q5InBohsmFhiEz8HVcoQLCfGxqqr68ZqJnrLmzsiK9tP7oKuvcSPPyHLCq5uXl1fXwda1655DIVA4itTXitjm42TS9WGrTZaAiI1D+G1qiVcCIZriIrUVzNoeqw/2mPFl6MxruIIeVVx5VPyWEGn07d+5+fH290doda2FSAVKReeSaMHaPUakWLx1cbKS9riYnVdVmFxYd3YqTL8HSa2n1++fxud6t7r13/6SWS9XOu6z5FkGbxWKlhpL8a0Uo9q2tIBk8tHvFY99SCWjLDWMsH6Qx+Eg04RBxEGs4Vuv2ILQlhZ3Nebbj/cgVYq6x0iSYXEQghfVlakTxJopfspZXg10neLi4sNdXV1WVmFsLFT8Hor279cfvTdnakfr+0ioLmc6zY1OyEdjyboXa/qhjDWqvFnUzZBBHRBT2BZFFlqLaWW1/o4dfx/Byy7d1n09M1KfRX3uXzIrbtte3tf7SCEta5w/IOSWllZSQNJkJUBrAlhNWNjY3U7dUxVYWFfSX5+fl9h9fBQ786Tu4++S6z9yBkvkkoCLGcqWJnIykQavzkNTisFMqxwZrBkoUftr8HXpN0E648T7k1cddb01Qwn3HctFVf37z/piJSVrZRHoKpWeleUp0q1zGBJrIirnZ2srOK+ksrKgoKjx44dA1r5pduFNStDoR14rtvId10jkNI9loTLFcxQzE7pilDprdQmeW3Eh/1XwKuN9qgFNifXPt6umiP/Da4SGJqQ+SuRvopz/6Zt7+dnkUhZKxIH5SEOe60ZwWIPxtksqbGMYDU0VJPBYRFYpaXj4+Mj7e3b22DsWPux/DpkvhAWSXNZAxQNPTKJqsOl5x+MUBnNWNfWytRajsvp0cHSllLKeUTs2pqeSppg/RFYDVKB0BgHRQ8flivceVTYsYLkQnlI11StKUil/bRMU+8CLspoLZ5itBAIi0tKgNbR9hHY6XGyEbaS6sWyhpFfHt+/fSfx4y7nHvBeDFynMpALXoxAE804eio+tbFQ9vLgK2VHOF2Bv46+dROqTg89Pb0XLqh+LTVGDcYSOKIBFc+7e7Xtph/DjtM/HCxRIFTdosxVMI5ez90Lt59FOspWyFutvCQEvtSU14LHQkKewUIsZLIEWCPjp5UxXgV1Zch0Pfvqwf7e3gVg5PHgqQgi6EcejyzxGDu4fNz+LFugReshN6pqjsvjcarvnevCiK0LqqlGXjJocuA+C7KmyUG5VCTnI9lweuQPj4Ob/THZ1cf1wSruk3FW3Hmw3RFaoYw6yaeVstb02PdKAc8VRCZLgkVvQiKr8iiTxd5q/DTwGuev+GakcqysbAx5rp/3E03XriPNxftKOZ6BFg6Kon+Lcw2GbnobN0vb5BCQ1GMqF0ahcZ1cH/MltyPpi2tAlreJ42HK6/DDn+z5o8E6nmxZ7t/S/BU+QT5qubLdubfSgbrf0DBl0cs0AfUWYEmnlQJWcUllqSRrZFx3WpohLArJdRX9EdedNir1wOdQKNML1MJrVegOS3ThS1OSnqSW7M1wEmaSLJxjoUei9Ft0K8rq9QSs02tTuLWyRpuZERs/hgGMPxQsanGPc6OMX8szBONBfEL373aUU069VyqmlVQ1BYaMIPWmm8FrLS7WNIxViywWuayCUqB1rH0kI1hkx7JaOSp+t3dnb70CYslDBR9+3VEtUaasXGpQI3hwjsMwzFFBwstGdXT6Vr001y3rXu8FK2suypwiJE5Pix3z05w6FZPUUnSZYL29vsqxO+GvAJbGFb0H8Rp8MhDqRYKhrGxCpc9TPFMaWKlvRO179lnksZgsBVaBAIvVO4H0VFdb2g8KqtvK6p5cvn8z8eNNl4XkPKelZFR0yVZpRkfTV2lWpSZk8S39GZtNnxzCwZ/19QsXWHNRpSfcZCU3Jrpr+E4U+S7uCRw0wTqUcHcs90dH/dTeLvJXcfoPfO/+Tv1wiLlaWZFdMbpngt56KVTamxB/Qa/SWadqlMcisvLhskoVWUZPlebA2ovbhlt/u/vo9v4dx3W50IgyEKIVnl6BgqygQW9JouTUo/BotAaAwaowLt210XPT5fJcuGAhkY/AKZrnwRYluNACQWgl7YMmWIcS7uFlNGBxw6jMX8EVVO19HqnvHS4fgstpW1mhrqsUb4UsfFkaV+maC7VnKuWwcCd3RWksUdABWPkSLJFzOBgKdb/VXrJY1vbvZ59fSYRR8pGtMTwcjQ/peviNaEvZ0qy228hp7KoKsd7GMPYvyGLfF8ehDfp9UVAiaS/6TVltra2ZYB0if0WJUZkWRRzEDlH6F7zr2r/cEQmVlw9L50OgrBjkU6tWIBweDr3ESJohhdUAnpQVMlbIvlP6vRLhcEQ9C19p4/kToZXtX+/9fCd8zcUK6/p151UkQ3ZVuYe/ypTpy3ZGGLHTViq51texz0tbuhukghCR5eAuCL49hsei2P+Q8+F1QfyBYGGCUPgr1lctnRDuLtv6/rN6cDUUkunPVgqHrSL6rXCjFXX5IVCK5pmhlF6sFLiG4bjAlngMslVWUk0HUMFltb/8aZjOVkFDKPTvZyj87K27r19HUyC66K//5NYHHX009hpUMTHDDgkdNbV/orMCdxXVbmfeMOGjd6QnIG4qNgmnhQwXVRM/SBH/h4E1mLPZH+3f8qs8Q1FVfDdo27v9ZAC8cKZdeiv+2ruiQl1vb0i1ZA3Jxr7hVKBEY5bs0AJdDdw0Iwo6BfwoJDvWzi/DNLCeZmarb3F4pf3ufcgtJ2IYuk5v3hTpBynlJVhqoL8qgymAxD5n2kJY4bIptrAkjhLDlKe3cC5CFKpJanH29APUWkf+MIeFjtF+0SjD+asrmBSc2Xvw2yTc1VCvnmmHt1pRCkpCNVQunZTq8DsYCvXeLH4bnqJXoajpcLaByTp2bDxT0uGpwCsNsfGSU6HWJ5e/2w9fu05u67bTo/Uxa+vb1KqIdKj0X5MarLMqL5fSD/y0FGS18IvYzRUgp9PL0xcJumdHT8TpD6+ceOQPgYpm6V0xHpxQeYYrQWfV3v2xSVAj5JUmzKWzojEJzVMZwt8Broa5p1T81aJeiDGLBsqRssjKZ691jKy9Pb2+8yobqesdmnj+1e07DveurUI1JLPfkoXpijQRnw6ZOm0AkrA63Elz2k6XjTd7dWKnHH7b5rK43DOxpeVZC/XInxQPxLU12rXFR2ZzTLBeFQYHk3avwV+RuW9e2X+00i24KtMrONQqQ85qRQRAJiedo0wSS++gmUAZuqEaX+pESOTumdJ2YQKs8fHx8TeRW5hlXGl/+GAvDPHu8bg0sFTfQ4UvxWOlLqzUXRYcVG40twjZLBcaDMllYX04L5NDFt8ddsxi+3jU7XM3ib0i5LTWeNn3B5TW+oPAQqJBLSmi/BUExnXX/uNQB2ev+DXIan2FWrBClA0NCWf18vCXbsLNUdc7eayGBgarLouLOu3tR1lpjSgTXB1A6+lB0dW+3TZU8/zRzYQ3aPBYhmUlVOdJB6uoSnyoX6aNhFX90RaQBbbW+Zo1rb7spNxEPGht6l+NLfdTL5HPmuCZMXohcs508LgJ1qsSWNN0GVWs/RD5q+D1va+RZgBXva0aWFp6KkS97kKtp4M1xF8oOKY+EfXMFrkt0TzD2feSyoKj0lMZsRofH3kjtzU+Xlo9FBp/mJ2wBl0eVlraahF9H5fwWiggxo2rdkmoE26gqKiiM69/tBM5eCfLrE5whWuLRfyvw2qZW41tLS/3+5zxrVlPEystklprH85mkf84WLQDK2cTaYbRUREHq+Kf0Q6r/YeYbUYcXJGtDIqqFSpFa7NeQyGJzpCIjMb3oYCLfqZ+g/6GPA9GOdNFGQtZv7ePiDehQkvB9UYxcXykr3U469f7TT/+hPZpJAnUXi40zbhl719cmbZjXj4I+RjLaIxSp53+0dwWIgs6C14sm1dCd87gyobVtrBQ4fVFY/ELVlf/aNxrnQJYPJG4meQ18oPve8/WfxwsePMcPAj9o6NqIAf97a6re3e7MSsxtNLL+QWJFcl2zE4AqyHxoZySGCcU9DTLX2SSYM3NzZgj7CbraCYiaVRM1HcoHBYWi1wW16FPy48D9jqvNVK5WN775N7elGWXWvPd7Hdshj5AhouKVJq4qhJpBXCV519dEq/BFn+uv4hlVkUnuOJd47gLVNUZWN+Yj7kSRUur/dbpRMI70z9rEYUeiK5NcQwqx/RYaS5rMBilThk/6ysk23fdV/aZq9AKlY5lMZCcVS+Jq4jRNUmGQtovRprV90zTZD1sYGCgfhLW3SHRCg0LvbVI2fhC7p2R5UJjJeeN2eLAWVAdWhl/fDvsCe5eF119Qb17WXdbRrDEjR+/f3lulaMm9j1n547mdla4nDYOhgiHuA1ExzUudM7NL9uawq5+yHj0Pkw53OGTPEYtBqlz3vcTBf/5UDhot2CAEGCpdX27u7b9u5MYlue0KKWwJFeUjgpxFBQRUMNqiGCLCGumKXs4qUlGqn6gVhrIIp/V0WxAC1oLsxWk4AtAlsiQnk6p67zMcT09SBblTYcj25d/vuPYvU4lnuuk4pXX0uNhClgtLXn+3P6FiwtOVmNxyjMgR0zXOwVZAIu0VktVYH1hIZq93pTwjq4u+R1TNORKs65r6mpPzvs97fofBSuHuQpzAkumGSgrCK46yF+FxEOujLLmYlSe/dWQJKs8JJwWcyXWNmDDTDNj1T05oCGlgzVJZBFaJN7w92MVj14H6iUtKJXBcDy1YqhTdVDMjxuDIf3kWOFKpPDhz3e8X+56sJ3yOtqu0iZ54nr6gdOg2Xn9udG58wvrqsBIysvf359dxU/DvDxxfKOzKHvdObex0LLusSaafLNhfckWDY2pCwXvsdf6T3usHK4Q0oNwRj4IXVeEvyoPqfR6Lz/5EAeHh9R2hnKDVsdPI8pddTQrZ0UwdXV11XbRD0AZx0Iiq1mAFZJCi8YM6woLqX2GfJZAh9yPcl2a5BLPxYx16nH5506PtOcvRsbuPkBLIPofIORtQeOYmEqaVlXoYOXmRje+nQ+oP0eeqwoyPuovIqHlz8MVYhyfwrWEC+ujfhvq0kBrSl/xzUbfTyWQjx80wVJcUYVQJBriYs5rff8hhbNyfN57pWwXXHGlecgg0zWTVJFKb+6WMdDgrIitAf5Fkln4YyIDFuLWPx5gxeuwhNtn2nV6UtyWnOLhzviMXRD0F4h60EhxWccE0Lpqo6Gx9dSNgD6f6l/Wwervv/jN3LoGFrcDVmXnRqO5/k7EQ9yfIhnfUtRpC1CzvId6TK1qoem0aNXiCf0EBsdMsBRZLTES7tr8oG9373I3sRKSOSfxEKSwGJLuSqUOROzTxBXtkAFX9fWp2krZgASrWYI1xCVEkTFF4x/NrxYIsrikM64i3bjBJ2lwjWSoV2t/fmSksKy5+u53dyxBD4HF7ctq75HP2DAjnoSj2Rc/mbPFg1rui70WJR+iUT//EQREf3ZnNq6aUd+WO3DBwWsBxVlElHcILM7GJ97fGuJ/VmMlc9ycGcVg6pdY/IEmpF1qv2pWcVB0JbC+Cmmbr3hlkYp9zeIrtFUHvBEegQh7B6ACVgQWR0LpsgRbw2L/3ynR8IDijoiH7cIvZQp7MiiiYG1UYynf4Ve3q8siOw9vT1/bdXkC61fXXe6U9eGs45ksehT2Zy/8z7mWlgrR2qw8G2UfyG1Fc4EVn2NENMR5swpqYw5gJrFJrEGaFsVDeCxkIdxT763L+o+CNWi30tFBf8sMPwhn4i5M42D9Hj0Ie+VjkHLqlFkfItwMrz+KfJp1RMBUR8ekSC3UZjIZCJV4F7mKkOpXPlWj+h1QOOSYeLS9vT1z0ZDA0n5LyTBdmPG37ds7vc07l2/fWcceE4qIqcsmWWtxzp1jYe7587FRtGTZ9GsFPtHl0JKLHfejdI8xD1i18JFPOK11bgDUroslElYLTVq74l7TY7FNU/qK4iAdLZnZDVbsfx7hhHsvZ0aRauBaDb4pF0GvPJUqxoR/UD/ZIaLggLIDkXBSPAqNYLGE7+XW5VNyKIwnLLirVLRqGWuHChtD3Sf1d06rYDjSXpJVE4ps39u3emhJjuemO40sEQ0BSzbyDf6F+eV+JsvmkjVsUQ/CBWJ/P9hCkg/5eurboo4IRZaYQwx4aLENhvU9rrjF1Fhkmyg8b/HmD/RfVXy5G9y7H5oEWEPDIcGVVgEsbxb+KtVZARJBFlxVx6QUV0pkGcmiDKkCq1mCVa4KiXLjHwbDGK5qbcERdT6UFGgt8QYPNZ4xNz+uf5AU296ZGGp+8mj/AnLx1y2qV0t1mYqWPpFwGI32Ly+s9mfT2I7e4izmxZCOF2xF+7PFjVgevnCKnntan+p10ECiw4IiuNs7+NGDhVaiZJw3yrSwx7pSFfTdfFBD24+HeHUa+vlCOlcdWgiMaM5KGtzVQH23RpQG1oCRKwVWc0Qo/nLVHSE6bUTnA+e1Fk9xWw0AY8SAV58YEmPtJV+NGeo+pxVggqzT48dK+xpay4eeP7jj3N39Sdykk3SptAIVCyHfQdZojPKfRQAr7fimUPn4M5Bb5LnykNOSfVw2tMl7+aqr1yn29Fq8yY8eLNS3nNSCxZMTyLfHncGbt/9dj0hIGateLc3AXNFibUMATAELD8GB7u56FugMkEgsGD2W/HXhspoFWGndD8MiZaYtAARhWImLBptqbQSROuTl3LS2RmR8/JjevjV+OiVvP471SHXVrc0TD2/foUy82t4gPBI3PtDRTo6FICu6Oh/L7XQZd39rEz9VVPzJo2eivIdNl4vzWmimTBytdslNzSZYJNzhr0bhr+CwqNjhurn/ZICSCCtqsnlYeJMh2haapqx0A1MDk5MDxJURLBkK1bfq10XFUCYcUtiSS3BlT6Eai8XY2KJwYLr8IuWli3etIUJ/JY5rIr+gOGtsorcZUmvdxyuRnGr1Q1C11HB+HWgBlqWF5dxOn9s4ui9uBQnf1iJ8G9BaXo6RpKdbxTaaubBYaJsN74HY/NjByhHC3T8Drshf+Xbd+89qAVA59/FRI8OwBEtxJYkSLksHa6B2clLnR6arJuvTPZaOlmhzKNf6bbS+rgNT+VT3pkyXGM0X8TGLlgCWUMfpiFomAqne3p7is0QFG79RWryzU91WXv7Lg7DTrV3EEGPT0hkhGBJZQKs/BqE1G9dPqhh7ukTfFv+5KJ9cH/Xn0QRGkC9tuJ1yA+XaxwwW9Q/hOsAo66vZlnhFlc3n/ukOCjnwJGpmkKgiEaT8FbGEOCm9lDRkGKgKaHz8DaQ4LM1pScAAFnNFsVX1c5FT1PuaVwzNg/jZyophS65Iecn+QEp6laa1CGoS7LRIxEPCl5YUYj4/MnZ5f69i95rlJvi6Tk012utQKnhyWrlRtCBDwmNjiFo6ov5YXGitljxBFqQ8QmER1D5P8vAFBN74Pf1ReyyanQhyPwMFQjqP6g4mvqrvoAjVq4M1RFcA0P9i9FcaWM387WRtVz3nRAd0sAZemnRgoSXKhc1aPUhgpOm5lbS+ecaLGqLFqE+r2ldTJ3WXUl3j0ntpHkum6MePVhZmnWpdiTy5P3Vt14njB/pyLfE65PkvpNeRBB3tX12IZXfaXIYzP1rGXvoslvHRUUqYFsU1sDw8NW31Tn3UYKEGH4hR/orO8FIhxx1suh+p76BP84rusKiTr7yZE+uRZiNUmk12daUWbwY436BzdlDAi1xWB6ccxAORHoUGH/WKvnkRLiVdGlzaKiQOiqLWIyBrP8qJVpA11tY21HZ5rym467rq4glXRZaS8OS00OngX15YyqXxVblXUst9+eSfy8smDQ/t7m8RyVJWV6ywsGfLG/6oM+85OENIC2VmZGuf233h05UB8lcaV+ywqCEGQUtT7N2pNlnPXHVRF0OX5rEGUgrQqd5qUiVJRforwjmtobLFxTZt58NK2tRP+nS1kGK0o4vz9SzqxcpJiooi3yXBwowGDGpsuzirDv+M8tP3E0iWoiTDYAmy5KoQ4bSoFwtCa7TF5jEcJnNpi91YkLHLwqMwW4BFxy+8vOaBbqmEBz9WsHgVz9os6oP+FjGS86XbjURDLecAVlZEdZAEFkmg5m71ENRoUobnYFfPwEBXl9Yco0rNup8Sv9Wlp7KUNJMZe4ityHBbdWFWXXXDYpsYXuzV/hcMpZtxKFZk7Nt4Wa6YyRCvRSnp29lfMViYt26vLB5rWJwIlT3c/xHJUs86iXhBlppp5bohKS0/Ca2WCpbkvL+U78MG1eMQ7Q657LBQOpSJUnH0Qp6h3nxP13n/brCo7T8ZH53Fg5DjYNXMrnN9/5ceruSEerXdHtzA16wAIHfVIbmSrmdyoKtH+CoDWXoc7JKW6rDSfB7cYaiGolkxsVXdcIro4gUjoYxk6XDJwChT9gSX0vPEFoZfmatSooqXjhRs71QvtpYNPb11Z532tq0r/WQzkEUKCj5rlISWz23YL29IO3SiL5761yhRypGQwfIqsBxr7+npw9/vsfAflHeLztHHuVWmyOdx7V2u7YaSGhJqR3xOSV9Furu10o3yVzJpgK9djV21PQofQyhUTVj8i13qOTgpAqHm8ITcKm8dQydWfkkfNoUUFxJdpybaeM2IInzopSb3QvCapMVTQnGV5FcWl5QSWZKqggLCrTK/oL2geKytt21l4vH+TTitdY8kS2760+o7uX6kFECWPx50y+3w2p/jUZ7O7H5yWBKsdaHa+fYTOSzH9EcLFnqRkb9qmY1TO4Mv3ukM7n0+OVlOXDFYmr8aKu/Qc+wCKwkWQQKuyC31dKVIrAEtDuruaoB/WeW3tAQqwOoYaigs2a7Mz68skdYHNVQ9hit0bbQCUHXtZACsPDSkKy6OipTnquP1SFnFBcQV1bEr5d85P//YsUoUD0O9K+XPb4evB9ZpuZZaMSmgYbLyCK3+XEj42Zkg3bXzGP8c5VPRTNOPXEM2afeg0wCWWO2dyHk/x6N/fyi0r9EhXqoPVlVgecau7faD1lqacNA2xYjP3FCEe6cMol15GvBVPwB/1dXT09VjDHkDaWFQI6tWpEf1BCp9bS4vq4aHoU4GaSXMAVxXVnX1qTKVij/VsEj18KFh/WadGFdE3/zQsIqNYsEpx8S6sbGsEmKKto709bE35DhZUoyU1kRo+/508Krn6u2bP/7krJD7AHnQghU8oiFiHYRWP4SWi9FSOp7+FP4IgcXz90Gu5AQMDgtdWoMfJ1gksPwtcmMf7sxjn8b+b13NSH0OqQSSHBUsb+aEk+TKGMLom64zPSlcGcEycJVC1oChk7S+u3m4gaJgpW70uOOlWURWW9kwO9CJLFyapsaaVnJfaX5LgSVrjdxDjxr2KeqkzyJGBVRAVazkKuiraxtuC608vnPtJ1wlQKrUxXNiovUvXiXehoiFyChQURri3AgWkg5xVu8MVpXIuovEKDmsJl69vGn/SMV7oJ/T7XHuRXZbbHt3uwgg7UEvV6hFBFfNiis9hJHA6mpsZKx6UjX6QK1MPnSlaXdd1svHYfNQWx2dZ8oX+9cqK+nHWDyTXwC+Cusa2mRqq7zmwf3LT7CgATOO5JPK1Oi16o1ISUbQ6kBVacTtOvJ9hdLktrfKndbh1onQr3s//nQN272d14U2D2pZeF7a4CeyVhfwOLQZwSKy0EZDrYG8MMTl9oh1kg6HAstqfU/V+5Hf67ASYiNynCcIgxbfna8GuiPNzdpnRw7hhJpJuBvclQEs8lfgKoUsQ4aBXFnPAbL04jSLq9bqvgKC6Zjc7CfAKi3Nr0Qkg7fSdHnH1/bBF/sPvrr7Ww28UxltM+XfFeFQHxSSeyPUaBHvTKqpK5R7KcViSrLtwsVhHJk6/fOdn3Zx0/WaokbkqnhBSDY3PET5cVjk1s7wCI+VASw+M61CoWP6IwyF+L+82YL6IHGFhejoJbGtPyivjVCNUP+vn+ss5dRqzPrKSJWcaq49c4bg6UkDiL9n3gy/kQ4WeiG6I8MNWSXsr9hlsScpET8sJmcls1Usyoe315LJE/gff2P//uPnIzXDtA6VMl7k0khlhfhD+C3WXeI12csTsQ1ZhTuybVCgVVJcWVk9PNywsvNo6qddT+A6OSJySoAmyOsc0CFDg6oQUv1opGmZcRkzpQAL+QYM4rfQShEOhazbHXzego8+JQY/vlCI3j4fp9v5UJwPCayrt3/rwSc6om/24PvOONssuepI5wpkdTWe6WmUXPV0pZkErpHR6jkIVjewaqsr7mMXVSC4EgJLhMBhLkvrZFWXf2VPnkgmkzfo/8GLvftf/3J0YoimtKkoXVY2bMzQi2U3ejZiaLi1ZierWi3TJbIg60vrhocXV1buTWNdfEAdnXO6KBSq2R3S8BgyWZpf6o+7NbBI46M1S4JFGstNYDkQBslpWcV5i/ezJet3gmX1q7kJugKyjtnUrkkwVC7qKNq1cHA1KbMMkzJrparKeA+eOdvY2JjusRgqwkr8VqOCTol31QBYPrzI1WORBBBA4ds+OuQrLkwPhbT1SCBrcejfL3KO4D8J0LXJqz9vvLj96OHz7Yny5gjOB7eKjGpveglIHqoeCrWOca+zXNZcWFi5vb1d3Do80bryECtMXXKpFpMlijucKeUkfH/e8vzSbItL6SzhsQ6A5dXAwvnDJuv7qd6P/C6BNeXnPuQg3ZsIui0V+/dqMQTRQQ6LnlflPDVPne00GyEEliEEcjpqAHGQuGpsTPNYPdJZpTEnE1lyYLW5vCGrLx9vtUq1OJmzV+SqykJD5caWZdmg1dbacc+evPGCVgXBcW1ugrAc4bsePx+vBopDpOrpzchJr6Eho/KinwyfYq52+CNrexuOa3sbj8OJ8rt3PDYOheL6iYtHVXl2R/gsfzQ3Nr/qn+FbrUJlIfEnwJopqlKhUHosDoQAa/rj8li0m3xzZmZW9jMEvwv+dP3mg5Va0cGir7HiJQzKX8kwODCgmmE0f2XwWfKjR4THRvk7AiqqR9fXqoUz8FZ1lFfCxuRtIawQ/rKQEOXbmqmmKs5lbcM7d5JJsTkvR3wlyOzHc47bb+x9//jZ07GVIVHJppw9KS+9P5+CPOIhStXVwGqHj2H08XbKxeG23rHHe9f/iU1aVyuo1d3N3AifJXUW+miQdujvDNLtc05M+GhZCLLz7PeVw3JoAiuMI084HDb4EYFFnwv3rMZV8Grwunv/SQ/efuVy15WYnKdhnG4xAGjgakBlOGvPnGWPpfDp0UxHTXNl+oQOe6vhxepilWLfFhXCumqEpFB5BhOiHF6odbHjoT15YCXj8ePYnEprOOx4M967+2R7BauUcKegpqa1jN6M5VpbDqXpJ8ZwD2Mni68kEliw6uHe7edf38QEtE8Oqrpl31WRUWflEllFtnWKhvQsFGDl0ZyApt0duruyhq0n38vjv78DLHsCedEWUld0iDfocd25S1w1qy1q2ui84kplrwxgdTX+/QyBdaYxlSPdU6VoetU2igxDpOxUHXcVc269GJ5qbAwBLKS8y0GyxKx0qAw73W/bMyriwSQZM3fjzoN7D5+3j/EpKdR32kQ2VdsHsMLHN+t4UzPTXVxS1xsCWVeuVMR30R+qDkoLmaXrLExZkM+yuUVOgsHCBhreAy89lkMJdysf02w6uflReSz0yrC7okFfNINcD+49mhzo5rmGciNZ5RDuMoGlgSUz5gO1jWfhsM6ckU6Lw1+j/HIALNWoRYmr8t4aPtabXyJaGaqrialybiAUTfSZ4BJvu7bF5l/syZzMXliwBd11RMr6x89+w5rucpEFQ2SUmitC4ZDBEodWSiqLC7LKyrOef/3zZ1/uxos+5UU7LnG8yaCz0Imci7bSaJHLnQGsdI9FDovuOm3mfBxgsSxJumbFHkg6wuZ27q7/vNMFeCLaZiIRB9lhUUOL4mpAlWLgtXr+LrnSwqH8tkf+qDEtDUE1nfqOobKGHX7tk07PqoZQp4n9lGGf5oxOi4wWh0Tug6ycTF4r5wabIEzEyxsIjb8+Havp5d5qKiNybqusgYTWDs3BIhr2UfWosG1o7Mnjn7O/nPF/SptJK9QqXLGPm3UW7W3IW52PzgT5LFicVjqg17QzLi5XsHjXPFYYp8tJaNHxipyPwWORFnEg0xAXDgtywuK+86wL6HSUp24lCgmuutWax0nVZkx8dZ3VwJIQ6d5KAaZJL46EmGRF2mpMZiiz6lBPJm3d3KwaSeXIqxowS6OLXRb0+9D2HRaJB1uAciC22AivEyco4XWCbjhPf/X15bvPnmzv1JT1cq0HYyINdWM7PKJIOqsgn0LyxFDb08ffYZIrT07P62Rh+6jQWdRIszQfbfHxqxD+LB0sg3hntKzexPsXDQ/nsfDvf83PxUGCirSBO4FSjnRYBrLQKkOZBgbLsOxRdL4QV8ZIqKFkcFjSZfFDEfM7kaG2Mc58Z1GLKCkqrQPHQBbFQonVAbAQy0KLi+Wk3zOCJbCCn2LHdeKEcF6bg+G5jfl/fP75V48fPnv+pB0NM3ggLkLXEVnEFiX6K7eLF4cniKz+WWpMZrjEBYsqcUKAfBZtMcpemt+aCXLr+0GwmCsRDMN0+7fJ4k1Mr71n536PHE5fYZxebFYDVjiN7HEGvvv/0NzXrXmIiB4IO9LAkpOoeBCCq7MGrHoaM3gsTWYhBJb3nqouLKyjvuMymstQZcdJ2UtKSk4OwYplSAfjIcCKhNoWW9tsQmblpL4M8TY8MchMnRgcPE6aa5Cei4PJFyDr4sVzGxtz8wvz859/9fXDX59kDbfW0Y43XgtBYBXjbVrdu/L03q2tWVpUxG5LHW9qyZZk0QCPv4XI4qGKl3gsKbPYY7mdYSbrw/dYgzmOWbqXirmJXdftK65d3/4TCCwsABlK2XdFPaPdHd16DzIPRkh/RcL9rFFfGV6EWiFH5rBqkbNqbcOuvpqJFR4h6zDWhSYNTcod3WpjzcsEPF2kayt//iKZzDl+48Tr3MBxrSyatCzNnQNc5zbm5ubmYV89G1sZ68siuJCkZcMLcbGslcjaoql5aifqZOPJZ75OQQ3LaP/LXobOYhGGKjQt+KvyVfAkBQ19cQXay+vY6GOmhe7Q8f25wQ/cY02zbvfF3QDryhXn7t7XtZwDiJRHtN18ZJxpMHJVrzWG9pw9myKwDiQcVL69Fr1WSEpSj8sKtc13p1Yb08Dq7tDBEhuVM4AFmRW5Z988fjznjf//syRLTnn6V5kuuK6NuX/ce15GiynrZKKUyCrpWyxbefJodDnGN9ZpIq5FgMVk0U+F22oBWZ1VtAFegiW6G3g6R4FlJaysidiSg1ZnTSffo2W3hwELi0Z9rK+CQSet8XG6178rH0BEalZgKbK6JyVYOguqga9LwyrNY3XpDTSCqsgQrS8lN9U9aagFpYFl8FkGsJozpRyottM6PLZ/5ETO2+jKQanKQNfowgbBNTf//eWJ1qw6ekYUsoRHx1ZJyalekLWFSzmY4aUVyXnZAq4W3chzVSzPx9DdB13PckyVdAKqfVSC1eSYWtgIhMlnrQ1+2GDZcxwt5K+grZBnwDrIqv1furqFwzJ4KxgaOw809lFRhjPuBzIN6d0NtdRpxUMYIKRbRlISZ1wMeglYHalgZSKLG/gaIs9u4MF3/M09Fl8iGRSPyeObe3kLc4iKPzze6S0k3Sd8FsDqKymeWFl5/n2UN33k+nl9n5/gYneVTU3IUPKdFZ0VMZBFiXkdLLfsINXBQkfW1MVLHtqrPDX1HpH11mCRN55u4R3mNBzgvunc9SEQNuPT2yFklVxSGyEP0605rFSPRZnRs2cyCSyVrhINfAyUnK1nP1WrdUW8zGOJraSGYBgpTwmInH/vRSkw9Mi+mRx8Cz9t/FdA360FYhsXN77a7kWmdIcXbwmVBbJ62+5+//0SyLo1imlo6Hg/vQXzOrm408JiHo9FZ/8CoiHpeszoQG35XDTIIwa/xBdksQDZloc2SE4hHL4/b8O3BwsdJy5yV5QoRu74isVj+3milnbwRTR1JT6hJLBkBkvLjZKzEoEQXJ09qLCM3Qsc+IzNfQMGOwCWwop9lkHAl2cia6UML8Pt/RvJQ4thmqe8cWNtfWvuq+1QHZUNZUspJUuL23pbHz5YwnqiW1HayjpKN/YwUpFXxBkt8k6UhbCtt6xitQPvUablWD5qqBG9yVbNANbJqXAiPDWVAFtr78vxpsN4LMdMME77B3jzk8sRR5f7JOWYIuqchPAUogcr5Uk4IDcxEFfqSXim0dDAQDtBVErCsK1BuxvwWrDEfpHmlJdhKldcNBzuXVms7n32O8CSSVT74PTVR/8eHsuqk2TRGE9lCeXgH98CWcu8oogMq7Bio2h6p70O4s49xgi9tlgMo18UKjur1NloMazapMAinQUNLzbBT619qB6LXoQ0KeB2cRnVve4O3G/uHuip74ikLH+M6LVng8dCKCSVhdKz5rKEulIHJ2q1jUVdabsaBoxNES8DC/+05lQBnykDT8FwpRX1RQTDQ3us4/YcSnHhDJz99nZZFs2JkWGUkWpNWa2hnc9jS+S0gBZ9wbKi5Zhf5EqLRD4eA/UB70y0Xy5+7+QXkZgAo54sVlphJipMy7pxaYcvobwXb8O391hJJxfuIQewGgqb51z7v9R21NYauBJwQc2rCcJJTbiLLqwuYkpLjvakDE9kWOmeKRKmbShNTWV1dKQK+AOJB57RaV2c2N4/nqR8qD3nkMV40HXjxQ377ZqVHRqd5g4tUvHFJTtl5acffb+0+v33sS2xsw/fLEexeIYnWTkdjzOZLo8jEJ/x4/oQ9mN1FmGTEb223QSXA76KFPsUuyv8IJEQp8HoeTr4wYFlt84G6S4DdnDSek3LLpoasNmxvjkdrMnJ7pQ5erXqinsaRAxMGZLoqq3VdoHUZgQtHazMOdIOvbhjBCtNZ9F9lMWdiWdU2SGwDu0DEA9RzX6w0la9WCeblUloFW+P9Zb/cn91iZwWW2wZP47RRR3yWZ0CLJczQGI94I5jbhVjrVhphIFpDaqTbAna0h1wBuh4BcCCzkJ54IMDay0e9LHA4kFxS+A65lMnawc6IobbEumpUeMgPIJhD7gy5qrkCplXua23AEuK947mjjSPlU4WMvk7E4+IrN8TWQaPIw2xab/XvIiDdrx5UlSlC4tPrYTu3lpdJbYAF75ZXVpdjYkTc0V80p5PDIgqjtV6Yd1ZYYsux73Ah/zUSYNNJbCd2+30JhKUz2paG0zmfGhg5XjifEgGIpMcFo5yPKqnNXyGZbXiEA6Ue3MqWLLxE0OEsB593qun69Wx8K1Doeaymg+gpeCihyHa98Z2SvduJJNH8MA7rMMaPH4DqdOk/XI37tnpYFGf2ARGpL8HWas/rC4BLPrR6lI0j3seilqky3KpHWuYm0hMOdf5ps7UtCJL8eWlXSJBNyl50LWW82F5LASMhHoP8gATdhreedJV31XbTRcrDZ/B5kmjw5o0AlDfQ+/BxjOyadTQw1f7pi6r/qAdXGiUAa7UlfBoDD1VWP3LixuDvwMsCoU3qF5940nHDl2llumsPhpEay3fube8urqwoIG1sLA8ykhVcQ0H70J+B5JaRzLU4XYAq/D06sYF5BZSzCH2AfoCCT6Jgvmid1zBvx1Y9k1uvnKTcqf/p15n+BE94iabI6mfP8rDZwSrnqZT9USDNnvT1VX7Wq50l1U/8DqwulVfVsfLwiH1ZbXVbNc8fJE8ciTn0GCJxkA8lvcmQjWnGnjbJJOFzQ5ZZZGn938QnkpgtTC/GsMKB3ZZJLPIZYmtowiGnqCXZPr0pvPi+TV4rKkDYFncLV6hujbf9cH7twuFg94478MXYFm8Fuc0OSxKNaR8/jq4lqMVc1ImVNHfLt+DPPaleaza16P1Ko/1MpfVnEZWs5bM4ousY6VZmAb7PWDlUD4r50jS/qgDFemaOpmCpwUl+Q1lQ89u/bDE0RBcUcfNwjLOCpC+YplV4aNOd74WYHXOBHCnyXoydn7O99lFx8kUn+WgVYBYleSbCdP51QSNseZ8KGBhjnDGKXYEs7/Cf2dNsQgFwo5IasTpru/WdhWlqexa4KRnRuVYl74C8g3BOuix9I2TaR7LsESQ2rQihpQDDc3nF+x8Z+eZ+0OChWQWZcM3N+13OyZqFqsFWCWF1PqH2k7oMQn4hR/IX6HVZm5udTmahzypjVZjEVnBIA8het1+p4NmcmJfLC1c2lrYODltBMvL/9LxZcYNbR9G6mHwgwELG4vccRq15K/rzsBVy08vfu2qp7YW4ykcfPbgsPQdo6kXcRrPNvLElyHjnpLIermSHzig4TPSle65Uv6n6WQNyTHD6qPb7RjawfAE5dIPJYqpkJ1zI3l8ejs0QcvaitXkDiYsFle2/7G8sACFtSDBml+O8RlfoNXZKcGiaNgfDDjQ2Df1jW15LvFt7t78XJMKhgiLlqBQth5fnNexTYWn6DX77gqttwqF4bjHZXFKsK5fu2r58fYEPtOTHYbPXrPIjWYGS+VGORAKlyWGnuUWEC2D1ZXJXR18HB70XBlUfLP4UPmsZtGuLDf49bYVtu88uTOIaEgDqzcOGxJzbhxHMAy1sX7PEpM7mKOtrJuI/EIvw6UFAmtuDn1cC8vRfgh4zB5WISZSkwjCXMA/SzrLMb16aS12/kbiUuyHSxtJPRxaOCcNsFwztOoPOa7wSSbr/QcLbe5cfQdYLLCuXVt3rX1NpZfutPEY2eaeESza/3HW2NlgHMKp7UpZFPl6sDJ5LfEPPai1dPke0fYU0WRFdf549d0XSbyybhyeK8o7DCbtz4YacDeYplhBFU9IF1S3lj+8tSCVO4G1Mb+0HPXzFQoii9tEPJ54FPvdkSud+mZ0/tInF3Nvnp/DAbEgnNUUZx489Mc4HM54mhAyE/iYfpcXKr85WIM5Xh8/TaiS4/ZcuxbweO/8hkXH9ULO6J9ArQsrDaxJWtSAjZBnKN8g3FbKNhCDhO96o1CYORyKl2i61kovHKot3K0Aa7zmMY2DDf4urm7cSObsoXW6hvV7ifBYWEVzamXi85h8EwIstAcuEFmdTFZRJ63pQSyMtiAUWDzhhUub5ze+OH/x2x/OzX/2yeo0slaULz3p5sEVImvGiSIigfVuPw3fvDXXPo1/AWJnGL61/Oj1eBIPOiDdJzWVLMHSi4RpYGHj9tme2oEe5srQ25C2ZuZ178PXgJUq47W5Hf204ZBYHDNMF6RbJwoB1sgYMvBJ5LOOHz80WTdenEjaHw+NgSw6QaDsWMnE0G+3lthnkcdCc+A80qT9kFku6kvurPChGD2zzGtvXeFLP/xw6du/XTqf+83Vc/Ox1SnKP6C5YSrIiwxogDPuFo1aFA03P4RQmPT49JMwFu813GNYu4tcw0C38XhXh2wbzeCxaJX7mbNdA7wQK60bK91tdf2HweoQs9EprX6tEERZhZUF2OE+Xlr36MaLTYB12E8U5RxOJAdftJedQhd8lrZTIj//aFZr5BkHw1X2WBfPzS3gZUj3AigYstpyxXLp/qHHGb54/rMfPtn45JtvvrgYvdSUIKqgqBwOAivOwTDuUmtv8TRMvrPB8M3BsvqcQbXl0BNwXLt69dreThdJ90jEEAsjzfWqb/QgWLVnG0VLVlfjmQwd7109Palr3v9zHqtDo4oDYBktRM6itVq8vh2b3HfuvSCXdfgMPBIPUFn/WBkrg8uSYFViYVfpseoy5BykywJYF9ll+Tv9aKbxs8+ytSzxnULKZn278WL+/CcX986/WP42QctmvG7fTP+W3B4MoR8PUnMpLODgpMP7DRaUO+YHtVAYuOAFWFPf15PDwhNew0rmsA56LHF/oudMT63qDO1JZUvb6fd6sg4VClX+ihZt4+lG+0RoKr40v6B0uyR//HTpxOUXKCffUONeb/svEoMZ1A9/41+hmrKJ6sIStVlwu+RYfk1oh7OkS/MbAOs8uazY6DJlS1eXqmy4fhmLuuhyBcmsvUvn/Zc2vj2/kfvJegLuKjjj39paWqqaYbLwNIz7aOjQG/D6gtapxNR7DRa1IwfkinIS77iH7Q1cu4btMvU9kykrE7hKmHLVa1IvEmIXVmPXwIBq1KvV0WpMayN9C5F1ECgdKZGlFbyLRe4EFSsgsVO5gE4CFFTSefv2Y9XP9+3JzSSehsftRw6ZMR203+odm2idGCvhAxYE1nbpscLF8ufRhR9+WKL5i/Pn4bIWOA1P355HE1Y28AqKAqzTEz737blvv/gs+olz6oLVGqfjYLGFZSwVyeZ8KlZuYfAQaDmxozo8FZ5+R9v+3gis41hZFMTIs9xw6EGbx4XAj9fu/BsMpIPVkQ7WpBGsHnVVYoCeiD2NZ86mOC1my6Dhu94eLGOitEO9CmmrFaAS4a+kQK7BzRdg0cEcOpnTXv3boxtoVOA2msPns54P103g8EpfPp3dIbAKjpUutg1dpgT86ufksaCy4Kzm4bfm5pbOnXPmRqO2KqHM8S/XnVj4NjoX/cSWQPeopaXFD9+2hHZ5Gk5EjZHBclgxeQcHZn13n4ZH3uy/w00XzXl5+IKVhffbe72JW921JN1TwZoUDckp170UWD1nxJiE2BFJszp6QZq81hl9Dkz0Kne9vuOvPmPhcFK/2hShFTG97Km41lJSoi1Y5iXLgiy6FtdeOHZ3n5ZkQcQfFqxB+/3e6lNY3F2MTAODVVlwtLRyIjTxaIlE1gY8FlwWTVLPLZy7dG5haX65c9kvwXJTitAVHr106YuiKchz7wz6/5ZWY3RhOk90NEPFB6CxPPNLCIrOJiYr5/0Fy+ryuPgEMoFFXEG9T1/uQa9x2vIg0YfVkeFsHHg606glzOXATuMZldJK0fIKrLcIhcZWQnGCnANgOZjiOgt1sohmlsoUtkgJFYCBUjpxWTA2/ugF13cOC9aR5IsnZXWLbTWFfZUq1JYeLdiZKH9yi1JZcwDrEoZd5+c35s5dwlD13NJqdKnIVuSj9kkuw1osF8JX7qA964LFN9OSu7qa28I3WPl4hQDL4U1sXdoiHU/prHdyxdFrwUJcwI41F/X1ubFs2s1zb/BZ1xx3fumpr02NhM3NymGlHLmUaNWe6RmoNxaRB9D0d1baQbYMy94N5+TewGOJ65iIf2jmmzglhxz0LiktESBMxcKCo8dwQC6/4fkD9BpzQDxMiMnZtD8arq5um8gqLCDxVkrU4ghdTU355VE0Zs2fO3/p0vlLG/Pz5zBMjcC4AQG/ULROyQQmi9d5r18AOwEnCtXZS0tYUOonsnBkgGuLMx7KkE6dO4/8j4f7twYH371d8K8Fi7hKBshF47I63WyXJ4R+tN5ewT3UtEiopHsmsEBRV22KywJlPWfTzFjr6epKu184cNBexhU6LhAD8UCrk8v+JVh9aWBJj0V2FGcJx8f7su7+fAPDN4dr/z2CXNZvbXWnWvEwpAPTpQV84bC0uKG17dH3eBcyWHgYzl/c2Lh0/tz5uVVEw9gFGy8ADHLSAS8kl9cRcLux1mFpidS7P4+PsFI7hAaW65uYBy2lYRLw76DMen0opLZR3CDkrCil3OkiB1ppr009omHltEjYXf8ysPA8bGxMczagosuAFH9JXRWSfpFC/yszgZX2a9gmgdNNi9r5G75/09eXDhaTVcD5rKNHjx0dOVZX+XAfKv5wXgBdyl+HshraGiifocAqwcuwJnT61hISDgALrgpBcGMOauviPE77rs5XrQfJZYlyIPWP4Cy0G/tLl1fzcFia5l3JZ+V1VhXFfajp4KRveHrjkhf7o6iH5l0U8G8Aln3T6QnSazBAYMnbVF5IrEYjWGKLnsi6ZwYLEistBUU5hzPpHuts6nYjber+VToLak1fDy/+NC/vxj+gu7xNHB3M0pbvpYNVQmAdYwaOlm5vHzs9Ul16ucmOybBDVHnRj7q/M1bd0FCHf444ncmXfQrGaiKXZ1d/mD8Hh4VSNK0UIa2FhNby0uqyGy18tGWFOh08liAclsftqlrd8NP1MLoajWlqCPiiGQEWOgIT7m9iFrfbSlXDxLsns16vsXB+IugUL2ExUMJoObx3fkFk6242gBWJNBtdWFr/Sr1INhhCIXuWnjPpaBlCYupWPz0PIUEznkUx5sEMDRFgf6ia10rKBWnFxSUHrFLpLOG1jh4dKalrf0gPxM3NQd7DhuZl3vb3JjVDNDmU4S5GDd1hEViRUTCcuLf8f6tzEO+sr7Bla2NpeTWK7SGY3sGMDs0cuqgJ3uL2hr1Oy8zyudgMLwDESlwM6oOuTlpP46K1DpgEmzvvRd8lNzokSBHmvF9g5UwH+fALXcv28MEzgdbeBBxQd8TYRIeGGaPmSu2LAkI9dJDJYNxR2qjD9Hf+oC+pej7T8iwjUBp++q3MAXV0bmByaJE9VuHLwTLorFJxUfzoSMHY9uXbGM+Vlyty3nT+eBBg3Z/Axvmx6kIFlshpVJ+K/AaVtXrxW2Sy8Byco+2ANB22vDyPTNW6q4IaHlyihwH7IeOjc0vxWdpbSkctwBX8Vj9SDlVBBis8Zf223+NyO2gkjAR8znsFFnYLWyRYFpqtdCiPFb7VTdsbm1PA6p5MEfMpYA3gxJdxrllrGdU91t9hZ8WXdDWfBpluZ1LbnFWQrBf5MmpDxD3frFSP1ZeBLEoNlJYW6E5rvHRs++7t4/RCVF0POW/QWHf8xqD9zkhhAVZmIZUlwKK//3ZlZc1Ex91bC0tzlwAWhULaO7mKQBhdnp9bXvavu6qqbDZu6MPW/Cbv7OrCDC9u4+2SdC0TZKFfvqiCe0jhshbOeV1BJ82zToXX7IPvl8eyJ/hoKFJ3AS+f0hMeyzL1VQ8VoNPB6ngZWCSxjAFM37LWeMbor5irv6egpamvM2fPpHCm/7RRm9QfMCa0GKxhuI6sVLBeRlaB7rdGjraPbFeX3P3uBTXU8L5b3qn8+mI0BqMfToxXkpjTwSpBaScLe7MwDrZ07ttL2Ah47hw5LAzeL0VjeBlGlzsDtqIK3uLD4dBqXY3OzLTQ2iO+Wk6bvLNzo9kAy8tgQVtd2goEfagYksx6xwT8kdelGjZVp4wnYLHogdAydRdpdOOmYi7n6LupFFra/oYuAZagqrHRyIfBZQmqDCaQe4md0Q6maClVw706ERQ7yuqy5IVBuWWozwBWZZ9BZxkDIkv5kaNZxb8+ILRoEn/Q/gZinoYr7Pd3TpcSTgVHj6oTd9t4GlafKh+/hZTD+W9JYc2j828JOx0wfL+McDgaq1i3dVYxWDRo7vQ2eXD4A0vaxJ5J3tqGC2IIhlY6wEoua/WcNe72gDEW8IPvksx6DVjoc8cKdwGWx+PVzQLtXk+KKiI/VCTURnU6WH4psDoEWF3iUFxjanh7OVYSLu37gwJfl/a12olobXUg/UJzq9qpYACLGocFXqlgVWpeC64GjQ/tSD7UPb//gq+hvBFYJzC8euLO05H2ozgbXNB+VHJF+f6Ckpq2ZkzdIxhShhSZ0SXCCjZahPn7WNTmxKuPN2NwqjTQZPVpe5eLaLV3ER176rRR5cNLrX6J83gYWsIiGCbeqXL0kVeXcuxrbotLc1kaVvgvZu/fPfX1KUl3EQlTPZYeEBmsnnRnZSDrZVidNbLFaP1d7YdP6T2t1Q7tiISWeiBEJrKMHqvYSFcaWCUGssR38Fzjx7KynqPQg1F8gPW6UJhzAi1/m/aH+afHj7Hvk1yJaJt1qmzlXmxp4dz5i6gWYj56ayvGYPkxMI3pHaezYoY3Y/DchMXpDQcqOqs04/lWm22dFmh5AxZv0/ToqsPiYLDCCes71QN/5DU5LAfvGWULcI1QotX0XQc3JSuHxctAJo17qToiqWD1nJFn4lTNWdSdFVgv81Z/zxAbU6eopXJLAYv8lfi9+vIa40HUFLSK08EqqdSkFvR7O/Kl+dsF46fHC2uefL5GmZfXf+Ywbv8CZR2ANX604CinSMWRTlbwYxMR9CmjsHORXBYehFtRXkUT7VylGen+dWTgfXTT10XNbyifNTXZsFiS9krG8YHtNOgrCXhRRPQFrLR8Zo1GLQgsxEIcvH93BPxrPNYaK3cRCaVyd9Du1UDifm1PbTefQyJ1RRxFmnmZXprJ1pVumoBWVDWKsUL9hXdGcnX2TaBK7a2p1X9gfGrii4iQ3WVjhnOoAi4dsQPpLJFz0jxW6THk5IEYGh+e3ruDgs0m2kRRoD4uXdcB0HKO0C4H++328fHxdmp7JrWm/gF9JVmnakIPt/5v/vPPGSwEwtwoCayoKxfT98hTrVPOwUVn6dx8q9ViTXhn6DSy2CaMjTOo9cRnZwJhjO5Ma8toxHY29JMOvh8aa9Ab1Oae2WExVqzd7/VgPKdZXNpSg/XdB7DSQiKD1Sh4Opg0OHP2738/+1quBFapmXiZcj9wSprEHD8Vm3GmK6suHazCTGBpZBUot1WgpR/a20smfnu8jyefOpXCTGUAC/Id9cLncFkjBfnHjpUawILVTbS1fb5Ek2DQ7mh9R3cy3oXLS6MV2MK8OjpatS6yWQwWL/ezJqxU7hE97zQjRrABKqZKoiV2s4WtU/b3wmNhPTK6ZRRYokYo0w0WFHQYrA7jYH138yvAkvGrsTFlnW2qx3o1Wtr6P04rSBmlpS669M1IhouHXc2LdQxWobo9z1zxd8XpOa10sAoMeS2MXGyPtV++jSmvJHIPN14WFLG4JgfjOg/7ANZRgEXJMe0fgM6dmlNDT79fQi/pAvBaohWStJENOYeqGFyYf9TmrOLBMBef9yWnhYVZHgEW6tROSCqej55mU2SxywqHHWvvh8ZKWjxO5bECXj05CrBOPjuTApY4b/IysJqNYDUeSHK+iceCt2rMwFWtTL/3GKs/jdqVp65aHI2uM4ZCVd4pTi9KZwJLvhCZq2PoBCw5VYLWBxJbJ468JFkqwSKRNdJekF9aWWoMhSUIhmOhh1/+3+r8HOjCgCEKOngY0uKsbAAWy8tdd/I9Otmq7KEThmF2WnGERIs1rHbQMFTKY00xV2iRT77zYKHP3T7l4iKh2CwjmRJ0eaZ/OTMwKa8hqbXX3R3NGWKhxKtW91QHwMJw9OvDoOIqJWsvIx7/TVm4nZF/f/mrPbUhIbF2Co1kKd9VzNdZjZmtjGAJtkh3HS2pKX724AblTJN0v+ngiCsBdyKZc3Nk/PTIyDHS7SzfNXyLG2omJv6xvLqMrDu9BEepVBhbQvIhWgXnhRnpgK2zSJR25OaVgBfJBE98djYe0LBirsSHDIYEltUbHnxHkg6vAiuJviDesePhNneHXoD2BhK/nRnoVpuB1EGml2FFZNUa/FM6VgTW3//+arjOCnVVqx1n1WqFB7MXhlhb2yvAKszKCFZxOlgl6WBJuI5ul1ZSlzyyDw1jz5DYevGCQmJOZrBOnHjxtGBkfPwYnFVfAYOlkZtVMzb85PvV2DIWz8BFRUdj6FnOhd5a8q9DyI/2Q2Z1FvEOEFH5p50OWPYXxiJlbZXDtM6VEFsnqRTdhBzE9DvyMjzyis7RhFwtQ89eR4rE8jqathsJLMM2WwFW5A3ASvdXPW/gseCyGntkDOQioHRVaal7bXBf/a0HyrBKQQXDDGAVp4Ol4NLGeGRaa7uggH6hdOQY6tNjSGxBbNG+hwMJ0hw6LJC0/1qMhMMxpDCK+woYLPlPOLo91taAl+FydHVjlfZ1R6NLC9w8s7xUsd4fW4pCZhW10DEBUfonshy8R5I+0uKgHg855RDG52fz3Vgj+XKwtGIOHJaeGpUOy3phpycVLDpN2BF5LVjaRV5dvTNYslT4yljYwweheRSjttaI1ZmXg1XftpOVlZWVGazCNwRL0oVgmE+zN+0jI1l1v3x1B179xIn0SxEoWNuTAOtx1jh5LICVVcJgyUawo9tZiw0TE1g5M0qlZ6rpwGMt9+dCai1VBKLL2H9rs3W2yE5lQVaAdo/S5LPaeTttjIVMF70LpxNuTIYl7e+4xwprE/UeTLIph3WB6Fq3Xq2pRRrL6LDK6QxmJH2drPbj2tQGl7QmmDOyt+FV1tildfdBXQlZpZWCzhqSp8Z/UPciLoJn5kpzWQfAOpiCwBCXbAwsRWbqWOmx8bqG08g+HNl8gR2m4iarsWA4aH8Ej9Xenr9dXEhNyiX8FGVFV1zQVz1W/q9YzB/bWEBJehkeKxZD6wJt7K6owhsxlodtIS1FyLKLzwAfbrJyElTunoGt4UMorGmlsabWAJbVMm1/F04MHHl532hQd1haCPQKsLwXrkwM0EbbzGBFUo9U6GD1HOys6uI0AR1bfZ14Nw7uyNKQ1myjVxJTuWpsxknwV4JVKMl6GVhy3sLQ/ICYiPnpkZGShpGHt2kQMXnkRLqIH7R/VwqwRgBWVl11McCSybNtLIsozaqZCH0dm51d3Vian1+CckfSYdTfT+VodCPDi2Hynq45VbjW10nhOtlnNUmyNJk1rYv3BGbFAFaYhvStNA/2zoJltze5LbL27FFpUc1jXbB+2ovyrhGsIeRHXwvWgX49sa1Beqyzr0yNNqaupOEx6tS/KCUSyrH95obXeCx1wrLkFcbiipGSKXnocVol0te2/fAKZk1A1on0/y73Twuw8GqorubXp/SQ25VH+2pqQtv3t/7Zjy0OGwtLF1f7cTUzNxvvw6VlZzaRlcvrbykJz28n9MJ5aQ2IJIvYmiaXJdNZJ8N0cCAxPR1wei1oAky+Awn4l4K16bK4PLIf2UrXZI0e60LTp6Gu+jSwujteBdaAyjYZqepSK9caXxEKNVwMDcr8HjyTGkDPHnBY+Euaq18LVuFrwULvev4xjoMYEjsq86XjZMeqC6mthha9p5H14un4afRGAKy6uoasEo0sqkWjM6tm6O4/v/R/D5f1+fw3lMzCEE4e57TWO7lHS5xk7eTjmCh7BMTqojAJeOmzVCg82YT/4KnXYbrJHbB6sXI48Q68DI9kbhvNwYiqhb0VJegc3nSP1XSrHGClPQqbU45gpgmugZ60+7yMlOBEnC98WXfD2dRrmWp9SKMoYZ9N6ag5Y0iWMcnldTpY6XAVqx/09fW9XGdV0hKGfCYJWdLSY/lH8/v4r+wjP3a0pC6L2mqQeRDdy9jfxqmkG//iRBaBhbsCmsti0VZaOTZ2quYfM9n/74f5W+e++DaPDjkxWVDy0UA2QMMG3E5x6xeHoxER1718BEWPhRQHCa1E2IGqNG6FITvqxHpcgBUIrP35LutIZuGesxmUBQWUPWm5SZrGaro1JD2Wtjc9omt545lVDaxGfTuDKL9onQl45TWezeyyzmpz0gezFCKLf9bYyHwmFayexq6hTGBlvRVYleiqorY9tLHj/nPh0aOnTz99+vQJ7CnZ6crq1idf7R/nTyVtUKaT4EDrX8fYYxFXBrCKxd+xpLow9Mt3/pbc+R++/5/znzFYkFl+qu/EKnJH6Y0Y9aMl2U8H54qK6A454SOLzdKQEcVcK6Q9bZ/xWLg9wBGgpfFJ+zvqsexW4a3oq9Xq0NPuDgVWSAdLHuw1eCwDWeqBWN8jS4MpS0dFo8tkKlhnDaFNXxqSRhf7LZFxMHBlzMIyW</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAYEBQYFBAYGBQYHBwYIChAKCgkJChQODwwQFxQYGBcUFhYaHSUfGhsjHBYWICwgIyYnKSopGR8tMC0oMCUoKSgBBwcHCggKEwoKEygaFhooKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKCgoKP/CABEIArwCvAMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAAAQIDBAUGBwj/2gAIAQEAAAAA/VIAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABEw0/nfH+j9vOAAAAAAAAAAACERq+T8p5ng8Dlc/gbbpb3b73ovWe19DaQAAAAAAAAAERj8p878F5DBMRWMHDy0jrZsVa07X0H6h9E2bTMyAAAAAAAACnI+UfK/O1U0+dzdDS1ur2ebPm9jc3Nzd2qxTo/WPtXrMlrzIAAAAAAACnn/AIr8s16Y+VwuJoTvbmzk5OrTH22DBrYs3S6u+xz9L/QXust7SAAAAAAAEcz4d8i16avm/N6vT7XW34pWmv5/D1NorGDS53PnrdTJE/W/0l6TJeQAAAAAAER80/PfIpp+T85s+n7+WIrWtaVrWlIpWBTncjS6PXyV6H6U+47FpAAAAAACGl+fPlMYvK+Q6Psu1StKUpAhVEIx48WMjU4Oj1uhNPrP6w7dgAAAAABDg/mLydef4TB7zu1piwYYmJQRWJhEorgwVNDzzs2r6r9ie5sAAAAABCPKflzjV4HhvWe6nDi1NcAhFZqRIRh1azHD4vZzup+wPqUyAAAAAIPH/lnmx5Tyv03vY8fP06WgmAiIRExMSQjX1zR8t0uhXc/X31m4kAAAAQPOfk7lPIef+ub2LW5GJEwlLlaOthwxfLs7nTyQFZV06Tg8l0N+u7+xfqEzIkAAACDnfkvzM+W4H2DZpzuNUIm/C4vLy2rFKxERTo9vvSImI1sTD5Dq7Ver+2fZTMzJIAABAr+Y/mLjeO+y7dOXxogMnA87KsCsVhCFvRd8QNfDOHxveR7L9sdO0zMzMgAAQHyP83xr/NvsvVx83hwgy87zN5iEPo2/HFtb59ArWPUdCsBgwtfxnqNZ9y/VE3my02kAAIDj/j7mT83+gewrpebQRl83zrqwg9V7HWtzfP8AmRCFet6OkRMNescrgeg1M37H+l2tN7XtIAAgK/nb49Pmud9gx4vMYkROTg4LOddFERsq01IRFYjYm276apExrxPkt2se4/a2fJa2S97AACA85+QNWnzD7fuV8/z4gzcnpZMPnt1EREViuOtIrWlKRi6iM/fomFcLD4j0+jP6x+vXvkyZMlwABAfn34tHlN36VTS81WUZOZuZqec3SIqrFK0rWtK0rFIt0sEb3fxhipPnKzX3P7Oz5M2TJmyAACBpfjflR8r+6bdfLadbROCt7+d3kIisVpFK1rStIitaxs3xT6PdCMbD4f0uhk/Y3vM+fLlz5QABA+X/AJspweR9fppeUqiZ0bX5drwiIpVSta0rWkRFYpDbwRb3FEwpFfJ7uvj+7fo3Y2M2fYzAACB+bPlk/PfoHqq8DiRBrY6OZuIiKK1ilMEWrFYiIrBmphj03XkVpHM4eenqP2jt7Oxn28wAAgxfjjjz8j++ZLeIxRETzta+ltIVisRXFrx0p51YiKqwIz6TN9AxBiU8H39Hc/YnrtzZ2dzOAAIPK/lDW0/n/wBwx4vHRERo00bam5BWqtcOHL6H2U+K4mLDWIqFc2lFfoGYMcR4js8+/wCm/rO9t7e7sAACD5b+dsPA531LHpeXisOdp684dxFYisRo5fun2zRnN8K+QU14iBEZdFHsOsTFax5XLqPu33job27v7IAAg+K/DMXifQe8x8vzdYV5/Jpi2M8RWqK4cXrf1bvYKZtD8n+driIRBqnqO8mEUnz3NT9W/RvT6O/0tkAAQfn74n4Xg/a/SYuN5usRHG5K25MVrERXFr/UP0RzdymPb/MfiJxiIRGGr0fokprWOL5DPvfSP0l1un0eptgACD8k/nTt9f3HpcXE8xEK4ORERFaqxWKY+3+wOnzq97zP460IqQKiPQd0mVXM5nncP0v9OdfrdPr7gAAg+F/nTb5XsPV4eN5OIVwcvFEVqrFYVxV95976uPi/n/yVSIBEJ9H2Epk5PK0dX3n6V7PV63Z3gABB8f8Az1paPoPZ05fioiGrqacVorVUrXFTJ7rQ8lW0xCAiDL6foSlc42hzbfYvrfZ6/X7fQAAEI+Rfnzn6u/8AQK6nz+IhrYuXWsRWIhFEUrtRrTMRBAiDa9ZmWTki3A5+jm+zfTOz2ez3eiAAIR8z/NvOjkfXcV/nGGIRqcmtYiKxEVhEIIREETEQOv6ikyvki3A4Ebv2v3Pb7Xa7/SAAEQ8n+Tee8r9kmnmOHEI1tLQhWIrCKlYEKzUQiDN6ffsTnMviNOOx9y9F2+33PQdMAARDW/F/KnzH0Ltxo+LQjFg49VYrEQiFYERAhBU6vqYkndxsHjdePZ/X+x2u73PRdMAARCv5U8Jh5V/pEPGaMIaWPlIrWIhVEQgiBECrb9PtTKdrJDg+bxZvp3v+v2e53/RdMAAVRHwn4rpV8f8AYs2PleYiERp6elFIiIiFUIIghBEZu33IsT18TY+aa8d/3Xu+v2e53fSdIAAVVeT/AB8r531nrMePyeohGLHzdKsRERCIhBCIIRGTqekTMuhmOT4ir33a951u13e76PogACqsYPxPrYMHnvrmPFpeaiIRj1tHRiIqhERAVQQjL0PR3WTl7WBsfM9F2vS+r9b1u32+/wCh6AAArERX84fGc9OF6f1Wvg5nJhETi0NfRrFSIqgKoIZup35mZT6LFXL5rxmOfpfmvrnX6vb7ve9DvAACtVY+d/k7b1cfnPqTBr83TmIQ5nPx4YIrCBEIRmz9vpJTL084o1/nGnX1Po+N9Y6PW7Xd73oN0AAUiIr5n4Z8R6lNPT+l87XxaeugRi5ehGOqsEKicuXpdi6ZlPrNrDir8148bX1/5v7H3fQ6va73e724AAKRWK4/ifw3lTHOye55mKmHXQQV52ppxFaxBdfd3ulYWlk9ds2jD8z4eKv1zg+W+z9bodTs9/u9zbAAGOIitfmPkfzj2sVeZueq59ZrrUCJI0tfFjrXJfNt7aUplO96fJky4fl/EwV+gd75t6D6rudHqdrud3s7QAAx1iIryPhfO+DekwTzr+q1BhwoJhEhEzCwlZfvdit8vP8AnPEpHq/o3yfR+vek3Oj1e13e31NoAAY6xWK4/j/mPI/JPQo0tL0uWExr45gRMTBYiUpmer2s15v5XxWhSvo/qPyrmeg+ubW90et2e5297aAAGKIrWMfI/PPQ8N819JVrcvp9W0ojDjiYlAkTEpy9DpbGXLfT8JxdXHHpPovzblU+zd3c3+l1e13OvtbQAAwxWIimH5j8j7viPmvo005WPsb9wrjpUEiZz7O3tMmXNXyfl9fWR631vgObh979G2t3e6nY7Pb6OfaAAGGK1iK11vzx5jo+R+fd3ax1w8+etu5U3m01rWEzkzZc1ptM5MXnvM4dekZPZdDw2LF3PsW3t7vQ63X7PZ2djZAAGOlIiK1xcX818/Lu/J8nRrSlNNu9HcyWvabzeVrzZFpryeDx61xxXf8AWaXA0J3fs3U293d6PV7PZ6eTY2QABWlK1itceHyX5t5nK9t5Pze/asVrq4290N6FrWsi04o2OfyeXitWFMna6fG0sOpufYe7tbu5v9Lrdnrb07GwAAFKUrFaVpreJ/M/kNX2/W8hr3pRVXV5l+h0NzYy2mrV0NPm5lqTWMm/0NXQpix5fr3oNnc3N7f6vW6/UyzsbAAAVrWtIrSuLV8h+aPnuHq+5xcHBTDFcPO34xY8eK9ZmMmXJGltQjPtbeDSpTHTofXOxsbe7u73R6nW627a2bYAABFaVrWtceLT85+fvkejTv8Ar45mLHq8DbIhQJmZY9fobGemDWpWla+l+o72xt7m7udHpdTqdPLN82cAAImIpSKxjx4tTi/Jvg3mqU7fqdzV5mj1dXWxYMeKJRkvn2M+xy1dfHFK1pm+ie3z7Gzube9v9Dp9Tp7U2tnygACAVrWla4sGtyfHfEvl/MbXvst+Fp48efb2L1hNKautq6uHbitYrV6j6X08uba3Nrd3uh0el09282tmygACACtMePFi1+Zw/A/IPBY/TZclpNfS1qYqVjHab0rWqsVd36L6W2bPt7W1u7u/v9Ho7+Va18mUAAQATFcePFi1dPkcDxHzjymtaxkiaVpjx48dKVpEViJ9R7r0l8uzsbGztbm7u7+/0d7LM3m2XIAAIABFcePDr6uhyOJ5jxHjeFqxCEVrWilaxFZ7XrPX9LJl2c+zn2dra293d397fyJta1stwABCAJBXHgw62roczjcjgeZ81wORr461rEViubqdzveh377GfZz5s+fY2tra293d3dvJK1pva9wABEAACuPDg19bT0Oby+boafL5urpYIvs7W9tXtly7GfLlzZsuxn2Nna29vc29mxabWtOSwAAhBAkARjxYdfXwamjqaepra2HFSIrabZbWyWyZcuXPn2NnPs7W3sZJTNl7L2sAAIQVAlJAiKYsOvr6+DDr4MOLHStaBa1smXJlz5tjY2NnPdKZmZtNrTYAAQgqAABEUx4MWHFhxY8VK44isxN75LZM2XPny5ZTKZTabLrSAAIIQgAAQEVpTHjx0pjrWAvkte+TJaZCyZTaZmZmQABBNSIAAIEEQiIUhWQsmEwmSZTMytMpkAAAQAAAIEJgQmAAAkJSEgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA/8QAGAEBAQEBAQAAAAAAAAAAAAAAAAECAwT/2gAIAQIQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAIWFAAAAAEmZGsq1qgAAABMZsADW6AAAA54oAA3sAAAHLNF1bZJmBroAAAOOdF3oAziDewAAHPlsvSgBOcLrYAAJwaXpQAJzheligAOfO11oABOQ3uCgA4ytdAAA55HZCgBOKutA89noAzzHWwoAZ5K60HHGNdeoM8x01CgBjmrrQZ46x6KCckvTUKAGeSumgHLpQM84ddQoAPPa10AADnmHawoAOMp1oABOUL2QoAOeKa6AAJzyN9EKABxDW6AExmDugoAGeYXegDOJEdtIKAAxmBbpYzkiOuyCgAGMAAIR12QKAAJzgASGutEFAAAziQSka6aCBQAACTOQ1dUEBQAAAAAICgAAAAAgCgABCgAJFBQAAQJaWIkpQoAABAgJbKCgAAAIAAKAAAAAgBQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAD//xAAXAQEBAQEAAAAAAAAAAAAAAAAAAQID/9oACAEDEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABUpAAAAABbqrnSM5gAAAAXpZQAziAAAAOm4AAMYAAAB11BMyJdaoZ5gAADtYTGQDW6M8wAAHTpknOABelGMKgAC98k5wAC9KOUogAOnTJygABeoxi2IADsM8wAA6aSc2kgAXtDlAMGwNdBylsgAa6w5QGQ0DXQc82sgBrrDlASXOqDXQc82sgBrrDnkBjYDXQc86MgBe0M8wAA6aLwaMgA7WHKAAF6lnFpIADfSGeYAC70Xni1IAB2DOIAF3orgtSAAa2pMZANbpqcYtSAAN6USZitaDV44NEgABvSgALpxwWwgAAu9ABVuOUFsQAADW7UNZ0k55DSEAAALq7gzmQFqEAAAAAAtQgAAAAALSCAAAqAALRBAAAFCEpbYQIAAAFFFiVAgAAABQACAAAAAFQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA//8QAKBAAAQMDBAIDAQADAQAAAAAAAQIDBAAFEQYQEiATQBQwUAcVYJAW/9oACAEBAAECAf8AviuTddaxf6BGvLbn+k5zl6TK1TJ109rl3Vjt4U9IdpI8iXWpjWo2dax/6BF11DvgOf38kztQztczNTOOZzknPJZB8iilTas5yTmHd4GvLdrViRnOc/r5nXC563uF5rOSXJC7m5d13VVwMuHKNyblXGeHUy03FN0TcUys1nMOfatfWrUHLIP6mbpdrvrN9/OVLeuD11dmFaUogptabV/i5cXyl3CbebeYBiKapDzc9E0KNZSuyaysmpgQf0pky96yedNEvSJF1elCmba1aEQgKOxpxDtuTAaY6GlMrhOQyhLjU1t6jSF6f1taLuCPz86g1VcbjWX5Eq5rdjQmLO2zsdjRo1jjxKCjx8COqkuQ3YuWZaHDWYM3S2uEL/NkyNR6sJpSplzdeiW6La6NHYnP2YKC2UdHY70QFmTmjWltZW24Z/Ku10v182lSpk2LEh2qjsolZPpEFsjd6M/HaeQvaw3vTWoM/kX283W47Tp7jlusqUGjSipz2FNlOxEmGCy8RVvnaQ1T+PqG83CbRq5XBlm22s7Kpx76z6GFI3kR3W476hUWRozVOfxL3dLnP2uk+DEhQzRp1xxf0JDlOXFd3N0VcPm/NE//ACSboi4Nrx9CkqTs80+zFfUmocnR2pc/hTpV/uu11nW6DGjGjT7xPdYdur07xgZznOc5znDU5m6Nn6FI2cbksRH1CrZN0ze81n3idZ3za5zIMSJGO0p/usPXNSOHDhw4ePx+LxeLxeLxePxFpsMXFH0KTs62+zFd20xebfNztn3Nc3kmpL9WyDtLf7NofnrrHUVZbLd9LW7SUzTUjS2qrF2IQY05Sey01iQyoc9v59qDOc+5dJtyl7XSXp23UakunsEzJoT9Dt9Ve0XkXa4X+9Xf6CIcwjsobT48N+Q1TLmiLznOc+znXt12vcrT0A0acWtXaSRD+IqKDjGMYo03IVLbluyOXLlz5c+flSOATEfHcja4x7e5tpK7tOg5zkbD1r5PkuU4tRgRTQEx3qgFSRT7quh7E7HbPTKSFE5ju9iNnW8vikq/nt1Bzkbj1v6Bcdr9I0pDNGpbmejaH3E0C64D9Oazsdsnq2tacgxJDiOqhtdWbYs7aSuaVAgihQpPqy37i/SjIXCjmgJLp3zUtQAOVr2zWemazWT9TC1VnNtd6nd1LapQphejZwKSCCKR6uvJazV5f0tGNGpi+vJqsgzXEjrnOc0Tk7Z+rNZQ6T1O91bYUdv51OSQQQRSPV11L2v7umGKNXRZ6u06sFS44rNZznbNZJLvlz9bS1prNmd6ne4t2tR209LQpJSQRTfqLVcX6NSS03TZcUemWFA5kms9M5rK1k+KM1KZ8JH1unaM+6juoNLloqIrTclJSU0mm/U1O+/tLXYWTs6rrMMkg5b652zTi0ioNoj6Vk6VnWuik/Uk7Goq+p3uKJBpB0E+2UlJSW/U/oDru18XpBo0anHq9UlWcxOucnY0DWk9MCMQKVH1Xpz62zvZldTveEp30A+2pJSU016mv1q2v8nSDRBq5dhSzlwsbk9XNtMRGVJffS1S3Xhe4qw4fo5b2Q9TveEx3NtEPNqQUFJa9TXhlSptzQ1ptBBF27LY+P8AF+MB9Chx/n5cQIkhgRBDbZ1gSF/Sa8fi8dk7He7CkOg6QLRbLZbpn1P6ZPWuJbJqdNkiruOrFH7FA1ZZ0F1SippaV36XLfXRP2Wj6Z4mIcbSrSL7ZaKC3THqf1CyNQ6uQ0xRo1d+zdOfarbTuooN7WtK7jqK/wB8+4Vax9FwqRWFs6EitFstluo/qf0Bc4VPGlaNYuieqqlD7SBSV2Zd1eJz9zYtw6je5Gcqm60dTRaLZbMb1P6I3PFSRpFe0lPWQJX3kcWn5D/ED7mRHT9FxqYumK0ohkslotVF9T+gIl7GtOuqFNl1HVoH8JhlSuiRsApzaINPoaLRaLVRfU1UyvfLSyauqOqqlI/AaTBR1QNkUle0FMBDVM0zTNRPUfbCNroLM9tNb6uIFH8BlrsobTlOb21humqZpktVE9XVTDqKuLenpJ3mNdXKlt+8ymI31jpNYAvi1mmUWlLdNU1TNM1E9X+nw3yaIaphdEz2+pDZkM+42iI0T1Kdm6cc2tTVpDVNU1TNM1E9XVEOEujV0b0/JNGjUpvq4hCn2vaQmOz2iNqNYvryt4rWnw3TVNUzTNRfVfRf2nQadTCcSs0S+hQ6uIDjzPsIRHZSnq02vdsyHtrVHuTllbbpqmqZpio3qmtdW6A7tcGtPzHAaJkt9loNOII9QUAxGA6gNtYw2i+SVHaBHkLYQ3TVM0zTNR/VNahbvUZwGjSk2+SSSS8ju5GJKfSCG0x4veLHIIxcZLp2sUO7P2dpIbpqmqYpmo/qmtQM6jt1rf2faiSeZJJK093ELjKPEj7AnggNw0jvEiEFJS869J2iscZLunGEBsNBqmaZpj1lgo1pao7+0pm1z3kk5pSfoUFQ1MKVgp44xjHHhhBTGbhgd20RY9Y4vrmynF7WG3XeZiIygNhqmgyGQz6+qWHm5cfJ2kM2ye6jdSSPqVFMIwvifE+IIYgpgtxvqjRmkChQEqROlvO7actl8mrVp+OgICA0GgyGQ16xq5Rm1322RnXE1h9iFN6qQfbSliETQoVNnvPKVtY7XcZrrhNnippAbDQaDIZDXrGjWrIbDuprPBkqSKNPMtuNySNyCj1xTMNpI2xU+6rUtW1otr78uQo2KIkICA2Gg0GQ2GvXNXGK4lp3UlkiS9jTrS0sSkq6EFHpoQ3FbAoUNpMubcFlR2tVsdelyVFKbbFSEBsNhoNBoJpr1zRrVttbdZev9kjyUq2NOx23mpCVdSjhj68JaTGQ1sKTQp12ZdyVOb2y2yJUmQpROnYKQgIDYbDQaDQFNeiaPU0acTqS2NuofftNMPZOy0qZQ+iQhfQbYLfiLPh8Ph8PgDAax1FOvyLspzKjs2iDBlzVOkmrRAbQkICA2Gg0loNimvSPY0auMS6QkOQnZsWdb2ZeaNGlJU0HUSUSEmhQ2xjHHjx4cOHEjdS3bi/cyaWvePFjtSJqlNEmHGhxkhISEBsNJaS0lIpr0TR7GjShe7ZOjMOuyY024WhJSs9DRa4B1Etub580Ow3B+S7dHLkp0iidjSEMRlOvv5UWjHZtkJISEBIQGw0lpLQ2b9I0aI2O5pQv1odiTihyBeJUR+IDg7Z2Jd2bkIuSLmmaJIf8vl85lKnrui7k8+kCs9EobYFLkkkk1Dj2u3gJCEpDaW0tJbS0lI2b9LBrB2xsQQtN3tl/sS05iT4s6RDcZooINEqUjbBBbLHxyz4gz4QwGAjFFXRLSWaU+pWSSTUOJAhAJCQkICEtpbS0ltI2FN+oRjGxFGiFonwtQabfaIBiXZiW5GcawWlMKFZz9Y2WlohgMBClqeKs5yTVstcaOAkJSlKAlLaG0toaSkbt+sRvggghxEhi+6euFrwRUe6RbitlTEmrdSmzFVFMYtKT0xgNhhMURAxcEtyVPqXnOSc001bbIlIASlKUpShKEIS2ltLaeiPXNYxjGCFBaHmrjbLzpyRD2g0lwOc3bcYWfni4CX5OZHDjnmqUu4m5KmqV4c5znOc1brNDh0kAJQlKUoShCENobQ2gDcUj2sYIIIIUhxqRHudkulgfhxRzC+fML5cltqiKt/wDC+J8X43xfBxJznOc5zmoNrgWigEhKUoSlKEIQhCUIQhCEjqj3MEYIIUlbbrEiNPss2xOs55c+fk8nk58+RUVFXIknOc9MgRLJDtFAJSEBASlCUJQhCEIQhCEJT2T7xBBCgpKkLadjuxpVumWCTaVNZznly5cuROckk5znePaounosPASEBCUBCUBCUJQlCUIQhCEJHcfgEEFJQpCkLacjuxXY0m3ybI/YHrUuMW8HfPRtlu0s6dYsEeJjgG0thAQEBCUJQlCUJQhCEIQhAT9CfwsEKSpCkKbW0uO5FciLiqiqjLty7OqyKsB09/54afFjRaG4fj8fi8SWQyGggN8A2GwhLaW0oShKENpQlAH0j8UpKCgoU2ppTKmFx1RlRVRTFMYxvjGN8f4/wAf44YDPi8Qa8Qa8YbDYbS2G0tpbS2ltKAn6x+PgpKChSC2Wy0Wi0WSyWSz4fD4vF4/F4/F4w0Gw14w2Gw2G0tpbDaWwn7R+XxKCgoLZQWy2Wi0Wy14/H4vF4/H4/GGw34/GGw2Gw2EY+8fnYKeBb8ZbLfjLfj8Xj8fi8Xi8XiDXiDYRwx/o2MFPHhw4cOHHGP08YxjGMYxjGMYxjGMYxx48ePHjx4cOPDhw4cOHDhw4cOHDhw4cOPHjx44xj/ut//EAE8QAAECAwQDDAcGBAQEBQUAAAECAwAEERIhMVEQQWEFEyAiMDJCcYGRofAUI0BSscHRM1BicpLhJENTgpOiwvElYGOyBhVEc5A0VHDS4v/aAAgBAQADPwH/AOfFhHPebHWoCNypFwtIUuaX/wBEVSO36ViRWoB+VmGqmlRRQjc2ZbC2Z6XUDfe4Ae7EQhxNW1pUPwmv/JrLCbT7qGxmpVI3Jl61md8UNTYJiWSf4eVdX+ZQT9YnVfYy7CBtqTG67lf4kIB91AHyjdJ25c9MUy3wiHF89xaus1iwm7HOL9G9LB1YGAcDE0x9hMvN/lWRG7DXNn3j+Y2vjG67fPLLv5kU+FIdFPSZFBGsoXSNy3ftkvM9aaiNzZyno84yo5FVD3QCLsP+QqRubJV32aQpfut8YxiJKVr+J0/IfWN1ZrGaU2nGjfF8YUskuLUonWTXhhe+JopSwi0Anr0UirLrp+zRS/NRwHz6hFQIu4U/JEeizbrdLqBV3dE+zQTbTcwnPmmNy5ugdWqWXk5h3w0+i2y4lac0mv37KyKLU2+hsbTeeyECqdz2LR99z6RPz9fSZhZSeiLh3cFpvnrT1QyitLStoj3UUOZh44WR1CH1dOHj/MX+qEoQsrBL2KHLRqjz52yzssoPyn8UTUvJcItdmEMtmq27euilEw7Oob32y2y0LLbaBSkKGBMPIwWqHxiqvWIV00pPVdDZ5yVDxhleDg7borhwJqRcC5R9xo7D8omWaJ3RZD6R0k3Kwjc7dMfw0wm17irj98ye5qLU06EnUgXqPZEy9aRII3hvC2b1Q4+4VvuKWs3kqNdIAJJoIZbwNo7IWeYAnxhxznLURl+0EwtZogFR2RMqwaI67oeOJQnrMZu9whHvqj0cilSk4GDrAVGSKQtw644otLNdkZOd4hY1pMODo918KSbxfChC0c0kdULHOooQ2rncWAoVSajMaShQUglKheCNUT+59lD6vSGRqViIkN1UjenQ27/TX96sSTO+zTqW0ZmHXLTW5id7R/UVzuzKHHnCt1alrVeSb9LbI46qbI/pCgzMLdPGUTClGgqYmHLymyM1QgfarKvy3RLt4Nprmb4AFALtN2hK0lKxUbYv9Uu7JX1hwG9SKbKmEtX85WZ4NYbVikdkJPNJ7YWMBXqhSYUg3E12QenfCHMDfkdKkKCkKKVC+oiakbLU769jCusRKbqMhyUdCtdnWPvKW3Pq1LUfmP8AKmJndB4uzbqlq26tKGU8dXZCjUN8UQpZJJh+YPERdmcIQn7dVo5CG2hRtCUjZwLuRMGDkeElXOFYSqtk02QtFbrsxCkQRcq8bYSsXHTMSL4dlXFIWL7oanLMvul6t/C3qUfPnXCVpCkkFJvBBx+7mpZlTz6whtN5Jh2btS8jVqXwJ6Sv22RU346AkVUaCKVDP6oUskkw/M30sI95UMMXkb4rNX0ig9izgGMjBHBQ5sOYhSLxeM4UgxW5ffFRUYaZncpQamyXpY59Hb58Yl90ZcPSqwtJv2jr+7JfcuX32ZVjzUjFXVEzus+Ss2WRzWwbhpRLp4xv1AQt9V5uyEPTbnq03e9qEMy4Cl+sczOA4AGMZRX2MHERlBGPAQ5fgdkLaN8FBvgODbpmtxZoOyyzY6SYld25UKaUEvC5Tf3UxuTL2nOM8ea3n+0P7pzSnpldThTIbNIZqlu9fgIW6vMmCqjk3xR7mswltASgBKRqGkDGK4e0g4QRjpBFDhGJa7oU2rqgLABxz0v7nzAelllKhlrhjdpgNOmxODEe9+/3QzuRLFSqKfVzEfMw9PzK35hZUpRrfpsgtsnrV9Iem3ghtNpRhuTFtdFve9qHVpoL8I9zviuPtdYyimOlLwyVnC2V0OPxi1xV98UOh2UfS8wqytMN7rspYmTZmhdf0vuZncmTU89eo3IRrUYe3RmlvzCrSlHzTTi00bsCR8odnnrLYu1qyhqTaCGhf0lazpDYvxygrN/dyJUaJFTkIS19u421q4yr+7HwiTQD6xbhGpKbu/8AaEV9VKkj8avpSJkn1bLSB1V+MTq9bQ6kCJ3/AO4id/rmJsdNB60xMV4yGiNgpArx2CB+ExLKxUpByUIQ59mtK+oxTHkaxTSl1NlffCmF34ajnAVRDnflBQaHQ5KPpdaNFDK6sN7sSyWnVATSc+n+/wDv9yNScq5MPmjbYqYd3VnlOuXJwSj3RlpsAstHjYKPyEOT79lNyBzlZQ3KshtkUA8evTY4qb1fCK3nHkA0i0+tLKThbuJ6hjDKbpZpTx95zijuicfFFO72g4pb4ohOupMAYDku+JhrBy0MlXw2q55BQcxeIS6m00oLGYv5C6KYYaUuIKVi6FMLvwOBgLSG3bqYHKKEg46HJCbQ8ypSSDW74w3uzIhYoHkUtp+Y+4qR/wCYTW8MK/hmjxfxH3vpp9FbKE/aqH6RnDs9MBCNd6lZDOG5RgNNC4a89FYpVDeOBPIJab3yYWGmzgTirqELvEi3vY/qrvUerLzfCnFlbqlLWdar9O3gbY2xtjbG2NojbG2NsbYU2sKbWUKGsXQRxZpFof1EY90JcbtsqDiMxq6+Qy0pdQUrF0KYcoewx6SgNEDfU806zs89WWl3cndBtbarsKajsPnbDU9KNzEuSW1jXiPuESkt6EyRvro45yTl2/DrgnHQmWYU6vqSMzDs7NUFVurV3mESMsEChWeerPq02AW0c7WeGpxVECpx6uuGmCUSll90fzDzE9Q1wt1wuPrU44ekrkJefl5RapbdFVsrCy2ptKXMbkWiK4X9UNt7oqa3NmUBhpsKfcmXEgNKOAJA6tXxhxe6ss1OPNrlHWlO79LOVqBQXEjMp1a4mkhDkiuXnWXHt6T6M7vlk6rRoNWuJtuWmXWpiSmDLCrzTLtpaOsU2HuiX3HU0JebbcNlKXWyurgVQ32ac3Dbfw6wtly2yooXmIbfol+yy8cCOYr6QUKooX8PLSl5uycc8oWw7Q3EQJlrfkUtC5wbc6eb+safRJj0WZX6lw0NTSyfe+R+4G9z5J2ZdwQLh7xyhydm3HnlWlrVUnR3Zx6TMcW5tNyY9HZ9JdHrnBcD0Rp3pN3PPhF+fCAbLrqt7ZTio/AbYVMp3ppJalvd6S/zRTkZpTW5qGw2z6B9kWwRXC9V+zxMT62HJlctua4zOJCnGVA2SU2+MQVY+rPcml8bs+mB5DMrvaJdQEuAN6S1rurhxca5ajfup6j0RmRlky8wkJZYACFrUCLzXK7HXWJ/0dwNsSclv7lXFSyaLWpNDxrz7w8RnDu6623JlmXQ8kEKcaRZU5hzj2ciCL4UykNv1cl9XvI6o4oWg221YKHDpp31u0kcdPjBl3gSKpNxB1jXG9qFk1QrjIOY8+I0FlwLT5EDdLc1LTi6vsgC/FSdR+Xt+/zfojJ9Uxzr8V/t8a6d6a3lB4671bBlHpczvjg9S1edpy0htBWrCCtZUrE8JDbRefVZaTddio5CJieUlSk2G0/Ztjow7lDsKSkla0pAzhB5q7QzCDAzV/hmE5r/AMMwM1/4Zgfj/wAMx+f/AAzH5/8ADMfn/wAMw82Ultx9JTcmyFCmv5nvh9SClT0yUklRBqbyLz21PjD7QWGnZhAVzgmor1w66ltLrj60oFEBQJsjIeHdGxf6I2L/AERsX+iNi/0RsX+iNi/0xsV+mKYg90KWKpF0Oe7Cx0YdllGiLTSuejPbCFthxk2mzd1bDw6HTva7aearwMb8yqXVzk1W2fiPOV2Ole5e6TaweLW9IPOTrHzG2EutocbNpCwFJI1j20bnbmPTF1sCiBmo4QXHSVEqJvqb9CW21LXzU3mHJ2cuFXHDcITJyiGUauccznoqbo31dE8xNw+vCSEqceVZZRziPgIVNuhxYsNpuab1JEUGhLLZWs0ELm1Au1S10W/mYphh7IWlVRhrT8xAUkEYaVMOFaBaSrno94QkoS40bTSr0n5HhV0h1CkqwMLlpi0klK0HEY1hKwh5oAIcFaDUdY86joKFBQxF8Cb3PMopVVs3o2o/Y/H23fJtMog8VgVVtUf2+J00QlgG83q6oqtU0sXJ4qOvPTvTNBz1+A4VtYA7zqj0p0JRUSrXNHvqzMU0JabK1mgEKmVh525I5iPmfZ97Vfeg4gfGCimBSoVSoYKGzRSAws272F8+nR/FBQog94+PI4OjqMb407LK/wDcRXURq7vgNJ3O3TacqbKTxhmg3GKioNRmPa0Sss6+5Ww2kqNIXMzC3XTVa1FZO3RZBJwEKmpskVqpVEiBKSjbKeiL9p0VVfhjWN9eUrVgOrhEJEs0aLdFVnJOXnZAQAlOA0+lu1/9OjAe8faaVbVzVYG1Syr6QQaEXjUdO+tGWWeO2CpsnWnWPnyIcbKTgboXLTSVpucbVUXaxCA6S19mqi031uN9K6LDyTqwj0vcRoK+0Y9UezDwp3e17zuYiWHOmF/5U3/GkVUdG9SagMVXRv26G+nmsi126tO9Spzcu7OElCVOL5iBUwoJU679s6anZs0lZDCDeq9RGoQEpCU4C72q20FdNNysL8j5779K2XEOtmi0G0IS4lDrX2bgtDZs5Gy6FjpQXtzkk1JYVYvPRVUgU67XfpsTpYUbn0f5k/ta9r37dhxAPFZQEfP5+Gm1MpbGCB4xvO5gWcXVWuzDTWYsDBAp28LfHW2OiPWL+QiqzTAaLCSo4C+Caur57l/KUhHvp74Qemnv5WwvjVsG5VMu8dfZBQspNKg0uIPjpttuyxxHrW/9Xh8OFdptyxzTfA35xtVgb42RVQw13bainbp9Enmnf6awu7Xsi7Z7SEIKlEBKbyYMxMOvK5zqysjz16TMTy6X2lUEby022LghNm7RRdTgmpgrWpRxN/C9S4+cXTUdWrTbKGvevPVyYSL/APeFq/APGE6xaO2+EKtqWDZQLVE3awMe3KGxYUhJsrBICr6XkY68IT0eKfw3QtOPGGYxi67Dk7TTa9dLBvvu/Yju0mWmmnhfYVWh1iAhwhJqnUdmfIVSQcoVKziHE0ttLBFdhgNzDiEm0lKqAjXt0UeG26PSdxZResIsn+275cG/2T0fcKcVmix+q75xxhs0b1LOLwISSI37dZgFNQk2yOrTYlXlfhs+fHhUYIGKuLFlKGxgBptvuKy4vJWRt1CL6m9WeicnKFpohJ6Srom0KCw/vbgwKa3fCJ1ZLhf3xZ1q8mJuSrv7SrOYv0a046xqMXAjA8l6p1JIGC+0Xf6vDgb7ufLLOIG9n+39qcjZmlZG+Lbcu5ZoFNJA/t4vy0UcSdsWtz3mdaHK9hH7Hg3+yBO5jDVeMt2tNgB+oj1itl2izuese8aeP7Ram3nfcR8dNJKnvODwB+vCtTLCcqr898VeVlhp9SCcVX8laVazw6tAWlE1PJ2pSYbaRRCaUih0IeRR1IUnbAlgZmSHExUj6aONT37u3zdyVHBQWiapA6wR8+BWTmEa0rSodov+A5GjqFZikKVudLrJuSpTSeyh/wBWi6KTMw1qW2F9xp/q4N/siVTMi0cUhRPUafSLzoQtsMoVUhVT57YIlnXMzTz3aaSzI/Gr5cKs6T7qIq4qms6PVr6ooyimXI1SRndoE5us2lXMTxjrp5rG90pcMtkINanCBS0CKQmlokUjVAdbKTgRHoe6bzQFkVqBFUGKqJ97jU8eRKKLTikg8D1kyn3mv9Q5H1aDrrFZXeyrBdoDO6/4DTve6jQ/qNlPhX5cG/2S1u03TosD4qMNS6auK7M4ceqlviI8YW6eICerVG97mqQcUkA/5tPqpf8Au+XCW9MuFDpbAoLhBOLqoTrWvvhvXU9ZigAGAu5G1QbR8YyJim667R/lnHz1QVIUkGhIpWHFIKEtNp4hTUK/aHVshKkpuUDS1XV1Q68222AhKEVJBvtHqFImA8FLpxUUtVxNfpBaZSk4pi3u27RV2zr/AHi41Ku+K02JA8KcjUQMzGSjB96CJ1VT/KX8OFdpqwPzaCOdhAULjH/F5Qn8X/aeDf7IuU3aeSi5xSAEk5WcfEwp1etSj2kwpXGf4o93XCWZUBoWRXV52RakHK42h89PqZf+75cL+Ie6gfjFOUqkiK353wdzt0mZgYJN/VDc2yl1o1QoVugIF2MVxiwqogLTDcjJLdWqyAIMzMuPKxWqtIqKZ3RUknXytJ0/+0v4cj6oQky8nd/KP/eqCm8QUm7GLe6cqnphWGynBv8AZEboyMvNIIQ80qwVH3TDcmpSUDjC61rOissdlI/gXM6p+B0/wsufxq+A4VJs/iR8P949Yrr5XuOh/ctW9qJXLnVjZ8+dcS062FNuJrjjAWi5X7wlpN6rh4RL7npNpxNvLE90TG671VkpZF4Ry94j1rxyap/mH78j6odcXNJPRQPG/wCei2bsYJ3bLigobwgm7M3fAng3+yKS3JIqbJKzTbd9TFJx4fjPx0fwT3UP+4Ral3fwpB8dNdz6+64PgeFZfaV/b2eaRR47b+WphhFYKFVQSkjWIm5lDi17oLbSgpHGoe0knijb87on5ZxIcnFqQtNpJSulR1V/bIxU3mpi/bFceWqoRRh5XvLCQeoV/wBQ5GiUDtgLeSU/02x22QNHrE9cU9Kp+H58G/2QmUlHNSVlPf8A7RSZNddFd4rotS7oPuGOM437yD9flptycwnXZtDsNfrwiWzZ5wvHXjAU2hxOB5euMZHvh5pp1pC6IduWM4ef3vfV2t7QG0bEjVG2KcvcSY3uVZScSm2etV/wpwsNJW+22kVVgBnWEuzj60CiFLJToq6IpLvL95dPD9+Dxuz2Qr3BCh0HUqPiPnFd6Wekj9vloGvDKPRp9IXgldFeeyLKiDiLtA3wBXNVcerCCh1SDik04VplbWtJp8x52fce+rbZOCsTsxVFtRVhXUNXBqRpqQBrj/ittCwje+Okn8ItfKmmrh2RY3PR+Ik+NPlwb+z2Qv8A/h+eQMQ3a/Sa/KAqVSdaVEdnmuned0lZHjXxbZQvMDTSYDgwcFe3hb3MJVqXxD14jztiy5XUr7htK2CKIW6elxE9Ws993CuJ7NNKq1JFfPhHEmF8TjcWh5wqa1Hd46eKpXZG9SzSMk/Lg39nsiXmXG181aSk9sFszcuuqVIOG0H9zpsPNu9nnxjfJSzrTl3fTTv0sQOcnjDhBbZSdcb+xRX2guPXFDf9wFRQ0i5a9eoZmAKJQKITxUjhWUhPaevTvW56zrXcPPnCKNto/voRrP7AabRYQdZqeFf2ey+gf+KniapaeNu1sUKK+cFtxSFChTcRo3yWVTEXxZcCVG5Xnz1RS446KXxvT5A5uI6uFvbm+jmm5cXWx2+3046o3psrVc44MPdTl52cKq6nmp4xipJOJ0FRAGMBcw2wk8VHmvxPbFpZOAyy0b46lOZgelbQm7hX9nstWZSdSOaS0o+I+BjfEtujppv137fOvRUEGDLThTkaiA6w2sdWm23UYp4V18b0rejzTzD8o3s1HNPh7baN+EB1VtQ9Ug3D3j9IJJJN54W9tBHSPGV57fHSG0rdVggYwXHFunFWmq1LOAuis24RghFO03/IcK/s9l9O3BnGAOMUWk9Yv+UW2XWDinjp+fy7tNLLycRFpJZJxvFeBvbppgb+EFpsqwMVq09er/u2xvZ/Dn7XaOyN+NBxW085XygAAJAAFwA1cIElxfMRqzOqCVEm8nRXCN6ZRKoxPOp580gYDAXaQxLJCtQqqLSHnTzlLofPbwr+z2UOtLbOCk0g7nbtb8hPEc9YAdfvD4wEr4htIN4OzQHEFJwMKlpizrQajaIDzCHkYK8/Lw0hxBGuLJoceEFi/rqNRzgg727jqPvRZvRh8Paa44QX8KpaHSGvqgJSEpFEjAcJTrgQjEwkANt8xOvM56UtNrfXgjDrgvvLdViq4DLTv0zaPNRfFhuwMT8IsSDVRerjeezRfwL/AGYvtTVkVdYWXRT3Tj52Rv8AKFsmq2bx+Wv1+OzTg6jFMJB3lf2bmGw+aRYUQf8AfTavGPDC02V3iFs8/jI97LrgKvTFDf7LXCAkVWYLt7oKW/d1nrigAFwGocKpuxj0dsp/mq55y2aStYSI3xxMq0aIRiTFTswA0+iygt848ZUKffonFRoBAQhKU4JFB7ZYm2ndTibBHVCtxd2iWx6o8dvak4p+IMC5TZq2sWknZ5+Giogy75HQVhs2R6dLWVf/AFCP823z8+BrTyFL2OL+E4RxrKxZVkYy9jrjBWbLKanwEJbNpzjuY1OA5D0ZNtf2x5o9z9+AmQlikfbK8PPnCCiqL7Z591Ozz8tO/v76v7NvxMWU72MTeY37dFGSKq8+Gi/2vfdzlkYt8fz2Vj/zTcr1YrMM8dv6d3jFr+FViTVsU6WXnX1xfoDrZBhyWeSoXOo8YTNy4mWB+dOR4F9RyCVposAjbCk3tKqPdV9YobLiSg5GMoI5UnVFMTBX9igr6or9uqv4U4QEiiQAMhyHo1HHhV/FKT0Np2xWtcTpRJsl1zndEQVrMwsq30n1YFwG2vnw0rmX0NN85XgIbkJIJGCR3wXFlSsTFGVvHFZoOr20KSUqFQbiM4MrNOMqxSoip17fhHok16YwPUPHjD3Veb49KZt3b4nngfHzryrptcZPOELlHbQ5puWk64StsPy97KvA7eBXDHkQoUUKjIwj+WVI2C8d0PI6KVj8N3hAHPBT+YUgHDQYMHIxsgwY2wlPOMV+yQpX5RDy+dZbG28w2L11cP4vpFMMOQU4sJQCpRwEJlL7lP56k9X1iulEq1vjuPRELm3C67e0DQCvOONPr8oU4sqWb+7zlp9El99dHrnPAZRvztlB9WnxMFxYSm9SjQDOAww22MEint29vNTSRcriKpnq87IbnJRxl4Wm3BQw9uNumW1gKs4VFziYC20uN3oVgcth01NtHO+MKllEc5o85JhK0b7Lm02b6ZcCvXFDybKsW01zF0I6K3E9tYXqf70Vh4YLb7QRExm14xMZteMPHFxA6kwrpPHsTSGxzlOK61QyilltPXSvJrfw4qBio6oQwkpZGOKjirgNyjdpznak/MwqbcK3Sd7HichCnVAmgSkWUpTcEjIedum2oTb44g5gOvbG9pLLZ46uccho32c3w81u/t5C/wBnE3Jusq6QuORzhTbikLuKTSkI3VkrIol5N7aj8IVJTK2n0qCa0cTrBzihFCFIUKpUMFDPTU2kYwuWcqnDpJOuG5hNtjHWj6cC6MvbCpQCQSTqEBN8xef6f1MVA1AYAab4blEkAhT2WNnr2+TlBmSp15at7Bx1qOQ+v+xtHAADADVp9Nc3x25hP+bZCJFgJRzzclI1QVkqUak6zFTHo0mhJHHVxlchf7RvEyJpA4jlyqe9FU3wJ9szEuP4pIw98fWN5O9PV3sn9Bih+mkL4wuOcLYcyIhExzjZXnnBBoceBWKe0VN2ME3umwMulCWhRoWRnrPbwKAkkAY1N0BAKJY0/Gbu7zXqi1aLtQOinWr9r/OMFdK6rgNJnXLS7mE4nOGdz5UUFALkoGuFvulazedHpM2FqHq27+s8hdHG9oROSjjK8FDGFykwtl25SDTQJkGbkk+uxWgdLaILQ3t2u9+KfOUXAi8G8EaQsUOOcKZVszi6yu8bYCub3cGvsql80Ex/UV2JhKOYLPBalh6w1V7gxh2ZNno6kJgIJBotyuAvSPr8IK1FSiVKN5J16VTarbnFZ+MMyEuKCgHNSNcLmHStw35aC4sJQKk3UgSkqhsY4qI1nkLo43tO+telsjjo51NYi+KwmZtTMoAHcVJ97bDkqVNLSbFb0nonz5wgLQFoNpB1/I8Chq13fSFINFRUX3wFYcIGDBy5SuELOrvj3ld0IT0a9fCQym06oJG3XBNUy/EHvdKFOcZZspOs316hr17I4pS2LKTcq+9V+s93dpvi2Q5Mi7UmG5RseCRC33Ctw35Zaf8A1Lu0I5Lje0hQIIqDdQwdzpsuN/YLvGyNsEQifS6GzYfaUQCekDePjTsh+RfKVgoUOck4GEPji8/WnRloSsccVhSOYbQ2YwRj3x/cISvA8MHVCYEbYOYg5wc4OcDWYT1wgaophw22R6xYSctfdBwYFnacYceUVElWaifn2QlOHHVmeb2Dv78IKjVRtHbfpUtVEiphLVFOcZfwhLIojjLyyhbqlLcNokm/SZx/jfZJvUc4CQAm4C6g5C7Rf7Uicllsui4+EO7mzRbc5uo7NFjdRY/qNA9x/wD6iV3UaN6VKSaWhqMPyLvGFUA0CxFaB7HC19Y7jwAvnDt1wRzONCgeNjnr74I+hhJpW6AoXHg7NByhWRhWRhWRhWR7oV7p7oV7qu6FZHugjEcBKBVRCRthlFbNVkdkOr5hsD8N3jC136jrN0JAv457hBXjq1fTgLdN/FTnDbCeL3mOiyf7vpo9UjqGhc28ltsVrjs2wiWZDbYuHjyN2i/2tvdCXKVCi+iqHZGZLTwIprzj/iaDk0oeKfpDknum8to87EEc4fP4wxug3ZIFvEoPnz2xvdVy/Ny8+eqFtKIN2YMBWFxyPBrzhaAzgdE064WK3VGy+CNd/dCx+8A84DsioFnvMZnkylV3hFgcYVEAcxI7YeXgqnVC1kmpJzjM9mMAYDvvgk1Jv28BS8B2wlF6rzCWhxu4a4U7dgjLT6tPVC33QhsWlHUITJM2Res84jlL/bG90Zcg0DnRV9Ydkt0XkvIUkpATf2xWaWoUxvofjlhCkqqgkKF+OHnzhAUAiauPv59fhshqYSCmmYI7/PXDjKqEVEUxw2xl3RTg15wB68e+G0IJ5pxuh+yDxb+jD7d1g9l8U56adkNHG6GVYKhk9MQ0f5ie+G/fT3w376e+GhitPfDI/mCGE9Iw0MBXthSuY1dnSHl1ti7KsJKUqCioHK6kAUuHbfXhKVgIAvVfASm+iRtj+n+oxU3m8314Dkw7vbaamsIkm/edPOV8hyVNN/tlYanWilxN+cOyTylU/uHzgpVQii8afGn0imXXqh6UVQGqBihUMTabNRU9BXyzgGpRjkfr/vCkLpQ1OAMZxXDugg3jTQEmN+XbWOIOaDhorjF1NWUJIwHdDZHNHXfCRrV2GBqU5+qPxr/VH43P1QPfc/VCdfG64QMEj4wkYCBo3ld44h8OCpUJGOMUF/FG2KcwdpgqvUanM8F2acstJrmcuuGpNsJbAtdJWfLX+21huZbKXU1EKatKaTab8+aQplXHrTC19YuHhT5RTDz1iHWgA56xGZN/fDE2ClJBOttWPdAI4p7FX+fhsgoxFB3+MVTUXpOsXg9sJPXsg6jBfWoE+rRzop7BUEGCFbyqtej9IWdkAYmsAc0QlNam/IXweiKbcYJxN/CcmyFL4jPvZ7BDcu0EMpsgePJ0HAv9vCwQRUbYQ9aW0KKMOyizQU2HAxfQiihqPyjzrjLv1Q+zS0Q4j8X/AO0MvkJvQvJWvqMIWSqllRutJuPfCxzVJUPxCh7xd4Q4hhfq12qahUQhDNCrja4bULwL9cJ1d0HUYcG2FjonsvhScQR18EwTgIWdUOHVC9cDWYbTqhCmaA0IvEBbYKq2sqQdQ74UrnG7LhrdWEtpKibqCAijk3xlY2PrFAAMNnJ3cG/2+sVENTKTbSKwpupQmqcv3hxk2aE06JxHVFTrtdx/eLzrOy490fxTdnMYfTTdEutVoW21Y1SYmEfYzNrXRV3jE62TaYCh+AwUAb6y4k9UMm61DJ6ae+G9kJOBhs4gQ1kmGhqENjKGhrTDScVCGU9LugE8RClbQImFDit2dpiYXznKdUA84qV18hWHpmi3fVtZnE9Q+cMyiLLKKHWo4nh38nf9w1ioIIuhp8XJocoW0Txag5/WFoupX8Ko/iEhVai+ihXx5BpfPbQesRLH+UOy6JfUCOow2MHHR2wNTznfH/Wcj/rOd8DW453w3rqesw0OhCRgByVYmZu9KLLfvruES8pRRG+uDpK+QjKK8pThX/cdYqCCLsoZerQWTjDrNVN4d4hxqttN2ftJUQBibomX6Fwb0g61Y90S0tQlO+LzV9OXp9110bIadrabvzF0JJO9+N0Ps6lU23+MOJxTXqv9jrE2/g0UjNd0JFDMuknJF3jDEsPUNJTqrr7/AGCn3dXTjDblbbYJz/eGV1s1TsN8LBNgoV4RMN/y19nGhaFUNxyMKgjUYOR5B137Jta/ypJidcAIYIB940h41315CB+EFX0iVRTfCtw5E0EMS/2LSE6qgfPQdOfK0+9dkbIriIZOLDdc7MSxxZ7jSJX+kf1GJc63B1GJf33u8RL++93j6RKg3lw9ZiS1tE9az9YlG8JdHbfDLR9Wy2j8qaRlB9kp977I2RsjZwtns1PvzZ/+RB/yYNAgQIH/ACkIGgQIECBAgQIECBAgQIECB/8AO/8A/8QALBABAAIBAwMDBAMBAQEBAQAAAQARITFBURBhcYGRobHB0fAgQOHxUDCQYP/aAAgBAQABPxD/APey5fapcvMUC2YdfSvrjBJ2xSRQgtBu/QbqD2AtiLpXI0dhe0EUYAFegpEyYQck7qiEe5BuXL//AIZYjmINZWXY/AIPi2VIdQ0fDQPvEwfzU+hF0K9Ei+Q+IUDZDXvl8wxXWoB7DUftx1t+qXLa5Ym9wfrBuy28sxY/ePaGrbUBuLj1tM7WxbOPI1GLW/cpjJWGxfSYbQxrWoIUBqS9kZhE+S94b+IyHJYT3FMEKFZE0qeG1y5csl/+2tbxgQqgGq4IUARd13bGB8pBLfLCyz0IaSxUMr2plPKxchWqS97lDYIcceJzdKidjziLNm/ExMp7yjQAG2qCpWcIVjUq3EEbsTOTtAoBzxeYApwnYhDd27wvJL2O20ZKqxToPgMxp6x5JCdSOQmE4iEEKIaeWIILAKCfK1hvxF3YuHAN6YgNfBoinJdaY5hY1haHdCB/9a4018y63lhiNLBlPAxlcqKaO4DXzfpFBul/GxFHP7/2U2MdsTymwudPWGNJGm2fbX4lUVBYFD71Eqj5Cz2qEUv1N7hFL9APtEM+4/MI1ECjYzlpFw1lvXARYXsOE3rblrl7xgyqAgo3SCCeRlDXpQFVcbqqq84AoKKn4cTSN639YthPA18VHuE8vqufGzQ94Rqe77qgRaH1i7mYozvEasOC2y+r0ysMKNJOMwEcKu8M9xWukFR0y43eIcOeYdIMH/0rmRg5mFt2jQrj0JbRe8RGucBDOS8F3sWcxIn2RLrdu9xwrTX5jrKbhIgFbarzxCkUrENlnfT2ZeBWy5H0PiXwozlR7MTQvczLmZsFfiA4Lx+pgQ9sS/giVivi37wEz5gCJaGatF8afj4hU2l22Zft7TJgXJ/yIjSVwVCsEwsBQu0rLO+KfvNC8RfxDtT6PoWURAcmZSY/faV6v3VFgqOSn3IeZJ3cnuSuHlLPiLFuDmPLPnO8aKNgitkZhkQaoaFPBnG62w4oNqUmmnOULxbpcta37dAYf+fct4Y1I8X6vAarq0XgZeyxSQorZpqq8uMJHXgp2Vbu9dcxOujMmeJbDTpbL4NYxZx2p6G0ujd2C4PBtKcUdAL+n2gYF9yvjWVSpuAB6yoXA0fugAANgKmmk0NYj0CaMUn69pckDZZj0fiAKnJJ7VHgLR/wJptBqPfM111gBSCOokA+yfSXSLtlLdAnK/jWPuEe5TL6TkqZpwd+jAMZ4DG9IsfTgiOsAtI+Y+dGrNE44KANjLStxPMlk1zWepppea06CuH/AJlxjTaUOO0g2ndNW0KO+bKicVgFQOAMBvQGWKbAeMb394xZAHYOWF6vq938RECuqtr5fyyyMb8Xu/EbFd7Gerq/Ex5jINfXWb5iZxtB5iQgdYioHhilxUU8e8XyxGs/BF5I8hHbLgtfYlU5x5hnSOI5robQ+RmFJkurJLAp8ggjcrW5kj5nvMer3HWYM+6OtQyUNaX7udS8JrEmD4E1FVR3a50KwwQNKAg2RMIw01g/+U9CcLb0B91cAZWgjbXG35bTSglNc3Y0IilWVd5e8fkHVXBAFKt0Y9InBXVW18ygzuuI9DVgQo9jB40e9yqAoDase00dDrbjzAFzfiL2AirqtTaJCJnSa5JXRJTz8Su8dd4h0D6TVivEtLK+I9ks7SsxJtXOsqHLXGH2l2FOzbzxDGomjBBmNtxAXI8ou0VlLZpTxESdSJWmttfLlbbMKGWwgTLsLxv2aaszAQ/8e+lxJRbGc5sPa3QsvUtWbEaA+7Wr3dCgaorHaPdllueqyxZabUweeYWEcLWLO/21hwlXcOA39YhtitO3Q649oI2L43l2BXeJqbhGX2lYhmEZtjq9L4iYnmVNrm1Q3Aw99dmO4Uc7SsXPSGvFbwtBfuMPk3lCFGyZH1heyHDpMca3j9uYj+7QscYhQCUtwnjTbivUEzrWTkQto8am2NkUGvOkv/x77S/IFSc7LeLYvd0GPUYpoNgGwW48uqre8vnWX7A1df8ASOlVdrqpAwKtlq8nH17TTzgFH/e+s0T6proO28RVid9ZlW2+8qBN49Nulx1qVLj0uVxGJzLhKlSs3EKyD2dJlFTGaHrtH66TXTEYgK1EsYLqnd6+kpDY7HUj51tWj5iDULxW0a/RYqKZNNEdHWA7KC4MHJxQbDWlKyAlXnpcv/xHIAbXXbBoHzp4y0GP1gDAbEreYGWDYboWTx+UcWrQ0O96FbrpvAuQai+wHXz/ALY7+e8SIRQAyu0ssCdxFsqV5m0Dqwem89ZTnXDxBVN15n7iVmJMc3GVN6SOm/R6PRmmYjBycTCpzxKtWDxNo8GkeLhLBv5iA0GTgcwgPh03ESp9E0TtCKbdYjV5umtcl83nWHxEWRmF15Od+yIAYP8AC/8AwHgLw2hF0cAZXbuoLdbADAcA2AwH3tn4i7AsMq0d27dnf8tn2Uy2A8rL86C0y7+Dg0O+YGs+/Rki1oNfXiWRYNBoT0jV0ZlTXTpUSVWfvBCEaAtV0Jjoi2CA9xcBQdUU16kYyFeze37IevBH7xmueKftMmo8B+Ipq3kPxG7fDH7QMIrZPoZ6pi/6kOLo6lD1LganDWN+NYpUKb0cSvrx0eqw1nDAOQs0d4rpybMCsz094hATUGo83DoW2Q0H7+7wRQC4W78do5GkB82WJ2rPhjEvvFVYDdWZISM02VC1rYGUNTDFhh8fMvpcvrf9h/havhN3gDdWg7spWLAbBbLOreVxbnijxP31g5KCPbn6C+m7ZTIBQwPu7Bv2LYWXXLlXK3f0ros4MvENKm46kIlFWq7xjiGNnrXEcFwoerSoc6g7gneP2bYM9lA3Zyp4ih9CkJXIVb5hcrVqrKqkeamGj++ke6Pqj5+8YX39488y3iKZQRLA3Y5uFBV7dPnPzKLd75UcnzFobquHk1PUnjOm5KlYj8Rx0caxBQljrEVw5lZ0zL2iz3Hk4f3tKGlyUYT8xYgavVrfqPw5KttTCBp7RgZBJdJuDuP3N5U2wJw2Y7TrWyJwsX0D36X1v+q/wAW6c7Er1LLD2mmnJuq3dJ4gypF4SupsOXbi71RhN8hpdVng+vLiOMAzTL3WapSqBuW0WGht2PzFV1m3RmOWF8RoLcEDnywtHuPnB3mOtORO6Dim1ZOUcGlqKWCDGNsGKiuX2zF/8S/L7R732PzHufb/AGPcO9Y+scL0eD8+sbaW9P8AYr/iK3B6fvMtC3CX4e0tWiJeB2xFyxYtj2iwLTpAGDOh0dKbbuLDtyvZgOTWs8M37QMfbrcvEe+m8MtHpPrKllRnqPJxG62ahon77Rq61XVTm/LqG7ovARHIn7/scxopfI4HXtOvZwzmWPAFKQwibIiYvS9G4QMGEDL6n9N/jrlqSi2mFZQ2cGzBjKrK5hcJJaeBqBnY1fbcjVwCOU+32iN0yO5z6DSXgwRylavzCQCii27Ezs9UmczGIoaArNAN04DlcEMhKkrSqre3u49MxLRrXt9D6QA3vz6RCtCNcRCUT0PaA4PaNWHcwsaICVmrejZEXCJTltIBJZdAWmZ5Q4YVW3ClS5pZulFLSKC7W6Ay0IqfbIll2UATIXbYLSVLmHRRAFUKWthtmIcE9pjgmOCYiDtB1a8hChd6tiNmjqxESVCpOO9pK0yYKy0YAGuRyJyJkelStOmvjpRkekpq7nlEeLUblMgVn6RHIVAS7YrqBxdWHACXEHUijSA7jTM+cZDZUoIYfv7++kIIGDBhLh/RuP8AFTdZbSmgeVx21cESIpeaVcBegGA0ADaHaAaqAFVgCrvxQvgiO3tmlNGq91z29IRU6BMr93fsnKRc3+6xYmHZXg4c+eIlStltXWeZ5lRmeYG1FGxfBv2HlozGFwmuqNFlWcBghAsACgCp6dGL0ZniV3lGHqsJLWIVyQAchTQcUR5AFgwuzTgWhsdr7XIN8jhlQyBFl6oW4kRbKoadlmWWht4BKFOoF3ZdJm+yFABubQAaAKARZUz0ZnjpWKqIACOo7/ukF4+Frbm1uXqbj4QU6DjPbs50fOiLVYdZxKhHnaay8oYdpWsS2a9Cvw3IYACMImjIg0uaswlIMJzDEgKKDQoNiJbSFqRe0f8AqnIYHRWNqmVNgtCYGlTVrkFykIIIIGDmGIf1u45gkVRECk1cOaY0EQyS9TvDsShqDYa2nuU9g5h52wLprnhi3sd4mmLMyXDAcvEea2tf34j7zzHXPS5TOdZ2DHc54PINTtaKhym68uYDb8em8zUgea/MFYVqEAlmuDVhfjEf1n6TgkMweSBG1oJmShtIOnREDbQpxlMbp1bgQSgJQILSgF1RDhl3U0JNKcHNmG9sSnA4BUAC4KBRihxFH5n5nd7z8xp+Z+Z+pfmX/wBn5lP9MTs/qiBYzlcK3VolVHcJ6n5iXq3PzrE4tQpQ4F4fHMWg9l1VZ4Hjn0Q6amJjXeBHOHSIhzpKnppn8ypPNmv0zMXtoBUKsvIgIW5oLTHDke+JeKiRkLEWOnYLoDsFuqhU1RWIWJ2RHoEEEcoMecf1mzqEpMDDcNUvQeIm8FJZVtVdXvrN4itA5M4287eUjyypPvgPAV6Ep2aqG/r6qDsBG1EIwvnYgi3ot3r5RYRjrN4lQ16psa7jWO1rQXKp4o7jV5XvvnWBQZd11eJjggSzxdavByxhQ82Uv6aflsoAABQGKl9FGXUUrSKcRrg9p7HmL2i8xReYwsU3inEuor9cRKWbekJ8DHTtFjP0zMGxz5lKJUunY7n44EdkJG1a8CKY7jonTbqEASpUOrDXh2f3iAgTIlAZETSkKfEQIK3YboWpTaC3RzHEW/OC/k9d4IqmylomNdyuABt0CCFcGDma/wCsy2YgtCEHNNIzqQbVZXeKxYataOD3L9CZPHyDq19A169poiCZWoU7/wClRQW9CJz0RkF2qUALVdgLfSAWQRDcp5sniwM0qAcrqwIMgdq/HvA5fAA+RhjBg4l9GXFixYsYWMLFii94wosWLL94SUU4lp2HI7bmMUJeFEJ2hQV5EppERBEGFXI7QCCsoMrYdy2zcXNqygpqkSxEsHImfGeld+rxM1mjKidpgDXDr2feXaVp2QhckAQrQqjA8U8M5jzwcrXAQEtNQcXXEMBLkQRO1azuTYioiiojt/q90A2QLo5XY3ZSYYsCm2jjLiUwlQBauADd7QW0LUUYA+kOY00ByL6s0QqlQFcALWNptgOBoResWXzMtYN7cRagg9TbLbK0+nBh2gAAbBp7fdmKYFrRS+KiXlUpsAavcNv+y+3iX0XGFixYveMLGFjC7xYsWLFjHzGLre8MUxLcDAWri2BtKabwikuGpBEfDmMGKII8wb4aTRzZumfC5vDrtBYnR01Ib9hlxxFVoGQgmMONTEoKBCGoAQ1S6eETaOGUy1YXhjtlyNAoBYXdWFuquluX0N6K2LP9W94EETWhU3ht6bl3NLxCWQrHzWHVrcoT1mP79YePLOfSej916MQaang2/aK67xbmJvCXgpJ6WGgd1xBtUrhtTYDTvC28AYk4Ow0dfVzCwAKHaWS4+YsXv0MMML0GFFjCxYsYxjGMQREsSq7TKEsAwo20XbYItagqYWOWsYkOvc2eyYTvDqqu3bbD5CI+L3jPH8Dm53tj2lKKBl7n6RxGthooDVgNeztcORlZBUqrW5C9jJ3alvSydJUTX/UZRgmS7FSz5ukVZmBiWY1CcLX0oPeKYRivhY+jGcN2VbYWvyX3ltY0ddHWFJbQPw03rbM2WlHeUQ1tCp8fpNJiWxobH1+JfUwwwsWMPmMELUDlYHX2ENF7AmRe3NxcXeIsuMWMej1I1I0wqty0ApQC6UXxGHSkgWNYCj6cxSNjluXtv4CgHkC+XMRqt6lcdKjB7J2jAWF4Hpr94VAC7igD5B+hmd0rEQtW+FSLz4IJ6wkIiixGx/g08TV6f1D3MocAFrCzAMbKq12te0TMwFrSKjteu5dH2hGwanIC/nPrF1hBmJfAL9ohFop5VuaJjjp5hTKgarwVb8RTFN7GgewMyXCWGWnhdmX3mmnp9ui5cWLGGF7xEszS9AM9gfvpF9clUZ9S6fMFbbkf3R9mNOJvEQ0crbG8o4VFqiKoU1XRmysXG2w8y+jSI2OQKHk0fiKNkNqs/dotRjGMuPVrcvzMz2FYHCAgaFXupiwagF2B6Ggj5FHzGOAi26yeoR9eu0ZWszenQzVjRPP6woMAll2FnkIFtDQBaA7NXFY190OW28sMoLXbaWvnL16srZsmp4/qIOC4K8h13BMbWmRl85+kq9JnayDzWJmo1WlC35Jlv+7xeJWzSgPdT7EMdyMueY6elDXK19L9oRUAIeCj6PQIVvkIXjd+ZcvvLlxhYvQsAHVtcj9u/wDpMp7N23YNv3WDtoHGh+3AqWqwq9cvoM2ZoIcEwqt4A2pdqtFGRXEeQg5Kgd+PWpd4+OZU1FgU9G+5s6wmpg1eyajwm/kdGXGLF/isBEVFZapQHiksLFgHXv8AMs9b35VR8ul3m0u9qnEtfnpjgllqqB3sz8jGoR4DDS76rejaTQz6wXlca6AKPdJZUtmKZCPLx/UtLBkb2F+GBohUVPAV9J4IFZkr8YP0UcSy48ipPk6OyGq4ED1ix6eZ2qk9Cj5itDYAdqPyvRQy4N30htpUU8qv4iy+8YveMMKLFRrLJ8i22z1f3SDbRDitoDg12dW8roVWW6ChAoA/eJcAV4xCXH7QUguLeqotq3/CXpmUabTOzi/Vdm9Ql/mLGV/C+jAManJHrY9ou0YyzWxrgQXv0HfoyrqbZUSdwj2N/djtkScC+q2LUW4ccLR2wPqgWZmebUek1vH9RuMBd0Hy5k15VYuLuvP7pAFACN1QkVCoyOTX6roDEdFi1+PzZ6xiTeL6zsYD3X618QkqxX5lf1mmO+AGMJfc6L0FixZcWWE1foVCGlVRittIa4rkKKwFNwQ+kIA1AAboFGXOm7nvKWFas3XniAyy1qDbDaMd1KhKlAM0cSidrNU+peISGocZBNPRs9JVTDWKdP2olKFADQsB8P8ACuj1bYoy9xE+kON5ZBlT9QQ7i/S/fowhp00XXQqA68VPW/xCogsp3AR+3sxztXZjpcU11n0EsxmZjM3ulreP6ggRdw4QH1IhONYGXVoekPHfhpyxu7Xwe8aCoW0X1cStAeeLX3JwTYgou7hY9LzAg+UbIutbneb4eCpZqfR+IeJVk+0AxQU8dFixY+eixZr+rubrFIA0Ph/MIqqiFMriijl9UVgwOClExAcIVcV4YctwR9AACW5pizUdY1YEoNgQG7p24mWbQ1AsK60ptveVRgUg2HrvCUqAdFUpNuBDsVi8sx6R2O6Xofs/gvRldCIOjrF9nwx4DzmIf5hIBXT7W+pN7lVCJ0F+qVK5IlItA/D+YiF5pvb9/SVhdDruQwgnJ+4hCmK9z/xmUzLUzMEWCPLx/UMhKhi4Ec5Ard7QNl4DcXQFb9vYlK7TYHIdLdtTHvUFKQ1VnBeNWhl4jKVmz2/DpJnSMJW59oY9E2jFRf8AU/hMlb9Li4jGLLixj0upSyrNoxYhQoaDpXuJ6Ro0HiXljTesPkgSgAq6sur9SncR0SLhncbMdqrtxnvKRL/EKKF9+d4W1BOfQ3fbKFlw/gQBoDoHYKPSUB77eN/oxNQJX1/g/wAU6PTIaV8tPqwh36PRMMq2BmBVykCAi2Jrev8AeYwsHDvBiq5H359YY+uGmqVp4tuPZEazMRFpNTx/TYbCQWW7Abo2gVlcmpfFZSboXfYzVFaG+Y6HaMutSfcPvEPhWOIGCG8iwarmn6MY9N4zAupPuqDR6Z/WJ3jGPRj5jF6riYOdQXs8+MHtNOISXFUyytoasy4xTolhbCQLDB33PUO0Lggo3qUbyYuJaLLvQHGbr3mDwGi5HShlvbblJf0NJ17vOuDQO6qOdTBfg5l223kovY/Q9jo8xl/yejBYbXUHvweX7JATWFcwlzZhzEzMcOtPXMaYb4CR8CIyOYIlRVUPcgOjEB7KPTtMxmZppRaRWvH9NhgJ4HCAj5ADy8wDgoA9IrEBaslHn8Ay4bsQL7A+vQw7a/ioPyEdIx6VOIWqe4v6g9YyWqB8P8Y+Y+Y9GMYy+rHSnT9+I1kXuNyIwM0UlafchRpWIiPMX64taKiAoxkZui6IMphCaqUI31FVNlNIyia2q/MoU3ZAy/8AIDkABuu/LO+r0XpUf4PWolowZlsnyRI6BMdNoKDvKgYlybv3EOSgacB3yRg2Lw+sBcKVK8gYvu+7L6maaUxEWfj+kxYAzMnuBIVeop6H3SoejLQ5QU+Qh3Fwa8FD3EYw61cJ3BfEOmjG+I5ly4pC2PCoHuEOVywu4lnx9Yxi9FjGMeix6fDzApS00dzw6kX+BcD8IAFEbNRqniBkxeg1VYVYW942KVXBg/PzAFBW70Y/wZXRj/ALajT0q4oiqHtZT1wenQejK0ZSAraVPpCwFABlUQ+0OMJjYWwjpcFOryvxLN2F6BjQncmhvFpFa/pHpbDTg2ED5EKGWh6Uo+I01gpZsajcvSJhmEcGp8veNVlFVnTWLA7oecK+FmBdiO41N+rHIlp4lxAKB2fgyHnslhpKdK+sY9GMYvRjHo9GPWujH+FRej/D63pLgIuLUqoeC41IWLRRZ0PGk4gTvtCUJ9fT/IiqysxgF2A8rX3iKYNUxaA8rR3Sd6zr8x0qKjYe2f8AGXDRd/TiNCd6aEek1/6Regslg+h9KmBm8OwgQ94alYTZhb0qA5OF+VgYZ1V6ph+S/XoL++sqJgp7MPyX6xnpNp2l9omwavDqPdTzCVTe7XeT6R6MYxYxjEjEiRi/wuL0YkTq9K/gwNXqd4wamy9iPasAd6TeVt0J336MeneXX4lcRmt4Snh0H3YsrtrUv6ACL8bwVUZbSbWmPeXMUkPnJ+bjwRGItItIs/1t/UFuzHkCJ7MWOwpMtJO1Wekd85m0QYc5N4DKHzFfa0sOCW+nqYtmsXeVstU96DJ7Z9JhBvWesxz1uSoVZqd/TCeIlKxadgmvhM+sCgERpOOjGMZcf4MWP8nqx6L/AATplaC7ajUCKsYDKVsArXbmIShhWoBi+W7V3VcXDoVEmnpUtMpD1Bb7Ae0qJDMQeqtiz6r6yl9cWqKUADuKDuvTfXiMCcYVmrt+LmNPeLJmLSXVL0TV/onosYS8kgWrkOctfES2pQUiNJLxKkBAGM2f5iECgIrkrf6j6IFIUGk4YwbA1IAakvlbdMcQjF4lyCwAODR9Lb7LxLae2J8vg6OejHo9WLGPV6+v8L6P8F6AFSgW3Qrd7fiOApsrHAnk4XVMCskvcKh0xNCobnY/YD1U/SWQKlr630GUqQDdbqoJekFCy72QUmWOAqDjOxtxGICWAem8Ul11HV0FPc95pqDSOqm2PSav9EvRjDFB3SpGk4GzyQac6EVVw5bqW9hKQsoEqMZgpO3EcuxBPKBS90q+9x6FeV3PpL2qVCJGAoAiUjxsSpfUszju5rTkO2WU1bbdw9GLHo9GMXHSur1x1f4PS+mSGOsIGamwLg7jC8tBuxEClq6ry8ytumIEvnHMt/gdxTA+BL5SpUSfTk3XVe4CncJdrahTgMaZ0DEdIxTWFHneWAaCLsFtXp7E1EOkMOk2zV/qGUILEdkA</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxIREBUQEBASEhIQERUQFhEQEBUSEBUQFxUWFhUVFRUYHSggGBolGxUXITEhJSkrLi4uFx8zODMsNygtLisBCgoKDg0OFQ8PGTUdICY3KzcyKy03LysrLzcrNy0rMS0tLS0uLSstLS03LisrLS0rLS0tMC0vKy03LS0rLTgtLf/CABEIAOEA4QMBIgACEQEDEQH/xAAbAAEAAgMBAQAAAAAAAAAAAAAABAUBAgMGB//aAAgBAQAAAAD7gAAAAAAAMaa6M9N8gANdddNNNNcY11w7WmQDjH48841xrrjVjLbfrNlhBkdIMLTO+jbbbO22dtsmdZ4eBpJfprPDrykIHeUxrjGuOjM8I1L56T67OccsAAhzNrABxg8+u2uwyDKjsp8oAY56664xjGNYu+/SqnWfYAAAVtbLjSrfIAAAV9RPi+hyAAACpgypc8AAACkiTLGSAAAB5KTLs+wAAAInkbWZa7gAAA5+Ps5VuAB56wp/T7AInmrCdZABBj8a+FaWdkBD8xb2EwAcuvmqqdxj+hnSwV3n7S27gCpjVfbfPKXMtwUdbY3W4BFz55rEkw/Rx78FNEmXAA5+V1xI52PPG98CriW8gAY8rG79qq/l0PppQIcOwkABG81FsJ0OHcXQEHhImZACm4aR41/agK/M7IAEONvY5AK2TJAAAAIUnoAAAAAAAAAAA//EABcBAQEBAQAAAAAAAAAAAAAAAAABAgP/2gAIAQIQAAAAoACUABKEiJrSUIDn1SgCTSUAc+hKATHQlASTZKAYuiUBMdBKASiUABKAAlAASgAJ/8QAFgEBAQEAAAAAAAAAAAAAAAAAAAEC/9oACAEDEAAAAAAAAAALRIAUNYAAtyABrIADWQALcgAakAA3gAAAAAAAAAAAAB//xAAjEAABBAEEAwEBAQAAAAAAAAAEAQIDBQASExQwBhEgQFBg/9oACAEBAAECAP5yuWZSVL5aEtnRe1cV6zKSpalKQsmvWsiyrPyEIgKa7pkJeY8nf31mWdSFI31l1+/XrSkbYmxAu+Z7aInUUQ5+pMRqNSFBkF4iBoGgaBoHxOLx9tUjf83yqSP5dReQrJ62Uje2GciXiCN5vN5ymcvluJjnSb0qfJQBvidh4h4PT6txJFVc2djY2NjY2NjY2NlR2Se43dEw0gaPSTW1yO169erVq1atXtFbM1A4OpWqOoihKDwOBweFw3C7zZGuTLMuvr4h/wA1xBE+JbYymrET89rM2OBAx2t/Rdo2fAWfpuHjo/BW/pnsRk9DJ+i3knGAyJIU7PeIvTOlygCionbZu5VPaNk6LLLLBY69vXbuqbXyWzEWJgdmBY/do5yJgDepxGW4RUcssTnsqMr5vq4dDj8ETquAhLuaeESaNiwZVvCf9eQ5XDvWFvTYGhHWkNcStUmGsHIjFCd9XiCNgH6iICAlZtEMa6siswnPo2fV5EC0RnU5LOOGcUofHRVZc8hE9aJ9W+VqIR12Ma16jCyQyJGYZR1f3crXoarU6yhoHxzPLhbVUvRdrXMaztnrXUUVG1vTeKCn67EWBn+E/8QAPhAAAgECBAIGCAMHAwUAAAAAAQIRAAMSITFRQWEiMFJxkaEQEyBCgbHB0TJA4QQUI5Ki8PFicoJDUGBj0v/aAAgBAQADPwD/ALcNxS70vOhtXKuVCp068bil3oVyo029Hf2BQ9BogzwOooESND1SjmeVHkKPaPjTDRj8anOhvQ9HKjRo70d/YNH0RKnvHtWkcozQRvpPfStmpB7iKOx8qY5AECjtR9MEj4+P+KNHajtRo0eoA1rpA6Cf7y9orecHtE/AnKmUyjFT/pJHyr9pte+HGzj6iv3pWODCyEAgGRB0I86n3aPZo7ejpD/b9aQCCcwdief1q2yMmIjEpWQpkSIkZVb4XruhHvHI/DnVu2SQ7mRBDAkazOmVJz/lNLs3hS7N4D70uz/DD96Gz+K/ehs/iPvQPBv5gKA4MZ3bF86nTz+1cTmay9q3c/GoPPjVtvwGKuCcInnVyw95rpkMqqARGYJJ+dLypaB9HS7lHmT9qUyYEk/p9KXYUvZFL2RS9kUvZFL2RS9kUvZHhS9keFL2R4Up4R3ZGil3ATr5iJB9EkDqVYZj4jI066dIctfCoyIjvy9ArU8T/Y631v7Szr+C2MM8CdPqaJqMzr1YOonvpOyKTbzNLu3jS9pvL7UO0fAV/r/p/Wj2x/L+tN2h50+6+J+1XBwB7jWcHI7H2Gdv3ez+I/jfgq8R30EUKoyHHc7mgPy+Qca6H6ekoAlvO5cyHIb0La7k5s3FmqNPzAAwxrnNEZ8DofRjuNdOpOFeQ/xHnUCNvzMEHfUUWgHILoBXRPPLxyrTvJ/NS8bZejId8+X615CP78PzVu42JWlWYqGggEgxlIzHMejpAf3mf0rInn+ZK2LhUEt6tgoGpYiFA5yRQt2FtEQUtqv/ACAE+dSoJ1IHyqX7vt+tdEeP5nId8+GfzFYhOzA+eYoFRGmlSSdzHif8dc9m96zg2YOvw566bUP2j9nLW2gsu+YO1G3cNu4TB31B0n70DoepOCQYjUb8IpXwBcmZ8xBgR3moGImSB3DTatO+fD/HWOLcpw/FGRjcRQcYbhAZROI5Bl3Oxq1bRUcYvWHIr7oHvc9aa1cw/A7Eb073Lly7bICMYbDBwn3ROugz50olHYBV0Y9nY0jjErYknDig5NsZ4Z9RFs/CpuoNgx+VdA+HjlWnJfn1ahsBYYjw+nf6PVtit5K2oHunXwoOVZkLm2CQmLChMgweR1iruIM2QKhhpIB934TV9URAfWY7jF2ILBUyyM6CJNKSWTNJIEjxHmKt+oFtBhjUcznNSuE6rl8Pb6Ec/pU3u5B866IG5ArI98eHVkg3EBPvFR+KQIld8gJFQAryTH4ozH3imU2rhS9cYs6KrNkwnO4QBkTOQ4AUgDC3d9aVYkgkSoJ+9MyqhwyHEK5iQNjvWDEDMnoFScIKmc5qFcFcFm2JGUtj3nif0pVwy0G4Mg2ROe1RejcsPr9PbYkBWwmJnLzkGsMycTMZLHjXTRe9j8NPlUKBy6oWVxEEyYypLqyp01HEfpStewoCC6l5A6AjjO88KKiGOIMMLYZHxA4GhZUC0rXfWnCWj8K8BA+fKit1Q6klCWU6CR7rHhnFXbptgWoDLiZp6K6iMXKPOnViceq4QYB+M8eHhSMEuvDuiDp6CRxjSpvJzYn+kn2+kO761nRN0sdICju1PVq6lXEg/wBzTWLhwvKGRkcwTvGhjxoi03q1dz0EW2CcCAZ4hznUnemUjEIOR3BHeNaxRdLnBbAi2phsfyivWs7eskmCFKgHmMvhTQQR0Bri07gONY4uBQsjTjHAkcKwW8HE/LjWK6z8La4f+Ta+Q8/bJUMNFyPx09HHfq5BG4irlhul0rbHouBnOx58uNDA2MsBdEBRokdxzmkFrAygKq9EqCXxE5zSYjbZsyhyiYETJ5xTLhvIT6tiRJGZjLhoaW4AGGa8OB76VFLNJJ0z8gKLHISznCqjfgK9VbCanVjux1Pt/wAFvh86yoiMQgHIEHrA1shhI1I5cahoBlTvtT2wHBDKZkoZAO00SrG2qi60dM6wddat3EZRDEQrHDGYHu8pBNLZMzntxonNu4KPkBRT+NdH8Qjor2F+/Ufwj3iujQcBVzM1AjrDbJgYrZ8Vnh3VaS36tZC7HM571bTQH4VhBFtVtgmSRqT31cvGLSlzxc5IO9jS2jjc+sudr3V/2j69T/DHNh9a6Oe1AaDrrbZxhO6mPLSkP/Uuf0f/ADVgGSpc/wDsYt5aeVACAAAOAEDquig3b6V0fzjXMOGOiTIPOKgQf/Bf/8QAIhEAAQQBBAIDAAAAAAAAAAAAAQACEVEwEhMhMTJBUGBh/9oACAECAQE/APgyY7WttrW21uNtbjLW6y017XdHDC0ilpFKBSgUoFJ7RII7zEwJQHs5jy4DMCCm+TjlKHaZ1ObiS5MENGUp3if3ORP0L//EACARAAEEAgIDAQAAAAAAAAAAAAEAAhEwElExQSEyUGD/2gAIAQMBAT8A+JidLE6WDtLB2lg7SLSOapKkqSpKkppMGbgJRPQuHhpN0I+ou6TtXaCdybhzfP4L/9k=</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxAPEBAQDw8QEA8VDw8VDxAVFRAPEBAQFRUWFhUVFRUYHSggGBolGxUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDQ0NDg8NDysZFRkrLS0rNysrNzcrLS0tKysrKysrKystLTcrKysrLSsrKysrKysrKysrKysrKysrKysrK//CABEIANcA6wMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAAAQIDBQYEBwj/2gAIAQEAAAAA9wFAAAAAAAAARQAAAAAAAABFAAAQUAAAAAAAEbU5HJXVxc9Pf1SqoIoAigNgqcz53BM6XnrpLHRaG+sO6ZVEFAKjE9M/QsFXV0NXYdrkqKzSb26t+5QASDzbRwiuklbOnFRZjg1unkVpZ3DkUExnZFI9UYxr5+hYuXoZEx803XZgCYKeSZ7lV42Nh0V/BdLNP0TR9cqgead8sz1c5woNrMkuv0cmR0FyzmsgG+XWU8sjh6qKiNxFHpfT5M95h0ei994BD5jYzSyOVXI8GpVee6zcZLwiW2sPadkBxec98sr3uFVVRGwYHS2Xm+W5bTq9o2oFXg+uZ73uUVQRkeLu+3pbkdWy31oFJjJ53yuVVUESNuTtOx5k9SlvsAKDJSSyvkVwKI1jcvZdgmT1KXGxUM7lXyyvkc4ARGx5mx7Yyv7UuNmoee8j5ZJVymj65FREIs339cNVh9VoLnageWeP6XTaLplbWQWFig1Ic/29fF5pkLj2W72gHL455c/svtJpbRUFa1sVH19GPzuN2HpdZ7EoNx3jPJbVtdDY6PQX3eNbFTz9OXt4MtlLX6dUBvLT0FHW11ZXcCWV5eXVhVS9VFj83z7j2TSKAAkNbR0VRx1tZW17Okmdz6K87NHtLRQABFRvJVUdLW81djeO27tDeanT2DgAAEUARnJWVWLzWx79Fo+pQAAAAQUAEajnAAAAAAigAAAAAJ//xAAWAQEBAQAAAAAAAAAAAAAAAAAAAQL/2gAIAQIQAAAAAAAAAIAoJLKKBkCrFMgFKZAFUkAKpklClJEUUoqSClBRJagALAAAP//EABYBAQEBAAAAAAAAAAAAAAAAAAABAv/aAAgBAxAAAAAAAAWACrCxAtAEhaAhC0BCGgCELQEIWgIQpQQgoKhAKBAAAAAD/8QAJxAAAQQCAgICAgIDAAAAAAAAAQIDBAUABgcREiAQExYwFEAXUGD/2gAIAQEAAQIA/wCI7/suOStmvuVf8tReRYe7tbA1srFsmUlz96lqmzdju9ruNgb3L8z+5OrSONRrydri8iQeQa7cWruNcolBX6r+8VaNV6GUyVOOw5Wov8ZzePmaBq9/OEzlaLP0RoU1/VmPYw7EH3nSa+K5F+rwxKku+X8VtlxiVRz9AseOXNE1/W0xPqIOAQZyFe3IMkFKwRngWDHLWIeblpkFp2MzKUFKUsBKENIYhO+pxxfmnEkEK8goHotqYKA8mysl1lziW0x0MoZSzPjxXvWtcQpKkkEHtOA9+RV5LTNYsp7jmpWCWkNctV2o2/anahXos68UKSQUq77BBJBKs7dG5wtZkV8hoZsO2aFvI5ig21M56TFa3iMQUlJBwHvBnZV33fR6VElmjsd75BkWolRlsbDoVh6XK9eCcSU4CMHwCCFdnOyZYaabylNloMvS10X4jB0vR4nptC6bEYMBGDO+x8d999nH8eS1lefsUqeryJ10+m6qrwkpKSMHoPQklzJaW8j4FE3KvLvXT6b4YwSUEYgjO/gfJw4cXkvG8YHebEMJ1s+nIOIxJBScTgIwg4M7JOHF5ODOM52TNrPInWiPTmK5Q6goKcSXWtf2CRcR3/g/JxeWGMY1new3auQKHZDmsevPzUC2r96rtwjyUEY/Hf1dVPUuDD8HDjhsAxjWPyORJkNDOHNV9bGFuPH6SkxZsDda/kGBfJUPgEk4SSvLAM4jN6tdlr4Lmq1bzkXch6LGzU1jotLrEjXX9efjBcG+gchQt/iXQJw525k4NlObRrFTX2Ds3dLC346hj1Ul+umavO1GVROxZFRI1p+jWkLhX8PkGHyLE2b7ZxSptVnstruvbqNW1/VX/wBBDsWVQTdQmaw/WvRpFHI1mRSOoBYmOWg2BewxY8LWWGI9bWatU1P7FNv1svV5mnytddr3WJFJaMkxtci6pX1cKmrNSh1CUf0OlsP1UnWJGn33Fp4zh6rG1Ws1WNBA/rkFv6Qj/T//xABHEAACAQICBQgGBwUGBwEAAAABAgMAEQQhEjFBUZEFEBMiYXGBoSAjMDJCsTNSYnJzssEUY5Ki0SRAQ4LC8CU0UFNgg+Hx/9oACAEBAAM/AP8AyIKLsQBtJIArCR3HShz9nMDvb3RxrCQgiORS32AcQw/hsg/iqJ2zkxZFxY6MI/lI/WoMr4kr2SQsPOMmopMkxOGc7hMEb+F7U9rlJLbwFkXitRnIsB3hlNRvqIPcVNJvt35UDqIP9wA1m1Rj4uAJorcRYWeQ/WYdGnHM+VcoBT0WH631VZYgO9nBJ8AK5adiTAFG/R6YjuLFvIVjksJRh5DbNWgK8CCpNYaTLE8nRNvKtY8HU/OuQcQbvFLAx26NxxRv0rkuYf2fHop2KzhSPBwPnWJHWhljlXYbX81uK5RwraSxvYHPo3KEjwrlTD5SSS2vksyLIO67AnzqQG02FgfeULwN8yPKsKduLgNs/cnQcCD5VDLbQxOGl7GJgk4NarC7LIg3i0icaR9To3ZfQbgaB13Hy40DqPs48Il2N2+FdpPZWJxbEliibFU2y7TtobWa/eadfclkXxvWIH+KGG5lU0T7+Hgft0dE+VYV/pMK6/dOkOBrk6XaEO50t5raomHqGRh9lwTwbPzrERBgCwU6wVIvbVnmKxkL9RpItzoza+3QzFcrQnRGIWe3wP0cp/nGl50QAuLwKMfi0dKI27muK5DxXvo+HY/WTL+KMn5VhJwTg8XG32QwJ4Ag+VYqHUhcfZIv/CwHzrGYM9SSfDtuvJGPLI1yrJYdAuMGkBdo1TLaTKujbZrvWICBmH7O+2NJDKnmP61KvvWfw0TxFK+XutuP6Hb7FYo2kY2VQST3VJyrO2IkuuHBsvaKRBooAAKNGjzqdYBqJtlj2ZU6+5K1txNxwNaX0kMb/aA0G4isNKLMpHY6iReNQvcoLdsbf6TUoPqnUm+phoHuuL/KsYSNCEq1/e6SNk79hrHwW6THyKuXqVPSpa37y/kKA151ahzkWVs+3fQIuMx6bSdDgoz1pnAbsjFi36edLh41giFlUAHtO3nFChzEURRHMp10jasjv1GpAOq+l9lxpDjrpC3RuOjl2KdTfdO2reiTzFH0D7rZp2NtHp9JyriZDmIIVVexmz+RFEm59gKB5iKK1YZ1FOpByOw6mB3g0Q/7PiD1x9HJ/wBxf6jmvs9EmMlffWzKe0Z10iK42gHuO0elpS8oyfWxhXwXL9Pag0RqpoXzOVDEICDZ1N0barDUaGIj0XFpUycf7/3mOeZ+TWmwzMs+FljxKaJIJEdw2rXYEnwpcdgsPil/xIlLdj2sw435gKt0ibFkJX7rZ/O/o2BPYavBK/1sXMfM+20hV0LDWDRJKk0cNiY5RkjkJJ46jxy8aBANAVgcMHjnlDMVIeJB0jWIsQdg8aj5JwuJw0kcjouJlOD1DTjY3sSdQ7c9tTl/+Vh6O/u6Th7fe1X8KXEQxzRk6DoGF9YvsPaKvM/bGvEE/wBfRtG53I3yNf2NDvllPn7fTjYdhopOR2kVpxkbbZdhGqg+GiY69AX8BUEOHljw04bEsNFSmYS56x0tV7X1VKzaOkbFsz8WfbSySHpCQuQFs7AahWGTO9z3Z0YiDBJIh7DYeI1GmxEcMrW0niOlbIX/ANj0dHDztuhkP8pq2Bw/cx8/b3U1ozn7xrKh0JQ+7eRbdhJHyrFNIVDRlDp6Fi9yNl+rYa9prlCKSxwruQR1k66N2g/1rEJL0RhcSkXEeidMjeBtHbXKFgf2SSxG+O/iNK4rHOetCIh9Z3S1u5STX7OsMIOloJo31Xy129HRwWKP7iT5VbCYYfYPz9v1TVpm+9WVWQ/fPyB/Xnty7gT9bBYpeAY8/rB94fI+jbk/Fn9w9Ww+HH7oe3yNeuPfWVer/wDYfyrz25Z5KO+PGD+Q/wBef1n+Zf19G3J2L/BPmRVoYB+5T2+VetPeKyr1R/F/0jntyryO328SOKDn6/8AmT5n0f8AhuK/DH5hVki/CT5ejb2frT4VkK9S34o/LzxTT4bEOWD4dpGjAsFYsLdbsFgcuf1n+ZPn6L4fDwQrohMRIyyscyETRaw3XJ19lKyxlSGHRpYggg5D0RIrIb2ZSptkbEWNjRg0cLi0aMIgWKVgQpWNXBLN29G1u6oVjaRWWS3wqRpFr2sd3bfVSyIrobqdRHAjwII8PYetPhWXhXqX/FX8vMmDj026zk2RN52k9grEMbKsIsTdrM1+wC/nUEwRCSkrE2U3IZibmxPaTlzes8V/X0ScLg3ANlxLgnYNJDa/Cp4PopWXsvlwqVcpo1kG8dU1hJbAuY23Nl50ji6OrDeCDzpIujIiup+FgGHn3msK5BVGiYaNijFR1SpW6m4NtAbKxcNzh8Yz5ECOYDRz0rHSAvcXXZsN6xRLriUUWCFJFIIbIaQOeu99mq3p+sPhWVeof8Zfy0kebuq95AoviMjdFhXQ3HSGlfzFXdRs20yspBJYOCp23vcc3rfFf19GKeNop41kjYWZGF1IrBxB5MM8kJCs3Rk9KmQvYXzHHnkiN45GQ9hIrFR20iso3MLHiKhawmjaM7x1hWFnt0cyHsJAPA1uz9j6zhWXhXqG/GH5aGHWFRHHJM7NoaYLKii2k1tp1CpMdBFjIIiToGOWNRcqUyBA3f8AytGQBsjmCDkQd1NiMQht6qNg0h2ZZhfE0qgszBV2kkAcTUcc8UOGbTlfEYdQwAKWMgDDPXdS2r0binlDW1EEcRWLhvogSKNXwtwNTrLpzoFjGldCblsssqib3SyHdrHnUq+6Vcfwngakj99GXvBtxq3Z5ViYT6ueQDde44GsQthKiSDf7reVYV8pFeI92kOIrDTfRzxsd2kAeB9Lr8Kyr1B/G/00cc8DrMsRj6QNpAsGVrarbbjzpcNCkKm4UZtq0mJuTxrCxK37T0NmJJDKhZ92Vrm1RxL0eChVFzsSAo7wo/Wp5zeWVm7Ng7hqFPPypgwiM4SdHkIBIRVzux2DL0gddRvrUVG+oWph7tSp8Jphky8ahf3owDvHVPlSn6OQjsYXHEVOmpdMb1N/LXTKbMCp3EEURWKh+jncdhNxwNYlcpEjkG/NT5Vh2ylikjO8WcVgpfcxCX+q3UPnSsLqwPaCDXX4ULeFeov++P5awuHuDJpv9RLMfE6hU8lxCBCu8dZ+OzwqWdjbTlc6zmx8TTo2gyODfaCP/wBrCPHHJioXMmk1102RWW/Vuo7KgVBHBDHCg+FFCjxtr9kjawKif4RQN9GpE1CpE1qavkygjtF6gf4NE71NvLVR/wAOTwYfqKxCfBpDepv5U6ZOrL3gj580ie5I69zEViCb9PJf7xrFAW6dj32rFyJ0TzMY730dQva1PM4jT3jfXkKRc5WLn6o6q/1NKgCogUbgLU0hHVv4U7WLC1LCO32oOsVG+tRUbagKI92pU+E1IutTWxluNxF6w764lB3rdPlQimkjW+irWF9drDmnkRXDRhWUEXJvY+FMDeSUW3KCTxNRxfRpn9Y5sfGpJCLKa1FxUcYyUUBqH9yU6wKibWoqJtQFDZUksjyxS6LNmVYXW9raxXKIcKVj0fr6WXC16ljjSO19FVW9tdhUh1ilWxYUkYyA/vIobhS7hQ3f9I//xAAbEQACAwEBAQAAAAAAAAAAAAAAEQEQMEAhYP/aAAgBAgEBPwDkejH8lGL7PBCELV2iYqIp6vk//8QAGhEBAAEFAAAAAAAAAAAAAAAAESAAATBAcP/aAAgBAwEBPwDVMZRMlbkn/9k=</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTERUSExIVFhUXFxUYGRcYGBkeGBgWGBgYGBkZGRkYHigiGx0lHhcYITEhJSorLi4uFyAzODMsNyovMC0BCgoKDg0OGxAQGzAlICYtLy0yLy0tLS03Mi0tLS0tLS0wMi0tLy0uLS0tLy0uLy0wKy0tMC0tLS0tLS8tLS0tLf/CABEIAOEA4QMBEQACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABAUCAwYBBwj/2gAIAQEAAAAA+4gAAAAAAAAAAAAAAAAAAAAAAAaeXlSd+eXueXvvp55jhjhr16o8SL1NnG/McBlP6HfFq/cvfffGO+LqtbWXhrg/XugjfmODJ66br2eaubqmXuV1v300y+2yqu/n9P0Eb8x6O402e7bsgxOVrfc9FtfabyshW2UzbU/VL+N+Y+kzsZceRYyaP35sysY+M+F0sjymscrD6bfRfhEnDf38HKNqixNXP8tutLC5gU8zsdddoqftt9F+SUu/G6nxaiT7OixqrmNE67gQ5i26TON9FvYv587+pzjIFrt8t7fm4nLc7n5ZyPNkyql3f1O8ifm77TL4SLpuovk3Cd0EKv53hTG4ssLCjk/aLuJ+evpPS/M4Wzs5fLb7LXG6isofOHi68Nt97V7Pvd1D+KdD1fznXj0fTwtNXBk49TRQcuW5/XhhPvqb9BXEP5Dh3vzvHb529jxO2fpjb86yDu5+g8RvPP0/cQvlGXf0nOQYHRdZ5zsb3sKPisJEaVCsN8Lns/0BbwvnWju3EVOiv+hWfHSOqpeF7nXXe9DQaIMHtPhn6kt4Pzyq72zqangdlt7edF88jypFTTb7KltKrmOzpP0VbQfnG+XIw907s9seihe7umn44asIOGvDV9BtAPIvNRNe26v/AGkoI22T0s3MANPOYbr/AHgDVz8XLopYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAf/EABsBAQADAQEBAQAAAAAAAAAAAAADBAUBAgYH/9oACAECEAAAAAAAAAAAAAAAAAAAAAAAAAAAACXz5DgAdB2SE+inealGGTU6HXfEsnycEVyXSzOPoZ63yWbK8vqt16RY8Xqbny9mGaXtnj6Lx8FYs1YI5Y/sNzvcqtNyha959b1FV1ePovjYLGPraWLn6MP6P7p1vFvK1adWvLJlwaXFbEv5uN9xXyfEK59Rq0NOrjR72YlsQ8g4o1KWvlZlrRtToqPv6ielc7Rn52KDK1eM+TG3sDux5rWs/H2/O5Z8eez2o6l2Op44n+awNvzt5ctjtrK+d+lu5+0LOnDkaFeHi98tlz6kOTS+2k5Ph/Ob/wBF8xr2He37VLtThgxRXrGBjfV7Frzz5/D2LtS7f76e7nujxichiks+/lK/6P14oVouWPVu0ise5oOMqOtFy/awsLQ+0z/PqpZkl9u+PVn33nGdUi85e5ox/FUvrL+DsyWex+pYOO3ZHGVT53C+j16+D40MO/oTe4a/LXI5pa9y7xD13zJ6dOjjjnPPvx4WOAHTgOnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH/xAAaAQEAAwEBAQAAAAAAAAAAAAAAAwQFAgEG/9oACAEDEAAAAAAAAAAAAAAAAAAAAAAAAAAAADn30AAAec9mZE9sW5I6Hnrw8e8c7lqOHmnbMyKzv2+PffMPI98S6XfHEX0EditV5jMyX6+lVsuLcvzuR5zq2qNa95zbtwzz5RmfYRZGxm59/UryfIeS27eVpUJbFiGLSkoGro5G5n/O69+XvmniZ+zhybdXP0Y/YbkY0LN3Av69OpmxUr2l1Sx5K0+jnXPOutXKNrG0M36ujiR6teS3BLm53vvkftqWrL72e6Fi/D8r7qdR1Z9PI56qeFero36UN0h2et75K7xaw/fIdDVxaGxRjPKcnvGid6/tvDsX4sPit3Jt2K0M3mT553HQ60jf5jivw5WtB81a860va/Vf1CtU/I7Rrcx1tmlQ0LObn6nnHNeOPnruT3jlIaMkXG5gZ8+9HzmXqVT07sT16nvro07+dHfys63q3sK5DSjdad2r5Xhuy43RPzzz1wA89PXp7JJHAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAD/8QAMBAAAgIBAwIFBAIBBAMAAAAAAgMBBAUABhESExAUISIzBxYjMRU0MiAwQXAkQlL/2gAIAQEAAQgA/wCkbbZEJKPvytEyJK3lXL9BuVU/oc6udRmlajMp1GWTqMmnUZBWvOr15xevNBrzQa82vXnF6m+rU5FOpyyNTmq+pz1fRbjr6LcyNHuxMaZvRUaZv9UaZ9R1f8YDJE9cmWsh8Zaz/wDasa410RofT9Uq9g+IXU21kSjnX8Ffj9WK2VXHOp3HcGeJjdFzX3Tc1G6rmvum5r7ot6+5reo3HbnU7gteuvO3pjnR5Sz/AMxkH6xFlks5KwCmyELsHKOZMk1bSZZFPD13xJA3aRgphs2T/XnwyPxlrPf2rHhRpm0ukMdttK/c1eZmZlVV63TMw1dOeI1C2h6xcYLB5s5jCSqOsNRqNRoOOfVQCR9kqvLJ6KR7WVM8lex6QLha8R0FywJlpSC6ZdcSui7BDWgWmVZ4kTjxW5UqKO5edUsA0w2V8E+GS+MtZ7+1Y1SqywoGELVVVJSa5ZxNga0yuO6myAzC092xM9MTXszALKWTJeoiIc9Odx3aPkdRpY8zERTskPJ6FPTEVBTZFccQe5FW/wAZYnbQSPGnYnokpqstMlZJZhd0IRzKwyVkWSbUZYVe+fcUEesuivKTOdmfAXhkvjLWe/tWNbZo9A9U+Y6zh+q1eQPo1OFfEE1pXoGIAZQ0VRLqWVAxWixfqmU9twrGWRDdw4HuomFGExMiWpuGroJa4lkd1OMd0wU6tvkz6IjBSa4nQMYifw4vd8yH53Llv5LNfHWLkH5S9jqoMJUVOoZ5NdwBiSO9ZgENc/ZvwT4ZL4i1XCvLrknc9qAWNQvdBjIDMj14S73VzBeQaJsUhZ1KrClLLLWh22MJUf5MuJD1n+brc6upq2eCPIbWmPVF+ODEZpDxKtVMklxRL6tVaiAm37RTEKi4sRDqLHev5ixvNp0Rq3uUXM8hUqbarCEyheCtMLtzkKRKLltm4UAyY2b8E+GS+ItVqS3+YAMot4tiHVS4Ajm6PrC9bayHRIN1eypOmYg7ED+mZY2z0JrYNzIiXKwdMS9+Pp0jMlFewtcCGW+QmOZVnsX5lcnH67k6VHprH5FieYDG2gL2o3I42MWg8m8+IVqxYlKwrV4oqUAzNHc1iOJsYnOi3217NkGn78jia5KMp2d8Hhk/iLT7k92zwGGS1UdFDBMYUdeMxnNoosLEeqSG3f7YxJBRY6JJqYjmRCbEH6y67MD0RiLfUuBavpYPabk8HCeJJfaAuWbwwsLgnIAfTURog59Jp5kxDtMo4NLCJqKigEyNrqbnEJ6PGkK+5FqpB+pjmrChgWW8mxtYg1s/4PDKfEWrp8X3a2E/uY+vOsmHu5jKmUMcqbDoWPWWLxptnvHXx5tZC2ZqmSuBOqkp9x1Z9J7VhoTyOsPlIIe05Tpie2y1SeMz21U5WzunuXYsT+an0+sxPTrjQzMTBQnOwUQFllM4iHJnKSZRLFIDjmWz1HIBZsfjII2jH4PDK/EWsvXXLHxP0rsc13LnMnABLCqckUySxGw4pK46ZGTnDq9JgskljImAYfTMS2KzG8S6nTiIjpzFRQDDJxm509cVWrdK5gDzGHKZJi5myEcpv4sbojNjJ41tdnafxrjRao3WIKSVVyiLE9LX49qgIl1zkYjTnR0EWtp/B4Zb4i1mMck+8evpoyAsNDW82cU2aut7daSisgQGFwpk9MHrE25GBIgnidZSjzMMGQABlhW82RRyqtWJhSYvw6ZUQFgM3KpipaF3ZmBPKZysRcqm82YkYt0Lj19lmV26a/2UccxM6nUL6pgdUc81PIhWvV7Me7P1yWPMbW+Dwy/wlo0epzrAPJdpfG7Vk6pPav21saC9MX+llE9Myek3fLvA5xxcRKpCeY9c1Tf3561Y4Rnrb3f/AF10c8yRoW72aTt03e8rqkVh6mlu5vqKGbls8+obptesFmaYtKWp6tTOv0HOpnQf/WmnJz1Ftf4PDMfCWqVXzCbEDT24YHL9YZcioYnemNR0S+cjiwWEcVZjmWEY8wXVgLZ9ketZx6FF6tDB40o5gpWdq1C+VxXrE04g6uEEVwdnc26FEHRWtVHy3tSvFuOTiX4WwqC6lVmEJMEMPZJfeGtgYtNiBy2yUKpC2cBt3G2JBbszisQqyFUd2YGa99lIPqHja9K35dO2Pg8Mz8JaoY6VDFlO5rjHLKDxyhhY8ZGuBKMDz9VxgIhn8dK5UENIRnzBUciabMWyxpwBSmO5AjMllsrDmTCcFgjdHUMsVVT7MzdO3jIYpIR1DOshz/PhGsQ8lnmDDZuQJlk0vvjFWlWqtz2cTWyAyyndgaGTs1b2RYzC1TZsyf8Az6+t2iBW7C2LxY2rFDKHm7rLNw7LNsfB4Zr4S0mrEhyLjGRYC9uRzVVEBXGJ5jJhwczrO42GVuoWHDGRpNAp64nbmRiUyqcrlitFIjgNswcQT8hl1qnpncGbhxzEYXNtqnMpzm5n2ghbPvu50jGozzAizOlZIxYDF5/ONts7rq/1HuLWIawW6rNRpmm7ue1aXC3HuLyjBYs8myxaN7MRup66x1dZPECX5FbZ+HwzXwlwGGbyMwvEWPf00cZdWEAqcbkJ/Zbful/l9qW5iRmNhM0Oxm6DY7I1Gym6ftqA9CzJJR/nX3nXFcLW3edfoITwVus70GtgkHPEfZ0anZkanZI6LYS9T9Plau7RBZAGm/TCvP7L6Yp440X03CP0X09iOeNvLIVcF/rIoj1l+SWMTM3PqNSAugT3Ted/WPDZix8iPpuJceZxGysfW4lMR4ZfaNGz87/pmkf6wbcy9f4R3Lkkf2Kv1KpyXQytmUnHVC2CUcj/ALdwzgJlZ/yrPSI2pYZ6vVsGhzEsqU1qHpV/tWawMHpY/YWPmeoD2W0J5QKMsr9YtjiDl3/Wf//EAEcQAAIBAgMFBAYFCAgHAQAAAAECEQMhABIxBCJBUWETMnGBEEJSkZKxI2KCocFyk6Ky0dLh8AUUIDAzQ1PCY3BzhKPi8fL/2gAIAQEACT8A/wCSMSOeKtAMpIKmqoIIMEEHiDh6R8KyH8cX8GU/I4V/cP24zD7Jw33H9mKg+/FRffiovvGKifEMOvvGHX4hh1+IYdfiGKifEMVE+IYqp8QxVT4hiqvvxVHuP7MOT4K37MZz4IcJV+EficI3mUH+7ApjxrIMGh+eB+QwoXeiBOkDn6f9ar+u3oAxbAqGdIYgHwJIB8sVairz7V5HipIONuc9BWf97FSsw+rULeeuNoqg8j/EY2hvhT93Fc/BT/cxX/QpfuYr/wDjpfuYrfoUv3MVv0Kf7mKx+Cn+CYrm2tkEdTu2w9eOeUgHwYAA+WK9b844Pum2K9f87U/ewaroqksYZ+KmTmYCLEG472CjsJ3OzWk5JhZJc5XABYxnNwLctjBVQdKKMxUEKLhZJlh6wgSeGNkVATvOmWnUUgi7A5xGszrPniii0wSiMz1AXC9582bLAIieJzRZZK1GjME7HK4ItDsyyALxwjU2vj2vwHp/1qv67egT8h/N/ceRxLt7It7z6vlfqRimXK6rQUQv5dYwqe8eGNo2emwMZV7TaaotN1SACfGOuK+0NxkbIgEXvDVZjFYcLVNnq0zfm9I1APGIxSBXTtlKuo0/zU7nhUAPTBz0z63ETpmj56f2Z4WAljJgKo4sxsB0JNgcKKjqDmpq+TZqOUSwq1EIas6i7sWVE4yd3CU6aK0PtWQ3qEdzZqUFpjSAahsZQYFStUOr1HdmNv8AhOoHxVPHG0UlYEDsy2aJIXeYM2W5vm0xdZhYkLUMwMrkRB58OXDEkJkEhiiJmJAFKkrgxY7zSx1JXQPkpqclXaQJrVKy37OgrAB1iJYkDfkZRGau9B2kL9JWqbRUIvCoh37C4CmBqcI5pvIYVFZA+8wOYsACW4ZSTfrGKFSkwRVFgyhRMQoCZQBAgLoPGaiNVNKtGSo1JwMoIGQFWIsZkGZPAAD2vwHp/wBar+u2OOCFAEsx4dB1/h0gOA102RDFRwe6+0NMoh5C/nYslOiBuUU3KVxEKiy9UW4yDcjrTJI9UKJgiBZBmA17xXroMNSpO1oZ0zSdLAOQepwRTrKm8huKgGr03CsSb3ThbpKI7D1qbRVHCLQ0dChwZU2KMoA6yo3VPhAPFFu2JyNOXmDxUzy9Ik8hqcStQlgtjNKBDvGuZVBUDUGIvjdG725EFrMIoDnlZlBHr1X5KMFVVVMmdynT1KqeI4s+rnplVa5VcoAp1JRKjGL1Hp7xpgSezGTMdWHBkcEW3fo4Ps0qZCqPHM31tQXexIJoEGnOhVs0ITzUZj4YpWOYsacUagzBVZiINJt0AcYBIsGM069Z1QJRAUCmgAspfMQWZhdxJJnWwD7PVqVIBz0qtJwpJIp06qyygTYFYnidcGvsnVyamzEnQtVoyDMgwyqb6jFSjUpkyzjs+zjKCb0Cl9bOG08ThWRWRhT41arb3dpqACBYlgLA36e2fkPT/rVf12xr+J/YMAMFYjZ0a6l1O9tDibqpkLzI88MhqMVl6hnMWkCRFpO6M2kWVxhSTJBh95gLFmbVUt3VE6dcAkG4W6U7mJWmkvU8TIPTFalstJgCoqbk5rqUoJrexklh7GkiqAxAp1zTdAtT1QGcAgmbEiDpeQMR2kSrkDsqwHtBrK3n5kQcJWpjQ2BHSGQ1Ao6SR0GuCGYAZQCN5lFgJJyuRIykwZsTEYBDAwQQQQRwINwfQQGLcZykAetF4kza9sU6R7NmbIlM9oXWAGvd6ech+B3RInEySRfW0iWnjdjfjVbiBgZgpG6dKlc3AbmiDeI4mxwc5JYsTvS2YySuoJN92MVGyyQQwLUzwOouNRJEeV8UioQKENOCKjkwlNF0JN4CkacBcPTUKoYo7E0aFOd16pWDUckNlQXY2GTfgdnshUKNquKrGzPlUZYAjsyi7oJJJYicNVq1id7I4GVspQO9slOFJiQzXO7eTmp1N6KyOzFxwzEAFjGp3tL8TgAJmnIMoNWqxhFbsxBYws2116I1TaaqMmWkVcUqZUB6VG4KBYOYgyTfis+0fkPTSBrLVrZWbfU5nIG626pBJ1B7puNMHK1Uhc3sq12b7KAnywo4JSRoICgbqkeyolm/jdmyl8zvMHj9KTzzZSByW1tLVEYo4+utj5HUdCMCnstCz1K6gNXqEnRMwhMp9ZpixUAaU+1retWc53J03q7kkCY0gTggo2q5RDCbzuFmFyRlUrfUcGzG9pLHwN6n3smKagfWIX9ZnGDs/wAdKfeEnCBjEB0qEvHiWiBygxeBfD5x7DWf7JsG+48gcCCqmQdQZNiPLGqqX8yxPyGB2b2ipT3VJ4Z8oJXhvAHyGKaq7QRULFtnrMYLMtRO5mIkgi55DFJhmk3cnKvHIQbzMSsjW84sqDQ7pA5C33cNYi+AFG+KamMqqP8AEq1ADpHeBmZCFbg4cNsIy5wc2es7AO2YkA9pKoGIgKkKpiIV0pojF/6soiQSrUh2e9TAzAlkUmdNLmVvFJmADNxBrge8MFPNsUSg72QkCmeILOTFXwEi/EXwlSi+oYd23rSWEAfVeOmGJAV1z5WAFm1JUZZzHUXzG+uPaPyHpo00qB2zVc2U3q1ADEHNoQfHhOKS01UOqstVXDM0KbC43O0swFpwTA3F6CA1QjqTC/YwQLZqh4AxaeEIvlppjNkI7KpMloQE0ahETJVch42WYNsHIkd2bkGI7Qi4DcAJmLBtRwk8BlvPXLEanM/VdMKas6m60joCZu1X8rejiwxVYKRZVPZprAEUyajHS2e8jScUy9SBKKd4MLG9E52nXeJ8cbLkqIqyr0gCwI3GGbWbyehm8nGy0l0ysamRmjicrZSYsRzvacVKkcFcrVHx02LAeIOEy7QqmII31WxWRZtLHUaaG3qqqD4QPmT6CCh71JxmptOsqfmIOGFNiZOy1zNFj/wqmqNyFjyiMJUpKq5nDnMJicobKcyqOMPG9M3OEH0ylTmBhVEBKYg2Zc2dvrED1RBPaPIBm6qTvVDyJMxygngMDKKYEMCVeRJzArfMSeHhin2wI7wbJtKLooNW4qwLlagYTiqHMgnZ6gVKs/8ASqHs6p1OZGDclw1RGQ3pv2jU9D30aK1KZ+tYR3SQaRRuzqZatEsachTYMhIXlDqDj2vwHp71LaaoKk2ZHdiuYcQdPLXGz7jqrBkpkRIDBkJEciCJFuOD2dGGZAARUVxVJdXDC4sTGu9EmJxlC7OoqV7yGYmUTqCZaNSFAIvGAQpbdBgm5kCNC0TbQXJtqbmyhZLFiIhJuTAu2pj1VEYEIO7SWN4kSog2cngW3OQbvBMxIXMLCmjCwkNmXwzFjyECMM1bWwYpQF5Izd5/AW5rhsi23Ka9mmo1CyxMHWV8MK4CxlYg51MA29YrfX388J3hItGYDQiNGH88gHYEmGVMxEaBsqyDGKlQSLFgQytwMuN7wYkYl6LkM5kHI15JAAhSYM3AMidP7E1aJy7jE5hlIYZW6ECxkWi2K7M285p1YzhjzIi3WCNL4pstVrEgmQFgbqtqtvVM2gA6mkSg7qpvb4uZVZO7yiZuRpgqycXUyg6MNVNuIGEsLLPDj3hox1ibWHAkkbVSWwStPbJNoo10h1JmNfI4MUER8tNiMzsVurtTQB0Uk5ZUZ9WJAlva/AenSpUrUj4l2amfiEeeJ3Van+bZkH3KMagq3+2PeAcFcrVjWLC5IKKKYPLKgAga+LQAZ7qqIzX9QcJJifDgAMDtCwOVUhrAiUAMWuCSYDC5IWBh2sCSwgLlkhaKgtmBGUkkDS9pEEGlJCgCKYm4LCd4m5gmDBnScHIut9be6AOBjTnfCKALGoxhBFrsbtEAECOccMFqzXlRu0x0MXb8q04BAGhJvTPC/Lrw44i/db1XHI9f4cwTWlPYcTHTNNx5TiitwVY05i/rFLA8jx1g8MAQRJozY9aR4fknyiIIIIJBBEEEagg3B6ekkEXBBgg9CNMLmX21F/trx8VjwbFTOrRDKwJMaLmIh49lxI4AG+DkddaqreQVINVSZMR6xYSZzLAGGyz/AJyy9FwdO1pGSgJESJSTacCFH+IVzZQBrHET908OFhlNisoFAJESAST7hE8sc/wHo/m+Ipv/AFgg1CWOXtA1WmwUEDVCPDFilYmLWDqp0/KD47qq8+GXN/tjzxck5mP1iZ/afh5YMUqQPgeDRwkyNY3J9ojFQpBC04sVzEBrqAYiSf8A9SBnRoYAQrHvLUA9lgQwAsDI7wJCJYAgsbs2oAsctxrrOnPANSpYikJyL1bmelhre8YaALKi+ryHJbWt78DKvIfeCcMtK5AYmCx5BRLN9kHAqBG3Ud0Crn9kXJEiYDAGxEQYwZU9yp+DHn19/M1dqvc06dYjxKBjH2Z8OWNorazlrIjAnnmFxfjimNn2ogBayXpVDHca8yPZaCOBIwmVuB1VhzRuI9xE3A/sPlJgMIBVwODqbMPHThGAKNWRlMkITyWoSShnQPu/WnDBgxiE35mzMyqCMwWdCGPW+AA4N1Y3nXei4jyOYMYuJMmCIggkkGSQRB0uZm08sc/wHo6fPFRy7vTOUUwFVqHaIQXLSdxiLLEjXBJ7SijX50mynziqPdjjkHvdcasLfa5eWDZd52uJa50MRAK2MwconXA3n7q2shNpB5wD5jlgqezRVqc+zJO+ST3aZm59XOdbY/k/z+GInj1/+8Os88MFAElmMCPHH0dM/wCa43m606bfrN8JwGvM1ahJqMOhPDwgcuWBIYXJOp68iDcEXBGDmRrU6rceSOeDjUHjqOMNNM91+KjqOXhp4SFD1DxKRkPXMSEnwM9MU0AYXVjnDDhuwBPgbeeKOdBFmptI6h85YHqDOEekeTmUPQNEg+M+WLESCORFj6TEzJ9lQJZvIAnF6RIiixOUAWBWDZo1PG+Bvm2RiBU1vkYWI0+6RphgVJiLSq2gHrMG3Ichjn+A9HT54E5qjH3kzbyb3HBXOO0CrmAznIxCELPeiLixIOoGFL3DZVG8VAOg4kGLDlacAlELEgypJpjuxEzE8OHlgzALVCbzGv6RjwGLs0BYsYbuqBzi3h1JxDSYqnhkYAEAcgLzxAPKAZyAZTxak05D1Nip4koSdRi/P+f5uMZXXNNKf8NV4MVAu+tyCOUYJqN10B6DSMWm6/swQAJzAmAI1JJsB188IaxA7oUgRNixMSsjvaTBFiMbyzuhm+jXiALZTGkhW8Rhs59lSQB82PLkeWKa01m2l/IYrkfVAB8ogn34fMvFalNSpHIjC5XMF6IMrMATSm/DuG97E2Hp71TTpSU/7mHuTrjTT9v7MHlHA62I+fuwxJkanwxz/Aejp88PFRa7IJBZQO0qMd1bk7pjlIwXBourO7hUpgjKxASTUaUYQN3vi+IzS0kLEAsWE7zcCvHj5YpL2soM4gMMzBQSxBkCeIODnIUdo4Jyuy2TiQufMWgaAHB9pEP1j3n9+6PA4O9MX1UjQeFtfDCntKAzRF6mzPrA1NlDAcWpAaHBkGLi8g6EHjzHPoMa8D95HnrgXGnUdMb7WKgHujgWbRRY35TExjM9Q3Wmg0+tBsoB9d+oAEjDgIhkU0nID9ZjvVTPOBYbtsO5qBgpkDLlg7wI1vHv0xTqNWMbrKZuJ0MGYvhajGmYdEU7pkrDQJmQRHTFB0CAM1rKrTBaNJg+44RiqRmYDdWdJPDFCoacTmCmCOfMjqBGuEqkm7diATHtENbzn32x/WRUNdqRDlQYhz3clpyjB2ha7sVAQjIAJCAEgxCqPvwdrzjaFpVc0BRTJKFlbLcBspnkDgE/SIKebVhVy9nprdsp6qcF2yrTDlmBJrPvECAIAUqfPHP8B6OnzxUZiarF6ahQAW7SC0KC8TxLXjSMKxFTKu9ABKuGG6sgjvetythmYEAjhYge/wAzOAoVgQZ0vxI4H34JYgPUJcm7rCCDFzBJg47qrkP5SxJke1r78DMIACe3W0yfk+seluOGzMWioeamAYHBRwA9nriMhHaUf+mSAyCPYYgQPVemOBwYA4/zqZ0jy4YUCLGprfiFGhP3Cbk8N2nc5zcu3ErPfa3fawtY3GAFm5J7zHSWOpPC+kYn6Ou3aAa5AHEnjG8h/wDmO7mWY0zTIkjw06Y5oY6dib/zywSrL2hUjUEPXgieOKjOu00mpEsSTIBK3PIZwOr4s+0bRnqjj2aOEE9O6fI42uumULGzrTJpMhWLRY3m8SCI4YZlLbQArCQy0CUIjioAd/C/LDtUJ2plzMSSVC1o3jrpEmce3/tbBG9Wr5RNxvtvAjTx8sEZKNCp/WGPt0JyE+DNUb7Ix/mVC+UaqGaQPIQJ6Y5/gPR0+eGdhVp1qeWWKrUHayYXcUyyiW3oHiMbOzVFZFLOwDEl8sqXJbvRERObFTcVRTBWN7IMhOYzIJHQ4F+Zkt7zve6cDk/+1vu+eAA6NlJ5hRKFuZyWnriezXdXnl9Z/Fjp/DCnlEax3R7vvOGAqbMQ9Mm2ZSCMp6MpZekg6xg5aQmSDqOh/H3dRlpju0tCw4ZxwU+xx9bUrhgDG6JGnTwjywYUGfE8Y6WHjioBmNwbq2puOnMRjs1UHMAixvCQDJJM34RhqcrEtk3mjgxnQ20AnDIBtEipI1ksTkE27554OQoysDqZUyPAWwVLBQgyiAFBJ0k8zg0qhUQr1EzVB9oMJ8SJ5zgp9J30dZRrkjdBERJ0jWMFCocOoVIykKUhb2WCbddcQ1ZDIBuqmCN7nroMH6SozMYsJYyco4Dphh2VSc1t4AgAgHgCBp1OmCBxy6La5y+yemnhjn+A9AJ0sBJ16Yp7RuvUcAJb6QgsplTKkgGOnjNLaB2mYNC00nMSTfICDJO9qOeKNRVE2D0hqSTxHEnCVB/3BA9yvj9LaKh/E47LKbEGo5BHUZYOE2QeC/8Apg7OPsfwxUoDwp4r0/zX/tjbKQPLs5PuDzjbaSfloqHyVqmY/CcNXdLnOlGvvEzJLhVJmeFtI0GP6wEYQTUpbRAHQwSviOWNsV+WUKzx1UMG/RxtazyZMrfCxBxVB+x/HDofFBjsvzY/ZhKB8aa/u4pbP5U1HyXGzl89s1NCVW4G+QRlF+WgONlpeTOPkwxsyx0qP+9ilUHhUn5zha4m3eQj9XClTOh8B/cEDxw1hxFx79MVUqPpkRu0Ynllohzj+j9pI4M6pQX312zR4JitsuzqeH0ldx4g5Kf6ONu2utzRWWjSP2KIB/SxsdFWHrlcz/G8t9/p2Si59ooA3xrDffja9r2e0BO07Wl8FYN88bTs1dRwYVKDnw7MtTnxXH9H1yPapinXXx+iKv8AoYcUn4rUJpMPs1wn44ex48Pi0+/BBHQz8v7xQzcFJifONcJslAc2q1Kp+BEpj9PH9I1T0oU6dIe9hUqfp4oGuw9baKlSsf8AyswHkMU0pryRQo9wH92iuvJlBHuONmFFvaoM9FvfRK4/pCuvIVlp1lHmVWofjwdl2gfl1aLe51rD7xhFR/ZVs1vGB/y0/8QALREAAgICAQMEAgEDBQEAAAAAAQIDBAAREgUTIRAUIjEjMzIgMEEGFTRRcEL/2gAIAQIBAQgA/wDEhC5GwUYfevXWazX9nWazWazWazXoFJ+hXkP161v1Lm83hAOWLNWH9p6nVI2h6rXxOpdOY6da9dxyX2kGezgz2cGeygz2UGexgz2NcfYpVs9vTHgrSrkbAqQZYPckPF4Z1xCX8ZDemrONDqt3exY614XtH1rfqX0t3IasfclvdbmfwY4rEnyX2KN+w0Kwz2UY/XE1uo3OLpXXIrn43/onmEKbISSXbv3OOwkSSSjaxyyRMCvUuqvGOCOgJ5GQFl26hx5IKuORHjzhOH1rfpXLduOrEZXt2p5rGsgqR1/kdM+2yS5Agz30rAtG/UhoFGslQDLJEk/5Iuh9TNyEpJ6DHPfk2Z35t21grI0fel7Mk45C1JPFruR9SYji/tqVgjUvTGjYvna3o4W34LcQNjuSA+T61v1LnWeo8pTIKsHto9sdJoubBu2OzkHTkHnErjfIdT6eqEzQVLQhI3LDWb5xVLprXkldGVhyXLLssi8ZJkTaipVMpWM3bA3sL1HttxMdtXGms04COUYftfFBK0jKxWGMjEqh1+NmCeHZdACwGH16pcsw8I1gUS2gCZF000i96yzSmZGglDpSvJYhEotdURTrDfnnfijQqg/Juufoxqcq9SlpjjFS/wBRK/id3WSYssp2W1K4pgpEIIZ4+2JOmS12LmrIzScVlftqNBe6M7R48j5JxrEKLoiyIhqHVSUEk+rRpK5M0cCVo3C3W2UgWhFvyOr1QrMgiDRAohrpD/yYqVqdNGKhUj/i1pIRow22kH45L7oxiaV6Uh3lG5JRmCyVh3JYxl5+U7YciuEeHQRNIzK0gsPtJNAccrgyMSZIPPJCdeJZemiRSYRWvRSaw+tzks+yzoDp5JIRbU5ABBBs2J5bkoRYxxfs1K1GGr5Nm6sX7AtmYbeKpEv11Cqsb96uZJI37qV77Wtqk1SbRMfQr0RlVHduTFsJ9CeQ4sjedj2Yli2rFIF4YLQZ+JDKw0fbedxSnbEA+vVIA1WKbHX5ZfTjPvLV73KIEKMp9pDDHHVTtR9Ssy165aLpsURhWaKWxFFnZnl8yx1408jqPTCNzwaIPcj6d1OKcBJblVLCaMXUJahEdvmCNjebwHIrLId5HZilHGSbpYA3HIJEbJHZF7WcABoH1KySQFcYg+c6jD3ApEbivGbGdPhNWIHGmkll7de/faaMRp0+2a4MeRVkrEhAwH1yyEPvY6r0wDdmuycvkvTutv4imfg4ImscumSbr1rUVhece83m8B1kF14/qx1CJl+KKQPJHgjD6/7i0XwUN83Bs+UOIgntJDl2yxACwIIU7eXlRpWKSr/9Do173EXYaJHkPFQscfjHYt/IEj66l00p+eBgHGxQt2YV7bSQ3HBZ46Ahfmi2JY/MgII2MBx5O2hbK+418qwb6IOjs+srflcFVTnyE6kjWdPR05u1V+5K0+NuVhCk8CzwmFH8/LIpXrTB0guixXV4gfGhkkqxjbPanlYpAUrVV3KnU55NpUFAyHcooVQNEU4l+oPxLwbWDD+SXWDB/wB4s7AEE+tqIRTFi1uy6hGK/YxAVOsqTERyKY1KRAYvjOqVeEocSLvxnRupe2l4SPtT5m6gB4j9sU+dppVMZZnqV5QGwIVPBQhP2oZfBH/ecT9qXfie2JZRGGau6gBSCD9Z/jD63C/MSBmrxn5oDxG5CqeWqujTalgmZ5ZBJWi7ng34hcQx5Js/IsOT/GmLdiNK2GWKkNV5rLudLDBqoqldNo43/IGKSOZyFiW0zN21VS8ipJ5Dfjdo2ZjApeH+YxpCrkhHDKCD5w+t0g7XEp/5PEsTsQop2L0fGcnDJ3BDYWweygiVW+iOrVeM3cXpnSS2yLF9FQwVXmfkVSrW7Y2ySNF/Ezs403uHwz63neIO8llaU7KWpNaMcxj2cltNJ8TDyJBEyjicScoOORWf8MfU10JJPt4/G/bxb3nYixq0D+WSNEACEA549N+m83m/Teb9PGaGcEwwxHOK52Y97w1YTgqxg7B/s69d/wBe/wD1f//EADwRAAEBBQUFBwIEBQUBAAAAAAEAAhEhMVFBYXGB8JGhscHRAxASICIy4UJyUmKy8XCCkqLiEyMwM0DC/9oACAECAQk/AP4JMnYh/wChk7D5KeQsjVJph/8AKNbl2J2BDw/cyRvkgCLkzx6pneeqZ3nqmd56pneeqZ3nqhvPVAbT1Q3tdUy/M9UyEfCHw5JqCIReBY8kJrJwTL4RfY+zLOzyU7i4ccEf9Nmgi0cfw5uwKZDAq1Em+MdgATbTW7qgf6k00zmCmn/bDazI7H3helulcL7thPlmi4HatYm03KVSfCNbUfFg8g5kAHamSy+ZI4deE1LWnWmxGAsPxM6CcNXQG08u4oeSi/c0Xq7UyFjF33VP04vd6m7WjIG7rOi2nUBeTmntnYNp5Ars4CbgS7OAgmXi+PMO2l67Ms3h4GxqB/qCa9Yi+RzHMEgVX/YxA3iw8jfG3yWcegEFACZ1abFDsxIV63VwQ8MYM6gTfF1iB5IPuaHP4egWDdEbv3TTLhaYYnVkBa8c/jihrj3O1U1uA2+SikyfCx91rWVl/hvXvai0aCnW/BF03ZTMeKaFpAshQfU0608EM2onZIbyKokkWvknfmZERiHQdUWTCf4TSY6jVy7Rl8x9O0QByccZEACRcXgsmD+eTpovHdYyd5dyQjODPSvJWxa1uC9rMGRfacBL90fnkhz+dhOCmaGGsnoR1O7UUYxmP00xnenm99784ohrcdv7Jkgm2YAxtWV15v8Am8+Rvws+EGEzc/8AZe3sxvHVo7IIwEcdc6KcgP8A5GU8YxMS6RB4IPakaA4XzFmLij4ju1gCn4M9fnJNBnN53P3ottG4AdV2Xabf8V2jbIo0yGhyIyQH3MvIzB9TOLiL0Xj0iGD+amSBsHVpCJEySeKJBdXhYeNxgi8C0DWVtroK2kQokwAqegmaB5T4GJ/Ea/bQc3qWtyMLuQkpHacU09/0zDsDACvtxTDjViWbJlk/yNn0mRMAJhz5BN+Jpoh9jnZmq+44mDI1VRdAczmdyxGfuG2IuKJPigXW5W/MaIvP4GZ/zHkNid2bFBDb8ktXJnxGpjx6Aoss7+pGbk2Tq5MNnIHORQPZtVALO6WxyIPZtGYk+sJXjc+dpLW8u4BWQ2d0Rv1cUAOJFpI0HUBTTjB1zH+c/tdUhS1DXNH0ifRQu1qiCanr9rBYHqPTHyCbIs/Du9p3LtH3Wf2hNPLRANwIcybrCoP4CZxMskMBzPM5Xj1N2t0uZoL5mQv9TfA5cBGp+lNPNBpww2gL/bZpacp7YUKYfe106kogEzALsweUxZBNPzfoJl5oSBuaa6rsiDd6hmGXuxHyC4hlwfbcDUOlN1k1b3yWvhGOtWVUhO816fs6d6ijFF5tN9BzOXk+lwOH7P3d1o+OiBkHj8xnvivefeaflwFtTDGdpv1sEBaTJ4BNoBhro8GLRmbQRYKQcQZl8HSUSdZ9ZuR8IpM7JDN5TMamJ3w3LMcxzFlkFB25BzXH50KInG3bylgYiLMg3yaFd+I9Sl5ChrlkoinT4dgUMrcjbgYo+ozNBTFSHkLx4XgOAkZEuJ4K1Vdt+XKftZxdE/yh2ZCHrb3a4voCogPJda7k+AqcQ6DJEeY27cHANe5wNABabTlY+cl7vxmZ+2go6zyOh7gOI6KdERc0Q/b121TDLQM3Q1duiiWuyMXGw2gHfSofFHqMRq7zMvb06ONYZuReTM3+URDxE1wQkXwvj3e1gRxm1vLsAvc1LCW0y2qDotGpHJmy95tQI8Rfc90Rid3pF/d7mRC9mmLNn5cEF6mtw1pyOVndK0U+D8FCKD6Az2AEkXOwKZDLJr4WB/eXwq5dowGrmicoMuIukgGhVlx2gWZDyZXmwZlRNuJn5jInVVIiceJ6qo2L3Fw2mKsgzy2COJRdU0dM5WXwm5BwHtq+pvatysAWeNvXAouILwdach4WTMD8VoPKoIw7yhc/GtgzyimvEaMw2tT2OTI7Nn8oniZk5pskpl+Z5IEDHiDDcjCvXrw75M/qPQbzd5w8mLnumH9bbEAGLgN5cyOKOtSRgdacg4st7AQ44+Es5vU2nE4fSzs9RxFO729p+ofJ3mnd7GoG6jWVtxNru6Jk++gqbgiQT9P1EX2Mi4RzCPhYk5mvMrxYFM9w7ggCaFABp8lOPXztSLoxcD0oL12pbaD5BwfzdiVPWrEXbkXPaDORMckHNBo6yUhM3UxO4PNiFkLnSCnI41z4hq5RKiQMPTZ4jYyJVIhj6+1cfXYLmKD8yi0bdaeolkknf17tQWpq2CtKJwVVN/dXznf0gi4Psg/WIKEa27THYSrUItwN5l+obwpzN56DgB3D0twONcjHaKqAHuaMgOtBaVBi02tGpPASHAF8lMopyIVvktUu+XlfFPLqk8HuQ4oJgHEAoAARgHRqh/yhAbEyNgQQ4ocf42f/xAAuEQADAAEDAwQBBAIBBQAAAAABAgMEABESBRMhEBQiMTIgIzNBJFFwFTBAQkP/2gAIAQMBAQgA/wCEuajW4/8AHJ213EH6LfmdbegJGpQvX8BgWHh/+n020cHKA+DUsh4t7imvcU17imvcU17imvcU17mmjk1/vu5BG4ORYHYm9NtQPCY5Jk4zLsGPEnVMad10cDF+jHpo3PP1t/IfTFxK5L8J4nTJ/wDzrXGj4oM6q+JDKzTr3OSf5HbGyBwp1DpNMYc1/RGLWYKrvOOyTEfp6XyYY5ApQTsh5dOw53PIihHxEwkySPdct00ZOvhHH9HYj69bfyHWHiUyqiSRhBYnamXXMPblSkcbZVXCzqKDR8DCn/Lj9PVgXumMj+Jo9MUha9Y6eMagefox2G+kPYjrHisk71M3LqKdiAoMQ+cD29d2jbBk53Ye7xvkiZpt8CaDYqy4q/c1OQhC04o4O3rb8zrp2B24LE5NWzrcEzMmtAZYkL4+BjBkv1GtDp35Aq3TcmyHi15d1OcVtlibTZodzAaJIIOx1NEZTyxMerjuNmZQnvRcbHKrsRisyBhkYEnIIg2RM8KEdwbtWSQRpkZOUWJ1kWolC2sSscghEq4I2Hr0np8cgGjZ9ymOzrlydEnhRo0OnRWC5M0JIDwZGMzi9IoRyYY+LjruEyKv/E3vB5Pdv9avhd/5Pfpe38XEpPYzAWUw37tnDVXMrGhaidSlZN50O/khe85Gq09t40r/ANaL7jYrKhIIWS5J/wAh8a0tgnq2RkYiJ7edny7SDdKqcmlMp+p5BehZ+nO2THhpcaUCGYWrlneNszDxW31Xrd6jcpiZl9nORj0x9xTE6d3JCi+1zlHi+L7uRBzP20camNl9KY3y5pWrrIckn7KPzgrUbuNTZF0lV24uYttylPqXbYCxy8akyyeuCVpjhSL5KtyTCyshcB56dWysgBZwj0zHO7r3F72Xn9Ye+6phdLvbZjIY2L4hXKox3OD32+LVx123QJCQ5M95Vn2j1LHyVmeYGw21t6Lujh0o7MArplrOnEnlVuY9qQu4PJD8RkK/xsCEG36On3KXeerjjQ6x2+Ox6Lge3Vr07i2/zbdQz6ZNOT9HMxkstMnNatXk8sWthufdY0/GPXItX88TMZGCs81deSWi6eVjekxxDRWvmZUjwdtba2/rVMcEfH96B3WPUQ/hgFI8tsvyHPc7n1DTWgOslCjBTigs3AdQAqy4a9b6gbU4rjdLx8fG7mbi9PljE8TKAYVpTKpnqHqR6VZAPPT8qhYIWQUBZL4KfkvbYfxwi2VJmakmQ+dtba20Rv4NcQNvtiRpPzSrhn30Nyw/R7HuLyOYrGU6HpK75a6zMjtxpfXQ8Lv19xbNu2VXuaEGnNVc+RrJn2K8xWqSHJ+Va+dJML+P15GLke48aZRUFlfpoYc3lm9OkwE2z8SxPL2WNkeMZlKkqdtbajLuOF1lbXYnTK6fcyCw29Zp+1Mi3caPFsCywtybrTMJSWVZDFw0xRHhjSOXWVaCprU/71aS0UoyYwSzCm3+ydTk9Dsq4scYCl65+VUkRPTYN+5l0zEUcUOXYncDKf71aps/M+hHah6H/Wu0NwR6yuzxVQsYBtxTbfxkM4lyTjTLyULdQuMjJ4qx31h2FFKa+9Z2MaKKIrB1BGN00sO5b34opTBTwwCG7SJAYljvTfb8WB+9bHQB28p97Fwo/GlTVuTeNEHfW3nx6wVREzfHlmV8JVjyO4Bfxpbrjxo6PNUmjJk1KbBMILj6I/vR8nw8MTpqnJyLi2c3LNSXI/K1dmJmCQfH/tof3oHfU4M42E8Z3XkOyq0RTkTXkQo+9CbNuVHnzoH9GMW3Us/U/kAKsOZOjRj9455KBpBwWkmxkNGNW2/rWA/cXgcrJl0uYLLOht7nJlAuN9ZGSCvBOW50x1y0iM52WPTwPLzkshstIS331RA+wNJhR4THP5NjkhhtkYIoOU2RkPFvU5DkAaFWH4mjt98joUYfTfLfcePr/tbnW51ybXNtc20aMdDJoBsBnXGrZDVHz/5q/8QAPBEAAQEFBAcHAgQFBQAAAAAAAREAAiExQVFhcYEDEpGhscHwECAiMlLR4UJyMGKC8TNwosLSEyNAkrL/2gAIAQMBCT8A/kkf+SRt/ABZ8DMtpRvZ4PYEc0ZQbwxYsWPBjwY8GO4MdwbgGO4ezPFnda1nIs6gbkrDNSzyIYZe/eHx1vYa5q8fKDd6iLlFC86WeL5sEBgg4PF4tow51YE4MRsLaMPZHjEME+7kabcmi5wxuv2gd4B57dssxnY0zhuEgGKH0gaz2ymaM6879wdB2B4kG7VZ8ECw8ajDKJg3XXRYeI0sINVp0WCjCGRmTsOLFbq5yLBGPd22C1oaEVq/efymQA8/2efwuSQTKcB/SL2dLzxVA6sbQqK8lwQSLPDRO2Cewe7aR8nFAtEWMTiz7xMIuHVRLRfbaG02tc+Af6nYjNWd8JhPWH6TXAgXK3kelddzF2HcmeHyWCkyFp/xd3wFrR0pmfT7G0/TjIF6EXxE5CYG+1ngt8TmvCTBDR532MdjwDPh4XzHB6H6hawOsZp4iep4xN0k+koRxzUDFn8j4d58O9WdQXyTNdzO0nzSPdm+NZ/7Ppc/VW7Wqhb+G6YWEiZNgTdiy6kAXgJmgX6XRQR3s6VQTiY0WQC2QE0oxTD3nwFzJGk1bJaiw286xCmn0mLaN5DA1EbKg7cmUoFChCCKYG2+KL2yUbo82MFRS8eBNAQqK0nfC6OB4vG8ox8T0XjUCzE/NGEOCUtg09mw/tiWeUC0R2/uxhxuDCxADC/WScKSFgZAFJRLQnBnS6tkRsssmz4QZKcJjZvaW2KBcodx3WIf1SpkEVU6wLQe0hQXAwGCOjbFvPpJmxwTl0ZVYdVJ6nKRaLp4M9C6ZFI8UisYKjI47fM5T2sFSr1s7QAcStgYE4BBtOruDzPAYkngHeLaZ3f/AJs469e6U4TzLEr6XoHIjwnAFghjxRpB1585n2cZ9XRRANhdTgzoedVYTGIr1ewUdT50ovZBx2JP7zUwdQFTJ4FkJedCV1Rj6rTPYEmwyotprnsaJErBhffsRnBD6pFaRESbF17g2kh6dJyeEz92rh3AEfdVQFjEFUSIKs4XQFRTMlLrFhYreUEh250IpzIU4NWJwoMhtJYeIdcJ3qwBeFbLU2RkkyjeX1mX6RDWx8Ln3N/uP2mOygGADt7HVBkkFz+SzpxeOqMlIXIMFsIiCdyI2lAOEQcdYcELPO6QXlDteAG0lgQ+7QzwNxoZWG36XXXM0C8Xu0o9aOYYqbr5WRzBWCqzqiK3v5J5JWkqsULT6j1XBhEybaPb5EJqWK9VszDO5jpNy3s91hXI9wyeIMUg9ES/MJWmxnADagXeVZ1BSCEhSSoWvA2tGMrzIZTzuYxRXnuQzgBMmhJbw6Ojhmaq/fUOeV2bxJiDqujropgAinwumpCk3gQKXkgVUs6rwrMj9R8LuDoVno3e5U8GdLwtNRYVmbDWsVWXD46vL5BudP8AaC2nABkvhIwJQ7itYQIVXlUSMJ5qvcgQ0Oo5lpNWSUHua/urQSvyzuY6Q7je2WF/c+riEI3gb2rHbFrxzacQLgILdZcBUKW/huxcFp9ZWp+gHyu+I+J46qpQUh1zMUA1Xi6PCRGVZBSqxMr4FggFF8wNSZmKgiAtUIW8LoZ3XPqMsjXIJRWeOAgN0d7G4E8DyNcZyqLPjq1JNAWU2c54yaBs9ukwMO6GLHVPXUdzHOhy6DDAWn2afcCFYmO2gaYhsPXy0yRxTm3lRXvskHT95BH2uvirBXXbMgu0jJLSwGs/Q/StB+YzJEguJHXuOpxd1nnVQD5RVhCVsm8tHBIfdV54VWANFC9ydDalD782EajmGGws8QeuuKhh4nZpNPUllLu+9quX9WWcGlTDumBYqoTZDbBr+Bab5QYSG4a2JLDwuSsLxjsAj+yNg6Lvd6ZyFGPi6TM21I7PK8Y3Pez0jenqLFOqN4Xd59m29hTSD+r5tFZixoPVFvXUfMdUW/JgG0hfediNQPPkHFwILwqFtE+h/KBu1gdzPEPel4ELgTAnAlpjtgKmwCZ2NAUuAgN29pd0KoG6GG5kCGUBuGdGsIzaKcQic80asXsJnadysFo6LSZbdwiYMVL3mwolztM6kluiwgeuvdiXnxU2UI4GURmewKz14+Klnf8ATHqfCvZOSH6o4s8dIbdIV2OwdH/Vb2dgOpMgyDJl8NMzv+ep9vmf/wDI/wAjuHfKBLFiCAdyHNovFakzCQEQNrQEPZjF0gxuIgx8L7uzVjzMbm8jkBjIn+0YFIHsMXUB/tPLCNW666i3nd3irue4gG1qsdV3lyDAaogXz5V/LV8/EhFvE/6np3p6RhG8shLFh3TBp+0u+7B4KL0sxhsbRu6MVU6xSspHEMEaLCICOgYLxYqCJ8828xlzOA3lBVpGd6zONW6sOfua9hRTATjcKk8VMIr4dGsNENx0hG5wZokYAZAAUFAGkYd7iwpv7RLvUTZcyps9uDCJjt2c2MOsmw5hj5YjCfApk1ZXCnzeTROyYhlQ5ezDX0r0HXBMnkBV6QxRntbS0TyuCxy+16dkImTSE7/woDsgdx9uDQI7iQAGzmyDIfvlJj2For+MWJYsWO4ezPbh7Mmz+df/2Q==</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAMCAgMCAgMDAwMEAwMEBQgFBQQEBQoHBwYIDAoMDAsKCwsNDhIQDQ4RDgsLEBYQERMUFRUVDA8XGBYUGBIUFRQBAwQEBQQFCQUFCRQNCw0UFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFBQUFP/CABEIAcoBygMBIgACEQEDEQH/xAAeAAEAAQUBAQEBAAAAAAAAAAAABAECAwUGCQcICv/aAAgBAQAAAAD1TAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH5H+aihS1WtVaKUpS2222/NepWlLaW220rnzXVVsyfvOSA8bPyNKiQaVKVClQAUqKKilaVoy9PoOm/oP3QDx3/HEMAFFQABRUAB2/8AQVugHkD+MIJnuKx7QArkssqAALrQ7z+gXdAPIr8U69Lj2FJWPECkrabSZS6LqNXGABIusuujWvoP9AG6AeSH4k10jDaCVFCu96KRrtVgybXZYue0FADNTEJcR9H9+9yA8kfxHrs+ABnwF3Ub7T6nopeXDF52X0ei5a0BdaF1r6V78bkB5I/iPXAAOk6Xld3u48zNjg5dPz3Y85zAAAfUPfLcgPI78Ta4ADYdppNrtMlckfKx4oHPdLx+rAvsC619W97NyA8ivxTr8+ABnwOr3Og7C6uTBdikW2Y+W20PjQMzCJkN9a96dwA8hfxdr5GG0EqNTN3ek6SXmUWX2XXY4PI9HxUYDPfRdGtfXveXcAPH/wDGcBLj2CTjxJ3a8t3+aLmaTR7be5o91/z3rON1oBRUfYveHcAPHr8bwTPcVj2k3ueS+h2Vk6vk77eo2F8KR8+7HhtcAAfZPd/cAPHb8dwQATe74/6JS2TE4ytnXT7Isr532XD60rKm5sUKLaH2b3d3ADx0/HkIAE7tea7eXjtpG5vfzaUzYeA6rkdYmdP0s+6yFz3LQB9n93NwA8cvx9CDNew2Fe6wTdnkurTU9DCUx6/Q7vg8ey7voMuLHdlt0vA6k+0e7e4AeOX4+hGe/BYzZMON0PT8h3dxsNBMyKWcJ1uh5iR3/VWc/q4kyd0d+h+cxKfZ/d3cAPHT8eQknFjBIsxZuzy6Psl2LV9HFtt5WVJ42N030TNyU/oo8rS6PrK8Fx77N7u7gB46fj2DlYgEuI2PYxtF1yPg6LDB5PYbXkdXf9D6zTa3smPM5rHvtB80w/ZPd/cAPHX8eQZUUKVEmNTZ9RM5bR29GsxdPTk9WfVd3xfV7JAn3RuH7fXfIKfYPePcAPHn8cQb7ABfYSN9l4LH1nSbGNqOfiD6xuuH7GfbAm5cXC9rC+O2/X/ePcgPHr8bwQAAZrcez2cGBGC/6R03MTOkrHkNToeq03yzF9i94dwA8dvx3ButAF1opUADs+8wcd2exiyo/FdRK4/5++y+724AeOH5AhSooClZUUArQBsfo+51/L7Gtdf0WyhfMdU+z+7m4AeNH5Hh5rcYCVFAJf6I+M8kA6Pvthh4Pmeh+gZ4vBctR9o929wA8YfybESsFgM9MIBn/QPy3iQF286nFzvP9p2mr43QWH2f3c3ADxc/KMUk1jUZM2LEKVCZ1Ol0gAkq0mStXED7N7u7gB4rflaMEiqzCAFVbbrQAUqA+y+724AeJ35cwABSoUV2EmfppWmToIAAPsXvDuAHiN+Y8IAApMiNjJ1my+gfK8XYceAAD6/7ybgB4gfmjEAAG/YpNt9l1tGisAAD7B7xbkB4dfm3GAUqClaK0VoVAAA+xe8O4Aed3zm+tVSluOyhRSlKUtpbfkvFKUpbS2ltKZalev8ASmYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA//EABoBAQADAQEBAAAAAAAAAAAAAAABAgQDBQb/2gAIAQIQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAIgAAAJkVgAAALSKwA4ZbVvssAWkVgDHxnhftz9GwC4VgFPP50mJ1R6AC0isAxc8rVy5207pAtIrAPPrmevn8+2nfZyvYtIrAMnDLOngnRvyfPZren9BNpFYBXzqc70nU1/JarRn3+/aRWAOGPtbhaPQ83x7Rac32FpFYAVrOHRpeV5ab1y/Y2kVgAA4/Jb+d+Gn6O0isAADzfD+k8Gv03S0isAAAc+haRWAETxtw7dQC0isAAABaRCUAAAJAAAAAAAAAAAAAAAAAAAAAAAAAAAAAP/EABwBAQACAgMBAAAAAAAAAAAAAAACBwEGAwQFCP/aAAgBAxAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAzkAAAIhLIAAAQDMgG0bv1+boV31QCAZkBYGy+rtnnaT2Kl6QCAZkD0rX3v3ePPBVvUqUBAMyBYu1WpPQNg9zy6mrDgAjgSyC1djsx8x75c/QqaqelnvdfgIBLIN93O1WiblLyqvqvZPpPberUFCcUAlkHat/a9n8f3OtU/n179l6Vw821VbQsAlkDZ7C83qbb4WKpsP6A9HYvYpXb/ieAZkA73Y47J1TUY2dd+2y2entw+HYBLIAB6f2dWG4cOdW+a4BmQAYyLDvj5ev70/mLowDMgAAO50yAZkAzjkxyccACASyAAAEAZABjIMMsAAAAAAAAAAAAAAAAAAAAAAAAAAAAAH/xABEEAABAwMCAQkFBgUCAwkAAAACAQMEAAUGERITBwgJEBQZITBWICIxNkEVJDI1QEYjJSgzRzhCFjSQQ1BRU1RXYXGB/9oACAEBAAEMAP8Apecu3SE2nkX5SbjiDWISL4+fS32NsyA8D2l3uNg9DJXe42D0MlL0uVhT9ipXe52H0Kld7nYfQqV3udg9CpS9LpYU/YqLXe7WL0Gld7tYvQaV3uti9CDSdLpYV/YopXe52D0MNd7lYfQw13uVh9DDS9LlYU/Yw13uVhX9ijXe52H0KNd7pYvQo0vS62P0GNL0u9jT9hDS9LzZPQKUvS9WVP8AH6LS9L5Z0/x6i0vS/WhP8d6030vlmJPe5PttD0utiL44IiV3uVh9DDXe5WH0MNd7nYfQw0vS52FP2KNd7pYfQo13uli9CDS9LtY0/YY0vS8WRP2ClL0vNl9AJS9L3Zk/x8i0vS+2dP8AHmtd7/aP/buk6X6zr/jzSm+l3sZ/HAUGh6XCwL8cHFK727H/AESNJ0tuPr+yRrvbMfX9kjS9LTYvQ1F0t1hBdFwZEVnpaLKUtgHeT2QjFsnt3W3RJrOvB8jntNKXOezlammDF7fJ1vitld7ap6jaAQZ8qG+yKR4ixz9rT/uOOShIaJE1Vy/SmwdccjVdJzdxkI6DKsrBH+ExWE/Jlh8nnqNbuc1m61evC7zE85f0HxrTzPr7EAf4DFYV8m2Hyeea3u5y2bLV9TS9TvYZhm6HEJRaa1iNfR19e1tJ8IbOnaI5/jioNdnYf/sPbTdaNk1BwVAvLECP8IEVJDkL/wBg5Rtm3+MCGtdevTzhbM01ECJFRRXRU0X2IA/d49YV8m2HyeeM1u5yWarWQppfZ6dYNBEbF14UNx59yQe5wty+wzLRQRmQiuMyY6xzT3kMPbi25+Z4th7sTH21NBcI33IloETIBjsskzbH3mD99zctuPsqOIrmrltdEm9puIkmzI48TRsMurIsDRESNkccpdtfhoquBqHmMRd7fFdLhMrNFnwjsg3RT5Jrqsh1aS4yETQnFdFEjy/BESM842bLhAYqJ9VvHWPHrC/k6w+Tzwh3c5DNKyPwv1w6obYpvfcTVp10nnCcNdxe1EJHhWKa+6QqJKipovsA2TpoIopFbrDtLc8HFdYtiSWEPelPOxm4yPaoJzswhsq0UdVI3syVZBONseAZa+KGnAbVAzA0ABJhNY2XRZEgdxEFMvR5DD4NruqTbgjsNqwSEtzx9N68EeC8YE2ZAYqJ+TEYR5xVNVFqTIWS5qqII+w2vbmOEXi91W4PusbWsL+TrF5PPA/1IZrWR/n9w6nnB7Kw0C6+3pX/ANeFTXBfdF1F1LrbaJ5wQAVIrZaxgaCqbnhihbm0fAtwXnKW4z6dl0dci2a65C4rhbhCNg0CAglOfRabbsUUVFmNxi7Zb1UVS3O7TSySUIXoitE/hNtnp9ykIhzbBdLERG2pqFoyj+I006ItGTDEhXHTMSK52hZgIriI2460bDhNuCon5AukDZAi6D7LThMuCYLtJfFVXqto6xY1YZ8n2LyeeAunORzWsj/P7h59itatIKqidojtpagFHtCC73p6a+cKEpOBYsRYgMJNnkik1Il3FVCC2kSMrFtiEouE5PktPTzXWLbW2B23vTTSOlOPXIF+8W9p8CG2Sl0VHLfJNyZbRFuQiTYV6xeNd2TmW9UErXd37O8UWS34GK3NpEMhEL1bUloe1d0n9DbR1hxawz5PsXk88Iv6kc1rIvz64edZoSSpO801atjDD6b3v7mU3txUW3j4njVhYs0FZ8z+9s7cvbrkvCjID91b1dLsMCPJFP4dqhoROxJRJvmXRGE7JA3LrdXNWobyCnY7sjhSpJgqN3SGLjYtvW1opMJztUMmUFEn2xVVL/Z2sjgLNjCIP45dUYdKNJ37p4q80KxmFEr7C4DwvgKI17YtEbRuJ4j7LTRPug2Cakvgqpr1WsPuUWsN+ULH5PPDLTnKZslZF+e3DqebHsrDoJp5Hx+HjU1sWHRaFNC6rNDViMyCN7iuc1IkEydThHh1qO83RZTy6oojdrgXE92A2o3Nw5cpVCDtW7CsmWfBhA7KuA/dkSDBQbXGcUNHJzvaWlBNLOSipWp8/wCKy5BPWXbWUXck+ELSR17bbVU2HVSOg3OEujTyt26U3OYRThZvZ1gTG5zKaN2Oe/c4A6OAhXa3k5HeYJdxae3FfSO7qSbm5MZY5pou9v2BHsDKmXg/1WsfuUSsN+ULH5PPFPTnL5vWQ/ns/qhuAu9h1drbrRMuE2abS19qGKMiso090iUiUlXVahsdplMtVbGDcdIwLYGZT1kKzH2qh26P9iYwKbNHn4xxoES3Nkm+Qx2yW1bm1RI2iXWSRGiBb/evCGSmsW3MTScVW7VDFBJ66doRlZrIuvzJLC7blDF9kRK2B2yG4r8Jwxt5hPjluiCgW64igDrCjxVFyZaXFRAOOl2x+RFc1J/GHhamOMOmoVMCOyYPAakVzj9lnvtaaJ7ceVwhVsxR1lYrT3iw8KV9mS/pHMk+zXx/uILCI4xE8W/vDzjhOmRmSkXVax1gw6w75Qsfk88gtOcxnFX9db3O6wdCW2LTxIDjzDkc9jgqK+wzERAR19VaZkyFkGnuoAdVl2jPAl1qAx92VeKquXIll5EiOp4TBR6fbIuu4Y7nEu86So6hHNY9jfkKKo9KY2MQ7awu0pTaXCaMJtUbi3nIzIuzxE4LKuvLIRf91pyJ+G5w3dXGg4dqmNG0quQIjHZp0q3EiKyIHIsj7Jlo7MeFfsu4JqqttrHyCSyKIIG4kLJyLZqkpxlYaojCoeQHxZ6OImn6C1J9wiVh3yjY/J55Zac5nOKvv5zN9hqYbYcMkR1pUiPfVyOXZWl+Etquzxx8TlotdpYZ/ss7ideN81Nw1Muu0ihSkqE0ycbYBqhsCq5IQ671TUsqFNNqxdUt91Pf7zzajbrW2hJp+LJDUqF7h2S4PprxI67jM1+JwpiNdq1ZQHS1bA08FiGT+LO66ayCTttpe3LujAKXG6tom4XNVxZtfBKlqiX+3Eq7qyAeFkjnCTRVKSsVdzQkt7XWQOvgvn2r8vh1h3yjY/J55hf1N5zV8/OJvm2jVZYolRHWTibAbXbqLGRrw9UQlAMkjOKqlUQNWbrGQfedIXLNCeTVEcNGL+y6iattRlP7QtpqgqYFBkmBoqITDBNaKiKCr2gxbBNUON2Szx4Pikh0FcvUKOKJpFd3Hd5W5BF8UDHIjXjvfTfkkQRREq9l2rJC1KjZdahKrcjVL4mkhvx1XrESMkERUibtjqro4QtK1j5mmqNvnX/DR6f2Hadx4wTVWpAU5a3EXRsxcU2yaJRMVAvZtKfy+HWHfKNj8nnmL/U7nVXvxu83zbIaBcmUVdEtbrjrXDbDbWQ74V7bk8PhpcHiWPb57YogmaRb2DimnBhtIhzbYZaIAHcrarG7ZKNPthpuRHXZcHY0bIXFbcFYs0rY6k9YW3+JHt8PH9Fe+8TWt0VSuVx047RlAhPTH1VJkhlYtujwNPvD4I/d4kNFThRHxkXG4TTXVuE4NwyInSRVbnIykXRpwhXI3EK6GCfDqh20pCip7hG3Y4qiiEnBGFj7UZtNAFpAtjI/7SWuxtCmnD1Ry3NOJ4AQ1LsTcgVHaDqXHG1QVEUQhnWo46koIWnsWpP5fCrDvlGyeTzzF/qdzur3+bzfaahvvJqDRkn2c8nx4Q19myF/CInTrDjC6ONk2vWBq2YkngtukG6Qk0u0Mvt5vw0cEkMcOmhdrO5BeL3o4FcLacRRVJbjh3OK3MaRBlkSzUG4w/dfFG7mXaYjnZZsq8HAUTk2/wC8WSUtxycHnURCahiyEiU22kiQUdI5druzm50dXD+0binDajvE2L11mJ4q4dttjr7iaysilf8AD+OJGE0V3D4LoockWuIlxkR3XxLh8NJT6yZDjpfGrXbCkmBKG9bLYhbRTLU3Go4MomxPHwTXT4k82C+Kjr29rx0KgkAX1GvBU8fgbIuJtNN1XayBIDcOqLeLSUdwyQUQ+u1/l8KsO+UbH5PPMT+p3O6vf5vM9hmIrgcVwkZZ7W2x4RmkRXX3H11ccJxepqa+ym0XF2oceV4EKRnH45xj2mmnXYJpLFVoSVHeHGeiABop0w89jF7Q0RUalmZizdoZ7iNdxjcrcm4diSy7fbS4bu6LdT1e1gTYMeeDqBKNuTHt7bbGZIDOmxYdzcuUpWHVZZdOHAe3vulcZTjJPbZl0NAYRe2l22V/DgRzWbIO5yEQYl6uRZLeU2qotQ4xWqIPZ3EIMguSrGItNrlQo6SHveReHj1nJE3mKIbbQgCCKeDrqNIqqtT8j1VW2BQqNybNXRTcUXrbMF8U4SUDUyIibHXQqHkDkctskdBZfF8EUfFFTX4+8l9tCPNKYKiFconZntRFRDqta62+HWHfKNj8nnl/6nM6q9+F4m9cdkAb7Q+mrb8g5J7jX248lBDgvIrjEmOsc0TVDCoUs4UkHgXxtk5qOqONqpDfrMV3hgu8d+LZI5YZRR3/ABZJgoxJNthcQG241zd40F3skp+b/tu0JUpbcxPa0gXA1OwsHFyplp5FQ37vBMZER90mlYfjMFpbIpSHXmW4pJKub/GdRt26r2qWqR4WWZP9qOJChLtj49aVtjZHJa1Ke62n9tzhsXCYU+UTq+A1jUBTNpNKhtI0wKaaU65sBVKrxdDmyFYbXULRjqGKOPJTMRpgUQARKeigctslBVU47bo6ECKl0sSEKm0lQ5p2aRwzVeztPI8CLqlOhxQUV8Kym2ILhoIrp1Wvwt0OsO+UbH5PPK/1OZ3V8/OJvVFY7Q8gqu0JUjtDu5E2h5EQkkNrFJaVFRdFTRatFy7KXCdVeBBmq6/o6glV7x0bs0DkcAbctd/n4vKJo0Igi3C05GIK2fZpU68SbDoEgwmxYuZWYHFeCIrcjHpzlyy1p8h0UoEVoJE1xjtTgvXSd7rLQQGpL9ssI8aW92mXeclm5JJRlkSbasuPNQyXtiKMh2a5E0YbTijeLiLv3ZgtWqYb4z7beulYrGR0OKiaIiInj9Mim9mi6b9p41bO1PcYh0ERQUREpFoh3Piui19K0rJLWhDxhHRcYlo7HVpS1VUX/wDcsj/dCdBPfmNizKdAF1CrYv8AL4VYd8o2PyeeUmvObzur5+cTerXgW/w8C8lFVFRU8FnpvMH08E6rbdezojTyqrUG5IANCuhDcrYzc2nG+Ai1OxV5lxOyOI+sy7SWy4L+j1Rrkwj4kscmyczBpTimywbDsTNpNuAhjgS1My68XoxbA1CoeMyprhFIJWltdmjQwQEFWX5s7iCbTiDrcrtxEJmORKHXjAcKKyOlD+HRazJxXrjBZVfdx9lGLeH0VVrVBTVfgdwaRzdqtNuI4CEnwq4so7FNKx/WPktwYTwFF1XWrw3viKi+KEm0lTqt3/IQ6w35Qsfk88gdecznVX385ndTjpOC2hfDyldImgbX8PXEnOw191UILffAI0UT0O65Y7Fb2pH4bkx8pLxOkuqslo571WW0tSpEPit7W2MdhKPD2Mo41Gji0pNAjTz1ybcRCZ0R+531tFRTJEcm3N6d7pLsa9jHdCjNqlImgotZcHDu9vNfhZTQ4LapWlGm4VSnDfVEb4bNRmlZZEVXWlqWukc1WrKvGy+aaeKIOgolXNdIiqvhTi7nCXqt/wCXw6w35Qsfk88f/UznVX386nfo2ZrzI7BPc24kST/dioKlAgkqaOvBUOW1FKN96IgeyoTcE+I8pP5CrhEQs7ikXKTJFRN1UD2WBE3mxNdoYs+ox2BL4prppWYQUkoy7rtrFLhvZ4J+Ba69RF95BNUr69WQTkiQz1XwxSAoOyZC6qal9aymT2W2uLr70tkWJLjYqpJVsHfb4dYb4YhY/J55B6c5vO0q+/nM3qNsm0BSTRPKVokbFxU939FjU9CP3i0pkt4CX1nxRlMEKpuReLZJ+7Vdttujc1kV1RC+P/zRH96BNUSkqZObiNkREmsyU9f7gDYLo1b4gxWRAE0FdEXVfhl9yTigHxRSUlVVXVatX5fDrDvlGx+Tzyz05zueJV6X+bzOpf41vFU8S8n4rU/+GTUfythbN+1dnkWaWTLyAn4rLdAksiu73E8fjV0tgTG/EfedjSrUak3+CJl5NDo+BIjuUCMps0NvZIzBTTayJGqNzb0aqfutWy1BEbRERVr/AMdfGrtPCDGMzJEq9zifdJC8D6rT+Xw6w75Rsfk88w9OdDnyVefG7S+qI+jDvvopNSWCjOqCqhJ5EMUaQpR6KJKpkpKupeRaLW9erpEgR0RX43Jfi1rw+HbLk6Tp8pGDphN3abYeKRB9tF0XVPBbJeVaJTXxW3XJqQ0HvotKqFomlOxWnxVHFRKv0BBdUmHFaL7Tl/8AqHKx+Oi3NtJBHIpiODSJ4eKrp8EXWXOCKCqRIi5BfllFv+LRGpkpEu4uq1fl8KsO+UbJ5PPQLTnRZ/V2XW6Sutl0H2kjvLtp5k47ig4O0vajRuMima8NiTI45CIjsa8mA5JamMnDVxJVrz3Gr9AhrflSFP5Vc1j5heWEhCSQPIbcJo0MFUStV6Jok2bQOPlrDTCo4exZ2bwHYZAKkTk29NSX3tiqQLWMSCS7M7BQ1KW00i6kiLcskZiN7ULQrzfTfVUdp5433FNwtxddrX+Xw6w75Rsfk89JdOdJygVdPzKV7DUtOGjT4cVpYPF8Yxo+hCoEokiiXUxHdklo02RqjDMbxfNHTkSTkKmugh5Vnu0ixXSNcIqiMlzldv7pkR9jUslyhzJezk7Ejx3PKCcWxAeFH2+FFe/tukwXYXi/AbbifZkr/wAkqjFMhPi6BgyT9/dVFQ5WqvXEy3I0nCT2bUutvh1h3yjY/J56p6c6flBSrn43GT7Q3GQIoKucQe3a/GOwtdvIfwssAr0x6QKC46RD5YipqgiikpCoqqKiiSNmQqSCSiiKq6fGnGjZLa4BAXmaJ5NrX+XQ6w75Rsfk89lxB51PKElXBdZ0hf0tguDdruzEp3iIF1vLE+6S5Io6gWG5JHxi5Rdr++3T24hskYmVZZemr7dBkMo/w+qNYrhLtz09mG87C/RWw0S3w6w35Qsfk8949Odbyh1N/wCbe/RQ7XInxZkhkQVrqx4Izl4jjL4SsXaLBW6zEjcPs7U15ho2mz2hYo0UjYfce4buSMWORl743l9rSWjQynkjqpMVbyx5ICsSCIJH6K3f8hDrDflCx+Tz4T/qu5RKlrrKd/RWq2RZEQzdbRSt9tjPg5xmEBYtvjOiKvBwaS025VTV5UT7KgbFXie8lotqnor6oKWqAoaq5oa2q3qv95Vo7XBTZtLfQWmIrbJbwIo9sinb3HCj6vPiIPuCP4f0NvT+Xw6w35PsXk8+U9vOx5RKk+Mhz9FpWleFaJWlaVpWlaVpWn6O3jrboVYb8oWPyech0budcsHLhk2ZWfI8ej2vuis8MlI8ixnVOiJzb65Djdd0TmnqHHK7onM/UGO13ROZ+oMcruicz9QY7XdE5l6gx2u6JzL1Bjtd0TmfqDHKXoic1+mQY5RdERnX+3IcZpeiIz76ZDi9d0Rn/qHF67ojP/UOL13RHKB6hxau6I5QPUOLV3RHKD6gxau6I5QfUGLV3RHKF6gxWu6I5RPUOKV3RHKL6hxSl6IflH9RYnS9EPyk/TIsSpeiH5SvUWJUvRD8pn0yLEaDoh+UnT38ixLUeiI5RPrkOKUnREcoH1yHFq7ojlA9Q4tXdEcoPqDFq7ojlB9QYtXdEcoXqDFaXoiOUP1Ditd0RyieocUpeiI5RvpkOJ0vRD8o/wBMixOl6IflJ+mRYlS9EPyl+osRpeiH5TfpkWIUvRDcp/0yPD6XohuVH6ZHh9d0Nyo+o8OoeiG5S/rkmI13Q3KT6kxKu6G5SfUmJV3Q3KV6kxKu6G5SfUmJ1aujD5TWVjMyshxMY9mt/wBk2eDBU+Iv/T2//8QAShAAAQICBAkJBQYEAwkBAAAAAQACAxESITFBBBMUUWGBsbPUECIwMnF0dZGhIEJSwdEjQGJy4fAFM0NTUJLxFTRjc4KQorLClP/aAAgBAQANPwD/ALXn8Potj4UcPGDtDy0OogYt5MgRXUmmRB/jgqP/AOdeODh144OHXjg4deODh144OHXjg4deODh146OHXjo4deOjh146OHXjg4deODh144OHXjo4deOjh146OHXjo4deOjh146OHXjw4dePDh148OGXj44ZePDh146OHXjg4deODh144OHXjo4deOjh146OHXjo4deOjh148OHXjw4ZePDhl4+OGXjw4deOjh144OHXjg4deODh144OHXjY4dZj/ABwcOnvaHxYP8XDyxpNZAMATkLphYTCZGZStouAI29DlLN0xNiupMJlMTsUjMF51eSpEk0p1Ss/woOBkDKdedAzJbFbUaxOX+XyUpOm4uLtfYpNX+z8H3behylm6YhFdt/w+i1ZBg+7b0OUs3bFjnbfY/uRDIarzqWeYYPmVpc8//SzwohG2a+CNVPsNnnJC4jpPwia/IV+IS+5aAtPs0WrIMH3behylm7asc/byuE2QjZLO7RoXoNAzezcfeZpafknCbHixw6AGRe6oea+CGJAa/wDRNvc2k5NJ5obIBC2xO+Jv0QE5youTfdeJtOv/AFVlNtY/TpQZUpTJOYC9fG8B7/Woal+cr4YvPHqrq+Y76bEDWDy0WrIIG7b0OUs3bVj37eSF7p951w/dwTjMn23mbCfdddqNiBkR7JqAF6tEJtg7Uz3LGNUOqR5rfK9CpwhiQKIlJziU6uu5NM6TTWERJwiikFWZsrb5FRObKc2n6K0wj1XdmbYm1FptHRMFJ7hcP3UgJNYLGjN7MMThuzgWt+nLRbsWQQN23ocpZu2rHv28lb3/AJibPIDz6F7QXj8V/nbr9hxkAL06p8W0M0BO6zbyM5NwUpfhGpPrm6ctQWZxl6D6oWFsIV+YQqNQ+iN7oY+QUpya75H6oWuhz9QgZYy49oUua1ps0tPyUvs4pEqWgppkQehdKYzys9ppmDp5aDdgWQQN23ocpZu2rHv29PFFVL3G506ZaXbSnOtFrim1yNY7BnKPWiutOtA2NsQEpvFaN1SArLQETVbJXRG1kDtQtEpV6R81OXPtac80BSND3hnGlQRU4WPbm+5UG7AsggbtvQ5UzdtWPft6aFznTvzBEzN3YFPnOt1Iippt/KEP5cHOmdUCqkE2oxnhOtYw2IWGkj7ryhVjmCxOthOrICbXFgfomDqXzzHQp8wzracyBmCapG8KNXIWB146BkqWv2nGQ5aDNgWQQN23ocqZu2LHv28hmx/5gbfIjy6FjQHn8V/lZq5XfaxBouH7zpgpCV7jYmOmC68/osFEpiwlQaoTc6hnmQxVSQqLzUStEyhnarjWE7rXkBf1IBuTzKNCzKOJRG3AlRDOYz3H95k6QrucLE4Y1lV4tG3oHCi9ucFOrY8WOHsxWya34Gm0nSbuWgzYFkMDdt6HKmbtix79vJFqpH3XXH9500yIPtsMmNPvPu8rUTMk8j3AJxlKVwrVriRaovNB0m0/vMo5pRHXrBwHPOdYNVL4pKHY2ykm1GK8SThTo3SnnUv5jBNO68I10QoxlEhiwTWGCy4EpwpwioE2id2b1ClNtcpEIOBEzcbUHGXZd0BMyw3HODcV/bjGiRrsKztFIeYX/FcB6Wq57hJjewX604zJN/Li2bAshgbtvQ5UzdsWOdt5WiUOKbJZnaNNyuzHsz+zd8T9AHzTRJjBY0coBAlcTUqM2tnKslBwBDcylTc31UBlETzrCHkA3qJzonYsGE4kr03mgMv7VRnbpTqnMfXUsKqIJmASozS6HO5YI6qWhEhjtKwiGXALGnm9qoub1bCKwnMbPUB9wxbNgWQwN23ocqZu2LHO2+x/biVgdmbUs0qbfkR6rSHD5LNDYXH1kvjjc70s2o3k+yaMnWyVOU0yF51IvImi8TGdQ4PNUSIWlyFSo0h9q3q21idqqUF82lOEjpTmTPkmxavNOhgGSxlU+1AmvtaqI+4YtmwLIYG7b0OVs3bFjXbelKotLyKpIPqJUWFUdSBLgFBeKRzKPDozTuezSpyOgozJ8wgsIeHFuhYOyk4qto8lFiAyz1qFCmZoxLR2qbpX2NVAT8vYNgAmvhPOd/lEz5rPRawepX/OZ9Fnk1+wr4TzHeRlPVNC0OEj7WLZsCyGBu29DlbN0xY523pXzZPtEgg1zSSLZVpxDhmTHSJ0XLCmS1o85hKwU1ZzJQOs01EptRBFTiiZS1odWG0VApwlCh5lhMwxptksIdScVgraTiM6YCxrhYEXl1k6kWGoG8lQ2tZrAr5XdVrRNz+wfNG1kM1n8zrT2CpaAs8pL8y0SK+Fwr9UP6UWsDsNoTa3Q3dZoz6RpHs4tmwLIYG7b0OVs3TFjXbfazyqX4ozB81+CI12wr8Ql7DTMKJKJMeqgmYlaQUBRA2H5LBTNs7ZBYMZPZeZJlUSFnTanQzVND+oLCnNcZBOeZTuQrhwQfkmfyYSNUFpWFmTQbQCo4IOeu302p/MGjOoU4j6vdaE9xdyO6jDYfxHQPVGVJ7v3UNCzyrPYtFZ81prK/ItIIX4qx5rMbdRQra9tRaU2tzWioj4h8xd7GLZsCyGBu29DljN0xY1232AZU3X6ALyv7kUBztQsC/EZ8ptY7nNOo1K5za2HtF2pGsEVhwzg8sE0m/lNv70otrLbwb9SJssm1EDGNbeM6/rQZ2odeBn1Jtl0yiOsUKUpWXKnW4mpSqFsih1IA+ihfy4RvUKeLhusqVKi0G4Z0GkBui8rCbG/DDH1OzkZznStOYDSbE7rSsAuaNAQs06SvU/ovi939dmlZmmiPSW0p0zIvdM2adKHu0iR6zX9xoq1i7VNETkD6go/wDkPqhWx0rP3YU4nm/CRaP3dLlxbNgWQwN23ocsZumLGu28s5MZe8/TOVKQAqDRmA9smy9pzjSnCbHixwz8jTWM4vCiCcMmvtaU1s2Gw9iJlIidE/RPriQQZiWhNrdDdUCUKhFYFdCe5Na8EeSDzWBaiP5jxUFOrB2mciodbYNkwEOaQ0SpaOxPE3PtoNUqUQCxjc3aVY1uYXDkEorp3k9UahM60RM9ivGwKcjL3j9B66kQDXyV1z7OS2WZE1j4dI+YRtIuNxRuzFRBSboeB8xMahy4tmwLIYG7b0OWN3bFjXbeQCk52ZotQFFjfhGboXGcIn3XZtdnkhdyOM5/Ac6o1ifW0jSrnj3tB0oGRhuOxG0ioz7FnMirg1Oa91eapGIZNFclKtxEkK5GuvsTqhCZf2q4nqt/VPnRpGz8TtCDqT3j33Z+wcjnATUR5cNAsA8gF8gnVA5ibTqCFxUuSRv7OUeShGhpomzWLNS+YUMiI3VWg40ey7kxbNgWQwN23ocsbu2LGu28kd3/AIt/XZ0QrBUZtIy+Kx3rXr5fdeOszs0InrA8x/0KtBcZPHZnUp0bHBNMi2MKRGu1Cv7OJV5EFQ2OYXMIFIGVqcZ/avmPIAI1BsFsj5q8OrcSm1zPXcdGZQ/enzG6Sc6NT4rus/6D2Gw27FIBF7ohHYjbyiY2I8kk9gfrUwfMItIQMuTFs2BZDA3behytu7Ysc7byMbRb2TJ+fRtJI1/6ewbWOsKlLFRnVanJthe2sDtTjOaKisic5zpAkS+qb7xcTSUMWMaGjzKBlKGJu1lCrFwTMn8zkDMQ22fqfZMMbFzUcY3WpcoaWh2LE5VX50OSSZBkSuapE+qJJ5MWzYFkEDdt6HLG7tixztv3P4Hik3yK+KA6j6GaAsLAfmoFItBhZ5adCaKqDA0bU610Z5d6CSNrGCiPT2nOAJFwTPs3doqUiPJQ3h4dmn8pyTapcsj8uWSjvAJPr5WKt3yCDJDtTDRmc4t5MWzYFkMDdt6HLG7tixztvI9tJukWfLo3EgHst2/c4oD/APqsd6yOtHaEQZDOLwpTOkZ/r+qI5JEbOQXTQMxOwnP2DagKLey8q3sAsUP7V2aqwazJGsnkxbNgWQwN23ocsbumLGu28kB1E/ldWPWfn0cJsnfmNZ+mropypSqnm6EOpw5/FeNYq8k683FWnRpVtVs84Xp+mzsXxSmPOxFrjOdlila0VedizXazfq80bSai76BWGV+gICbiohpvGYe6356+XFM2BZDA3behy1u6Ysa7byOFF4F4P7nqVrXCxwuPQwzJgPvPu8rUayehwmK2EydkyZVrCMMnDe+JQdEi0Jc0TF11fnUsKYYkB7usADItPZVXmI6G2Kwf+4+Y1ojmuWb6FfFYQmhxLmVUpL8ydDDxSrkSri75BG68/RAVke6gfsmH3z8R0D1KJmSb+XFs2BZDA3behy1u6YsY7byj+XEPunMdB9EPbb1nnYM5TBJjMw+vRB04ZhTpT0SrWAPbhBgYVBiThRB7zZDO6YnnFVSwNhhwnPBBeSa3S1AauhaZgi5E1wXGTXHO03HRYm2w4gkRqR6oIsWILWnSeTJ2zmszaz5o2NbW5yugA/8Aufl5o2n2MUzYFkMDdt6HLm7pixjtvsCyuTmdh+S+Cx41fSaFoIkRyi2Qs7V/ahHa76JvVY2prR0eDvpwy4TE+xOlMnBmzMpSmdQ8lDpF74DaOMc6UyRZ7oqHRiwPtHYbV8MUTHmPoj8EQLUmto8+I0VeaPu4O3/6PyCda6c3u7XfT2sWzYFkMDdt6HLm7pixjtvtCwRAHAea/JJZxDB2oWNnIDV0hsAE0LQbk20gVDk+Fwkfu2LZsCyGBu29Dlzd0xUzt+6spAmDKmJtImJ3iaixKYDwC54kBJ3l6qNSohhbQdNoHOmZ1SnUmPpFjQJPzV6EIYZPCSC81k1y7ZauWB/MjtbNrO06/ueLZsCyGBu29Dlzd0xUz9ywRgiRS6I1pDS4NEgTM1kVCfLXMR3UWE0TKkbhOSEWTcTE5jBIVidonPyTrQmRWnrSlIiVSh4JCbDa6IWtFZnWCa5SkJ17A9whl1pbOqerkOAvitex5oGNi4kmOrqNKhnsl9zxbNgWQwN23ocvbumKkfuQhgh1MiZvvr7EITnib3CbgSKOxFszJj3yMyJVHMp1nJ4lVf5s1aAmBiIlZlOXWz1KlKeTxLKUp9bNX6KjOjiIltGcutnq9VMj/d4lk3V9bQ3/ADaEXNBGJeJAmszpXJwm5lCICDOyc5WX6UDzeea66qp3iuaDiB5/csWzYFkEDdt6HLm7pipH/D8UzYFkMDdt6H+LRmx2QMOix2R4ZDGtIIbBc2XNtmjWZYbhPDLvuE8Mu+4Twy77hPDLvuE8Mu/YTwy79hPDLv2E8Mu/YTwy04dhPDLTh2E8Mu/YTwy79hPDLv2FcMu/YVwy79hXDLv2FcKu/wCFcKu/YVwy79hXCrv2FcKu/YVwq79hXCrv2FcKu/YXwq0YdhXCrRh2FcKu/YVwy79hXDLv2FcKu/4Vwq7/AIVwq79hXDLv2FcKu/YVwq79hXCrv2FcKu/YXwq79hfCrv2F8Ku/YXwq79hfCrRhuFcMu+4Vwy77hXDLvuFcMu+4VwyYWtc+DhWFOcGi0gHBwCZaQsGgQ4NOUqVFoE/T/t7/AP/EADURAAEEAAMCDQIHAQEAAAAAAAEAAgMREiExBEEQEyAiMDJRYXGBwdHwQKEFFEJwkbHhI4L/2gAIAQIBAT8A/bAq1atWrVq1atWrVq1atWrVq1atWrQ+tHJPQyTNYuNlk6oXFynNVMxN2ijTk1wcLHRDknoJpcPNbqhG1gxyp0zjkMvDVF/afumyOGh9UJGyZSDzRxQO7k1wcLHTHlvdhbaiAJMr9AnPLjiPzuHeu4/5/qF7vQKs8/b7hX89CoyHjizpu9lC4xuwHoRyTy9pdlSfzWNb5oX5+p9kO74O3xKZASLNDxzTmFmRHsfYrI/Nx0/hB1Z79f41U2Tw4b0DYvoB0m1Xkp93gVv8/RNNAeSveptGjvX6fL1yR3/+lPowFM6o4TNGNXD+U17XdU3yB0m0tttonHE1/YqrL53FaZ/B49yje9rSdwCx49T7+AXf8vcPJNbiIaPD3UpxSADcgKFLaNpbAO0qWeSY848AJGYKg257DhkzCa4OFjTgHSObiFJjuKeWu0KkjMZrdu9ivDX7/wCpgyeb3aVSBcdR6fda/P6900cS3G7XcFAyzjKkeI2Fx3J7zI4vcmxsjaHy79AhtTm9VoAXGtkylb5hSRGM1qDoVsExa7ijodOAdLLEJB3przH/AM5BYTYmPORsdidAACGb1+XfeZHzuWKOLPUprHTHE9AACgvxB1RgdqgYHyNB09k9xkeXFEIixkhzonMP6cwmuwPDhu4B0zmNdqmRtj6oTw4imriJHdYpkDW6rTg/ERcYK2ZwErbVYHFp3K6zC0Caaje/tyQGIho4B9LNHxsZYiC04TqEHN2kDOnj7oxTA0WoRSEXJzR3qWUOprMmj5a2GIySYzoP74ByT9DtWycdz2ar8tMTWErZmvazC5ba4mUX2KDZZJzegUcbYmhjdOAfUmJhOIjP6IkNFk8HN43TOvVYA3ERvWzSB7AGtIyCleWCwL6IfWjk0q4aVKlSpUqVKlSpUqVKlSpUqVftl//EAEERAAECBAMEBQcJCAMAAAAAAAECAwAEBREhMUEGElFhEyJxofAUIDAyQoGRBxAjQFJiwdHhFTM0cHKCsfEkQ6L/2gAIAQMBAT8A/lgItFotFotFotFotFotFotFotFotFotFotFot5w+uj0NM2fmqjiBYf58eBAolHpYCpx0aHiSDy4jlBqez7fUSCcCLi/uOMJf2cnjuk7pJGffnhnE3smlbRfk1gi18MdbWHHt+AMTMq9KOFt5Nj6ceg2coXlZ8qmMEDXQdvb40hyozVTeNOoad1KcVL0TbMg5AeBzk9lJBhPTzH0yj7SyUoJ+6B11914bpDQT9EyLfdlwR8Vm5iboVPeG4+yi/NKmVe44oJ7YmKFO0ZZfpK1HdxU2r1gMyRbBQ+8nGGzJ7USxCU2dGY5nUn/AAfdbQzkquTeLS9PTDz6dKmcmUtWw1isOOoSzQqePpHcCQLXBwsRp+V9DFMpjMjLplWACgZXyWpPrOL+4nJIyMIT1gtBJKsjYFahxF8G0DQ8IWGSevuk81OOH3lOHwhJG4ejPVGe6StP9za+sBzELYSEWOATjgb7o+22fs39ZPCNoZFymvisywG+kgOAeqd7JY0svuVG0UqioyaKiwDYi+QA7uX4D0w8/Y2XC5lTpTe3O3b8YoCVT9VnagT1k2bSeazug9oAMFDSQR7GPH923hb+9WcLCsUrG8okAjLeWRcJvohAzEVHa5mXd8nYK3N02JQdxHYkAd5+EU2ry9WR5Q0s9U2JVbfbJwBJHro0N8o66RdKbKG8QOC0+ukX9lacbRNybcyky2aFXb49VxO83y6qsBFAs7TX5Vy12ycwb8u+H2+idUgaEj0o8/Yrc+k3rXxzzy0/E6RsRYB8HR9u+Ol1DtzgABjH7B46O3V+sTiFuFxKPWKnQP6lJG78RgIS24UFoK3VIvcZG98DGyYW5MTT6fU6MpJ4qNgPeTjAsH7n7Z/8tWV35xY7radf+OPfcn/EbPXM1UFovu7xytxVoYnf4ld+PzAEmwhNPnFi6WVEf0n8ocYeZ/eII7QR6EefshNdDOFsk9bhFM3qfXpmnqNunF0nAdcHeT3giEuhZ6RIuDdQGOIIs6jtBxtBAcAR61wNbFaR6qknRaciMzFdp1OnZuXYWr6dxYSohJSSk2HWBw3hyzhqninISlhASgYpHsJ0C1q9pXAcYATbo72BScTmEXutauBXknlFUnxJsLm3BbcBctwJG60n4YxRmvJKM7MPWBcOoINjqD3w6vpHFL4kmKDs/M114IaFk6mKPsbT6Ym6khSuJ8eNI6OUZG6AkfD8Yep0lOJIWgG/jsjaH5PkFCn6dgR7Pjxxh1pbKy24LEZjzx58rMKlXkuoNiInmP25Itz0lg81iLZ4W17x+sUSuN1hkuYhwWK0j1kqH/Yjjf20xvp3d5ZTuKxJxLajxuMW1d14qcwtU1T2uiJT0qSHN8LGY6oIHcYUiXaUegdCiSSbkrKTc4JbGo5w45uKKCOt6xBOJt7bpyCRmERU5pW0k4KfKqJZQd5a7YKVx5DRI0GMbT1FLTSadLmyRoDce73YfEaRJyy5yYQwjNRihUmXo0kltAsbYmJ2tVGuTiqdQsEpwU5oOQz+OOOXGJn5PS42HJmaWtwkXNzbE2Od4f2Vq9CT5RSZkrA9hWII8cLRQa61WWTdO66nBSTmD+XD/Yj5Q6AhCRU5dNtFePGHnj0FErbtKdAzQTiIfprVUIqlHc6N8Y4am3IYHnr3xNbU1WQQUTDO499tJsFW+0nFCueUS21z0y6y7UHAEsrSsJQgDfNxe5GFwOML25pqmR0DbiVHNKd1O8ScyvFXwEFNY2hAYKRLy5PqjAqtxJxKv6iBwidqUrQGfJaf63HXnvaHt/1Drinlla8zGwUsiYrCSvIePwja6fXI0d1xs2UQAO1Rt3XvGyNKapVKaSkdZQCj2mJ6ZZl0J6ZQGIz5EXi6VAFOUVeXFG2ml5lkWS/dKhxOY77d8V6VTOU19ki90nx8fPHoZWdmJJQWwoiJ+qTdTUFTK962XART3Zdl8LmU3SLYe8Xv7rwNpaRJ/wAKxc5ZBOGh1xBif2nnZwFKTug5215wpSlneUbn5vk+fQzVwF6iNt2FTFEd3Bimx+BBPdGzk61UKWw8g+yAe0ZxWKZLVFCA+L2NviQDDbSWkBCchhG0byZ/aKRkm8S3dauWGHfaKs8iWkHnVZJSfzg4+cPqFMnVU+bbmU+yYkpuXrEklxGKVDHx47oR5dsPNLU0guSijewzR+ng83duaLMsJcQ7qm41GIif2+llXlqQkvOnKwwHMnhGzlEelVOVCoK3ph3M6AfZHIeMhf5Ra4mWlP2a0eu5nyH6/n54+o7LbWO0Fzo3Os0dOEObZUVcuXS6kndJ3Try7fFoqzzExMqdZTYEnKPk+RLtU9xzAdc5i2g11/CNodt5OloLcsd93gMh2xPTr9RmFTMwq6leePqiJyZbbLSHCEnQE2jP0A9CATl82O5yvG8TYHSHUlKiSbwhO8cfTj69eLxeLxeLxeLxeLxeL/NeLxeLxeL/AD3i/wDLL//Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="14"/>
       <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,51 +197,56 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -325,27 +436,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="39.71"/>
-    <col customWidth="1" min="2" max="2" width="22.57"/>
-    <col customWidth="1" min="3" max="3" width="27.29"/>
-    <col customWidth="1" min="4" max="4" width="17.86"/>
-    <col customWidth="1" min="6" max="6" width="51.0"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -365,7 +481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -376,36 +492,196 @@
         <v>8</v>
       </c>
       <c r="D2" s="4">
-        <v>969.0</v>
+        <v>419</v>
       </c>
       <c r="E2" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="4">
+        <v>89</v>
+      </c>
+      <c r="E3" s="4">
+        <v>21</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4">
-        <v>89.0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6">
+        <v>21.45</v>
+      </c>
+      <c r="E4" s="6">
+        <v>21</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6">
+        <v>29.9</v>
+      </c>
+      <c r="E5" s="6">
+        <v>21</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6">
+        <v>927</v>
+      </c>
+      <c r="E6" s="6">
+        <v>21</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6">
+        <v>379</v>
+      </c>
+      <c r="E7" s="6">
+        <v>21</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="6">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6">
+        <v>21</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6">
+        <v>280</v>
+      </c>
+      <c r="E9" s="6">
+        <v>21</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="6">
+        <v>387.95</v>
+      </c>
+      <c r="E10" s="6">
+        <v>21</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6">
+        <v>24.49</v>
+      </c>
+      <c r="E11" s="6">
+        <v>21</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>